<commit_message>
feat: correction de certaines disciplines
</commit_message>
<xml_diff>
--- a/content/personnel/liste-personnel.xlsx
+++ b/content/personnel/liste-personnel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projets\coquille-web\content\personnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF7AB39-CBC2-4F71-8C54-C01F8AF368A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E9CB65-25B0-4A0F-9C50-E1AF9F0F9A28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -327,9 +327,6 @@
     <t>caroline-pateneaude.jpg</t>
   </si>
   <si>
-    <t>Sociologie, anthropologie,  données statistiques</t>
-  </si>
-  <si>
     <t>514 343-6111, poste 5239</t>
   </si>
   <si>
@@ -609,9 +606,6 @@
     <t>emilie-dalpe.jpg</t>
   </si>
   <si>
-    <t>Littératures de langue française, littératures et langues du monde, culture québécoise</t>
-  </si>
-  <si>
     <t>514 343-6111, poste 2628</t>
   </si>
   <si>
@@ -996,9 +990,6 @@
     <t>Julia</t>
   </si>
   <si>
-    <t>Science politique, démographie, coopération internationale</t>
-  </si>
-  <si>
     <t>514 343-6111, poste 2623</t>
   </si>
   <si>
@@ -1512,9 +1503,6 @@
     <t>nino-gabrielli.jpg</t>
   </si>
   <si>
-    <t>Études religieuses, études classiques et médiévales, philosophie et études asiatiques</t>
-  </si>
-  <si>
     <t>514 343-6111, poste 2627</t>
   </si>
   <si>
@@ -1990,6 +1978,18 @@
   </si>
   <si>
     <t>Sciences de l’éducation, didacthèque</t>
+  </si>
+  <si>
+    <t>Sociologie, anthropologie,  données statistiques, études autochtones, études féministes</t>
+  </si>
+  <si>
+    <t>Littératures de langue française, littératures et langues du monde, littérature comparée, études anglaises, études allemandes, études hispaniques</t>
+  </si>
+  <si>
+    <t>Science politique, démographie et sciences de la population, études internationales</t>
+  </si>
+  <si>
+    <t>Études religieuses, études classiques, études médiévales, philosophie, études asiatiques</t>
   </si>
 </sst>
 </file>
@@ -2594,8 +2594,8 @@
   <dimension ref="A1:I105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C91" sqref="C91"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2612,31 +2612,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>633</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>634</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="G1" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>637</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>636</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>635</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>638</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>639</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>640</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2653,7 +2653,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>4</v>
@@ -2959,7 +2959,7 @@
         <v>89</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9" t="s">
@@ -3014,30 +3014,30 @@
         <v>11</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>100</v>
+        <v>651</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G15" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="H15" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="I15" s="18" t="s">
         <v>102</v>
-      </c>
-      <c r="I15" s="18" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="C16" s="11" t="s">
         <v>105</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>106</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>22</v>
@@ -3049,204 +3049,204 @@
         <v>32</v>
       </c>
       <c r="G16" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H16" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="I16" s="11" t="s">
         <v>108</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>110</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>111</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="H17" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="H17" s="9" t="s">
+      <c r="I17" s="9" t="s">
         <v>115</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13" t="s">
         <v>24</v>
       </c>
       <c r="G18" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H18" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="H18" s="13" t="s">
+      <c r="I18" s="13" t="s">
         <v>120</v>
-      </c>
-      <c r="I18" s="13" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="4" customFormat="1">
       <c r="A19" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>122</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>123</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>69</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="I19" s="18" t="s">
         <v>125</v>
-      </c>
-      <c r="I19" s="18" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="E20" s="11" t="s">
         <v>130</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>131</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>62</v>
       </c>
       <c r="G20" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H20" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="I20" s="11" t="s">
         <v>133</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="C21" s="9" t="s">
         <v>136</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>137</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="G21" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="H21" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="I21" s="9" t="s">
         <v>141</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="C22" s="11" t="s">
         <v>144</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>145</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>47</v>
       </c>
       <c r="G22" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="H22" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="I22" s="11" t="s">
         <v>148</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="C23" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="D23" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="E23" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="F23" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="G23" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="H23" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="H23" s="9" t="s">
+      <c r="I23" s="9" t="s">
         <v>157</v>
-      </c>
-      <c r="I23" s="9" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -3254,96 +3254,96 @@
         <v>97</v>
       </c>
       <c r="B24" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>160</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F24" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G24" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="H24" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="I24" s="13" t="s">
         <v>163</v>
-      </c>
-      <c r="I24" s="13" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>167</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>168</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>69</v>
       </c>
       <c r="G25" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="H25" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="H25" s="17" t="s">
+      <c r="I25" s="17" t="s">
         <v>170</v>
-      </c>
-      <c r="I25" s="17" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="C26" s="11" t="s">
         <v>173</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>174</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F26" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="H26" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="H26" s="11" t="s">
+      <c r="I26" s="11" t="s">
         <v>177</v>
-      </c>
-      <c r="I26" s="11" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>179</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>180</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="9" t="s">
@@ -3353,716 +3353,716 @@
         <v>5</v>
       </c>
       <c r="H27" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="I27" s="9" t="s">
         <v>181</v>
-      </c>
-      <c r="I27" s="9" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="C28" s="11" t="s">
         <v>184</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>185</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="F28" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="G28" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="H28" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="H28" s="11" t="s">
+      <c r="I28" s="11" t="s">
         <v>189</v>
-      </c>
-      <c r="I28" s="11" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="C29" s="9" t="s">
         <v>192</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>193</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>194</v>
+        <v>652</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G29" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="I29" s="9" t="s">
         <v>195</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="I29" s="9" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="11" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F30" s="11" t="s">
         <v>83</v>
       </c>
       <c r="G30" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="I30" s="16" t="s">
         <v>201</v>
-      </c>
-      <c r="H30" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="I30" s="16" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="D31" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="E31" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="F31" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G31" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="H31" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="F31" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="G31" s="9" t="s">
+      <c r="I31" s="9" t="s">
         <v>209</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="C32" s="11" t="s">
         <v>212</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>214</v>
       </c>
       <c r="D32" s="11" t="s">
         <v>55</v>
       </c>
       <c r="E32" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="H32" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F32" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="G32" s="11" t="s">
+      <c r="I32" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="H32" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="I32" s="11" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="9" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B33" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>219</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>221</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>55</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F33" s="9" t="s">
         <v>62</v>
       </c>
       <c r="G33" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="I33" s="18" t="s">
         <v>223</v>
-      </c>
-      <c r="H33" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="I33" s="18" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="H34" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="I34" s="11" t="s">
         <v>229</v>
-      </c>
-      <c r="H34" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="I34" s="11" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="C35" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="D35" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="C35" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>235</v>
-      </c>
       <c r="E35" s="10" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="F35" s="18" t="s">
         <v>24</v>
       </c>
       <c r="G35" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="H35" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="I35" s="18" t="s">
         <v>236</v>
-      </c>
-      <c r="H35" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="I35" s="18" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="D36" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E36" s="15" t="s">
         <v>240</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>242</v>
       </c>
       <c r="F36" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G36" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="I36" s="16" t="s">
         <v>243</v>
-      </c>
-      <c r="H36" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="I36" s="16" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="C37" s="9" t="s">
         <v>246</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>248</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>83</v>
       </c>
       <c r="G37" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="I37" s="9" t="s">
         <v>250</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="I37" s="9" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="C38" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="D38" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="E38" s="11" t="s">
         <v>255</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>257</v>
       </c>
       <c r="F38" s="11" t="s">
         <v>83</v>
       </c>
       <c r="G38" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="I38" s="11" t="s">
         <v>258</v>
-      </c>
-      <c r="H38" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="I38" s="11" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="C39" s="18" t="s">
         <v>261</v>
-      </c>
-      <c r="B39" s="18" t="s">
-        <v>262</v>
-      </c>
-      <c r="C39" s="18" t="s">
-        <v>263</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E39" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="G39" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="F39" s="18" t="s">
+      <c r="H39" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="G39" s="18" t="s">
+      <c r="I39" s="18" t="s">
         <v>266</v>
-      </c>
-      <c r="H39" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="I39" s="18" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="C40" s="11" t="s">
         <v>269</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>271</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E40" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="G40" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="F40" s="11" t="s">
+      <c r="H40" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="G40" s="11" t="s">
+      <c r="I40" s="11" t="s">
         <v>274</v>
-      </c>
-      <c r="H40" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="I40" s="11" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="D41" s="9" t="s">
         <v>278</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>280</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="H41" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="I41" s="9" t="s">
         <v>282</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="I41" s="9" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E42" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="G42" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="F42" s="11" t="s">
+      <c r="H42" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="G42" s="11" t="s">
+      <c r="I42" s="11" t="s">
         <v>289</v>
-      </c>
-      <c r="H42" s="11" t="s">
-        <v>290</v>
-      </c>
-      <c r="I42" s="11" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="9" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F43" s="9" t="s">
         <v>62</v>
       </c>
       <c r="G43" s="9"/>
       <c r="H43" s="17" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I43" s="17" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="C44" s="11" t="s">
         <v>297</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>298</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>299</v>
       </c>
       <c r="D44" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="F44" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="H44" s="11" t="s">
         <v>300</v>
       </c>
-      <c r="G44" s="11" t="s">
+      <c r="I44" s="11" t="s">
         <v>301</v>
-      </c>
-      <c r="H44" s="11" t="s">
-        <v>302</v>
-      </c>
-      <c r="I44" s="11" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="9" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="F45" s="9" t="s">
         <v>62</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="H45" s="9"/>
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="11" t="s">
         <v>51</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="F46" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="H46" s="16" t="s">
+        <v>642</v>
+      </c>
+      <c r="I46" s="11" t="s">
         <v>306</v>
-      </c>
-      <c r="G46" s="11" t="s">
-        <v>307</v>
-      </c>
-      <c r="H46" s="16" t="s">
-        <v>646</v>
-      </c>
-      <c r="I46" s="11" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>309</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>311</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G47" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="I47" s="9" t="s">
         <v>312</v>
-      </c>
-      <c r="H47" s="9" t="s">
-        <v>313</v>
-      </c>
-      <c r="I47" s="9" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="13" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C48" s="13"/>
       <c r="D48" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E48" s="13"/>
       <c r="F48" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="G48" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="H48" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="G48" s="13" t="s">
+      <c r="I48" s="13" t="s">
         <v>318</v>
-      </c>
-      <c r="H48" s="13" t="s">
-        <v>319</v>
-      </c>
-      <c r="I48" s="13" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C49" s="9"/>
       <c r="D49" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>323</v>
+        <v>653</v>
       </c>
       <c r="F49" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="I49" s="9" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="11" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>22</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="F50" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="H50" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="I50" s="11" t="s">
         <v>330</v>
-      </c>
-      <c r="G50" s="11" t="s">
-        <v>331</v>
-      </c>
-      <c r="H50" s="11" t="s">
-        <v>332</v>
-      </c>
-      <c r="I50" s="11" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="9" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C51" s="9"/>
       <c r="D51" s="9" t="s">
         <v>55</v>
       </c>
       <c r="E51" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="H51" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="I51" s="9" t="s">
         <v>336</v>
-      </c>
-      <c r="F51" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="G51" s="9" t="s">
-        <v>337</v>
-      </c>
-      <c r="H51" s="9" t="s">
-        <v>338</v>
-      </c>
-      <c r="I51" s="9" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="11" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D52" s="11" t="s">
         <v>55</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F52" s="11" t="s">
         <v>83</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="9" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>3</v>
@@ -4074,273 +4074,273 @@
         <v>83</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="H53" s="9" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="I53" s="9" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="11" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C54" s="11"/>
       <c r="D54" s="11" t="s">
         <v>55</v>
       </c>
       <c r="E54" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="G54" s="11" t="s">
+        <v>352</v>
+      </c>
+      <c r="H54" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="I54" s="11" t="s">
         <v>354</v>
-      </c>
-      <c r="F54" s="11" t="s">
-        <v>281</v>
-      </c>
-      <c r="G54" s="11" t="s">
-        <v>355</v>
-      </c>
-      <c r="H54" s="11" t="s">
-        <v>356</v>
-      </c>
-      <c r="I54" s="11" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="9" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C55" s="9"/>
       <c r="D55" s="9" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="E55" s="19"/>
       <c r="F55" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G55" s="18" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="I55" s="17" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="11" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C56" s="11"/>
       <c r="D56" s="11" t="s">
+        <v>363</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>364</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="H56" s="11" t="s">
         <v>366</v>
       </c>
-      <c r="E56" s="11" t="s">
+      <c r="I56" s="11" t="s">
         <v>367</v>
-      </c>
-      <c r="F56" s="11" t="s">
-        <v>317</v>
-      </c>
-      <c r="G56" s="11" t="s">
-        <v>368</v>
-      </c>
-      <c r="H56" s="11" t="s">
-        <v>369</v>
-      </c>
-      <c r="I56" s="11" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="9" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="H57" s="9" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="I57" s="9" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="11" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C58" s="11"/>
       <c r="D58" s="11" t="s">
         <v>51</v>
       </c>
       <c r="E58" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>378</v>
+      </c>
+      <c r="H58" s="11" t="s">
         <v>379</v>
       </c>
-      <c r="F58" s="11" t="s">
+      <c r="I58" s="11" t="s">
         <v>380</v>
-      </c>
-      <c r="G58" s="11" t="s">
-        <v>381</v>
-      </c>
-      <c r="H58" s="11" t="s">
-        <v>382</v>
-      </c>
-      <c r="I58" s="11" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="E59" s="10" t="s">
         <v>384</v>
-      </c>
-      <c r="B59" s="9" t="s">
-        <v>385</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>386</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="E59" s="10" t="s">
-        <v>387</v>
       </c>
       <c r="F59" s="9" t="s">
         <v>4</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="H59" s="9" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="I59" s="9" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="11" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D60" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E60" s="15" t="s">
+        <v>391</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="G60" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="H60" s="13" t="s">
+        <v>393</v>
+      </c>
+      <c r="I60" s="13" t="s">
         <v>394</v>
-      </c>
-      <c r="F60" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="G60" s="13" t="s">
-        <v>395</v>
-      </c>
-      <c r="H60" s="13" t="s">
-        <v>396</v>
-      </c>
-      <c r="I60" s="13" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="E61" s="19" t="s">
         <v>398</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>399</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>400</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="E61" s="19" t="s">
-        <v>401</v>
       </c>
       <c r="F61" s="9" t="s">
         <v>62</v>
       </c>
       <c r="G61" s="9"/>
       <c r="H61" s="9" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="I61" s="9" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="11" t="s">
+        <v>401</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>402</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>403</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E62" s="15" t="s">
         <v>404</v>
-      </c>
-      <c r="B62" s="11" t="s">
-        <v>405</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>406</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="E62" s="15" t="s">
-        <v>407</v>
       </c>
       <c r="F62" s="11" t="s">
         <v>62</v>
       </c>
       <c r="G62" s="11" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="H62" s="11" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="I62" s="11" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="9" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D63" s="9" t="s">
         <v>3</v>
@@ -4352,311 +4352,311 @@
         <v>62</v>
       </c>
       <c r="G63" s="18" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H63" s="18" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="I63" s="18" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>415</v>
+      </c>
+      <c r="D64" s="11" t="s">
         <v>416</v>
       </c>
-      <c r="B64" s="11" t="s">
+      <c r="E64" s="14" t="s">
         <v>417</v>
       </c>
-      <c r="C64" s="11" t="s">
+      <c r="F64" s="11" t="s">
+        <v>417</v>
+      </c>
+      <c r="G64" s="13" t="s">
         <v>418</v>
       </c>
-      <c r="D64" s="11" t="s">
+      <c r="H64" s="13" t="s">
         <v>419</v>
       </c>
-      <c r="E64" s="14" t="s">
+      <c r="I64" s="11" t="s">
         <v>420</v>
-      </c>
-      <c r="F64" s="11" t="s">
-        <v>420</v>
-      </c>
-      <c r="G64" s="13" t="s">
-        <v>421</v>
-      </c>
-      <c r="H64" s="13" t="s">
-        <v>422</v>
-      </c>
-      <c r="I64" s="11" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="4" customFormat="1">
       <c r="A65" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="E65" s="19" t="s">
         <v>424</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>425</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>426</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="E65" s="19" t="s">
-        <v>427</v>
       </c>
       <c r="F65" s="9" t="s">
         <v>62</v>
       </c>
       <c r="G65" s="18"/>
       <c r="H65" s="17" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="I65" s="18" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="11" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="D66" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="H66" s="11" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="I66" s="11" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="5" customFormat="1">
       <c r="A67" s="9" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C67" s="9"/>
       <c r="D67" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="F67" s="9" t="s">
         <v>62</v>
       </c>
       <c r="G67" s="9" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="H67" s="9" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="I67" s="9" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="11" t="s">
+        <v>438</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>439</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="E68" s="11" t="s">
         <v>441</v>
-      </c>
-      <c r="B68" s="11" t="s">
-        <v>442</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>443</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="E68" s="11" t="s">
-        <v>444</v>
       </c>
       <c r="F68" s="11" t="s">
         <v>62</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="H68" s="11" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="I68" s="11" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="9" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D69" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="H69" s="9" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="I69" s="9" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="11" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="D70" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="F70" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="G70" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="H70" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="I70" s="20" t="s">
         <v>457</v>
-      </c>
-      <c r="G70" s="11" t="s">
-        <v>458</v>
-      </c>
-      <c r="H70" s="11" t="s">
-        <v>459</v>
-      </c>
-      <c r="I70" s="20" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="9" t="s">
+        <v>458</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="E71" s="19" t="s">
         <v>461</v>
-      </c>
-      <c r="B71" s="9" t="s">
-        <v>462</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>463</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="E71" s="19" t="s">
-        <v>464</v>
       </c>
       <c r="F71" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="H71" s="9" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="I71" s="9" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="11" t="s">
+        <v>465</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="C72" s="11" t="s">
+        <v>467</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="E72" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="F72" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="G72" s="11" t="s">
         <v>468</v>
       </c>
-      <c r="B72" s="11" t="s">
+      <c r="H72" s="11" t="s">
         <v>469</v>
       </c>
-      <c r="C72" s="11" t="s">
+      <c r="I72" s="11" t="s">
         <v>470</v>
-      </c>
-      <c r="D72" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="E72" s="15" t="s">
-        <v>281</v>
-      </c>
-      <c r="F72" s="11" t="s">
-        <v>281</v>
-      </c>
-      <c r="G72" s="11" t="s">
-        <v>471</v>
-      </c>
-      <c r="H72" s="11" t="s">
-        <v>472</v>
-      </c>
-      <c r="I72" s="11" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="18" t="s">
+        <v>471</v>
+      </c>
+      <c r="B73" s="18" t="s">
+        <v>472</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>473</v>
+      </c>
+      <c r="D73" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="E73" s="18" t="s">
         <v>474</v>
       </c>
-      <c r="B73" s="18" t="s">
+      <c r="F73" s="18" t="s">
+        <v>647</v>
+      </c>
+      <c r="G73" s="18" t="s">
         <v>475</v>
       </c>
-      <c r="C73" s="9" t="s">
+      <c r="H73" s="18" t="s">
         <v>476</v>
       </c>
-      <c r="D73" s="18" t="s">
-        <v>379</v>
-      </c>
-      <c r="E73" s="18" t="s">
+      <c r="I73" s="18" t="s">
         <v>477</v>
-      </c>
-      <c r="F73" s="18" t="s">
-        <v>651</v>
-      </c>
-      <c r="G73" s="18" t="s">
-        <v>478</v>
-      </c>
-      <c r="H73" s="18" t="s">
-        <v>479</v>
-      </c>
-      <c r="I73" s="18" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="4" customFormat="1">
       <c r="A74" s="11" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C74" s="11"/>
       <c r="D74" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E74" s="11" t="s">
         <v>56</v>
@@ -4665,429 +4665,429 @@
         <v>83</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="H74" s="11" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="I74" s="11" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="9" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F75" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="H75" s="17" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="I75" s="17" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="11" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D76" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E76" s="15" t="s">
-        <v>495</v>
+        <v>654</v>
       </c>
       <c r="F76" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="H76" s="11" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="I76" s="11" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="77" spans="1:9" s="4" customFormat="1">
       <c r="A77" s="9" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D77" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="F77" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G77" s="9" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="H77" s="9" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="I77" s="9" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="11" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="F78" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="H78" s="11" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="I78" s="11" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="9" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D79" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="F79" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G79" s="9" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="H79" s="9" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="I79" s="12" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="11" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="D80" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E80" s="15" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="F80" s="11" t="s">
         <v>69</v>
       </c>
       <c r="G80" s="11" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="H80" s="11" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="I80" s="11" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="9" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="D81" s="9" t="s">
         <v>55</v>
       </c>
       <c r="E81" s="19" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="F81" s="9" t="s">
         <v>62</v>
       </c>
       <c r="G81" s="9"/>
       <c r="H81" s="17" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="I81" s="17" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="11" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D82" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E82" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F82" s="11" t="s">
         <v>69</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="H82" s="11" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="I82" s="11" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" s="9" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="C83" s="9"/>
       <c r="D83" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="G83" s="9" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="H83" s="9" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="I83" s="9" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="11" t="s">
+        <v>541</v>
+      </c>
+      <c r="B84" s="11" t="s">
+        <v>542</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>543</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>416</v>
+      </c>
+      <c r="E84" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="F84" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="G84" s="11" t="s">
+        <v>544</v>
+      </c>
+      <c r="H84" s="11" t="s">
         <v>545</v>
       </c>
-      <c r="B84" s="11" t="s">
+      <c r="I84" s="11" t="s">
         <v>546</v>
-      </c>
-      <c r="C84" s="11" t="s">
-        <v>547</v>
-      </c>
-      <c r="D84" s="11" t="s">
-        <v>419</v>
-      </c>
-      <c r="E84" s="15" t="s">
-        <v>317</v>
-      </c>
-      <c r="F84" s="11" t="s">
-        <v>317</v>
-      </c>
-      <c r="G84" s="11" t="s">
-        <v>548</v>
-      </c>
-      <c r="H84" s="11" t="s">
-        <v>549</v>
-      </c>
-      <c r="I84" s="11" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B85" s="9" t="s">
+        <v>547</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>548</v>
+      </c>
+      <c r="D85" s="9" t="s">
+        <v>549</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G85" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H85" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="I85" s="9" t="s">
         <v>551</v>
-      </c>
-      <c r="C85" s="9" t="s">
-        <v>552</v>
-      </c>
-      <c r="D85" s="9" t="s">
-        <v>553</v>
-      </c>
-      <c r="E85" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="F85" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="G85" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="H85" s="9" t="s">
-        <v>554</v>
-      </c>
-      <c r="I85" s="9" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" s="11" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="D86" s="11" t="s">
         <v>22</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="F86" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="H86" s="11" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="I86" s="11" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="9" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="D87" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="F87" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G87" s="18" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="H87" s="18" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="I87" s="18" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="11" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="F88" s="11" t="s">
         <v>4</v>
       </c>
       <c r="G88" s="11" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="H88" s="11" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="I88" s="11" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" s="9" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E89" s="9" t="s">
         <v>76</v>
@@ -5096,338 +5096,338 @@
         <v>4</v>
       </c>
       <c r="G89" s="9" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="H89" s="9" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="I89" s="9" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="11" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="D90" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E90" s="15" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="F90" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="H90" s="11" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="I90" s="11" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" s="9" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="D91" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E91" s="19" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="F91" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G91" s="9" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="H91" s="9" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="I91" s="9" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="11" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="B92" s="11" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="D92" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E92" s="11" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="F92" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G92" s="13" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="I92" s="11" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" s="9" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="D93" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E93" s="19" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="F93" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G93" s="18" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="H93" s="18" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="I93" s="18" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
     <row r="94" spans="1:9" s="4" customFormat="1">
       <c r="A94" s="11" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E94" s="15" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="F94" s="11" t="s">
         <v>62</v>
       </c>
       <c r="G94" s="11"/>
       <c r="H94" s="11" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="I94" s="11" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
     </row>
     <row r="95" spans="1:9" s="4" customFormat="1">
       <c r="A95" s="9" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="D95" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="F95" s="9" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="G95" s="9" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="H95" s="9" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="I95" s="9" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" s="13" t="s">
+        <v>619</v>
+      </c>
+      <c r="B96" s="13" t="s">
+        <v>613</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="D96" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="E96" s="13" t="s">
+        <v>621</v>
+      </c>
+      <c r="F96" s="13" t="s">
+        <v>622</v>
+      </c>
+      <c r="G96" s="13" t="s">
         <v>623</v>
       </c>
-      <c r="B96" s="13" t="s">
-        <v>617</v>
-      </c>
-      <c r="C96" s="11" t="s">
+      <c r="H96" s="13" t="s">
         <v>624</v>
       </c>
-      <c r="D96" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="E96" s="13" t="s">
+      <c r="I96" s="13" t="s">
         <v>625</v>
-      </c>
-      <c r="F96" s="13" t="s">
-        <v>626</v>
-      </c>
-      <c r="G96" s="13" t="s">
-        <v>627</v>
-      </c>
-      <c r="H96" s="13" t="s">
-        <v>628</v>
-      </c>
-      <c r="I96" s="13" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="97" spans="1:9" s="4" customFormat="1">
       <c r="A97" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="B97" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="D97" t="s">
         <v>11</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="F97" t="s">
         <v>13</v>
       </c>
       <c r="G97" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="H97" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="I97" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="98" spans="1:9">
       <c r="A98" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="B98" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="D98" t="s">
         <v>11</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="F98" t="s">
         <v>13</v>
       </c>
       <c r="G98" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="H98" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="I98" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="99" spans="1:9">
       <c r="A99" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="B99" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="D99" t="s">
         <v>11</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="F99" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="H99" s="4" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="I99" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
     </row>
     <row r="100" spans="1:9">
       <c r="A100" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="B100" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="D100" t="s">
         <v>11</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="F100" t="s">
         <v>32</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="H100" s="4" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="I100" s="4" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
     <row r="101" spans="1:9" s="5" customFormat="1">
       <c r="A101" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="B101" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="C101" s="8"/>
       <c r="D101" t="s">
@@ -5440,117 +5440,117 @@
         <v>13</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="H101" s="4" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="I101" s="4" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
     </row>
     <row r="102" spans="1:9">
       <c r="A102" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="B102" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="D102" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="F102" t="s">
         <v>62</v>
       </c>
       <c r="H102" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="I102" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
     </row>
     <row r="103" spans="1:9">
       <c r="A103" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="B103" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="D103" t="s">
         <v>11</v>
       </c>
       <c r="E103" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="F103" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="G103" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="H103" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="I103" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>613</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>620</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E104" s="21" t="s">
+        <v>621</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>622</v>
+      </c>
+      <c r="G104" s="4" t="s">
         <v>623</v>
       </c>
-      <c r="B104" s="4" t="s">
-        <v>617</v>
-      </c>
-      <c r="C104" s="7" t="s">
+      <c r="H104" s="4" t="s">
         <v>624</v>
       </c>
-      <c r="D104" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="E104" s="21" t="s">
+      <c r="I104" s="4" t="s">
         <v>625</v>
-      </c>
-      <c r="F104" s="4" t="s">
-        <v>626</v>
-      </c>
-      <c r="G104" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="H104" s="4" t="s">
-        <v>628</v>
-      </c>
-      <c r="I104" s="4" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="105" spans="1:9">
       <c r="A105" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="B105" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D105" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E105" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="F105" t="s">
         <v>62</v>
       </c>
       <c r="G105" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
   </sheetData>
@@ -5581,26 +5581,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f6670ae2-8190-4e72-909e-d717fe03ced5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="00db0817-461a-4a69-8eb5-8daf0756d296" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007812637FDE95774892D21861907C1625" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="9e26b686a71b543072340cfd27a56c29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f6670ae2-8190-4e72-909e-d717fe03ced5" xmlns:ns3="00db0817-461a-4a69-8eb5-8daf0756d296" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8d151e41c23af60827e9e8828a6e0ebd" ns2:_="" ns3:_="">
     <xsd:import namespace="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
@@ -5835,10 +5815,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f6670ae2-8190-4e72-909e-d717fe03ced5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="00db0817-461a-4a69-8eb5-8daf0756d296" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{141ACCEB-C60B-4854-82C0-9885432D8ACB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
+    <ds:schemaRef ds:uri="00db0817-461a-4a69-8eb5-8daf0756d296"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5861,20 +5872,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{141ACCEB-C60B-4854-82C0-9885432D8ACB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
-    <ds:schemaRef ds:uri="00db0817-461a-4a69-8eb5-8daf0756d296"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: Mise à jour personnel
</commit_message>
<xml_diff>
--- a/content/personnel/liste-personnel.xlsx
+++ b/content/personnel/liste-personnel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projets\coquille-web\content\personnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E9CB65-25B0-4A0F-9C50-E1AF9F0F9A28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA4E192-E17C-4902-867A-9C2178882272}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="661">
   <si>
     <t>Borsi</t>
   </si>
@@ -852,30 +852,12 @@
     <t>https://teams.microsoft.com/l/chat/0/0?users=graham.lavender@umontreal.ca</t>
   </si>
   <si>
-    <t>Viart</t>
-  </si>
-  <si>
-    <t>Guillaume</t>
-  </si>
-  <si>
-    <t>guillaume-viart.jpg</t>
-  </si>
-  <si>
-    <t>Technicien en coordination du travail de bureau</t>
-  </si>
-  <si>
     <t>Direction de l'engagement et de l'innovation sociale</t>
   </si>
   <si>
     <t>514 343-6111, poste 1049</t>
   </si>
   <si>
-    <t>guillaume.viart@umontreal.ca</t>
-  </si>
-  <si>
-    <t>https://teams.microsoft.com/l/chat/0/0?users=guillaume.viart@umontreal.ca</t>
-  </si>
-  <si>
     <t>Brazeau</t>
   </si>
   <si>
@@ -1074,12 +1056,6 @@
     <t>https://teams.microsoft.com/l/chat/0/0?users=khalid.jouamaa@umontreal.ca</t>
   </si>
   <si>
-    <t>Gignac</t>
-  </si>
-  <si>
-    <t>Laurie-Anne</t>
-  </si>
-  <si>
     <t>Expérience utilisateur</t>
   </si>
   <si>
@@ -1990,6 +1966,48 @@
   </si>
   <si>
     <t>Études religieuses, études classiques, études médiévales, philosophie, études asiatiques</t>
+  </si>
+  <si>
+    <t>Marie-Pierre</t>
+  </si>
+  <si>
+    <t>Gadoua</t>
+  </si>
+  <si>
+    <t>marie-pierre.gadoua@umontreal.ca</t>
+  </si>
+  <si>
+    <t>Conseillère</t>
+  </si>
+  <si>
+    <t>Engagement et en innovation sociale</t>
+  </si>
+  <si>
+    <t>François-Xavier</t>
+  </si>
+  <si>
+    <t>Panaccio</t>
+  </si>
+  <si>
+    <t>Technopédagoque</t>
+  </si>
+  <si>
+    <t>francois-xavier.panaccio@umontreal.ca</t>
+  </si>
+  <si>
+    <t>Vanessa</t>
+  </si>
+  <si>
+    <t>Technicienne en coordination de travail de bureau</t>
+  </si>
+  <si>
+    <t>vanessa.martin.2@umontreal.ca</t>
+  </si>
+  <si>
+    <t>Poste</t>
+  </si>
+  <si>
+    <t>vacant</t>
   </si>
 </sst>
 </file>
@@ -2164,7 +2182,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2191,6 +2209,9 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -2244,16 +2265,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A0AF7E1-A614-44BF-8C48-5C26377DC552}" name="Tableau1" displayName="Tableau1" ref="A1:I105" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:I105" xr:uid="{4F6A1D8F-9220-4675-A202-2173F3493722}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A0AF7E1-A614-44BF-8C48-5C26377DC552}" name="Tableau1" displayName="Tableau1" ref="A1:I107" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:I107" xr:uid="{4F6A1D8F-9220-4675-A202-2173F3493722}">
     <filterColumn colId="5">
       <filters>
         <filter val="Direction de la recherche et des initiatives numériques"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState ref="A2:I104">
-    <sortCondition ref="B1:B104"/>
+  <sortState ref="A2:I106">
+    <sortCondition ref="B1:B106"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4B04E1AF-0079-4AD2-81CA-E8A433733E21}" name="nom"/>
@@ -2591,11 +2612,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:I107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E61" sqref="E61"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2612,31 +2633,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>625</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>629</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>633</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>632</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>631</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>634</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>635</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>636</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2653,7 +2674,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>4</v>
@@ -3014,7 +3035,7 @@
         <v>11</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>32</v>
@@ -3402,7 +3423,7 @@
         <v>11</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>32</v>
@@ -3570,7 +3591,7 @@
         <v>233</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>639</v>
+        <v>631</v>
       </c>
       <c r="F35" s="18" t="s">
         <v>24</v>
@@ -3615,314 +3636,308 @@
       </c>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="11" t="s">
+        <v>653</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>652</v>
+      </c>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11" t="s">
+        <v>654</v>
+      </c>
+      <c r="E37" s="15"/>
+      <c r="F37" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11" t="s">
+        <v>655</v>
+      </c>
+      <c r="I37" s="23"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B38" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C38" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D38" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E38" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F38" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="G38" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="H37" s="9" t="s">
+      <c r="H38" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="I37" s="9" t="s">
+      <c r="I38" s="9" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="11" t="s">
+    <row r="39" spans="1:9">
+      <c r="A39" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B39" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C39" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D39" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E39" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F39" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="G38" s="11" t="s">
+      <c r="G39" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="H38" s="11" t="s">
+      <c r="H39" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="I38" s="11" t="s">
+      <c r="I39" s="11" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="18" t="s">
+    <row r="40" spans="1:9">
+      <c r="A40" s="18" t="s">
         <v>259</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="B40" s="18" t="s">
         <v>260</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="C40" s="18" t="s">
         <v>261</v>
       </c>
-      <c r="D39" s="9" t="s">
+      <c r="D40" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E39" s="18" t="s">
+      <c r="E40" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="F39" s="18" t="s">
+      <c r="F40" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="G39" s="18" t="s">
+      <c r="G40" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="H39" s="18" t="s">
+      <c r="H40" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="I39" s="18" t="s">
+      <c r="I40" s="18" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="11" t="s">
+    <row r="41" spans="1:9">
+      <c r="A41" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B41" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C41" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D41" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E40" s="11" t="s">
+      <c r="E41" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="F40" s="11" t="s">
+      <c r="F41" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="G40" s="11" t="s">
+      <c r="G41" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="H40" s="11" t="s">
+      <c r="H41" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="I40" s="11" t="s">
+      <c r="I41" s="11" t="s">
         <v>274</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="I41" s="9" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="11" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="9" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="9" t="s">
         <v>197</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="F43" s="9" t="s">
         <v>62</v>
       </c>
       <c r="G43" s="9"/>
       <c r="H43" s="17" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="I43" s="17" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="11" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="D44" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="9" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="9" t="s">
         <v>197</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
       <c r="F45" s="9" t="s">
         <v>62</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>628</v>
+        <v>620</v>
       </c>
       <c r="H45" s="9"/>
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="11" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="11" t="s">
         <v>51</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="H46" s="16" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="9" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
       <c r="F47" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="I47" s="9" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="13" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="C48" s="13"/>
       <c r="D48" s="13" t="s">
@@ -3930,116 +3945,116 @@
       </c>
       <c r="E48" s="13"/>
       <c r="F48" s="13" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="H48" s="13" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="I48" s="13" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="9" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C49" s="9"/>
       <c r="D49" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
       <c r="F49" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="I49" s="9" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="11" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>22</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="9" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="C51" s="9"/>
       <c r="D51" s="9" t="s">
         <v>55</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="H51" s="9" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="I51" s="9" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="11" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D52" s="11" t="s">
         <v>55</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="F52" s="11" t="s">
         <v>83</v>
@@ -4048,21 +4063,21 @@
         <v>199</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="9" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>3</v>
@@ -4074,1483 +4089,1529 @@
         <v>83</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="H53" s="9" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="I53" s="9" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="11" t="s">
-        <v>349</v>
+        <v>659</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>350</v>
+        <v>660</v>
       </c>
       <c r="C54" s="11"/>
       <c r="D54" s="11" t="s">
         <v>55</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="9" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="C55" s="9"/>
       <c r="D55" s="9" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="E55" s="19"/>
       <c r="F55" s="9" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="G55" s="18" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="I55" s="17" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="11" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="C56" s="11"/>
       <c r="D56" s="11" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="H56" s="11" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="I56" s="11" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="9" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
       <c r="F57" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="H57" s="9" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="I57" s="9" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="11" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="C58" s="11"/>
       <c r="D58" s="11" t="s">
         <v>51</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="9" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>254</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="F59" s="9" t="s">
         <v>4</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="H59" s="9" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="I59" s="9" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="11" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="D60" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E60" s="15" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="G60" s="13" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="H60" s="13" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="I60" s="13" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="9" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>197</v>
       </c>
       <c r="E61" s="19" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="F61" s="9" t="s">
         <v>62</v>
       </c>
       <c r="G61" s="9"/>
       <c r="H61" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="I61" s="9" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="9" t="s">
+        <v>648</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>647</v>
+      </c>
+      <c r="C62" s="17"/>
+      <c r="D62" s="9" t="s">
+        <v>650</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>651</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="G62" s="9"/>
+      <c r="H62" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="I62" s="22"/>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E63" s="15" t="s">
+        <v>396</v>
+      </c>
+      <c r="F63" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="H63" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="I63" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="I61" s="9" t="s">
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="9" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="62" spans="1:9">
-      <c r="A62" s="11" t="s">
+      <c r="B64" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B62" s="11" t="s">
+      <c r="C64" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="C62" s="11" t="s">
+      <c r="D64" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G64" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="H64" s="18" t="s">
         <v>403</v>
       </c>
-      <c r="D62" s="11" t="s">
+      <c r="I64" s="18" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="11" t="s">
+        <v>405</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>406</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>407</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>409</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="G65" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="H65" s="13" t="s">
+        <v>411</v>
+      </c>
+      <c r="I65" s="11" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" s="4" customFormat="1">
+      <c r="A66" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="D66" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="E62" s="15" t="s">
-        <v>404</v>
-      </c>
-      <c r="F62" s="11" t="s">
+      <c r="E66" s="19" t="s">
+        <v>416</v>
+      </c>
+      <c r="F66" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G62" s="11" t="s">
-        <v>405</v>
-      </c>
-      <c r="H62" s="11" t="s">
-        <v>406</v>
-      </c>
-      <c r="I62" s="11" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="9" t="s">
+      <c r="G66" s="18"/>
+      <c r="H66" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="I66" s="18" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" s="11" t="s">
+        <v>419</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="F67" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="H67" s="11" t="s">
+        <v>422</v>
+      </c>
+      <c r="I67" s="11" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" s="5" customFormat="1">
+      <c r="A68" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="F68" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G68" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="H68" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="I68" s="9" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" s="11" t="s">
+        <v>430</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>431</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>432</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>433</v>
+      </c>
+      <c r="F69" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G69" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="H69" s="11" t="s">
+        <v>435</v>
+      </c>
+      <c r="I69" s="11" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="F70" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="G70" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="H70" s="9" t="s">
+        <v>441</v>
+      </c>
+      <c r="I70" s="9" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>444</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>445</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E71" s="11" t="s">
+        <v>638</v>
+      </c>
+      <c r="F71" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="G71" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="H71" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="I71" s="20" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="9" t="s">
+        <v>450</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>451</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="H72" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="I72" s="9" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" s="11" t="s">
+        <v>457</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>459</v>
+      </c>
+      <c r="D73" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="E73" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="F73" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="G73" s="11" t="s">
+        <v>460</v>
+      </c>
+      <c r="H73" s="11" t="s">
+        <v>461</v>
+      </c>
+      <c r="I73" s="11" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" s="18" t="s">
+        <v>463</v>
+      </c>
+      <c r="B74" s="18" t="s">
+        <v>464</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D74" s="18" t="s">
+        <v>368</v>
+      </c>
+      <c r="E74" s="18" t="s">
+        <v>466</v>
+      </c>
+      <c r="F74" s="18" t="s">
+        <v>639</v>
+      </c>
+      <c r="G74" s="18" t="s">
+        <v>467</v>
+      </c>
+      <c r="H74" s="18" t="s">
+        <v>468</v>
+      </c>
+      <c r="I74" s="18" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" s="4" customFormat="1">
+      <c r="A75" s="11" t="s">
+        <v>470</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>471</v>
+      </c>
+      <c r="C75" s="11"/>
+      <c r="D75" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F75" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="G75" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="H75" s="11" t="s">
+        <v>473</v>
+      </c>
+      <c r="I75" s="11" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" s="9" t="s">
+        <v>475</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>477</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G76" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="H76" s="17" t="s">
+        <v>479</v>
+      </c>
+      <c r="I76" s="17" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" s="11" t="s">
+        <v>481</v>
+      </c>
+      <c r="B77" s="11" t="s">
+        <v>482</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>483</v>
+      </c>
+      <c r="D77" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77" s="15" t="s">
+        <v>646</v>
+      </c>
+      <c r="F77" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G77" s="11" t="s">
+        <v>484</v>
+      </c>
+      <c r="H77" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="I77" s="11" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" s="4" customFormat="1">
+      <c r="A78" s="9" t="s">
+        <v>487</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>488</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E78" s="9" t="s">
+        <v>490</v>
+      </c>
+      <c r="F78" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G78" s="9" t="s">
+        <v>491</v>
+      </c>
+      <c r="H78" s="9" t="s">
+        <v>492</v>
+      </c>
+      <c r="I78" s="9" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" s="11" t="s">
+        <v>494</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>495</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>496</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="F79" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G79" s="11" t="s">
+        <v>498</v>
+      </c>
+      <c r="H79" s="11" t="s">
+        <v>499</v>
+      </c>
+      <c r="I79" s="11" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" s="9" t="s">
+        <v>501</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>502</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>503</v>
+      </c>
+      <c r="D80" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G80" s="9" t="s">
+        <v>505</v>
+      </c>
+      <c r="H80" s="9" t="s">
+        <v>506</v>
+      </c>
+      <c r="I80" s="12" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" s="11" t="s">
+        <v>508</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>509</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="D81" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" s="15" t="s">
+        <v>511</v>
+      </c>
+      <c r="F81" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G81" s="11" t="s">
+        <v>512</v>
+      </c>
+      <c r="H81" s="11" t="s">
+        <v>513</v>
+      </c>
+      <c r="I81" s="11" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82" s="9" t="s">
+        <v>515</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>516</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>517</v>
+      </c>
+      <c r="D82" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E82" s="19" t="s">
+        <v>518</v>
+      </c>
+      <c r="F82" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G82" s="9"/>
+      <c r="H82" s="17" t="s">
+        <v>519</v>
+      </c>
+      <c r="I82" s="17" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83" s="11" t="s">
+        <v>521</v>
+      </c>
+      <c r="B83" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="D83" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="F83" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G83" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="H83" s="11" t="s">
+        <v>525</v>
+      </c>
+      <c r="I83" s="11" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" s="9" t="s">
+        <v>527</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>528</v>
+      </c>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="F84" s="9" t="s">
+        <v>529</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>530</v>
+      </c>
+      <c r="H84" s="9" t="s">
+        <v>531</v>
+      </c>
+      <c r="I84" s="9" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" s="11" t="s">
+        <v>533</v>
+      </c>
+      <c r="B85" s="11" t="s">
+        <v>534</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>535</v>
+      </c>
+      <c r="D85" s="11" t="s">
         <v>408</v>
       </c>
-      <c r="B63" s="9" t="s">
-        <v>409</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>410</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E63" s="19" t="s">
+      <c r="E85" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="F85" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="G85" s="11" t="s">
+        <v>536</v>
+      </c>
+      <c r="H85" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="I85" s="11" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>539</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>540</v>
+      </c>
+      <c r="D86" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G86" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H86" s="9" t="s">
+        <v>542</v>
+      </c>
+      <c r="I86" s="9" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" s="11" t="s">
+        <v>544</v>
+      </c>
+      <c r="B87" s="11" t="s">
+        <v>539</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>545</v>
+      </c>
+      <c r="D87" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E87" s="11" t="s">
+        <v>641</v>
+      </c>
+      <c r="F87" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="G87" s="11" t="s">
+        <v>546</v>
+      </c>
+      <c r="H87" s="11" t="s">
+        <v>547</v>
+      </c>
+      <c r="I87" s="11" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88" s="9" t="s">
+        <v>549</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>539</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D88" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G88" s="18" t="s">
+        <v>551</v>
+      </c>
+      <c r="H88" s="18" t="s">
+        <v>552</v>
+      </c>
+      <c r="I88" s="18" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
+      <c r="A89" s="11" t="s">
+        <v>554</v>
+      </c>
+      <c r="B89" s="11" t="s">
+        <v>555</v>
+      </c>
+      <c r="C89" s="11" t="s">
+        <v>556</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="E89" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="F89" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G89" s="11" t="s">
+        <v>557</v>
+      </c>
+      <c r="H89" s="11" t="s">
+        <v>558</v>
+      </c>
+      <c r="I89" s="11" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>562</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G90" s="9" t="s">
+        <v>563</v>
+      </c>
+      <c r="H90" s="9" t="s">
+        <v>564</v>
+      </c>
+      <c r="I90" s="9" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
+      <c r="A91" s="11" t="s">
+        <v>566</v>
+      </c>
+      <c r="B91" s="11" t="s">
+        <v>567</v>
+      </c>
+      <c r="C91" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="D91" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E91" s="15" t="s">
+        <v>569</v>
+      </c>
+      <c r="F91" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G91" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="H91" s="11" t="s">
+        <v>571</v>
+      </c>
+      <c r="I91" s="11" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
+      <c r="A92" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>575</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E92" s="19" t="s">
+        <v>576</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G92" s="9" t="s">
+        <v>577</v>
+      </c>
+      <c r="H92" s="9" t="s">
+        <v>578</v>
+      </c>
+      <c r="I92" s="9" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="A93" s="11" t="s">
+        <v>580</v>
+      </c>
+      <c r="B93" s="11" t="s">
+        <v>581</v>
+      </c>
+      <c r="C93" s="11" t="s">
+        <v>582</v>
+      </c>
+      <c r="D93" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E93" s="11" t="s">
+        <v>642</v>
+      </c>
+      <c r="F93" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="G93" s="13" t="s">
+        <v>584</v>
+      </c>
+      <c r="H93" s="13" t="s">
+        <v>585</v>
+      </c>
+      <c r="I93" s="11" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="A94" s="9" t="s">
+        <v>587</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>588</v>
+      </c>
+      <c r="D94" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E94" s="19" t="s">
+        <v>589</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G94" s="18" t="s">
+        <v>590</v>
+      </c>
+      <c r="H94" s="18" t="s">
+        <v>591</v>
+      </c>
+      <c r="I94" s="18" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="A95" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>656</v>
+      </c>
+      <c r="C95" s="9"/>
+      <c r="D95" s="9" t="s">
+        <v>657</v>
+      </c>
+      <c r="E95" s="19"/>
+      <c r="F95" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="G95" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="H95" s="17" t="s">
+        <v>658</v>
+      </c>
+      <c r="I95" s="24"/>
+    </row>
+    <row r="96" spans="1:9" s="4" customFormat="1">
+      <c r="A96" s="11" t="s">
+        <v>598</v>
+      </c>
+      <c r="B96" s="11" t="s">
+        <v>599</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>600</v>
+      </c>
+      <c r="D96" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E96" s="15" t="s">
+        <v>601</v>
+      </c>
+      <c r="F96" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F63" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G63" s="18" t="s">
-        <v>316</v>
-      </c>
-      <c r="H63" s="18" t="s">
-        <v>411</v>
-      </c>
-      <c r="I63" s="18" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
-      <c r="A64" s="11" t="s">
-        <v>413</v>
-      </c>
-      <c r="B64" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="C64" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="D64" s="11" t="s">
-        <v>416</v>
-      </c>
-      <c r="E64" s="14" t="s">
-        <v>417</v>
-      </c>
-      <c r="F64" s="11" t="s">
-        <v>417</v>
-      </c>
-      <c r="G64" s="13" t="s">
-        <v>418</v>
-      </c>
-      <c r="H64" s="13" t="s">
-        <v>419</v>
-      </c>
-      <c r="I64" s="11" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" s="4" customFormat="1">
-      <c r="A65" s="9" t="s">
-        <v>421</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>422</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="D65" s="9" t="s">
+      <c r="G96" s="11"/>
+      <c r="H96" s="11" t="s">
+        <v>602</v>
+      </c>
+      <c r="I96" s="11" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" s="4" customFormat="1">
+      <c r="A97" s="9" t="s">
+        <v>604</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>605</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>606</v>
+      </c>
+      <c r="D97" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>607</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>446</v>
+      </c>
+      <c r="G97" s="9" t="s">
+        <v>608</v>
+      </c>
+      <c r="H97" s="9" t="s">
+        <v>609</v>
+      </c>
+      <c r="I97" s="9" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" s="13" t="s">
+        <v>611</v>
+      </c>
+      <c r="B98" s="13" t="s">
+        <v>605</v>
+      </c>
+      <c r="C98" s="11" t="s">
+        <v>612</v>
+      </c>
+      <c r="D98" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="E65" s="19" t="s">
-        <v>424</v>
-      </c>
-      <c r="F65" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G65" s="18"/>
-      <c r="H65" s="17" t="s">
-        <v>425</v>
-      </c>
-      <c r="I65" s="18" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
-      <c r="A66" s="11" t="s">
-        <v>427</v>
-      </c>
-      <c r="B66" s="11" t="s">
-        <v>422</v>
-      </c>
-      <c r="C66" s="11" t="s">
-        <v>428</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E66" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="F66" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="G66" s="11" t="s">
-        <v>429</v>
-      </c>
-      <c r="H66" s="11" t="s">
-        <v>430</v>
-      </c>
-      <c r="I66" s="11" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" s="5" customFormat="1">
-      <c r="A67" s="9" t="s">
-        <v>432</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>433</v>
-      </c>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>434</v>
-      </c>
-      <c r="F67" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G67" s="9" t="s">
-        <v>435</v>
-      </c>
-      <c r="H67" s="9" t="s">
-        <v>436</v>
-      </c>
-      <c r="I67" s="9" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
-      <c r="A68" s="11" t="s">
-        <v>438</v>
-      </c>
-      <c r="B68" s="11" t="s">
-        <v>439</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>440</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="E68" s="11" t="s">
-        <v>441</v>
-      </c>
-      <c r="F68" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G68" s="11" t="s">
-        <v>442</v>
-      </c>
-      <c r="H68" s="11" t="s">
-        <v>443</v>
-      </c>
-      <c r="I68" s="11" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
-      <c r="A69" s="9" t="s">
-        <v>446</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>445</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>447</v>
-      </c>
-      <c r="D69" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E69" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="F69" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="G69" s="9" t="s">
-        <v>448</v>
-      </c>
-      <c r="H69" s="9" t="s">
-        <v>449</v>
-      </c>
-      <c r="I69" s="9" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
-      <c r="A70" s="11" t="s">
-        <v>451</v>
-      </c>
-      <c r="B70" s="11" t="s">
-        <v>452</v>
-      </c>
-      <c r="C70" s="11" t="s">
-        <v>453</v>
-      </c>
-      <c r="D70" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E70" s="11" t="s">
-        <v>646</v>
-      </c>
-      <c r="F70" s="11" t="s">
-        <v>454</v>
-      </c>
-      <c r="G70" s="11" t="s">
-        <v>455</v>
-      </c>
-      <c r="H70" s="11" t="s">
-        <v>456</v>
-      </c>
-      <c r="I70" s="20" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
-      <c r="A71" s="9" t="s">
-        <v>458</v>
-      </c>
-      <c r="B71" s="9" t="s">
-        <v>459</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>460</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="E71" s="19" t="s">
-        <v>461</v>
-      </c>
-      <c r="F71" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G71" s="9" t="s">
-        <v>462</v>
-      </c>
-      <c r="H71" s="9" t="s">
-        <v>463</v>
-      </c>
-      <c r="I71" s="9" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
-      <c r="A72" s="11" t="s">
-        <v>465</v>
-      </c>
-      <c r="B72" s="11" t="s">
-        <v>466</v>
-      </c>
-      <c r="C72" s="11" t="s">
-        <v>467</v>
-      </c>
-      <c r="D72" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="E72" s="15" t="s">
-        <v>279</v>
-      </c>
-      <c r="F72" s="11" t="s">
-        <v>279</v>
-      </c>
-      <c r="G72" s="11" t="s">
-        <v>468</v>
-      </c>
-      <c r="H72" s="11" t="s">
-        <v>469</v>
-      </c>
-      <c r="I72" s="11" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9">
-      <c r="A73" s="18" t="s">
-        <v>471</v>
-      </c>
-      <c r="B73" s="18" t="s">
-        <v>472</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>473</v>
-      </c>
-      <c r="D73" s="18" t="s">
-        <v>376</v>
-      </c>
-      <c r="E73" s="18" t="s">
-        <v>474</v>
-      </c>
-      <c r="F73" s="18" t="s">
-        <v>647</v>
-      </c>
-      <c r="G73" s="18" t="s">
-        <v>475</v>
-      </c>
-      <c r="H73" s="18" t="s">
-        <v>476</v>
-      </c>
-      <c r="I73" s="18" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" s="4" customFormat="1">
-      <c r="A74" s="11" t="s">
-        <v>478</v>
-      </c>
-      <c r="B74" s="11" t="s">
-        <v>479</v>
-      </c>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="E74" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="F74" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="G74" s="11" t="s">
-        <v>480</v>
-      </c>
-      <c r="H74" s="11" t="s">
-        <v>481</v>
-      </c>
-      <c r="I74" s="11" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9">
-      <c r="A75" s="9" t="s">
-        <v>483</v>
-      </c>
-      <c r="B75" s="9" t="s">
-        <v>484</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>485</v>
-      </c>
-      <c r="D75" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>340</v>
-      </c>
-      <c r="F75" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G75" s="9" t="s">
-        <v>486</v>
-      </c>
-      <c r="H75" s="17" t="s">
-        <v>487</v>
-      </c>
-      <c r="I75" s="17" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9">
-      <c r="A76" s="11" t="s">
-        <v>489</v>
-      </c>
-      <c r="B76" s="11" t="s">
-        <v>490</v>
-      </c>
-      <c r="C76" s="11" t="s">
-        <v>491</v>
-      </c>
-      <c r="D76" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E76" s="15" t="s">
-        <v>654</v>
-      </c>
-      <c r="F76" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G76" s="11" t="s">
-        <v>492</v>
-      </c>
-      <c r="H76" s="11" t="s">
-        <v>493</v>
-      </c>
-      <c r="I76" s="11" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" s="4" customFormat="1">
-      <c r="A77" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="B77" s="9" t="s">
-        <v>496</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>497</v>
-      </c>
-      <c r="D77" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>498</v>
-      </c>
-      <c r="F77" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G77" s="9" t="s">
-        <v>499</v>
-      </c>
-      <c r="H77" s="9" t="s">
-        <v>500</v>
-      </c>
-      <c r="I77" s="9" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9">
-      <c r="A78" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="B78" s="11" t="s">
-        <v>503</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>504</v>
-      </c>
-      <c r="D78" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="E78" s="11" t="s">
-        <v>505</v>
-      </c>
-      <c r="F78" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G78" s="11" t="s">
-        <v>506</v>
-      </c>
-      <c r="H78" s="11" t="s">
-        <v>507</v>
-      </c>
-      <c r="I78" s="11" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9">
-      <c r="A79" s="9" t="s">
-        <v>509</v>
-      </c>
-      <c r="B79" s="9" t="s">
-        <v>510</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>511</v>
-      </c>
-      <c r="D79" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E79" s="9" t="s">
-        <v>512</v>
-      </c>
-      <c r="F79" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G79" s="9" t="s">
-        <v>513</v>
-      </c>
-      <c r="H79" s="9" t="s">
-        <v>514</v>
-      </c>
-      <c r="I79" s="12" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9">
-      <c r="A80" s="11" t="s">
-        <v>516</v>
-      </c>
-      <c r="B80" s="11" t="s">
-        <v>517</v>
-      </c>
-      <c r="C80" s="11" t="s">
-        <v>518</v>
-      </c>
-      <c r="D80" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E80" s="15" t="s">
-        <v>519</v>
-      </c>
-      <c r="F80" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="G80" s="11" t="s">
-        <v>520</v>
-      </c>
-      <c r="H80" s="11" t="s">
-        <v>521</v>
-      </c>
-      <c r="I80" s="11" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9">
-      <c r="A81" s="9" t="s">
-        <v>523</v>
-      </c>
-      <c r="B81" s="9" t="s">
-        <v>524</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>525</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E81" s="19" t="s">
-        <v>526</v>
-      </c>
-      <c r="F81" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G81" s="9"/>
-      <c r="H81" s="17" t="s">
-        <v>527</v>
-      </c>
-      <c r="I81" s="17" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9">
-      <c r="A82" s="11" t="s">
-        <v>529</v>
-      </c>
-      <c r="B82" s="11" t="s">
-        <v>530</v>
-      </c>
-      <c r="C82" s="11" t="s">
-        <v>531</v>
-      </c>
-      <c r="D82" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E82" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="F82" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="G82" s="11" t="s">
-        <v>532</v>
-      </c>
-      <c r="H82" s="11" t="s">
-        <v>533</v>
-      </c>
-      <c r="I82" s="11" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9">
-      <c r="A83" s="9" t="s">
-        <v>535</v>
-      </c>
-      <c r="B83" s="9" t="s">
-        <v>536</v>
-      </c>
-      <c r="C83" s="9"/>
-      <c r="D83" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E83" s="9" t="s">
-        <v>648</v>
-      </c>
-      <c r="F83" s="9" t="s">
-        <v>537</v>
-      </c>
-      <c r="G83" s="9" t="s">
-        <v>538</v>
-      </c>
-      <c r="H83" s="9" t="s">
-        <v>539</v>
-      </c>
-      <c r="I83" s="9" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9">
-      <c r="A84" s="11" t="s">
-        <v>541</v>
-      </c>
-      <c r="B84" s="11" t="s">
-        <v>542</v>
-      </c>
-      <c r="C84" s="11" t="s">
-        <v>543</v>
-      </c>
-      <c r="D84" s="11" t="s">
-        <v>416</v>
-      </c>
-      <c r="E84" s="15" t="s">
-        <v>315</v>
-      </c>
-      <c r="F84" s="11" t="s">
-        <v>315</v>
-      </c>
-      <c r="G84" s="11" t="s">
-        <v>544</v>
-      </c>
-      <c r="H84" s="11" t="s">
-        <v>545</v>
-      </c>
-      <c r="I84" s="11" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9">
-      <c r="A85" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="B85" s="9" t="s">
-        <v>547</v>
-      </c>
-      <c r="C85" s="9" t="s">
-        <v>548</v>
-      </c>
-      <c r="D85" s="9" t="s">
-        <v>549</v>
-      </c>
-      <c r="E85" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="F85" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G85" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="H85" s="9" t="s">
-        <v>550</v>
-      </c>
-      <c r="I85" s="9" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9">
-      <c r="A86" s="11" t="s">
-        <v>552</v>
-      </c>
-      <c r="B86" s="11" t="s">
-        <v>547</v>
-      </c>
-      <c r="C86" s="11" t="s">
-        <v>553</v>
-      </c>
-      <c r="D86" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E86" s="11" t="s">
-        <v>649</v>
-      </c>
-      <c r="F86" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="G86" s="11" t="s">
-        <v>554</v>
-      </c>
-      <c r="H86" s="11" t="s">
-        <v>555</v>
-      </c>
-      <c r="I86" s="11" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9">
-      <c r="A87" s="9" t="s">
-        <v>557</v>
-      </c>
-      <c r="B87" s="9" t="s">
-        <v>547</v>
-      </c>
-      <c r="C87" s="9" t="s">
-        <v>558</v>
-      </c>
-      <c r="D87" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E87" s="9" t="s">
-        <v>512</v>
-      </c>
-      <c r="F87" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G87" s="18" t="s">
-        <v>559</v>
-      </c>
-      <c r="H87" s="18" t="s">
-        <v>560</v>
-      </c>
-      <c r="I87" s="18" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9">
-      <c r="A88" s="11" t="s">
-        <v>562</v>
-      </c>
-      <c r="B88" s="11" t="s">
-        <v>563</v>
-      </c>
-      <c r="C88" s="11" t="s">
-        <v>564</v>
-      </c>
-      <c r="D88" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="E88" s="11" t="s">
-        <v>474</v>
-      </c>
-      <c r="F88" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G88" s="11" t="s">
-        <v>565</v>
-      </c>
-      <c r="H88" s="11" t="s">
+      <c r="E98" s="13" t="s">
+        <v>613</v>
+      </c>
+      <c r="F98" s="13" t="s">
+        <v>614</v>
+      </c>
+      <c r="G98" s="13" t="s">
+        <v>615</v>
+      </c>
+      <c r="H98" s="13" t="s">
+        <v>616</v>
+      </c>
+      <c r="I98" s="13" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" s="4" customFormat="1">
+      <c r="A99" t="s">
         <v>566</v>
       </c>
-      <c r="I88" s="11" t="s">
+      <c r="B99" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="89" spans="1:9">
-      <c r="A89" s="9" t="s">
+      <c r="C99" s="8" t="s">
         <v>568</v>
-      </c>
-      <c r="B89" s="9" t="s">
-        <v>569</v>
-      </c>
-      <c r="C89" s="9" t="s">
-        <v>570</v>
-      </c>
-      <c r="D89" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="E89" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="F89" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="G89" s="9" t="s">
-        <v>571</v>
-      </c>
-      <c r="H89" s="9" t="s">
-        <v>572</v>
-      </c>
-      <c r="I89" s="9" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9">
-      <c r="A90" s="11" t="s">
-        <v>574</v>
-      </c>
-      <c r="B90" s="11" t="s">
-        <v>575</v>
-      </c>
-      <c r="C90" s="11" t="s">
-        <v>576</v>
-      </c>
-      <c r="D90" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E90" s="15" t="s">
-        <v>577</v>
-      </c>
-      <c r="F90" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G90" s="11" t="s">
-        <v>578</v>
-      </c>
-      <c r="H90" s="11" t="s">
-        <v>579</v>
-      </c>
-      <c r="I90" s="11" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9">
-      <c r="A91" s="9" t="s">
-        <v>581</v>
-      </c>
-      <c r="B91" s="9" t="s">
-        <v>582</v>
-      </c>
-      <c r="C91" s="9" t="s">
-        <v>583</v>
-      </c>
-      <c r="D91" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E91" s="19" t="s">
-        <v>584</v>
-      </c>
-      <c r="F91" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G91" s="9" t="s">
-        <v>585</v>
-      </c>
-      <c r="H91" s="9" t="s">
-        <v>586</v>
-      </c>
-      <c r="I91" s="9" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9">
-      <c r="A92" s="11" t="s">
-        <v>588</v>
-      </c>
-      <c r="B92" s="11" t="s">
-        <v>589</v>
-      </c>
-      <c r="C92" s="11" t="s">
-        <v>590</v>
-      </c>
-      <c r="D92" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E92" s="11" t="s">
-        <v>650</v>
-      </c>
-      <c r="F92" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="G92" s="13" t="s">
-        <v>592</v>
-      </c>
-      <c r="H92" s="13" t="s">
-        <v>593</v>
-      </c>
-      <c r="I92" s="11" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9">
-      <c r="A93" s="9" t="s">
-        <v>595</v>
-      </c>
-      <c r="B93" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="C93" s="9" t="s">
-        <v>596</v>
-      </c>
-      <c r="D93" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E93" s="19" t="s">
-        <v>597</v>
-      </c>
-      <c r="F93" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G93" s="18" t="s">
-        <v>598</v>
-      </c>
-      <c r="H93" s="18" t="s">
-        <v>599</v>
-      </c>
-      <c r="I93" s="18" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" s="4" customFormat="1">
-      <c r="A94" s="11" t="s">
-        <v>606</v>
-      </c>
-      <c r="B94" s="11" t="s">
-        <v>607</v>
-      </c>
-      <c r="C94" s="11" t="s">
-        <v>608</v>
-      </c>
-      <c r="D94" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="E94" s="15" t="s">
-        <v>609</v>
-      </c>
-      <c r="F94" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G94" s="11"/>
-      <c r="H94" s="11" t="s">
-        <v>610</v>
-      </c>
-      <c r="I94" s="11" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" s="4" customFormat="1">
-      <c r="A95" s="9" t="s">
-        <v>612</v>
-      </c>
-      <c r="B95" s="9" t="s">
-        <v>613</v>
-      </c>
-      <c r="C95" s="9" t="s">
-        <v>614</v>
-      </c>
-      <c r="D95" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E95" s="9" t="s">
-        <v>615</v>
-      </c>
-      <c r="F95" s="9" t="s">
-        <v>454</v>
-      </c>
-      <c r="G95" s="9" t="s">
-        <v>616</v>
-      </c>
-      <c r="H95" s="9" t="s">
-        <v>617</v>
-      </c>
-      <c r="I95" s="9" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9">
-      <c r="A96" s="13" t="s">
-        <v>619</v>
-      </c>
-      <c r="B96" s="13" t="s">
-        <v>613</v>
-      </c>
-      <c r="C96" s="11" t="s">
-        <v>620</v>
-      </c>
-      <c r="D96" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="E96" s="13" t="s">
-        <v>621</v>
-      </c>
-      <c r="F96" s="13" t="s">
-        <v>622</v>
-      </c>
-      <c r="G96" s="13" t="s">
-        <v>623</v>
-      </c>
-      <c r="H96" s="13" t="s">
-        <v>624</v>
-      </c>
-      <c r="I96" s="13" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" s="4" customFormat="1">
-      <c r="A97" t="s">
-        <v>574</v>
-      </c>
-      <c r="B97" t="s">
-        <v>575</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>576</v>
-      </c>
-      <c r="D97" t="s">
-        <v>11</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>577</v>
-      </c>
-      <c r="F97" t="s">
-        <v>13</v>
-      </c>
-      <c r="G97" t="s">
-        <v>578</v>
-      </c>
-      <c r="H97" t="s">
-        <v>579</v>
-      </c>
-      <c r="I97" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9">
-      <c r="A98" t="s">
-        <v>581</v>
-      </c>
-      <c r="B98" t="s">
-        <v>582</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>583</v>
-      </c>
-      <c r="D98" t="s">
-        <v>11</v>
-      </c>
-      <c r="E98" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="F98" t="s">
-        <v>13</v>
-      </c>
-      <c r="G98" t="s">
-        <v>585</v>
-      </c>
-      <c r="H98" t="s">
-        <v>586</v>
-      </c>
-      <c r="I98" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9">
-      <c r="A99" t="s">
-        <v>588</v>
-      </c>
-      <c r="B99" t="s">
-        <v>589</v>
-      </c>
-      <c r="C99" s="8" t="s">
-        <v>590</v>
       </c>
       <c r="D99" t="s">
         <v>11</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>591</v>
+        <v>569</v>
       </c>
       <c r="F99" t="s">
-        <v>186</v>
-      </c>
-      <c r="G99" s="4" t="s">
-        <v>592</v>
-      </c>
-      <c r="H99" s="4" t="s">
-        <v>593</v>
+        <v>13</v>
+      </c>
+      <c r="G99" t="s">
+        <v>570</v>
+      </c>
+      <c r="H99" t="s">
+        <v>571</v>
       </c>
       <c r="I99" t="s">
-        <v>594</v>
+        <v>572</v>
       </c>
     </row>
     <row r="100" spans="1:9">
       <c r="A100" t="s">
-        <v>595</v>
+        <v>573</v>
       </c>
       <c r="B100" t="s">
-        <v>589</v>
+        <v>574</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>596</v>
+        <v>575</v>
       </c>
       <c r="D100" t="s">
         <v>11</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>597</v>
+        <v>576</v>
       </c>
       <c r="F100" t="s">
-        <v>32</v>
-      </c>
-      <c r="G100" s="4" t="s">
-        <v>598</v>
-      </c>
-      <c r="H100" s="4" t="s">
-        <v>599</v>
-      </c>
-      <c r="I100" s="4" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" s="5" customFormat="1">
+        <v>13</v>
+      </c>
+      <c r="G100" t="s">
+        <v>577</v>
+      </c>
+      <c r="H100" t="s">
+        <v>578</v>
+      </c>
+      <c r="I100" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
       <c r="A101" t="s">
-        <v>601</v>
+        <v>580</v>
       </c>
       <c r="B101" t="s">
-        <v>602</v>
-      </c>
-      <c r="C101" s="8"/>
+        <v>581</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>582</v>
+      </c>
       <c r="D101" t="s">
-        <v>17</v>
-      </c>
-      <c r="E101" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>583</v>
       </c>
       <c r="F101" t="s">
-        <v>13</v>
+        <v>186</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>603</v>
+        <v>584</v>
       </c>
       <c r="H101" s="4" t="s">
-        <v>604</v>
-      </c>
-      <c r="I101" s="4" t="s">
-        <v>605</v>
+        <v>585</v>
+      </c>
+      <c r="I101" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="102" spans="1:9">
       <c r="A102" t="s">
-        <v>606</v>
+        <v>587</v>
       </c>
       <c r="B102" t="s">
-        <v>607</v>
+        <v>581</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>608</v>
+        <v>588</v>
       </c>
       <c r="D102" t="s">
+        <v>11</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="F102" t="s">
+        <v>32</v>
+      </c>
+      <c r="G102" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="H102" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="I102" s="4" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" s="5" customFormat="1">
+      <c r="A103" t="s">
+        <v>593</v>
+      </c>
+      <c r="B103" t="s">
+        <v>594</v>
+      </c>
+      <c r="C103" s="8"/>
+      <c r="D103" t="s">
+        <v>17</v>
+      </c>
+      <c r="E103" t="s">
+        <v>18</v>
+      </c>
+      <c r="F103" t="s">
+        <v>13</v>
+      </c>
+      <c r="G103" s="4" t="s">
+        <v>595</v>
+      </c>
+      <c r="H103" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="I103" s="4" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104" t="s">
+        <v>598</v>
+      </c>
+      <c r="B104" t="s">
+        <v>599</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>600</v>
+      </c>
+      <c r="D104" t="s">
         <v>197</v>
       </c>
-      <c r="E102" s="3" t="s">
-        <v>609</v>
-      </c>
-      <c r="F102" t="s">
+      <c r="E104" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="F104" t="s">
         <v>62</v>
       </c>
-      <c r="H102" t="s">
-        <v>610</v>
-      </c>
-      <c r="I102" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9">
-      <c r="A103" t="s">
-        <v>612</v>
-      </c>
-      <c r="B103" t="s">
-        <v>613</v>
-      </c>
-      <c r="C103" s="8" t="s">
-        <v>614</v>
-      </c>
-      <c r="D103" t="s">
-        <v>11</v>
-      </c>
-      <c r="E103" t="s">
-        <v>615</v>
-      </c>
-      <c r="F103" t="s">
-        <v>454</v>
-      </c>
-      <c r="G103" t="s">
-        <v>616</v>
-      </c>
-      <c r="H103" t="s">
-        <v>617</v>
-      </c>
-      <c r="I103" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9">
-      <c r="A104" s="4" t="s">
-        <v>619</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>613</v>
-      </c>
-      <c r="C104" s="7" t="s">
-        <v>620</v>
-      </c>
-      <c r="D104" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="E104" s="21" t="s">
-        <v>621</v>
-      </c>
-      <c r="F104" s="4" t="s">
-        <v>622</v>
-      </c>
-      <c r="G104" s="4" t="s">
-        <v>623</v>
-      </c>
-      <c r="H104" s="4" t="s">
-        <v>624</v>
-      </c>
-      <c r="I104" s="4" t="s">
-        <v>625</v>
+      <c r="H104" t="s">
+        <v>602</v>
+      </c>
+      <c r="I104" t="s">
+        <v>603</v>
       </c>
     </row>
     <row r="105" spans="1:9">
       <c r="A105" t="s">
-        <v>626</v>
+        <v>604</v>
       </c>
       <c r="B105" t="s">
-        <v>303</v>
+        <v>605</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>606</v>
       </c>
       <c r="D105" t="s">
+        <v>11</v>
+      </c>
+      <c r="E105" t="s">
+        <v>607</v>
+      </c>
+      <c r="F105" t="s">
+        <v>446</v>
+      </c>
+      <c r="G105" t="s">
+        <v>608</v>
+      </c>
+      <c r="H105" t="s">
+        <v>609</v>
+      </c>
+      <c r="I105" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>612</v>
+      </c>
+      <c r="D106" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="E105" t="s">
-        <v>627</v>
-      </c>
-      <c r="F105" t="s">
+      <c r="E106" s="21" t="s">
+        <v>613</v>
+      </c>
+      <c r="F106" s="4" t="s">
+        <v>614</v>
+      </c>
+      <c r="G106" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="H106" s="4" t="s">
+        <v>616</v>
+      </c>
+      <c r="I106" s="4" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
+      <c r="A107" t="s">
+        <v>618</v>
+      </c>
+      <c r="B107" t="s">
+        <v>297</v>
+      </c>
+      <c r="D107" t="s">
+        <v>197</v>
+      </c>
+      <c r="E107" t="s">
+        <v>619</v>
+      </c>
+      <c r="F107" t="s">
         <v>62</v>
       </c>
-      <c r="G105" t="s">
-        <v>628</v>
+      <c r="G107" t="s">
+        <v>620</v>
       </c>
     </row>
   </sheetData>
@@ -5566,16 +5627,17 @@
     <hyperlink ref="H46" r:id="rId9" display="mailto:isabelle.lagadec@bib.umontreal.ca" xr:uid="{4822C834-E5A8-42FD-9734-374BFC718C85}"/>
     <hyperlink ref="H55" r:id="rId10" display="mailto:magalie.beaudoin@umontreal.ca" xr:uid="{2D976BF0-B68A-46E5-8412-BA8BC43FD26D}"/>
     <hyperlink ref="I55" r:id="rId11" xr:uid="{8AB273DE-5C86-4A48-AF36-BE5967CA61FD}"/>
-    <hyperlink ref="H65" r:id="rId12" display="mailto:mathieu.pigeon@umontreal.ca" xr:uid="{F73DFC6E-4D6D-42F3-84C0-454956AEC7E8}"/>
-    <hyperlink ref="H75" r:id="rId13" display="mailto:nadege.arsa@bib.umontreal.ca" xr:uid="{408AF5A3-35ED-4BF5-92B9-1B21C0C475D9}"/>
-    <hyperlink ref="I75" r:id="rId14" xr:uid="{DD84AED2-20C7-4DA6-BFBF-EEC1E7D79E1B}"/>
-    <hyperlink ref="H81" r:id="rId15" display="mailto:simon.blais.longtin@umontreal.ca" xr:uid="{EA917AC7-9087-435B-A6E7-3AE1885514AA}"/>
-    <hyperlink ref="I81" r:id="rId16" xr:uid="{CDCAA32A-F6EB-49BF-B7CF-1AA918DBB62B}"/>
+    <hyperlink ref="H66" r:id="rId12" display="mailto:mathieu.pigeon@umontreal.ca" xr:uid="{F73DFC6E-4D6D-42F3-84C0-454956AEC7E8}"/>
+    <hyperlink ref="H76" r:id="rId13" display="mailto:nadege.arsa@bib.umontreal.ca" xr:uid="{408AF5A3-35ED-4BF5-92B9-1B21C0C475D9}"/>
+    <hyperlink ref="I76" r:id="rId14" xr:uid="{DD84AED2-20C7-4DA6-BFBF-EEC1E7D79E1B}"/>
+    <hyperlink ref="H82" r:id="rId15" display="mailto:simon.blais.longtin@umontreal.ca" xr:uid="{EA917AC7-9087-435B-A6E7-3AE1885514AA}"/>
+    <hyperlink ref="I82" r:id="rId16" xr:uid="{CDCAA32A-F6EB-49BF-B7CF-1AA918DBB62B}"/>
+    <hyperlink ref="H95" r:id="rId17" xr:uid="{8ABC26E9-CF81-491C-8A28-B209E6620D2A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
   <tableParts count="1">
-    <tablePart r:id="rId18"/>
+    <tablePart r:id="rId19"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
retrait de la ligne poste vacant
</commit_message>
<xml_diff>
--- a/content/personnel/liste-personnel.xlsx
+++ b/content/personnel/liste-personnel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tardimat\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96434A8E-5F81-48C7-A2C2-7788165A98FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78926830-204D-4497-8F38-0865C1FA9312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2670" yWindow="5010" windowWidth="47100" windowHeight="23445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15360" yWindow="3150" windowWidth="34200" windowHeight="26295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="655">
   <si>
     <t>Borsi</t>
   </si>
@@ -1050,18 +1050,6 @@
     <t>https://teams.microsoft.com/l/chat/0/0?users=khalid.jouamaa@umontreal.ca</t>
   </si>
   <si>
-    <t>Expérience utilisateur</t>
-  </si>
-  <si>
-    <t>514 343-6111, poste 5775</t>
-  </si>
-  <si>
-    <t>laurie-anne.gignac@umontreal.ca</t>
-  </si>
-  <si>
-    <t>https://teams.microsoft.com/l/chat/0/0?users=laurie-anne.gignac@umontreal.ca</t>
-  </si>
-  <si>
     <t>Beaudoin</t>
   </si>
   <si>
@@ -1987,12 +1975,6 @@
   </si>
   <si>
     <t>vanessa.martin.2@umontreal.ca</t>
-  </si>
-  <si>
-    <t>Poste</t>
-  </si>
-  <si>
-    <t>vacant</t>
   </si>
   <si>
     <t>Direction des bibliothèques sociétés et création</t>
@@ -2264,16 +2246,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A0AF7E1-A614-44BF-8C48-5C26377DC552}" name="Tableau1" displayName="Tableau1" ref="A1:I103" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:I103" xr:uid="{4F6A1D8F-9220-4675-A202-2173F3493722}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A0AF7E1-A614-44BF-8C48-5C26377DC552}" name="Tableau1" displayName="Tableau1" ref="A1:I102" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:I102" xr:uid="{4F6A1D8F-9220-4675-A202-2173F3493722}">
     <filterColumn colId="5">
       <filters>
         <filter val="Direction de la recherche et des initiatives numériques"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I103">
-    <sortCondition ref="A1:A103"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I102">
+    <sortCondition ref="A1:A102"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4B04E1AF-0079-4AD2-81CA-E8A433733E21}" name="nom"/>
@@ -2577,11 +2559,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I103"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A101" sqref="A101:XFD101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2598,31 +2580,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>619</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>620</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="G1" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>623</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>622</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>621</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>624</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>626</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2656,42 +2638,42 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>195</v>
@@ -2703,13 +2685,13 @@
         <v>30</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2758,7 +2740,7 @@
         <v>74</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>75</v>
@@ -2772,114 +2754,114 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="B8" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="F8" t="s">
         <v>184</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="I8" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="7" t="s">
         <v>307</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>403</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="F10" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>404</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="H10" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="I10" s="9" t="s">
         <v>406</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>407</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>407</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>408</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>409</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -3019,87 +3001,87 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>53</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="15" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="B18" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="F18" t="s">
         <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="H18" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="I18" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -3141,7 +3123,7 @@
         <v>3</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>4</v>
@@ -3187,39 +3169,39 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9" t="s">
@@ -3232,13 +3214,13 @@
         <v>81</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -3270,16 +3252,16 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="E25" s="13" t="s">
         <v>307</v>
@@ -3288,13 +3270,13 @@
         <v>307</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -3326,58 +3308,58 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>67</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -3411,31 +3393,31 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>195</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -3496,13 +3478,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>11</v>
@@ -3514,42 +3496,42 @@
         <v>67</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>184</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -3566,7 +3548,7 @@
         <v>11</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>30</v>
@@ -3583,13 +3565,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>231</v>
@@ -3601,13 +3583,13 @@
         <v>273</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="I36" s="9" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -3624,7 +3606,7 @@
         <v>11</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>290</v>
@@ -3707,7 +3689,7 @@
         <v>11</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>184</v>
@@ -3724,31 +3706,31 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>252</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>4</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3782,80 +3764,80 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="9" t="s">
         <v>49</v>
       </c>
       <c r="E43" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="I43" s="9" t="s">
         <v>366</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>367</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>368</v>
-      </c>
-      <c r="H43" s="9" t="s">
-        <v>369</v>
-      </c>
-      <c r="I43" s="9" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="F44" s="9" t="s">
         <v>30</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="C45" s="15"/>
       <c r="D45" s="7" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>273</v>
       </c>
       <c r="G45" s="7"/>
       <c r="H45" s="7" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="I45" s="7"/>
     </row>
@@ -3918,13 +3900,13 @@
         <v>176</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>110</v>
@@ -3936,39 +3918,39 @@
         <v>111</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>195</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="F49" s="9" t="s">
         <v>60</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="I49" s="9" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -3983,7 +3965,7 @@
         <v>11</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>30</v>
@@ -4000,7 +3982,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>295</v>
@@ -4010,13 +3992,13 @@
         <v>195</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
@@ -4052,89 +4034,89 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>195</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="F53" s="9" t="s">
         <v>30</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="H53" s="9" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="I53" s="9" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E54" s="17" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="B55" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="F55" t="s">
         <v>13</v>
       </c>
       <c r="G55" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="H55" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="I55" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -4207,7 +4189,7 @@
         <v>49</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="F58" s="9" t="s">
         <v>296</v>
@@ -4216,7 +4198,7 @@
         <v>297</v>
       </c>
       <c r="H58" s="14" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="I58" s="9" t="s">
         <v>298</v>
@@ -4253,13 +4235,13 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>252</v>
@@ -4271,42 +4253,42 @@
         <v>4</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="I60" s="7" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F61" s="9" t="s">
         <v>269</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="H61" s="9" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="I61" s="9" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -4369,60 +4351,60 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>252</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>4</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="I64" s="7" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="D65" s="9" t="s">
         <v>252</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="F65" s="9" t="s">
         <v>60</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="H65" s="9" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="I65" s="9" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -4466,10 +4448,10 @@
         <v>22</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="G67" s="11" t="s">
         <v>23</v>
@@ -4506,14 +4488,14 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="C69" s="7"/>
       <c r="D69" s="7" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="E69" s="17"/>
       <c r="F69" s="7" t="s">
@@ -4523,48 +4505,48 @@
         <v>274</v>
       </c>
       <c r="H69" s="15" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="I69" s="16"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="F70" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="I70" s="7" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D71" s="7" t="s">
         <v>11</v>
@@ -4576,13 +4558,13 @@
         <v>261</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="H71" s="7" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="I71" s="7" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -4744,10 +4726,10 @@
         <v>231</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="F77" s="16" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="G77" s="16" t="s">
         <v>232</v>
@@ -4761,29 +4743,29 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C78" s="9"/>
       <c r="D78" s="9" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="F78" s="9" t="s">
         <v>307</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="H78" s="9" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="I78" s="9" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -4825,7 +4807,7 @@
         <v>22</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="F80" s="9" t="s">
         <v>319</v>
@@ -4842,14 +4824,14 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="C81" s="9"/>
       <c r="D81" s="9" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="E81" s="13"/>
       <c r="F81" s="9" t="s">
@@ -4857,61 +4839,61 @@
       </c>
       <c r="G81" s="9"/>
       <c r="H81" s="9" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="I81" s="18"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="D82" s="9" t="s">
         <v>195</v>
       </c>
       <c r="E82" s="13" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="F82" s="9" t="s">
         <v>60</v>
       </c>
       <c r="G82" s="9"/>
       <c r="H82" s="9" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="I82" s="9" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="B83" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="C83" s="22" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="D83" t="s">
         <v>195</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="F83" t="s">
         <v>60</v>
       </c>
       <c r="H83" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="I83" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -4957,7 +4939,7 @@
         <v>11</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="F85" s="7" t="s">
         <v>30</v>
@@ -5003,153 +4985,153 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="D87" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="F87" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G87" s="16" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="H87" s="16" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="I87" s="16" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D88" s="7" t="s">
         <v>195</v>
       </c>
       <c r="E88" s="17" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="F88" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G88" s="16"/>
       <c r="H88" s="15" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="I88" s="16" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D89" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E89" s="13" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="F89" s="9" t="s">
         <v>296</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="H89" s="11" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="I89" s="11" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="D90" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E90" s="17" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="F90" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G90" s="16" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="H90" s="16" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="I90" s="16" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="B91" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="C91" s="22" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="D91" t="s">
         <v>11</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="F91" t="s">
         <v>30</v>
       </c>
       <c r="G91" s="4" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="H91" s="4" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="B92" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="C92" s="19"/>
       <c r="D92" t="s">
@@ -5162,24 +5144,24 @@
         <v>13</v>
       </c>
       <c r="G92" s="4" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="H92" s="4" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
     </row>
     <row r="93" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="D93" s="7" t="s">
         <v>3</v>
@@ -5194,10 +5176,10 @@
         <v>308</v>
       </c>
       <c r="H93" s="16" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="I93" s="16" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="94" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -5227,31 +5209,31 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="D95" s="11" t="s">
         <v>195</v>
       </c>
       <c r="E95" s="11" t="s">
+        <v>607</v>
+      </c>
+      <c r="F95" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="G95" s="11" t="s">
+        <v>609</v>
+      </c>
+      <c r="H95" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="I95" s="11" t="s">
         <v>611</v>
-      </c>
-      <c r="F95" s="11" t="s">
-        <v>612</v>
-      </c>
-      <c r="G95" s="11" t="s">
-        <v>613</v>
-      </c>
-      <c r="H95" s="11" t="s">
-        <v>614</v>
-      </c>
-      <c r="I95" s="11" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -5267,7 +5249,7 @@
       </c>
       <c r="E96" s="11"/>
       <c r="F96" s="11" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="G96" s="11" t="s">
         <v>116</v>
@@ -5281,69 +5263,69 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C97" s="20"/>
       <c r="D97" s="7" t="s">
         <v>127</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F97" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G97" s="7" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="I97" s="7" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="16" t="s">
+        <v>457</v>
+      </c>
+      <c r="B98" s="16" t="s">
+        <v>458</v>
+      </c>
+      <c r="C98" s="20" t="s">
+        <v>459</v>
+      </c>
+      <c r="D98" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="E98" s="16" t="s">
+        <v>460</v>
+      </c>
+      <c r="F98" s="16" t="s">
+        <v>651</v>
+      </c>
+      <c r="G98" s="16" t="s">
         <v>461</v>
       </c>
-      <c r="B98" s="16" t="s">
+      <c r="H98" s="16" t="s">
         <v>462</v>
       </c>
-      <c r="C98" s="20" t="s">
+      <c r="I98" s="16" t="s">
         <v>463</v>
-      </c>
-      <c r="D98" s="16" t="s">
-        <v>366</v>
-      </c>
-      <c r="E98" s="16" t="s">
-        <v>464</v>
-      </c>
-      <c r="F98" s="16" t="s">
-        <v>657</v>
-      </c>
-      <c r="G98" s="16" t="s">
-        <v>465</v>
-      </c>
-      <c r="H98" s="16" t="s">
-        <v>466</v>
-      </c>
-      <c r="I98" s="16" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="99" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C99" s="21" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D99" s="9" t="s">
         <v>11</v>
@@ -5355,13 +5337,13 @@
         <v>151</v>
       </c>
       <c r="G99" s="9" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="H99" s="9" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="I99" s="9" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -5392,83 +5374,56 @@
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="9" t="s">
-        <v>655</v>
-      </c>
-      <c r="B101" s="9" t="s">
-        <v>654</v>
-      </c>
-      <c r="C101" s="21"/>
-      <c r="D101" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E101" s="9" t="s">
-        <v>341</v>
-      </c>
-      <c r="F101" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="G101" s="9" t="s">
-        <v>342</v>
-      </c>
-      <c r="H101" s="9" t="s">
-        <v>343</v>
-      </c>
-      <c r="I101" s="9" t="s">
-        <v>344</v>
+      <c r="A101" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="C101" s="20" t="s">
+        <v>383</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="E101" s="17" t="s">
+        <v>384</v>
+      </c>
+      <c r="F101" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G101" s="7"/>
+      <c r="H101" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="I101" s="7" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="7" t="s">
-        <v>385</v>
-      </c>
-      <c r="B102" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="C102" s="20" t="s">
-        <v>387</v>
-      </c>
-      <c r="D102" s="7" t="s">
+      <c r="A102" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C102" s="9"/>
+      <c r="D102" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="E102" s="17" t="s">
-        <v>388</v>
-      </c>
-      <c r="F102" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G102" s="7"/>
-      <c r="H102" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="I102" s="7" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="B103" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="C103" s="9"/>
-      <c r="D103" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="E103" s="9" t="s">
+      <c r="E102" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="F103" s="9" t="s">
+      <c r="F102" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G103" s="9" t="s">
+      <c r="G102" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="H103" s="9" t="s">
+      <c r="H102" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="I103" s="14" t="s">
+      <c r="I102" s="14" t="s">
         <v>199</v>
       </c>
     </row>
@@ -5478,7 +5433,7 @@
     <hyperlink ref="I32" r:id="rId2" xr:uid="{574D93C5-0522-4DEE-A777-CB1BD468A7B3}"/>
     <hyperlink ref="H26" r:id="rId3" display="mailto:delphine.cado@umontreal.ca" xr:uid="{0E0BF38D-BCA7-4652-84E3-BBE8A015792A}"/>
     <hyperlink ref="I26" r:id="rId4" xr:uid="{27792995-CED1-460A-9DC6-1C7D908E58F9}"/>
-    <hyperlink ref="I103" r:id="rId5" xr:uid="{FA15E077-C7FD-42E7-A5F3-AC50929F77F4}"/>
+    <hyperlink ref="I102" r:id="rId5" xr:uid="{FA15E077-C7FD-42E7-A5F3-AC50929F77F4}"/>
     <hyperlink ref="I31" r:id="rId6" xr:uid="{2D74694A-18E3-4092-AA2F-BC65E158D410}"/>
     <hyperlink ref="H15" r:id="rId7" display="mailto:hugo.bernier@umontreal.ca" xr:uid="{3F591457-DA50-462E-B1CA-F2F56ED9E3DD}"/>
     <hyperlink ref="I15" r:id="rId8" xr:uid="{11A3F440-1028-45FC-8DC2-DE60A7EA0AD9}"/>
@@ -5501,6 +5456,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f6670ae2-8190-4e72-909e-d717fe03ced5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="00db0817-461a-4a69-8eb5-8daf0756d296" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007812637FDE95774892D21861907C1625" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="9e26b686a71b543072340cfd27a56c29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f6670ae2-8190-4e72-909e-d717fe03ced5" xmlns:ns3="00db0817-461a-4a69-8eb5-8daf0756d296" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8d151e41c23af60827e9e8828a6e0ebd" ns2:_="" ns3:_="">
     <xsd:import namespace="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
@@ -5735,17 +5701,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f6670ae2-8190-4e72-909e-d717fe03ced5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="00db0817-461a-4a69-8eb5-8daf0756d296" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5756,6 +5711,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="00db0817-461a-4a69-8eb5-8daf0756d296"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{141ACCEB-C60B-4854-82C0-9885432D8ACB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5774,23 +5746,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="00db0817-461a-4a69-8eb5-8daf0756d296"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Organiser les images des collections spéciales et ajuster la taille pour que certaines images trop grandes soient plus adaptées au web.
</commit_message>
<xml_diff>
--- a/content/personnel/liste-personnel.xlsx
+++ b/content/personnel/liste-personnel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p1212882\siteWeb\coquille-web\content\personnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671346F1-2081-4FA7-8D22-F2E870AC72F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05E1D86-CFBC-4BE4-9D74-8AC31707E252}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15360" yWindow="3150" windowWidth="34200" windowHeight="26295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2595,9 +2595,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2774,7 +2774,7 @@
         <v>74</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>75</v>
@@ -5376,26 +5376,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f6670ae2-8190-4e72-909e-d717fe03ced5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="00db0817-461a-4a69-8eb5-8daf0756d296" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007812637FDE95774892D21861907C1625" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="9e26b686a71b543072340cfd27a56c29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f6670ae2-8190-4e72-909e-d717fe03ced5" xmlns:ns3="00db0817-461a-4a69-8eb5-8daf0756d296" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8d151e41c23af60827e9e8828a6e0ebd" ns2:_="" ns3:_="">
     <xsd:import namespace="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
@@ -5630,32 +5610,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="00db0817-461a-4a69-8eb5-8daf0756d296"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f6670ae2-8190-4e72-909e-d717fe03ced5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="00db0817-461a-4a69-8eb5-8daf0756d296" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{141ACCEB-C60B-4854-82C0-9885432D8ACB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5672,4 +5647,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="00db0817-461a-4a69-8eb5-8daf0756d296"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ajout de Laurence Charest au répertoire
</commit_message>
<xml_diff>
--- a/content/personnel/liste-personnel.xlsx
+++ b/content/personnel/liste-personnel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p1212882\siteWeb\coquille-web\content\personnel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tardimat\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05E1D86-CFBC-4BE4-9D74-8AC31707E252}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{02CEEDCE-0652-4C68-BEF8-B1439F073ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="3150" windowWidth="34200" windowHeight="26295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1065" yWindow="8190" windowWidth="43200" windowHeight="23445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="661">
   <si>
     <t>Borsi</t>
   </si>
@@ -1990,13 +1990,31 @@
   </si>
   <si>
     <t>Direction des bibliothèques sociétés et création; Bibliothèque d'aménagement; Bibliothèque de droit; Bibliothèque Thérèse-Gouin-Décarie; Bibliothèque du Campus de Laval; Bibliothèque de musique</t>
+  </si>
+  <si>
+    <t>Laurence</t>
+  </si>
+  <si>
+    <t>Charest</t>
+  </si>
+  <si>
+    <t>Papyrus</t>
+  </si>
+  <si>
+    <t>514-343-6111, poste 4019</t>
+  </si>
+  <si>
+    <t>laurence.charest@umontreal.ca</t>
+  </si>
+  <si>
+    <t>https://teams.microsoft.com/l/chat/0/0?users=laurence.charest@umontreal.ca</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2246,16 +2264,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A0AF7E1-A614-44BF-8C48-5C26377DC552}" name="Tableau1" displayName="Tableau1" ref="A1:I98" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:I98" xr:uid="{4F6A1D8F-9220-4675-A202-2173F3493722}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A0AF7E1-A614-44BF-8C48-5C26377DC552}" name="Tableau1" displayName="Tableau1" ref="A1:I99" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:I99" xr:uid="{4F6A1D8F-9220-4675-A202-2173F3493722}">
     <filterColumn colId="5">
       <filters>
         <filter val="Direction de la recherche et des initiatives numériques"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState ref="A2:I98">
-    <sortCondition ref="A1:A98"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I99">
+    <sortCondition ref="A1:A99"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4B04E1AF-0079-4AD2-81CA-E8A433733E21}" name="nom"/>
@@ -2273,9 +2291,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2313,9 +2331,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2348,26 +2366,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2400,26 +2401,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2593,14 +2577,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="3" width="18.85546875" customWidth="1"/>
@@ -2612,7 +2596,7 @@
     <col min="9" max="9" width="75.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>615</v>
       </c>
@@ -2641,7 +2625,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>8</v>
       </c>
@@ -2670,7 +2654,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>598</v>
       </c>
@@ -2699,7 +2683,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>469</v>
       </c>
@@ -2728,7 +2712,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>169</v>
       </c>
@@ -2757,7 +2741,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>71</v>
       </c>
@@ -2786,7 +2770,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>437</v>
       </c>
@@ -2815,7 +2799,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>574</v>
       </c>
@@ -2844,7 +2828,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>341</v>
       </c>
@@ -2869,7 +2853,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>399</v>
       </c>
@@ -2898,7 +2882,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>78</v>
       </c>
@@ -2925,7 +2909,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>124</v>
       </c>
@@ -2954,7 +2938,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>34</v>
       </c>
@@ -2983,7 +2967,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>34</v>
       </c>
@@ -3008,7 +2992,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>282</v>
       </c>
@@ -3033,7 +3017,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>509</v>
       </c>
@@ -3060,7 +3044,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>560</v>
       </c>
@@ -3089,7 +3073,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>305</v>
       </c>
@@ -3114,7 +3098,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>0</v>
       </c>
@@ -3143,7 +3127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>208</v>
       </c>
@@ -3172,7 +3156,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>495</v>
       </c>
@@ -3201,7 +3185,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>464</v>
       </c>
@@ -3228,7 +3212,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>275</v>
       </c>
@@ -3255,7 +3239,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>527</v>
       </c>
@@ -3284,7 +3268,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>162</v>
       </c>
@@ -3311,2066 +3295,2094 @@
         <v>168</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>521</v>
+        <v>656</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>522</v>
+        <v>655</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>657</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>658</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>659</v>
+      </c>
+      <c r="I26" s="15" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>632</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>523</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G27" s="7" t="s">
         <v>524</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H27" s="7" t="s">
         <v>525</v>
       </c>
-      <c r="I26" s="7" t="s">
+      <c r="I27" s="7" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="9" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>502</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B28" s="9" t="s">
         <v>503</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C28" s="9" t="s">
         <v>504</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D28" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E28" s="13" t="s">
         <v>505</v>
       </c>
-      <c r="F27" s="9" t="s">
+      <c r="F28" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G28" s="9" t="s">
         <v>506</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="H28" s="9" t="s">
         <v>507</v>
       </c>
-      <c r="I27" s="9" t="s">
+      <c r="I28" s="9" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="7" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B29" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C29" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E29" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F29" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G29" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="H28" s="7" t="s">
+      <c r="H29" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="I28" s="7" t="s">
+      <c r="I29" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="7" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B30" s="7" t="s">
         <v>445</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C30" s="7" t="s">
         <v>446</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D30" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E30" s="17" t="s">
         <v>447</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F30" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G30" s="7" t="s">
         <v>448</v>
       </c>
-      <c r="H29" s="7" t="s">
+      <c r="H30" s="7" t="s">
         <v>449</v>
       </c>
-      <c r="I29" s="7" t="s">
+      <c r="I30" s="7" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="9" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B31" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C31" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D31" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="E31" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="F31" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G30" s="9" t="s">
+      <c r="G31" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="H30" s="9" t="s">
+      <c r="H31" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="I30" s="14" t="s">
+      <c r="I31" s="14" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="7" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B32" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C32" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D32" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7" t="s">
+      <c r="E32" s="7"/>
+      <c r="F32" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G31" s="7" t="s">
+      <c r="G32" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H31" s="7" t="s">
+      <c r="H32" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="I31" s="15" t="s">
+      <c r="I32" s="15" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="9" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
         <v>515</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B33" s="9" t="s">
         <v>516</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C33" s="9" t="s">
         <v>517</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D33" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="E33" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="F32" s="9" t="s">
+      <c r="F33" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G32" s="9" t="s">
+      <c r="G33" s="9" t="s">
         <v>518</v>
       </c>
-      <c r="H32" s="9" t="s">
+      <c r="H33" s="9" t="s">
         <v>519</v>
       </c>
-      <c r="I32" s="9" t="s">
+      <c r="I33" s="9" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="7" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B34" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C34" s="7" t="s">
         <v>356</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>630</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>357</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>358</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>190</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="7" t="s">
+        <v>630</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>635</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F35" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G34" s="7" t="s">
+      <c r="G35" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="H34" s="7" t="s">
+      <c r="H35" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="I34" s="7" t="s">
+      <c r="I35" s="7" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="9" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>451</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B36" s="9" t="s">
         <v>452</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C36" s="9" t="s">
         <v>453</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D36" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="E35" s="13" t="s">
+      <c r="E36" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="F35" s="9" t="s">
+      <c r="F36" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="G35" s="9" t="s">
+      <c r="G36" s="9" t="s">
         <v>454</v>
       </c>
-      <c r="H35" s="9" t="s">
+      <c r="H36" s="9" t="s">
         <v>455</v>
       </c>
-      <c r="I35" s="9" t="s">
+      <c r="I36" s="9" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="9" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B37" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C37" s="9" t="s">
         <v>289</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>625</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>290</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>182</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="9" t="s">
+        <v>625</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F38" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="G38" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="H37" s="9" t="s">
+      <c r="H38" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="I37" s="9" t="s">
+      <c r="I38" s="9" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="7" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B39" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7" t="s">
+      <c r="C39" s="7"/>
+      <c r="D39" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7" t="s">
+      <c r="E39" s="7"/>
+      <c r="F39" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="G38" s="7" t="s">
+      <c r="G39" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="H38" s="7" t="s">
+      <c r="H39" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="I38" s="7" t="s">
+      <c r="I39" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="7" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B40" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C40" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D40" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E40" s="7" t="s">
         <v>628</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="F40" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="G39" s="7" t="s">
+      <c r="G40" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="H39" s="7" t="s">
+      <c r="H40" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="I39" s="7" t="s">
+      <c r="I40" s="7" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="9" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
         <v>548</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B41" s="9" t="s">
         <v>549</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C41" s="9" t="s">
         <v>550</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D41" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E41" s="9" t="s">
         <v>460</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F41" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G40" s="9" t="s">
+      <c r="G41" s="9" t="s">
         <v>551</v>
       </c>
-      <c r="H40" s="9" t="s">
+      <c r="H41" s="9" t="s">
         <v>552</v>
       </c>
-      <c r="I40" s="9" t="s">
+      <c r="I41" s="9" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="9" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B42" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C42" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D42" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="E42" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F41" s="9" t="s">
+      <c r="F42" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="G42" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="H41" s="9" t="s">
+      <c r="H42" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="I41" s="9" t="s">
+      <c r="I42" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="9" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
         <v>360</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B43" s="9" t="s">
         <v>361</v>
       </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9" t="s">
+      <c r="C43" s="9"/>
+      <c r="D43" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E42" s="9" t="s">
+      <c r="E43" s="9" t="s">
         <v>362</v>
       </c>
-      <c r="F42" s="9" t="s">
+      <c r="F43" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="G42" s="9" t="s">
+      <c r="G43" s="9" t="s">
         <v>364</v>
       </c>
-      <c r="H42" s="9" t="s">
+      <c r="H43" s="9" t="s">
         <v>365</v>
       </c>
-      <c r="I42" s="9" t="s">
+      <c r="I43" s="9" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="9" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
         <v>475</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B44" s="9" t="s">
         <v>476</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C44" s="9" t="s">
         <v>477</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D44" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E43" s="13" t="s">
+      <c r="E44" s="13" t="s">
         <v>637</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="F44" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G43" s="9" t="s">
+      <c r="G44" s="9" t="s">
         <v>478</v>
       </c>
-      <c r="H43" s="9" t="s">
+      <c r="H44" s="9" t="s">
         <v>479</v>
       </c>
-      <c r="I43" s="9" t="s">
+      <c r="I44" s="9" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="7" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
         <v>639</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B45" s="7" t="s">
         <v>638</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="7" t="s">
+      <c r="C45" s="15"/>
+      <c r="D45" s="7" t="s">
         <v>641</v>
       </c>
-      <c r="E44" s="17" t="s">
+      <c r="E45" s="17" t="s">
         <v>642</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="F45" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7" t="s">
+      <c r="G45" s="7"/>
+      <c r="H45" s="7" t="s">
         <v>640</v>
       </c>
-      <c r="I44" s="7"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="9" t="s">
+      <c r="I45" s="7"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B46" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="C46" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D46" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="9" t="s">
+      <c r="E46" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F45" s="9" t="s">
+      <c r="F46" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G45" s="9" t="s">
+      <c r="G46" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="H45" s="9" t="s">
+      <c r="H46" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="I45" s="9" t="s">
+      <c r="I46" s="9" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H46" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="I46" s="7" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>176</v>
       </c>
       <c r="B47" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B48" s="7" t="s">
         <v>533</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C48" s="7" t="s">
         <v>534</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D48" s="7" t="s">
         <v>535</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="E48" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="F47" s="7" t="s">
+      <c r="F48" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="G47" s="7" t="s">
+      <c r="G48" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="H47" s="7" t="s">
+      <c r="H48" s="7" t="s">
         <v>536</v>
       </c>
-      <c r="I47" s="7" t="s">
+      <c r="I48" s="7" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="9" t="s">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B49" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C49" s="9" t="s">
         <v>389</v>
       </c>
-      <c r="D48" s="9" t="s">
+      <c r="D49" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="E48" s="13" t="s">
+      <c r="E49" s="13" t="s">
         <v>390</v>
       </c>
-      <c r="F48" s="9" t="s">
+      <c r="F49" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="G48" s="9" t="s">
+      <c r="G49" s="9" t="s">
         <v>391</v>
       </c>
-      <c r="H48" s="9" t="s">
+      <c r="H49" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="I48" s="9" t="s">
+      <c r="I49" s="9" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="7" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B50" s="7" t="s">
         <v>312</v>
-      </c>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>636</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="H49" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="I49" s="7" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="7" t="s">
-        <v>612</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>295</v>
       </c>
       <c r="C50" s="7"/>
       <c r="D50" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>612</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E50" s="7" t="s">
+      <c r="E51" s="7" t="s">
         <v>613</v>
       </c>
-      <c r="F50" s="7" t="s">
+      <c r="F51" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G50" s="7" t="s">
+      <c r="G51" s="7" t="s">
         <v>614</v>
       </c>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="7" t="s">
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B52" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C52" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D52" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="E52" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F51" s="7" t="s">
+      <c r="F52" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G51" s="7" t="s">
+      <c r="G52" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H51" s="7" t="s">
+      <c r="H52" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I51" s="7" t="s">
+      <c r="I52" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
-      <c r="A52" s="9" t="s">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
         <v>488</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B53" s="9" t="s">
         <v>489</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C53" s="9" t="s">
         <v>490</v>
       </c>
-      <c r="D52" s="9" t="s">
+      <c r="D53" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="E52" s="9" t="s">
+      <c r="E53" s="9" t="s">
         <v>491</v>
       </c>
-      <c r="F52" s="9" t="s">
+      <c r="F53" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G52" s="9" t="s">
+      <c r="G53" s="9" t="s">
         <v>492</v>
       </c>
-      <c r="H52" s="9" t="s">
+      <c r="H53" s="9" t="s">
         <v>493</v>
       </c>
-      <c r="I52" s="9" t="s">
+      <c r="I53" s="9" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
-      <c r="A53" t="s">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>567</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>568</v>
       </c>
-      <c r="C53" s="22" t="s">
+      <c r="C54" s="22" t="s">
         <v>569</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>11</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E54" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F54" t="s">
         <v>13</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G54" t="s">
         <v>571</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H54" t="s">
         <v>572</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I54" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
-      <c r="A54" s="7" t="s">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B55" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C55" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D55" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="E55" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="F54" s="7" t="s">
+      <c r="F55" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G54" s="7" t="s">
+      <c r="G55" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="H54" s="7" t="s">
+      <c r="H55" s="7" t="s">
         <v>339</v>
       </c>
-      <c r="I54" s="7" t="s">
+      <c r="I55" s="7" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="7" t="s">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B56" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C56" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D56" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="E56" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F55" s="7" t="s">
+      <c r="F56" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G55" s="7" t="s">
+      <c r="G56" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H55" s="7" t="s">
+      <c r="H56" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I55" s="7" t="s">
+      <c r="I56" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="9" t="s">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B57" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9" t="s">
+      <c r="C57" s="9"/>
+      <c r="D57" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E56" s="9" t="s">
+      <c r="E57" s="9" t="s">
         <v>626</v>
       </c>
-      <c r="F56" s="9" t="s">
+      <c r="F57" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="G56" s="9" t="s">
+      <c r="G57" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="H56" s="14" t="s">
+      <c r="H57" s="14" t="s">
         <v>627</v>
       </c>
-      <c r="I56" s="9" t="s">
+      <c r="I57" s="9" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
-      <c r="A57" s="9" t="s">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B58" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C57" s="9" t="s">
+      <c r="C58" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D57" s="9" t="s">
+      <c r="D58" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E57" s="9" t="s">
+      <c r="E58" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F57" s="9" t="s">
+      <c r="F58" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G57" s="9" t="s">
+      <c r="G58" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="H57" s="9" t="s">
+      <c r="H58" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="I57" s="9" t="s">
+      <c r="I58" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
-      <c r="A58" s="7" t="s">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
         <v>554</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B59" s="7" t="s">
         <v>555</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C59" s="7" t="s">
         <v>556</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D59" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="E58" s="7" t="s">
+      <c r="E59" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F58" s="7" t="s">
+      <c r="F59" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G58" s="7" t="s">
+      <c r="G59" s="7" t="s">
         <v>557</v>
       </c>
-      <c r="H58" s="7" t="s">
+      <c r="H59" s="7" t="s">
         <v>558</v>
       </c>
-      <c r="I58" s="7" t="s">
+      <c r="I59" s="7" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
-      <c r="A59" s="9" t="s">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
         <v>538</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B60" s="9" t="s">
         <v>533</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="C60" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="D59" s="9" t="s">
+      <c r="D60" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E59" s="9" t="s">
+      <c r="E60" s="9" t="s">
         <v>633</v>
       </c>
-      <c r="F59" s="9" t="s">
+      <c r="F60" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="G59" s="9" t="s">
+      <c r="G60" s="9" t="s">
         <v>540</v>
       </c>
-      <c r="H59" s="9" t="s">
+      <c r="H60" s="9" t="s">
         <v>541</v>
       </c>
-      <c r="I59" s="9" t="s">
+      <c r="I60" s="9" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
-      <c r="A60" s="9" t="s">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="B61" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="C60" s="9" t="s">
+      <c r="C61" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="D60" s="9" t="s">
+      <c r="D61" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E60" s="9" t="s">
+      <c r="E61" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="F60" s="9" t="s">
+      <c r="F61" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G60" s="9" t="s">
+      <c r="G61" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="H60" s="9" t="s">
+      <c r="H61" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="I60" s="9" t="s">
+      <c r="I61" s="9" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="61" spans="1:9" s="4" customFormat="1">
-      <c r="A61" s="9" t="s">
+    <row r="62" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="B62" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="C61" s="9" t="s">
+      <c r="C62" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="D61" s="9" t="s">
+      <c r="D62" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="E61" s="9" t="s">
+      <c r="E62" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="F61" s="9" t="s">
+      <c r="F62" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G61" s="9" t="s">
+      <c r="G62" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="H61" s="9" t="s">
+      <c r="H62" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="I61" s="9" t="s">
+      <c r="I62" s="9" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
-      <c r="A62" s="7" t="s">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B63" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C63" s="7" t="s">
         <v>369</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D63" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="E62" s="8" t="s">
+      <c r="E63" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="F62" s="7" t="s">
+      <c r="F63" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G62" s="7" t="s">
+      <c r="G63" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="H62" s="7" t="s">
+      <c r="H63" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="I62" s="7" t="s">
+      <c r="I63" s="7" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="63" spans="1:9" s="5" customFormat="1">
-      <c r="A63" s="9" t="s">
+    <row r="64" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="9" t="s">
         <v>424</v>
       </c>
-      <c r="B63" s="9" t="s">
+      <c r="B64" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="C63" s="9" t="s">
+      <c r="C64" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="D63" s="9" t="s">
+      <c r="D64" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="E63" s="9" t="s">
+      <c r="E64" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="F63" s="9" t="s">
+      <c r="F64" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="G63" s="9" t="s">
+      <c r="G64" s="9" t="s">
         <v>428</v>
       </c>
-      <c r="H63" s="9" t="s">
+      <c r="H64" s="9" t="s">
         <v>429</v>
       </c>
-      <c r="I63" s="9" t="s">
+      <c r="I64" s="9" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
-      <c r="A64" s="7" t="s">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B65" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="C65" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D65" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="E64" s="7" t="s">
+      <c r="E65" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="F64" s="7" t="s">
+      <c r="F65" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="G64" s="7" t="s">
+      <c r="G65" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="H64" s="7" t="s">
+      <c r="H65" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="I64" s="7" t="s">
+      <c r="I65" s="7" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
-      <c r="A65" s="11" t="s">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B65" s="11" t="s">
+      <c r="B66" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11" t="s">
+      <c r="C66" s="11"/>
+      <c r="D66" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E65" s="12" t="s">
+      <c r="E66" s="12" t="s">
         <v>370</v>
       </c>
-      <c r="F65" s="11" t="s">
+      <c r="F66" s="11" t="s">
         <v>652</v>
       </c>
-      <c r="G65" s="11" t="s">
+      <c r="G66" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H65" s="11" t="s">
+      <c r="H66" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I65" s="11" t="s">
+      <c r="I66" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
-      <c r="A66" s="7" t="s">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B67" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E66" s="7"/>
-      <c r="F66" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G66" s="7"/>
-      <c r="H66" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="I66" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
-      <c r="A67" s="7" t="s">
-        <v>395</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>647</v>
       </c>
       <c r="C67" s="7"/>
       <c r="D67" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I67" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>647</v>
+      </c>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7" t="s">
         <v>648</v>
       </c>
-      <c r="E67" s="17"/>
-      <c r="F67" s="7" t="s">
+      <c r="E68" s="17"/>
+      <c r="F68" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="G67" s="16" t="s">
+      <c r="G68" s="16" t="s">
         <v>274</v>
       </c>
-      <c r="H67" s="15" t="s">
+      <c r="H68" s="15" t="s">
         <v>649</v>
       </c>
-      <c r="I67" s="16"/>
-    </row>
-    <row r="68" spans="1:9">
-      <c r="A68" s="7" t="s">
+      <c r="I68" s="16"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B69" s="7" t="s">
         <v>482</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C69" s="7" t="s">
         <v>483</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>484</v>
-      </c>
-      <c r="F68" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G68" s="7" t="s">
-        <v>485</v>
-      </c>
-      <c r="H68" s="7" t="s">
-        <v>486</v>
-      </c>
-      <c r="I68" s="7" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
-      <c r="A69" s="7" t="s">
-        <v>432</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>431</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>433</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E69" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="I69" s="7" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="F69" s="7" t="s">
+      <c r="F70" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="G69" s="7" t="s">
+      <c r="G70" s="7" t="s">
         <v>434</v>
       </c>
-      <c r="H69" s="7" t="s">
+      <c r="H70" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="I69" s="7" t="s">
+      <c r="I70" s="7" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="70" spans="1:9" s="4" customFormat="1">
-      <c r="A70" s="7" t="s">
+    <row r="71" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B71" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C71" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D71" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E70" s="7" t="s">
+      <c r="E71" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="F70" s="7" t="s">
+      <c r="F71" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G70" s="7" t="s">
+      <c r="G71" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="H70" s="7" t="s">
+      <c r="H71" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="I70" s="7" t="s">
+      <c r="I71" s="7" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
-      <c r="A71" s="7" t="s">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B72" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C71" s="7" t="s">
+      <c r="C72" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E71" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="G71" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="H71" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="I71" s="7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
-      <c r="A72" s="16" t="s">
-        <v>257</v>
-      </c>
-      <c r="B72" s="16" t="s">
-        <v>258</v>
-      </c>
-      <c r="C72" s="16" t="s">
-        <v>259</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E72" s="16" t="s">
+      <c r="E72" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="G72" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="H72" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="I72" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="C73" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E73" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="F72" s="16" t="s">
+      <c r="F73" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="G72" s="16" t="s">
+      <c r="G73" s="16" t="s">
         <v>262</v>
       </c>
-      <c r="H72" s="16" t="s">
+      <c r="H73" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="I72" s="16" t="s">
+      <c r="I73" s="16" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="73" spans="1:9" s="4" customFormat="1">
-      <c r="A73" s="9" t="s">
+    <row r="74" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="B73" s="9" t="s">
+      <c r="B74" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="C73" s="9" t="s">
+      <c r="C74" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="D73" s="9" t="s">
+      <c r="D74" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E73" s="9" t="s">
+      <c r="E74" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="F73" s="9" t="s">
+      <c r="F74" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G73" s="9" t="s">
+      <c r="G74" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="H73" s="9" t="s">
+      <c r="H74" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="I73" s="9" t="s">
+      <c r="I74" s="9" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
-      <c r="A74" s="9" t="s">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B74" s="9" t="s">
+      <c r="B75" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C74" s="9" t="s">
+      <c r="C75" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D74" s="9" t="s">
+      <c r="D75" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E74" s="13" t="s">
+      <c r="E75" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F74" s="9" t="s">
+      <c r="F75" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G74" s="9" t="s">
+      <c r="G75" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="H74" s="9" t="s">
+      <c r="H75" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="I74" s="9" t="s">
+      <c r="I75" s="9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
-      <c r="A75" s="16" t="s">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="B75" s="16" t="s">
+      <c r="B76" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="C75" s="16" t="s">
+      <c r="C76" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="D75" s="16" t="s">
+      <c r="D76" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="E75" s="8" t="s">
+      <c r="E76" s="8" t="s">
         <v>650</v>
       </c>
-      <c r="F75" s="16" t="s">
+      <c r="F76" s="16" t="s">
         <v>654</v>
       </c>
-      <c r="G75" s="16" t="s">
+      <c r="G76" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="H75" s="16" t="s">
+      <c r="H76" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="I75" s="16" t="s">
+      <c r="I76" s="16" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
-      <c r="A76" s="9" t="s">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="B77" s="9" t="s">
         <v>348</v>
-      </c>
-      <c r="C76" s="9"/>
-      <c r="D76" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="E76" s="9" t="s">
-        <v>350</v>
-      </c>
-      <c r="F76" s="9" t="s">
-        <v>307</v>
-      </c>
-      <c r="G76" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="H76" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="I76" s="9" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9">
-      <c r="A77" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="B77" s="9" t="s">
-        <v>223</v>
       </c>
       <c r="C77" s="9"/>
       <c r="D77" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="F77" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="G77" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="H77" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="I77" s="9" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E77" s="9"/>
-      <c r="F77" s="9" t="s">
+      <c r="E78" s="9"/>
+      <c r="F78" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="G77" s="9" t="s">
+      <c r="G78" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="H77" s="9" t="s">
+      <c r="H78" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="I77" s="9" t="s">
+      <c r="I78" s="9" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
-      <c r="A78" s="9" t="s">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B79" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="C78" s="9" t="s">
+      <c r="C79" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="D78" s="9" t="s">
+      <c r="D79" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E78" s="11" t="s">
+      <c r="E79" s="11" t="s">
         <v>629</v>
       </c>
-      <c r="F78" s="9" t="s">
+      <c r="F79" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="G78" s="9" t="s">
+      <c r="G79" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="H78" s="9" t="s">
+      <c r="H79" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="I78" s="9" t="s">
+      <c r="I79" s="9" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
-      <c r="A79" s="9" t="s">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="s">
         <v>644</v>
       </c>
-      <c r="B79" s="9" t="s">
+      <c r="B80" s="9" t="s">
         <v>643</v>
       </c>
-      <c r="C79" s="9"/>
-      <c r="D79" s="9" t="s">
+      <c r="C80" s="9"/>
+      <c r="D80" s="9" t="s">
         <v>645</v>
       </c>
-      <c r="E79" s="13"/>
-      <c r="F79" s="9" t="s">
+      <c r="E80" s="13"/>
+      <c r="F80" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="G79" s="9"/>
-      <c r="H79" s="9" t="s">
+      <c r="G80" s="9"/>
+      <c r="H80" s="9" t="s">
         <v>646</v>
       </c>
-      <c r="I79" s="18"/>
-    </row>
-    <row r="80" spans="1:9">
-      <c r="A80" t="s">
+      <c r="I80" s="18"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>592</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B81" t="s">
         <v>593</v>
       </c>
-      <c r="C80" s="22" t="s">
+      <c r="C81" s="22" t="s">
         <v>594</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D81" t="s">
         <v>195</v>
       </c>
-      <c r="E80" s="3" t="s">
+      <c r="E81" s="3" t="s">
         <v>595</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F81" t="s">
         <v>60</v>
       </c>
-      <c r="H80" t="s">
+      <c r="H81" t="s">
         <v>596</v>
       </c>
-      <c r="I80" t="s">
+      <c r="I81" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
-      <c r="A81" s="7" t="s">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="B81" s="7" t="s">
+      <c r="B82" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="C81" s="7" t="s">
+      <c r="C82" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="D81" s="7" t="s">
+      <c r="D82" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E81" s="17" t="s">
+      <c r="E82" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="F81" s="7" t="s">
+      <c r="F82" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G81" s="16" t="s">
+      <c r="G82" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="H81" s="16" t="s">
+      <c r="H82" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="I81" s="16" t="s">
+      <c r="I82" s="16" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
-      <c r="A82" s="7" t="s">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B82" s="7" t="s">
+      <c r="B83" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C82" s="7" t="s">
+      <c r="C83" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D82" s="7" t="s">
+      <c r="D83" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E82" s="7" t="s">
+      <c r="E83" s="7" t="s">
         <v>634</v>
       </c>
-      <c r="F82" s="7" t="s">
+      <c r="F83" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G82" s="16" t="s">
+      <c r="G83" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="H82" s="16" t="s">
+      <c r="H83" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="I82" s="16" t="s">
+      <c r="I83" s="16" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
-      <c r="A83" s="9" t="s">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B83" s="9" t="s">
+      <c r="B84" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="C83" s="9" t="s">
+      <c r="C84" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="D83" s="9" t="s">
+      <c r="D84" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E83" s="9" t="s">
+      <c r="E84" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F83" s="9" t="s">
+      <c r="F84" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G83" s="11" t="s">
+      <c r="G84" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="H83" s="11" t="s">
+      <c r="H84" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="I83" s="11" t="s">
+      <c r="I84" s="11" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
-      <c r="A84" s="7" t="s">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="7" t="s">
         <v>543</v>
       </c>
-      <c r="B84" s="7" t="s">
+      <c r="B85" s="7" t="s">
         <v>533</v>
       </c>
-      <c r="C84" s="7" t="s">
+      <c r="C85" s="7" t="s">
         <v>544</v>
       </c>
-      <c r="D84" s="7" t="s">
+      <c r="D85" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E84" s="7" t="s">
+      <c r="E85" s="7" t="s">
         <v>498</v>
       </c>
-      <c r="F84" s="7" t="s">
+      <c r="F85" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G84" s="16" t="s">
+      <c r="G85" s="16" t="s">
         <v>545</v>
       </c>
-      <c r="H84" s="16" t="s">
+      <c r="H85" s="16" t="s">
         <v>546</v>
       </c>
-      <c r="I84" s="16" t="s">
+      <c r="I85" s="16" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
-      <c r="A85" s="7" t="s">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="B85" s="7" t="s">
+      <c r="B86" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="C85" s="7" t="s">
+      <c r="C86" s="7" t="s">
         <v>409</v>
       </c>
-      <c r="D85" s="7" t="s">
+      <c r="D86" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E85" s="17" t="s">
+      <c r="E86" s="17" t="s">
         <v>410</v>
       </c>
-      <c r="F85" s="7" t="s">
+      <c r="F86" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G85" s="16"/>
-      <c r="H85" s="15" t="s">
+      <c r="G86" s="16"/>
+      <c r="H86" s="15" t="s">
         <v>411</v>
       </c>
-      <c r="I85" s="16" t="s">
+      <c r="I86" s="16" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
-      <c r="A86" s="9" t="s">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="9" t="s">
         <v>374</v>
       </c>
-      <c r="B86" s="9" t="s">
+      <c r="B87" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="C86" s="9" t="s">
+      <c r="C87" s="9" t="s">
         <v>376</v>
       </c>
-      <c r="D86" s="9" t="s">
+      <c r="D87" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E86" s="13" t="s">
+      <c r="E87" s="13" t="s">
         <v>377</v>
       </c>
-      <c r="F86" s="9" t="s">
+      <c r="F87" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="G86" s="11" t="s">
+      <c r="G87" s="11" t="s">
         <v>378</v>
       </c>
-      <c r="H86" s="11" t="s">
+      <c r="H87" s="11" t="s">
         <v>379</v>
       </c>
-      <c r="I86" s="11" t="s">
+      <c r="I87" s="11" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
-      <c r="A87" t="s">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>581</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>575</v>
       </c>
-      <c r="C87" s="22" t="s">
+      <c r="C88" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D88" t="s">
         <v>11</v>
       </c>
-      <c r="E87" s="3" t="s">
+      <c r="E88" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F88" t="s">
         <v>30</v>
       </c>
-      <c r="G87" s="4" t="s">
+      <c r="G88" s="4" t="s">
         <v>584</v>
       </c>
-      <c r="H87" s="4" t="s">
+      <c r="H88" s="4" t="s">
         <v>585</v>
       </c>
-      <c r="I87" s="4" t="s">
+      <c r="I88" s="4" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
-      <c r="A88" t="s">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>587</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B89" t="s">
         <v>588</v>
       </c>
-      <c r="C88" s="19"/>
-      <c r="D88" t="s">
+      <c r="C89" s="19"/>
+      <c r="D89" t="s">
         <v>17</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E89" t="s">
         <v>18</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F89" t="s">
         <v>13</v>
       </c>
-      <c r="G88" s="4" t="s">
+      <c r="G89" s="4" t="s">
         <v>589</v>
       </c>
-      <c r="H88" s="4" t="s">
+      <c r="H89" s="4" t="s">
         <v>590</v>
       </c>
-      <c r="I88" s="4" t="s">
+      <c r="I89" s="4" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="89" spans="1:9" s="4" customFormat="1">
-      <c r="A89" s="7" t="s">
+    <row r="90" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="B89" s="7" t="s">
+      <c r="B90" s="7" t="s">
         <v>395</v>
       </c>
-      <c r="C89" s="7" t="s">
+      <c r="C90" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="D89" s="7" t="s">
+      <c r="D90" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E89" s="17" t="s">
+      <c r="E90" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="F89" s="7" t="s">
+      <c r="F90" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G89" s="16" t="s">
+      <c r="G90" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="H89" s="16" t="s">
+      <c r="H90" s="16" t="s">
         <v>397</v>
       </c>
-      <c r="I89" s="16" t="s">
+      <c r="I90" s="16" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="90" spans="1:9" s="4" customFormat="1">
-      <c r="A90" s="7" t="s">
+    <row r="91" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B90" s="7" t="s">
+      <c r="B91" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C90" s="7"/>
-      <c r="D90" s="7" t="s">
+      <c r="C91" s="7"/>
+      <c r="D91" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E90" s="17" t="s">
+      <c r="E91" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="F90" s="7" t="s">
+      <c r="F91" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G90" s="16"/>
-      <c r="H90" s="16" t="s">
+      <c r="G91" s="16"/>
+      <c r="H91" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="I90" s="16" t="s">
+      <c r="I91" s="16" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
-      <c r="A91" s="11" t="s">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="11" t="s">
         <v>605</v>
       </c>
-      <c r="B91" s="11" t="s">
+      <c r="B92" s="11" t="s">
         <v>599</v>
       </c>
-      <c r="C91" s="9" t="s">
+      <c r="C92" s="9" t="s">
         <v>606</v>
       </c>
-      <c r="D91" s="11" t="s">
+      <c r="D92" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="E91" s="11" t="s">
+      <c r="E92" s="11" t="s">
         <v>607</v>
       </c>
-      <c r="F91" s="11" t="s">
+      <c r="F92" s="11" t="s">
         <v>608</v>
       </c>
-      <c r="G91" s="11" t="s">
+      <c r="G92" s="11" t="s">
         <v>609</v>
       </c>
-      <c r="H91" s="11" t="s">
+      <c r="H92" s="11" t="s">
         <v>610</v>
       </c>
-      <c r="I91" s="11" t="s">
+      <c r="I92" s="11" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
-      <c r="A92" s="11" t="s">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="B92" s="11" t="s">
+      <c r="B93" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="C92" s="23"/>
-      <c r="D92" s="11" t="s">
+      <c r="C93" s="23"/>
+      <c r="D93" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="E92" s="11"/>
-      <c r="F92" s="11" t="s">
+      <c r="E93" s="11"/>
+      <c r="F93" s="11" t="s">
         <v>653</v>
       </c>
-      <c r="G92" s="11" t="s">
+      <c r="G93" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="H92" s="11" t="s">
+      <c r="H93" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="I92" s="11" t="s">
+      <c r="I93" s="11" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
-      <c r="A93" s="7" t="s">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="7" t="s">
         <v>418</v>
       </c>
-      <c r="B93" s="7" t="s">
+      <c r="B94" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="C93" s="20"/>
-      <c r="D93" s="7" t="s">
+      <c r="C94" s="20"/>
+      <c r="D94" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E93" s="7" t="s">
+      <c r="E94" s="7" t="s">
         <v>420</v>
       </c>
-      <c r="F93" s="7" t="s">
+      <c r="F94" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G93" s="7" t="s">
+      <c r="G94" s="7" t="s">
         <v>421</v>
       </c>
-      <c r="H93" s="7" t="s">
+      <c r="H94" s="7" t="s">
         <v>422</v>
       </c>
-      <c r="I93" s="7" t="s">
+      <c r="I94" s="7" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
-      <c r="A94" s="16" t="s">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="16" t="s">
         <v>457</v>
       </c>
-      <c r="B94" s="16" t="s">
+      <c r="B95" s="16" t="s">
         <v>458</v>
       </c>
-      <c r="C94" s="20" t="s">
+      <c r="C95" s="20" t="s">
         <v>459</v>
       </c>
-      <c r="D94" s="16" t="s">
+      <c r="D95" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="E94" s="16" t="s">
+      <c r="E95" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="F94" s="16" t="s">
+      <c r="F95" s="16" t="s">
         <v>651</v>
       </c>
-      <c r="G94" s="16" t="s">
+      <c r="G95" s="16" t="s">
         <v>461</v>
       </c>
-      <c r="H94" s="16" t="s">
+      <c r="H95" s="16" t="s">
         <v>462</v>
       </c>
-      <c r="I94" s="16" t="s">
+      <c r="I95" s="16" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="95" spans="1:9" s="5" customFormat="1">
-      <c r="A95" s="9" t="s">
+    <row r="96" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="B95" s="9" t="s">
+      <c r="B96" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="C95" s="21" t="s">
+      <c r="C96" s="21" t="s">
         <v>414</v>
       </c>
-      <c r="D95" s="9" t="s">
+      <c r="D96" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E95" s="9" t="s">
+      <c r="E96" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="F95" s="9" t="s">
+      <c r="F96" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="G95" s="9" t="s">
+      <c r="G96" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="H95" s="9" t="s">
+      <c r="H96" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="I95" s="9" t="s">
+      <c r="I96" s="9" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
-      <c r="A96" s="7" t="s">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="B96" s="7" t="s">
+      <c r="B97" s="7" t="s">
         <v>324</v>
       </c>
-      <c r="C96" s="20"/>
-      <c r="D96" s="7" t="s">
+      <c r="C97" s="20"/>
+      <c r="D97" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E96" s="7" t="s">
+      <c r="E97" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="F96" s="7" t="s">
+      <c r="F97" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="G96" s="7" t="s">
+      <c r="G97" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="H96" s="7" t="s">
+      <c r="H97" s="7" t="s">
         <v>327</v>
       </c>
-      <c r="I96" s="7" t="s">
+      <c r="I97" s="7" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
-      <c r="A97" s="7" t="s">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="7" t="s">
         <v>381</v>
       </c>
-      <c r="B97" s="7" t="s">
+      <c r="B98" s="7" t="s">
         <v>382</v>
       </c>
-      <c r="C97" s="20" t="s">
+      <c r="C98" s="20" t="s">
         <v>383</v>
       </c>
-      <c r="D97" s="7" t="s">
+      <c r="D98" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E97" s="17" t="s">
+      <c r="E98" s="17" t="s">
         <v>384</v>
       </c>
-      <c r="F97" s="7" t="s">
+      <c r="F98" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G97" s="7"/>
-      <c r="H97" s="7" t="s">
+      <c r="G98" s="7"/>
+      <c r="H98" s="7" t="s">
         <v>385</v>
       </c>
-      <c r="I97" s="7" t="s">
+      <c r="I98" s="7" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
-      <c r="A98" s="9" t="s">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="B98" s="9" t="s">
+      <c r="B99" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="C98" s="9"/>
-      <c r="D98" s="9" t="s">
+      <c r="C99" s="9"/>
+      <c r="D99" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="E98" s="9" t="s">
+      <c r="E99" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="F98" s="9" t="s">
+      <c r="F99" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G98" s="9" t="s">
+      <c r="G99" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="H98" s="9" t="s">
+      <c r="H99" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="I98" s="14" t="s">
+      <c r="I99" s="14" t="s">
         <v>199</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H11" r:id="rId1" display="mailto:audrey.begin-poissant@umontreal.ca" xr:uid="{708FEBAC-F938-40E8-8D55-B34C4326210F}"/>
-    <hyperlink ref="I31" r:id="rId2" xr:uid="{574D93C5-0522-4DEE-A777-CB1BD468A7B3}"/>
+    <hyperlink ref="I32" r:id="rId2" xr:uid="{574D93C5-0522-4DEE-A777-CB1BD468A7B3}"/>
     <hyperlink ref="H25" r:id="rId3" display="mailto:delphine.cado@umontreal.ca" xr:uid="{0E0BF38D-BCA7-4652-84E3-BBE8A015792A}"/>
     <hyperlink ref="I25" r:id="rId4" xr:uid="{27792995-CED1-460A-9DC6-1C7D908E58F9}"/>
-    <hyperlink ref="I98" r:id="rId5" xr:uid="{FA15E077-C7FD-42E7-A5F3-AC50929F77F4}"/>
-    <hyperlink ref="I30" r:id="rId6" xr:uid="{2D74694A-18E3-4092-AA2F-BC65E158D410}"/>
+    <hyperlink ref="I99" r:id="rId5" xr:uid="{FA15E077-C7FD-42E7-A5F3-AC50929F77F4}"/>
+    <hyperlink ref="I31" r:id="rId6" xr:uid="{2D74694A-18E3-4092-AA2F-BC65E158D410}"/>
     <hyperlink ref="H15" r:id="rId7" display="mailto:hugo.bernier@umontreal.ca" xr:uid="{3F591457-DA50-462E-B1CA-F2F56ED9E3DD}"/>
     <hyperlink ref="I15" r:id="rId8" xr:uid="{11A3F440-1028-45FC-8DC2-DE60A7EA0AD9}"/>
-    <hyperlink ref="H56" r:id="rId9" display="mailto:isabelle.lagadec@bib.umontreal.ca" xr:uid="{4822C834-E5A8-42FD-9734-374BFC718C85}"/>
+    <hyperlink ref="H57" r:id="rId9" display="mailto:isabelle.lagadec@bib.umontreal.ca" xr:uid="{4822C834-E5A8-42FD-9734-374BFC718C85}"/>
     <hyperlink ref="H9" r:id="rId10" display="mailto:magalie.beaudoin@umontreal.ca" xr:uid="{2D976BF0-B68A-46E5-8412-BA8BC43FD26D}"/>
     <hyperlink ref="I9" r:id="rId11" xr:uid="{8AB273DE-5C86-4A48-AF36-BE5967CA61FD}"/>
-    <hyperlink ref="H85" r:id="rId12" display="mailto:mathieu.pigeon@umontreal.ca" xr:uid="{F73DFC6E-4D6D-42F3-84C0-454956AEC7E8}"/>
+    <hyperlink ref="H86" r:id="rId12" display="mailto:mathieu.pigeon@umontreal.ca" xr:uid="{F73DFC6E-4D6D-42F3-84C0-454956AEC7E8}"/>
     <hyperlink ref="H4" r:id="rId13" display="mailto:nadege.arsa@bib.umontreal.ca" xr:uid="{408AF5A3-35ED-4BF5-92B9-1B21C0C475D9}"/>
     <hyperlink ref="I4" r:id="rId14" xr:uid="{DD84AED2-20C7-4DA6-BFBF-EEC1E7D79E1B}"/>
     <hyperlink ref="H16" r:id="rId15" display="mailto:simon.blais.longtin@umontreal.ca" xr:uid="{EA917AC7-9087-435B-A6E7-3AE1885514AA}"/>
     <hyperlink ref="I16" r:id="rId16" xr:uid="{CDCAA32A-F6EB-49BF-B7CF-1AA918DBB62B}"/>
-    <hyperlink ref="H67" r:id="rId17" xr:uid="{8ABC26E9-CF81-491C-8A28-B209E6620D2A}"/>
+    <hyperlink ref="H68" r:id="rId17" xr:uid="{8ABC26E9-CF81-491C-8A28-B209E6620D2A}"/>
+    <hyperlink ref="I26" r:id="rId18" xr:uid="{28692D92-728B-4DFE-B003-A38AA753D55A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
   <tableParts count="1">
-    <tablePart r:id="rId19"/>
+    <tablePart r:id="rId20"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5611,15 +5623,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="f6670ae2-8190-4e72-909e-d717fe03ced5">
@@ -5628,6 +5631,15 @@
     <TaxCatchAll xmlns="00db0817-461a-4a69-8eb5-8daf0756d296" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5650,14 +5662,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -5672,4 +5676,12 @@
     <ds:schemaRef ds:uri="00db0817-461a-4a69-8eb5-8daf0756d296"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Correction des données répertoire de Laurence C
</commit_message>
<xml_diff>
--- a/content/personnel/liste-personnel.xlsx
+++ b/content/personnel/liste-personnel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tardimat\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02CEEDCE-0652-4C68-BEF8-B1439F073ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2FAE6E-1C02-40D0-A5B5-AF48E760366F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="8190" windowWidth="43200" windowHeight="23445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="662">
   <si>
     <t>Borsi</t>
   </si>
@@ -2001,13 +2001,16 @@
     <t>Papyrus</t>
   </si>
   <si>
-    <t>514-343-6111, poste 4019</t>
-  </si>
-  <si>
     <t>laurence.charest@umontreal.ca</t>
   </si>
   <si>
     <t>https://teams.microsoft.com/l/chat/0/0?users=laurence.charest@umontreal.ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                </t>
+  </si>
+  <si>
+    <t>laurence-charest.jpg</t>
   </si>
 </sst>
 </file>
@@ -2579,9 +2582,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2787,7 +2790,7 @@
         <v>631</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>440</v>
+        <v>660</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>441</v>
@@ -3302,7 +3305,9 @@
       <c r="B26" s="7" t="s">
         <v>655</v>
       </c>
-      <c r="C26" s="7"/>
+      <c r="C26" s="7" t="s">
+        <v>661</v>
+      </c>
       <c r="D26" s="7" t="s">
         <v>164</v>
       </c>
@@ -3312,14 +3317,12 @@
       <c r="F26" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="7"/>
+      <c r="H26" s="15" t="s">
         <v>658</v>
       </c>
-      <c r="H26" s="15" t="s">
+      <c r="I26" s="15" t="s">
         <v>659</v>
-      </c>
-      <c r="I26" s="15" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -5623,6 +5626,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="f6670ae2-8190-4e72-909e-d717fe03ced5">
@@ -5631,15 +5643,6 @@
     <TaxCatchAll xmlns="00db0817-461a-4a69-8eb5-8daf0756d296" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5662,6 +5665,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -5676,12 +5687,4 @@
     <ds:schemaRef ds:uri="00db0817-461a-4a69-8eb5-8daf0756d296"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ajout d'un champ 'direction' pour la liste de personels
</commit_message>
<xml_diff>
--- a/content/personnel/liste-personnel.xlsx
+++ b/content/personnel/liste-personnel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tardimat\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p1212882\siteWeb\coquille-web\content\personnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2FAE6E-1C02-40D0-A5B5-AF48E760366F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C7D500-A826-4E1D-A374-68A30F7BEF9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="664">
   <si>
     <t>Borsi</t>
   </si>
@@ -2011,13 +2011,19 @@
   </si>
   <si>
     <t>laurence-charest.jpg</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>test direction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2267,22 +2273,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A0AF7E1-A614-44BF-8C48-5C26377DC552}" name="Tableau1" displayName="Tableau1" ref="A1:I99" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:I99" xr:uid="{4F6A1D8F-9220-4675-A202-2173F3493722}">
-    <filterColumn colId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A0AF7E1-A614-44BF-8C48-5C26377DC552}" name="Tableau1" displayName="Tableau1" ref="A1:J99" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:J99" xr:uid="{4F6A1D8F-9220-4675-A202-2173F3493722}">
+    <filterColumn colId="6">
       <filters>
         <filter val="Direction de la recherche et des initiatives numériques"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I99">
+  <sortState ref="A2:J99">
     <sortCondition ref="A1:A99"/>
   </sortState>
-  <tableColumns count="9">
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{4B04E1AF-0079-4AD2-81CA-E8A433733E21}" name="nom"/>
     <tableColumn id="2" xr3:uid="{1806D27F-AC1F-4E36-9BA8-C129073C454B}" name="prenom"/>
     <tableColumn id="9" xr3:uid="{0ACCD680-F0E8-4E63-BE6D-84E7AE033942}" name="photo"/>
     <tableColumn id="3" xr3:uid="{0FE88E88-BACD-4136-9DE5-D5CF43012561}" name="fonction"/>
+    <tableColumn id="10" xr3:uid="{11859D3A-4F24-4371-AA7F-C9DB16F12327}" name="direction"/>
     <tableColumn id="8" xr3:uid="{EAABD870-1607-4CF3-AAF5-8E02FDD82AD3}" name="disciplines"/>
     <tableColumn id="4" xr3:uid="{05DDFE09-1E34-4D35-BAB3-F489E7BA0330}" name="bibliotheque"/>
     <tableColumn id="5" xr3:uid="{46B2E408-5C8E-434E-9C2D-03D2C880B796}" name="telephone"/>
@@ -2294,9 +2301,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2334,9 +2341,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2369,9 +2376,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2404,9 +2428,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2580,26 +2621,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I99"/>
+  <dimension ref="A1:J99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="45" customWidth="1"/>
-    <col min="5" max="5" width="79.42578125" customWidth="1"/>
-    <col min="6" max="6" width="116.85546875" customWidth="1"/>
-    <col min="7" max="7" width="44.28515625" customWidth="1"/>
-    <col min="8" max="8" width="36.42578125" customWidth="1"/>
-    <col min="9" max="9" width="75.85546875" customWidth="1"/>
+    <col min="4" max="5" width="45" customWidth="1"/>
+    <col min="6" max="6" width="79.42578125" customWidth="1"/>
+    <col min="7" max="7" width="116.85546875" customWidth="1"/>
+    <col min="8" max="8" width="44.28515625" customWidth="1"/>
+    <col min="9" max="9" width="36.42578125" customWidth="1"/>
+    <col min="10" max="10" width="75.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>615</v>
       </c>
@@ -2613,22 +2654,25 @@
         <v>618</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>617</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>620</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>621</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>622</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="9" t="s">
         <v>8</v>
       </c>
@@ -2641,23 +2685,24 @@
       <c r="D2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="7" t="s">
         <v>598</v>
       </c>
@@ -2670,23 +2715,24 @@
       <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7" t="s">
         <v>601</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>440</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>602</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>603</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="7" t="s">
         <v>469</v>
       </c>
@@ -2699,23 +2745,24 @@
       <c r="D4" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
         <v>332</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>472</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="I4" s="15" t="s">
         <v>473</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="J4" s="15" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="9" t="s">
         <v>169</v>
       </c>
@@ -2728,23 +2775,24 @@
       <c r="D5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="9"/>
+      <c r="F5" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="I5" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="J5" s="9" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="7" t="s">
         <v>71</v>
       </c>
@@ -2758,22 +2806,25 @@
         <v>22</v>
       </c>
       <c r="E6" s="7" t="s">
+        <v>663</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>654</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="I6" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="9" t="s">
         <v>437</v>
       </c>
@@ -2786,23 +2837,24 @@
       <c r="D7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="9"/>
+      <c r="F7" s="9" t="s">
         <v>631</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="G7" s="9" t="s">
         <v>660</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>441</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="I7" s="9" t="s">
         <v>442</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="J7" s="7" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>574</v>
       </c>
@@ -2815,23 +2867,23 @@
       <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>184</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>578</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>579</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="7" t="s">
         <v>341</v>
       </c>
@@ -2842,21 +2894,22 @@
       <c r="D9" s="7" t="s">
         <v>343</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="7" t="s">
+      <c r="E9" s="7"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="H9" s="16" t="s">
         <v>344</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="I9" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="J9" s="15" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="9" t="s">
         <v>399</v>
       </c>
@@ -2869,23 +2922,24 @@
       <c r="D10" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="9"/>
+      <c r="F10" s="12" t="s">
         <v>403</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="H10" s="11" t="s">
         <v>404</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="I10" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="J10" s="9" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="9" t="s">
         <v>78</v>
       </c>
@@ -2896,23 +2950,24 @@
       <c r="D11" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="9"/>
+      <c r="F11" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="H11" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="I11" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="J11" s="9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="9" t="s">
         <v>124</v>
       </c>
@@ -2925,23 +2980,24 @@
       <c r="D12" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="G12" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="H12" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="I12" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="J12" s="9" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="9" t="s">
         <v>34</v>
       </c>
@@ -2954,23 +3010,24 @@
       <c r="D13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="9"/>
+      <c r="F13" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="G13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="H13" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="I13" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="J13" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="9" t="s">
         <v>34</v>
       </c>
@@ -2982,20 +3039,21 @@
         <v>49</v>
       </c>
       <c r="E14" s="9"/>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="9"/>
+      <c r="G14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="H14" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="I14" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="J14" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="7" t="s">
         <v>282</v>
       </c>
@@ -3006,21 +3064,22 @@
       <c r="D15" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="7"/>
+      <c r="F15" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="G15" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="7"/>
+      <c r="I15" s="15" t="s">
         <v>285</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="J15" s="15" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="7" t="s">
         <v>509</v>
       </c>
@@ -3033,21 +3092,22 @@
       <c r="D16" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="7"/>
+      <c r="F16" s="17" t="s">
         <v>512</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="G16" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="15" t="s">
+      <c r="H16" s="7"/>
+      <c r="I16" s="15" t="s">
         <v>513</v>
       </c>
-      <c r="I16" s="15" t="s">
+      <c r="J16" s="15" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>560</v>
       </c>
@@ -3060,23 +3120,23 @@
       <c r="D17" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>563</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>13</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>564</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>565</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="11" t="s">
         <v>305</v>
       </c>
@@ -3088,20 +3148,21 @@
         <v>115</v>
       </c>
       <c r="E18" s="11"/>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="11"/>
+      <c r="G18" s="11" t="s">
         <v>307</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="H18" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="I18" s="11" t="s">
         <v>309</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="J18" s="11" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="7" t="s">
         <v>0</v>
       </c>
@@ -3114,23 +3175,24 @@
       <c r="D19" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="7"/>
+      <c r="F19" s="8" t="s">
         <v>624</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="G19" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="H19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="I19" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="J19" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="9" t="s">
         <v>208</v>
       </c>
@@ -3143,23 +3205,24 @@
       <c r="D20" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="9"/>
+      <c r="F20" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="G20" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="H20" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="I20" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="I20" s="9" t="s">
+      <c r="J20" s="9" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="7" t="s">
         <v>495</v>
       </c>
@@ -3172,23 +3235,24 @@
       <c r="D21" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="7"/>
+      <c r="F21" s="7" t="s">
         <v>498</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="G21" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="H21" s="7" t="s">
         <v>499</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="I21" s="7" t="s">
         <v>500</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="J21" s="10" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="9" t="s">
         <v>464</v>
       </c>
@@ -3199,23 +3263,24 @@
       <c r="D22" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="9"/>
+      <c r="F22" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="G22" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="H22" s="9" t="s">
         <v>466</v>
       </c>
-      <c r="H22" s="9" t="s">
+      <c r="I22" s="9" t="s">
         <v>467</v>
       </c>
-      <c r="I22" s="9" t="s">
+      <c r="J22" s="9" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="9" t="s">
         <v>275</v>
       </c>
@@ -3226,23 +3291,24 @@
       <c r="D23" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="9"/>
+      <c r="F23" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="G23" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="H23" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="H23" s="9" t="s">
+      <c r="I23" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="I23" s="9" t="s">
+      <c r="J23" s="9" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="9" t="s">
         <v>527</v>
       </c>
@@ -3255,23 +3321,24 @@
       <c r="D24" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="9"/>
+      <c r="F24" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="G24" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="H24" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="I24" s="9" t="s">
         <v>531</v>
       </c>
-      <c r="I24" s="9" t="s">
+      <c r="J24" s="9" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="7" t="s">
         <v>162</v>
       </c>
@@ -3282,23 +3349,24 @@
       <c r="D25" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="7"/>
+      <c r="F25" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="G25" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="H25" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="H25" s="15" t="s">
+      <c r="I25" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="I25" s="15" t="s">
+      <c r="J25" s="15" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="7" t="s">
         <v>656</v>
       </c>
@@ -3311,21 +3379,22 @@
       <c r="D26" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="7"/>
+      <c r="F26" s="7" t="s">
         <v>657</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="G26" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G26" s="7"/>
-      <c r="H26" s="15" t="s">
+      <c r="H26" s="7"/>
+      <c r="I26" s="15" t="s">
         <v>658</v>
       </c>
-      <c r="I26" s="15" t="s">
+      <c r="J26" s="15" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="7" t="s">
         <v>521</v>
       </c>
@@ -3336,23 +3405,24 @@
       <c r="D27" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="7"/>
+      <c r="F27" s="7" t="s">
         <v>632</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="G27" s="7" t="s">
         <v>523</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="H27" s="7" t="s">
         <v>524</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="I27" s="7" t="s">
         <v>525</v>
       </c>
-      <c r="I27" s="7" t="s">
+      <c r="J27" s="7" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="9" t="s">
         <v>502</v>
       </c>
@@ -3365,23 +3435,24 @@
       <c r="D28" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="9"/>
+      <c r="F28" s="13" t="s">
         <v>505</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="G28" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="H28" s="9" t="s">
         <v>506</v>
       </c>
-      <c r="H28" s="9" t="s">
+      <c r="I28" s="9" t="s">
         <v>507</v>
       </c>
-      <c r="I28" s="9" t="s">
+      <c r="J28" s="9" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="7" t="s">
         <v>200</v>
       </c>
@@ -3394,23 +3465,24 @@
       <c r="D29" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="7"/>
+      <c r="F29" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="G29" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="H29" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="H29" s="7" t="s">
+      <c r="I29" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="I29" s="7" t="s">
+      <c r="J29" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="7" t="s">
         <v>444</v>
       </c>
@@ -3423,23 +3495,24 @@
       <c r="D30" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="7"/>
+      <c r="F30" s="17" t="s">
         <v>447</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="G30" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="H30" s="7" t="s">
         <v>448</v>
       </c>
-      <c r="H30" s="7" t="s">
+      <c r="I30" s="7" t="s">
         <v>449</v>
       </c>
-      <c r="I30" s="7" t="s">
+      <c r="J30" s="7" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="9" t="s">
         <v>235</v>
       </c>
@@ -3452,23 +3525,24 @@
       <c r="D31" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="E31" s="9"/>
+      <c r="F31" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="G31" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="H31" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="H31" s="9" t="s">
+      <c r="I31" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="I31" s="14" t="s">
+      <c r="J31" s="14" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="7" t="s">
         <v>85</v>
       </c>
@@ -3482,20 +3556,21 @@
         <v>150</v>
       </c>
       <c r="E32" s="7"/>
-      <c r="F32" s="7" t="s">
+      <c r="F32" s="7"/>
+      <c r="G32" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G32" s="7" t="s">
+      <c r="H32" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H32" s="7" t="s">
+      <c r="I32" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="I32" s="15" t="s">
+      <c r="J32" s="15" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="9" t="s">
         <v>515</v>
       </c>
@@ -3508,23 +3583,24 @@
       <c r="D33" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="13" t="s">
+      <c r="E33" s="9"/>
+      <c r="F33" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="F33" s="9" t="s">
+      <c r="G33" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="H33" s="9" t="s">
         <v>518</v>
       </c>
-      <c r="H33" s="9" t="s">
+      <c r="I33" s="9" t="s">
         <v>519</v>
       </c>
-      <c r="I33" s="9" t="s">
+      <c r="J33" s="9" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="7" t="s">
         <v>354</v>
       </c>
@@ -3537,23 +3613,24 @@
       <c r="D34" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="7"/>
+      <c r="F34" s="7" t="s">
         <v>630</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="G34" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="G34" s="7" t="s">
+      <c r="H34" s="7" t="s">
         <v>357</v>
       </c>
-      <c r="H34" s="7" t="s">
+      <c r="I34" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="I34" s="7" t="s">
+      <c r="J34" s="7" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="7" t="s">
         <v>188</v>
       </c>
@@ -3566,23 +3643,24 @@
       <c r="D35" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="7"/>
+      <c r="F35" s="7" t="s">
         <v>635</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="G35" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G35" s="7" t="s">
+      <c r="H35" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="H35" s="7" t="s">
+      <c r="I35" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="I35" s="7" t="s">
+      <c r="J35" s="7" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="9" t="s">
         <v>451</v>
       </c>
@@ -3595,23 +3673,24 @@
       <c r="D36" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="E36" s="13" t="s">
+      <c r="E36" s="9"/>
+      <c r="F36" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="F36" s="9" t="s">
+      <c r="G36" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="G36" s="9" t="s">
+      <c r="H36" s="9" t="s">
         <v>454</v>
       </c>
-      <c r="H36" s="9" t="s">
+      <c r="I36" s="9" t="s">
         <v>455</v>
       </c>
-      <c r="I36" s="9" t="s">
+      <c r="J36" s="9" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="9" t="s">
         <v>287</v>
       </c>
@@ -3624,23 +3703,24 @@
       <c r="D37" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E37" s="9"/>
+      <c r="F37" s="9" t="s">
         <v>625</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="G37" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="H37" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="H37" s="9" t="s">
+      <c r="I37" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="I37" s="9" t="s">
+      <c r="J37" s="9" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="9" t="s">
         <v>180</v>
       </c>
@@ -3653,23 +3733,24 @@
       <c r="D38" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E38" s="9"/>
+      <c r="F38" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="F38" s="9" t="s">
+      <c r="G38" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="G38" s="9" t="s">
+      <c r="H38" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="H38" s="9" t="s">
+      <c r="I38" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="I38" s="9" t="s">
+      <c r="J38" s="9" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="7" t="s">
         <v>107</v>
       </c>
@@ -3681,20 +3762,21 @@
         <v>109</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="7" t="s">
+      <c r="F39" s="7"/>
+      <c r="G39" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="G39" s="7" t="s">
+      <c r="H39" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="H39" s="7" t="s">
+      <c r="I39" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="I39" s="7" t="s">
+      <c r="J39" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="7" t="s">
         <v>299</v>
       </c>
@@ -3707,23 +3789,24 @@
       <c r="D40" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E40" s="7" t="s">
+      <c r="E40" s="7"/>
+      <c r="F40" s="7" t="s">
         <v>628</v>
       </c>
-      <c r="F40" s="7" t="s">
+      <c r="G40" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="G40" s="7" t="s">
+      <c r="H40" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="H40" s="7" t="s">
+      <c r="I40" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="I40" s="7" t="s">
+      <c r="J40" s="7" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="9" t="s">
         <v>548</v>
       </c>
@@ -3736,23 +3819,24 @@
       <c r="D41" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="E41" s="9"/>
+      <c r="F41" s="9" t="s">
         <v>460</v>
       </c>
-      <c r="F41" s="9" t="s">
+      <c r="G41" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="H41" s="9" t="s">
         <v>551</v>
       </c>
-      <c r="H41" s="9" t="s">
+      <c r="I41" s="9" t="s">
         <v>552</v>
       </c>
-      <c r="I41" s="9" t="s">
+      <c r="J41" s="9" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="9" t="s">
         <v>101</v>
       </c>
@@ -3765,23 +3849,24 @@
       <c r="D42" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E42" s="9" t="s">
+      <c r="E42" s="9"/>
+      <c r="F42" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F42" s="9" t="s">
+      <c r="G42" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G42" s="9" t="s">
+      <c r="H42" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="H42" s="9" t="s">
+      <c r="I42" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="I42" s="9" t="s">
+      <c r="J42" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="9" t="s">
         <v>360</v>
       </c>
@@ -3792,23 +3877,24 @@
       <c r="D43" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E43" s="9"/>
+      <c r="F43" s="9" t="s">
         <v>362</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="G43" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="G43" s="9" t="s">
+      <c r="H43" s="9" t="s">
         <v>364</v>
       </c>
-      <c r="H43" s="9" t="s">
+      <c r="I43" s="9" t="s">
         <v>365</v>
       </c>
-      <c r="I43" s="9" t="s">
+      <c r="J43" s="9" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="9" t="s">
         <v>475</v>
       </c>
@@ -3821,23 +3907,24 @@
       <c r="D44" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E44" s="13" t="s">
+      <c r="E44" s="9"/>
+      <c r="F44" s="13" t="s">
         <v>637</v>
       </c>
-      <c r="F44" s="9" t="s">
+      <c r="G44" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G44" s="9" t="s">
+      <c r="H44" s="9" t="s">
         <v>478</v>
       </c>
-      <c r="H44" s="9" t="s">
+      <c r="I44" s="9" t="s">
         <v>479</v>
       </c>
-      <c r="I44" s="9" t="s">
+      <c r="J44" s="9" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="7" t="s">
         <v>639</v>
       </c>
@@ -3848,19 +3935,20 @@
       <c r="D45" s="7" t="s">
         <v>641</v>
       </c>
-      <c r="E45" s="17" t="s">
+      <c r="E45" s="7"/>
+      <c r="F45" s="17" t="s">
         <v>642</v>
       </c>
-      <c r="F45" s="7" t="s">
+      <c r="G45" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7" t="s">
+      <c r="H45" s="7"/>
+      <c r="I45" s="7" t="s">
         <v>640</v>
       </c>
-      <c r="I45" s="7"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" s="7"/>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" s="9" t="s">
         <v>140</v>
       </c>
@@ -3873,23 +3961,24 @@
       <c r="D46" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="E46" s="9"/>
+      <c r="F46" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F46" s="9" t="s">
+      <c r="G46" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G46" s="9" t="s">
+      <c r="H46" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="H46" s="9" t="s">
+      <c r="I46" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="I46" s="9" t="s">
+      <c r="J46" s="9" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="7" t="s">
         <v>176</v>
       </c>
@@ -3901,20 +3990,21 @@
         <v>115</v>
       </c>
       <c r="E47" s="7"/>
-      <c r="F47" s="7" t="s">
+      <c r="F47" s="7"/>
+      <c r="G47" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G47" s="7" t="s">
+      <c r="H47" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H47" s="7" t="s">
+      <c r="I47" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="I47" s="7" t="s">
+      <c r="J47" s="7" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="7" t="s">
         <v>176</v>
       </c>
@@ -3927,23 +4017,24 @@
       <c r="D48" s="7" t="s">
         <v>535</v>
       </c>
-      <c r="E48" s="7" t="s">
-        <v>110</v>
-      </c>
+      <c r="E48" s="7"/>
       <c r="F48" s="7" t="s">
         <v>110</v>
       </c>
       <c r="G48" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H48" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="H48" s="7" t="s">
+      <c r="I48" s="7" t="s">
         <v>536</v>
       </c>
-      <c r="I48" s="7" t="s">
+      <c r="J48" s="7" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="9" t="s">
         <v>387</v>
       </c>
@@ -3956,23 +4047,24 @@
       <c r="D49" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="E49" s="13" t="s">
+      <c r="E49" s="9"/>
+      <c r="F49" s="13" t="s">
         <v>390</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="G49" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="G49" s="9" t="s">
+      <c r="H49" s="9" t="s">
         <v>391</v>
       </c>
-      <c r="H49" s="9" t="s">
+      <c r="I49" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="I49" s="9" t="s">
+      <c r="J49" s="9" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="7" t="s">
         <v>311</v>
       </c>
@@ -3983,23 +4075,24 @@
       <c r="D50" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E50" s="7" t="s">
+      <c r="E50" s="7"/>
+      <c r="F50" s="7" t="s">
         <v>636</v>
       </c>
-      <c r="F50" s="7" t="s">
+      <c r="G50" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G50" s="7" t="s">
+      <c r="H50" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="H50" s="7" t="s">
+      <c r="I50" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="I50" s="7" t="s">
+      <c r="J50" s="7" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="7" t="s">
         <v>612</v>
       </c>
@@ -4010,19 +4103,20 @@
       <c r="D51" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="E51" s="7"/>
+      <c r="F51" s="7" t="s">
         <v>613</v>
       </c>
-      <c r="F51" s="7" t="s">
+      <c r="G51" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G51" s="7" t="s">
+      <c r="H51" s="7" t="s">
         <v>614</v>
       </c>
-      <c r="H51" s="7"/>
       <c r="I51" s="7"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" s="7"/>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" s="7" t="s">
         <v>41</v>
       </c>
@@ -4035,23 +4129,24 @@
       <c r="D52" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="7" t="s">
+      <c r="E52" s="7"/>
+      <c r="F52" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F52" s="7" t="s">
+      <c r="G52" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G52" s="7" t="s">
+      <c r="H52" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H52" s="7" t="s">
+      <c r="I52" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I52" s="7" t="s">
+      <c r="J52" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="9" t="s">
         <v>488</v>
       </c>
@@ -4064,23 +4159,24 @@
       <c r="D53" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="E53" s="9" t="s">
+      <c r="E53" s="9"/>
+      <c r="F53" s="9" t="s">
         <v>491</v>
       </c>
-      <c r="F53" s="9" t="s">
+      <c r="G53" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G53" s="9" t="s">
+      <c r="H53" s="9" t="s">
         <v>492</v>
       </c>
-      <c r="H53" s="9" t="s">
+      <c r="I53" s="9" t="s">
         <v>493</v>
       </c>
-      <c r="I53" s="9" t="s">
+      <c r="J53" s="9" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" t="s">
         <v>567</v>
       </c>
@@ -4093,23 +4189,23 @@
       <c r="D54" t="s">
         <v>11</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="F54" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>13</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>571</v>
       </c>
-      <c r="H54" t="s">
+      <c r="I54" t="s">
         <v>572</v>
       </c>
-      <c r="I54" t="s">
+      <c r="J54" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="7" t="s">
         <v>335</v>
       </c>
@@ -4122,23 +4218,24 @@
       <c r="D55" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E55" s="7"/>
+      <c r="F55" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="F55" s="7" t="s">
+      <c r="G55" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G55" s="7" t="s">
+      <c r="H55" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="H55" s="7" t="s">
+      <c r="I55" s="7" t="s">
         <v>339</v>
       </c>
-      <c r="I55" s="7" t="s">
+      <c r="J55" s="7" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="7" t="s">
         <v>26</v>
       </c>
@@ -4151,23 +4248,24 @@
       <c r="D56" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E56" s="7" t="s">
+      <c r="E56" s="7"/>
+      <c r="F56" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F56" s="7" t="s">
+      <c r="G56" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G56" s="7" t="s">
+      <c r="H56" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H56" s="7" t="s">
+      <c r="I56" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I56" s="7" t="s">
+      <c r="J56" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="9" t="s">
         <v>294</v>
       </c>
@@ -4178,23 +4276,24 @@
       <c r="D57" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E57" s="9" t="s">
+      <c r="E57" s="9"/>
+      <c r="F57" s="9" t="s">
         <v>626</v>
       </c>
-      <c r="F57" s="9" t="s">
+      <c r="G57" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="G57" s="9" t="s">
+      <c r="H57" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="H57" s="14" t="s">
+      <c r="I57" s="14" t="s">
         <v>627</v>
       </c>
-      <c r="I57" s="9" t="s">
+      <c r="J57" s="9" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="9" t="s">
         <v>50</v>
       </c>
@@ -4207,23 +4306,24 @@
       <c r="D58" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E58" s="9" t="s">
+      <c r="E58" s="9"/>
+      <c r="F58" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F58" s="9" t="s">
+      <c r="G58" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G58" s="9" t="s">
+      <c r="H58" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="H58" s="9" t="s">
+      <c r="I58" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="I58" s="9" t="s">
+      <c r="J58" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="7" t="s">
         <v>554</v>
       </c>
@@ -4236,23 +4336,24 @@
       <c r="D59" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="E59" s="7" t="s">
+      <c r="E59" s="7"/>
+      <c r="F59" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F59" s="7" t="s">
+      <c r="G59" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G59" s="7" t="s">
+      <c r="H59" s="7" t="s">
         <v>557</v>
       </c>
-      <c r="H59" s="7" t="s">
+      <c r="I59" s="7" t="s">
         <v>558</v>
       </c>
-      <c r="I59" s="7" t="s">
+      <c r="J59" s="7" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="9" t="s">
         <v>538</v>
       </c>
@@ -4265,23 +4366,24 @@
       <c r="D60" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E60" s="9" t="s">
+      <c r="E60" s="9"/>
+      <c r="F60" s="9" t="s">
         <v>633</v>
       </c>
-      <c r="F60" s="9" t="s">
+      <c r="G60" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="G60" s="9" t="s">
+      <c r="H60" s="9" t="s">
         <v>540</v>
       </c>
-      <c r="H60" s="9" t="s">
+      <c r="I60" s="9" t="s">
         <v>541</v>
       </c>
-      <c r="I60" s="9" t="s">
+      <c r="J60" s="9" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="9" t="s">
         <v>265</v>
       </c>
@@ -4294,23 +4396,24 @@
       <c r="D61" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E61" s="9" t="s">
+      <c r="E61" s="9"/>
+      <c r="F61" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="F61" s="9" t="s">
+      <c r="G61" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G61" s="9" t="s">
+      <c r="H61" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="H61" s="9" t="s">
+      <c r="I61" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="I61" s="9" t="s">
+      <c r="J61" s="9" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="62" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" s="4" customFormat="1">
       <c r="A62" s="9" t="s">
         <v>249</v>
       </c>
@@ -4323,23 +4426,24 @@
       <c r="D62" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="E62" s="9" t="s">
+      <c r="E62" s="9"/>
+      <c r="F62" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="F62" s="9" t="s">
+      <c r="G62" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G62" s="9" t="s">
+      <c r="H62" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="H62" s="9" t="s">
+      <c r="I62" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="I62" s="9" t="s">
+      <c r="J62" s="9" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="7" t="s">
         <v>367</v>
       </c>
@@ -4352,23 +4456,24 @@
       <c r="D63" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="E63" s="8" t="s">
+      <c r="E63" s="7"/>
+      <c r="F63" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="F63" s="7" t="s">
+      <c r="G63" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G63" s="7" t="s">
+      <c r="H63" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="H63" s="7" t="s">
+      <c r="I63" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="I63" s="7" t="s">
+      <c r="J63" s="7" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="64" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" s="5" customFormat="1">
       <c r="A64" s="9" t="s">
         <v>424</v>
       </c>
@@ -4381,23 +4486,24 @@
       <c r="D64" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="E64" s="9" t="s">
+      <c r="E64" s="9"/>
+      <c r="F64" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="F64" s="9" t="s">
+      <c r="G64" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="G64" s="9" t="s">
+      <c r="H64" s="9" t="s">
         <v>428</v>
       </c>
-      <c r="H64" s="9" t="s">
+      <c r="I64" s="9" t="s">
         <v>429</v>
       </c>
-      <c r="I64" s="9" t="s">
+      <c r="J64" s="9" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="7" t="s">
         <v>147</v>
       </c>
@@ -4410,23 +4516,24 @@
       <c r="D65" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="E65" s="7" t="s">
+      <c r="E65" s="7"/>
+      <c r="F65" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="F65" s="7" t="s">
+      <c r="G65" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="G65" s="7" t="s">
+      <c r="H65" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="H65" s="7" t="s">
+      <c r="I65" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="I65" s="7" t="s">
+      <c r="J65" s="7" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="11" t="s">
         <v>20</v>
       </c>
@@ -4437,23 +4544,24 @@
       <c r="D66" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E66" s="12" t="s">
+      <c r="E66" s="11"/>
+      <c r="F66" s="12" t="s">
         <v>370</v>
       </c>
-      <c r="F66" s="11" t="s">
+      <c r="G66" s="11" t="s">
         <v>652</v>
       </c>
-      <c r="G66" s="11" t="s">
+      <c r="H66" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H66" s="11" t="s">
+      <c r="I66" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I66" s="11" t="s">
+      <c r="J66" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="7" t="s">
         <v>20</v>
       </c>
@@ -4465,18 +4573,19 @@
         <v>49</v>
       </c>
       <c r="E67" s="7"/>
-      <c r="F67" s="7" t="s">
+      <c r="F67" s="7"/>
+      <c r="G67" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G67" s="7"/>
-      <c r="H67" s="7" t="s">
+      <c r="H67" s="7"/>
+      <c r="I67" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I67" s="7" t="s">
+      <c r="J67" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="7" t="s">
         <v>395</v>
       </c>
@@ -4487,19 +4596,20 @@
       <c r="D68" s="7" t="s">
         <v>648</v>
       </c>
-      <c r="E68" s="17"/>
-      <c r="F68" s="7" t="s">
+      <c r="E68" s="7"/>
+      <c r="F68" s="17"/>
+      <c r="G68" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="G68" s="16" t="s">
+      <c r="H68" s="16" t="s">
         <v>274</v>
       </c>
-      <c r="H68" s="15" t="s">
+      <c r="I68" s="15" t="s">
         <v>649</v>
       </c>
-      <c r="I68" s="16"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J68" s="16"/>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69" s="7" t="s">
         <v>481</v>
       </c>
@@ -4512,23 +4622,24 @@
       <c r="D69" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E69" s="7" t="s">
+      <c r="E69" s="7"/>
+      <c r="F69" s="7" t="s">
         <v>484</v>
       </c>
-      <c r="F69" s="7" t="s">
+      <c r="G69" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G69" s="7" t="s">
+      <c r="H69" s="7" t="s">
         <v>485</v>
       </c>
-      <c r="H69" s="7" t="s">
+      <c r="I69" s="7" t="s">
         <v>486</v>
       </c>
-      <c r="I69" s="7" t="s">
+      <c r="J69" s="7" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="7" t="s">
         <v>432</v>
       </c>
@@ -4541,23 +4652,24 @@
       <c r="D70" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E70" s="7" t="s">
+      <c r="E70" s="7"/>
+      <c r="F70" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="F70" s="7" t="s">
+      <c r="G70" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="G70" s="7" t="s">
+      <c r="H70" s="7" t="s">
         <v>434</v>
       </c>
-      <c r="H70" s="7" t="s">
+      <c r="I70" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="I70" s="7" t="s">
+      <c r="J70" s="7" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="71" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" s="4" customFormat="1">
       <c r="A71" s="7" t="s">
         <v>242</v>
       </c>
@@ -4570,23 +4682,24 @@
       <c r="D71" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E71" s="7" t="s">
+      <c r="E71" s="7"/>
+      <c r="F71" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="F71" s="7" t="s">
+      <c r="G71" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G71" s="7" t="s">
+      <c r="H71" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="H71" s="7" t="s">
+      <c r="I71" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="I71" s="7" t="s">
+      <c r="J71" s="7" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="7" t="s">
         <v>132</v>
       </c>
@@ -4599,23 +4712,24 @@
       <c r="D72" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E72" s="7" t="s">
+      <c r="E72" s="7"/>
+      <c r="F72" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="F72" s="7" t="s">
+      <c r="G72" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="G72" s="7" t="s">
+      <c r="H72" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="H72" s="7" t="s">
+      <c r="I72" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="I72" s="7" t="s">
+      <c r="J72" s="7" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="16" t="s">
         <v>257</v>
       </c>
@@ -4628,23 +4742,24 @@
       <c r="D73" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E73" s="16" t="s">
+      <c r="E73" s="7"/>
+      <c r="F73" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="F73" s="16" t="s">
+      <c r="G73" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="G73" s="16" t="s">
+      <c r="H73" s="16" t="s">
         <v>262</v>
       </c>
-      <c r="H73" s="16" t="s">
+      <c r="I73" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="I73" s="16" t="s">
+      <c r="J73" s="16" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="74" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" s="4" customFormat="1">
       <c r="A74" s="9" t="s">
         <v>329</v>
       </c>
@@ -4657,23 +4772,24 @@
       <c r="D74" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E74" s="9" t="s">
+      <c r="E74" s="9"/>
+      <c r="F74" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="F74" s="9" t="s">
+      <c r="G74" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G74" s="9" t="s">
+      <c r="H74" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="H74" s="9" t="s">
+      <c r="I74" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="I74" s="9" t="s">
+      <c r="J74" s="9" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="9" t="s">
         <v>63</v>
       </c>
@@ -4686,23 +4802,24 @@
       <c r="D75" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E75" s="13" t="s">
+      <c r="E75" s="9"/>
+      <c r="F75" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F75" s="9" t="s">
+      <c r="G75" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G75" s="9" t="s">
+      <c r="H75" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="H75" s="9" t="s">
+      <c r="I75" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="I75" s="9" t="s">
+      <c r="J75" s="9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="16" t="s">
         <v>228</v>
       </c>
@@ -4715,23 +4832,24 @@
       <c r="D76" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="E76" s="8" t="s">
+      <c r="E76" s="16"/>
+      <c r="F76" s="8" t="s">
         <v>650</v>
       </c>
-      <c r="F76" s="16" t="s">
+      <c r="G76" s="16" t="s">
         <v>654</v>
       </c>
-      <c r="G76" s="16" t="s">
+      <c r="H76" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="H76" s="16" t="s">
+      <c r="I76" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="I76" s="16" t="s">
+      <c r="J76" s="16" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="9" t="s">
         <v>347</v>
       </c>
@@ -4742,23 +4860,24 @@
       <c r="D77" s="9" t="s">
         <v>349</v>
       </c>
-      <c r="E77" s="9" t="s">
+      <c r="E77" s="9"/>
+      <c r="F77" s="9" t="s">
         <v>350</v>
       </c>
-      <c r="F77" s="9" t="s">
+      <c r="G77" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="G77" s="9" t="s">
+      <c r="H77" s="9" t="s">
         <v>351</v>
       </c>
-      <c r="H77" s="9" t="s">
+      <c r="I77" s="9" t="s">
         <v>352</v>
       </c>
-      <c r="I77" s="9" t="s">
+      <c r="J77" s="9" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="9" t="s">
         <v>222</v>
       </c>
@@ -4770,20 +4889,21 @@
         <v>109</v>
       </c>
       <c r="E78" s="9"/>
-      <c r="F78" s="9" t="s">
+      <c r="F78" s="9"/>
+      <c r="G78" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="G78" s="9" t="s">
+      <c r="H78" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="H78" s="9" t="s">
+      <c r="I78" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="I78" s="9" t="s">
+      <c r="J78" s="9" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="9" t="s">
         <v>316</v>
       </c>
@@ -4796,23 +4916,24 @@
       <c r="D79" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E79" s="11" t="s">
+      <c r="E79" s="9"/>
+      <c r="F79" s="11" t="s">
         <v>629</v>
       </c>
-      <c r="F79" s="9" t="s">
+      <c r="G79" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="G79" s="9" t="s">
+      <c r="H79" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="H79" s="9" t="s">
+      <c r="I79" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="I79" s="9" t="s">
+      <c r="J79" s="9" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="9" t="s">
         <v>644</v>
       </c>
@@ -4823,17 +4944,18 @@
       <c r="D80" s="9" t="s">
         <v>645</v>
       </c>
-      <c r="E80" s="13"/>
-      <c r="F80" s="9" t="s">
+      <c r="E80" s="9"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="G80" s="9"/>
-      <c r="H80" s="9" t="s">
+      <c r="H80" s="9"/>
+      <c r="I80" s="9" t="s">
         <v>646</v>
       </c>
-      <c r="I80" s="18"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J80" s="18"/>
+    </row>
+    <row r="81" spans="1:10">
       <c r="A81" t="s">
         <v>592</v>
       </c>
@@ -4846,20 +4968,20 @@
       <c r="D81" t="s">
         <v>195</v>
       </c>
-      <c r="E81" s="3" t="s">
+      <c r="F81" s="3" t="s">
         <v>595</v>
       </c>
-      <c r="F81" t="s">
+      <c r="G81" t="s">
         <v>60</v>
       </c>
-      <c r="H81" t="s">
+      <c r="I81" t="s">
         <v>596</v>
       </c>
-      <c r="I81" t="s">
+      <c r="J81" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="7" t="s">
         <v>216</v>
       </c>
@@ -4872,23 +4994,24 @@
       <c r="D82" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E82" s="17" t="s">
+      <c r="E82" s="7"/>
+      <c r="F82" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="F82" s="7" t="s">
+      <c r="G82" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G82" s="16" t="s">
+      <c r="H82" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="H82" s="16" t="s">
+      <c r="I82" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="I82" s="16" t="s">
+      <c r="J82" s="16" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="7" t="s">
         <v>95</v>
       </c>
@@ -4901,23 +5024,24 @@
       <c r="D83" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E83" s="7" t="s">
+      <c r="E83" s="7"/>
+      <c r="F83" s="7" t="s">
         <v>634</v>
       </c>
-      <c r="F83" s="7" t="s">
+      <c r="G83" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G83" s="16" t="s">
+      <c r="H83" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="H83" s="16" t="s">
+      <c r="I83" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="I83" s="16" t="s">
+      <c r="J83" s="16" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="9" t="s">
         <v>95</v>
       </c>
@@ -4930,23 +5054,24 @@
       <c r="D84" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E84" s="9" t="s">
+      <c r="E84" s="9"/>
+      <c r="F84" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F84" s="9" t="s">
+      <c r="G84" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G84" s="11" t="s">
+      <c r="H84" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="H84" s="11" t="s">
+      <c r="I84" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="I84" s="11" t="s">
+      <c r="J84" s="11" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="7" t="s">
         <v>543</v>
       </c>
@@ -4959,23 +5084,24 @@
       <c r="D85" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E85" s="7" t="s">
+      <c r="E85" s="7"/>
+      <c r="F85" s="7" t="s">
         <v>498</v>
       </c>
-      <c r="F85" s="7" t="s">
+      <c r="G85" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G85" s="16" t="s">
+      <c r="H85" s="16" t="s">
         <v>545</v>
       </c>
-      <c r="H85" s="16" t="s">
+      <c r="I85" s="16" t="s">
         <v>546</v>
       </c>
-      <c r="I85" s="16" t="s">
+      <c r="J85" s="16" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="7" t="s">
         <v>407</v>
       </c>
@@ -4988,21 +5114,22 @@
       <c r="D86" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E86" s="17" t="s">
+      <c r="E86" s="7"/>
+      <c r="F86" s="17" t="s">
         <v>410</v>
       </c>
-      <c r="F86" s="7" t="s">
+      <c r="G86" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G86" s="16"/>
-      <c r="H86" s="15" t="s">
+      <c r="H86" s="16"/>
+      <c r="I86" s="15" t="s">
         <v>411</v>
       </c>
-      <c r="I86" s="16" t="s">
+      <c r="J86" s="16" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="9" t="s">
         <v>374</v>
       </c>
@@ -5015,23 +5142,24 @@
       <c r="D87" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E87" s="13" t="s">
+      <c r="E87" s="9"/>
+      <c r="F87" s="13" t="s">
         <v>377</v>
       </c>
-      <c r="F87" s="9" t="s">
+      <c r="G87" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="G87" s="11" t="s">
+      <c r="H87" s="11" t="s">
         <v>378</v>
       </c>
-      <c r="H87" s="11" t="s">
+      <c r="I87" s="11" t="s">
         <v>379</v>
       </c>
-      <c r="I87" s="11" t="s">
+      <c r="J87" s="11" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" t="s">
         <v>581</v>
       </c>
@@ -5044,23 +5172,23 @@
       <c r="D88" t="s">
         <v>11</v>
       </c>
-      <c r="E88" s="3" t="s">
+      <c r="F88" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="F88" t="s">
+      <c r="G88" t="s">
         <v>30</v>
       </c>
-      <c r="G88" s="4" t="s">
+      <c r="H88" s="4" t="s">
         <v>584</v>
       </c>
-      <c r="H88" s="4" t="s">
+      <c r="I88" s="4" t="s">
         <v>585</v>
       </c>
-      <c r="I88" s="4" t="s">
+      <c r="J88" s="4" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" t="s">
         <v>587</v>
       </c>
@@ -5071,23 +5199,23 @@
       <c r="D89" t="s">
         <v>17</v>
       </c>
-      <c r="E89" t="s">
+      <c r="F89" t="s">
         <v>18</v>
       </c>
-      <c r="F89" t="s">
+      <c r="G89" t="s">
         <v>13</v>
       </c>
-      <c r="G89" s="4" t="s">
+      <c r="H89" s="4" t="s">
         <v>589</v>
       </c>
-      <c r="H89" s="4" t="s">
+      <c r="I89" s="4" t="s">
         <v>590</v>
       </c>
-      <c r="I89" s="4" t="s">
+      <c r="J89" s="4" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="90" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" s="4" customFormat="1">
       <c r="A90" s="7" t="s">
         <v>394</v>
       </c>
@@ -5100,23 +5228,24 @@
       <c r="D90" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E90" s="17" t="s">
+      <c r="E90" s="7"/>
+      <c r="F90" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="F90" s="7" t="s">
+      <c r="G90" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G90" s="16" t="s">
+      <c r="H90" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="H90" s="16" t="s">
+      <c r="I90" s="16" t="s">
         <v>397</v>
       </c>
-      <c r="I90" s="16" t="s">
+      <c r="J90" s="16" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="91" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" s="4" customFormat="1">
       <c r="A91" s="7" t="s">
         <v>119</v>
       </c>
@@ -5127,21 +5256,22 @@
       <c r="D91" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E91" s="17" t="s">
+      <c r="E91" s="7"/>
+      <c r="F91" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="F91" s="7" t="s">
+      <c r="G91" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G91" s="16"/>
-      <c r="H91" s="16" t="s">
+      <c r="H91" s="16"/>
+      <c r="I91" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="I91" s="16" t="s">
+      <c r="J91" s="16" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="11" t="s">
         <v>605</v>
       </c>
@@ -5154,23 +5284,24 @@
       <c r="D92" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="E92" s="11" t="s">
+      <c r="E92" s="11"/>
+      <c r="F92" s="11" t="s">
         <v>607</v>
       </c>
-      <c r="F92" s="11" t="s">
+      <c r="G92" s="11" t="s">
         <v>608</v>
       </c>
-      <c r="G92" s="11" t="s">
+      <c r="H92" s="11" t="s">
         <v>609</v>
       </c>
-      <c r="H92" s="11" t="s">
+      <c r="I92" s="11" t="s">
         <v>610</v>
       </c>
-      <c r="I92" s="11" t="s">
+      <c r="J92" s="11" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="11" t="s">
         <v>114</v>
       </c>
@@ -5182,20 +5313,21 @@
         <v>115</v>
       </c>
       <c r="E93" s="11"/>
-      <c r="F93" s="11" t="s">
+      <c r="F93" s="11"/>
+      <c r="G93" s="11" t="s">
         <v>653</v>
       </c>
-      <c r="G93" s="11" t="s">
+      <c r="H93" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="H93" s="11" t="s">
+      <c r="I93" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="I93" s="11" t="s">
+      <c r="J93" s="11" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="7" t="s">
         <v>418</v>
       </c>
@@ -5206,23 +5338,24 @@
       <c r="D94" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E94" s="7" t="s">
+      <c r="E94" s="7"/>
+      <c r="F94" s="7" t="s">
         <v>420</v>
       </c>
-      <c r="F94" s="7" t="s">
+      <c r="G94" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G94" s="7" t="s">
+      <c r="H94" s="7" t="s">
         <v>421</v>
       </c>
-      <c r="H94" s="7" t="s">
+      <c r="I94" s="7" t="s">
         <v>422</v>
       </c>
-      <c r="I94" s="7" t="s">
+      <c r="J94" s="7" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="16" t="s">
         <v>457</v>
       </c>
@@ -5235,23 +5368,24 @@
       <c r="D95" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="E95" s="16" t="s">
+      <c r="E95" s="16"/>
+      <c r="F95" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="F95" s="16" t="s">
+      <c r="G95" s="16" t="s">
         <v>651</v>
       </c>
-      <c r="G95" s="16" t="s">
+      <c r="H95" s="16" t="s">
         <v>461</v>
       </c>
-      <c r="H95" s="16" t="s">
+      <c r="I95" s="16" t="s">
         <v>462</v>
       </c>
-      <c r="I95" s="16" t="s">
+      <c r="J95" s="16" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="96" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" s="5" customFormat="1">
       <c r="A96" s="9" t="s">
         <v>413</v>
       </c>
@@ -5264,23 +5398,24 @@
       <c r="D96" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E96" s="9" t="s">
+      <c r="E96" s="9"/>
+      <c r="F96" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="F96" s="9" t="s">
+      <c r="G96" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="G96" s="9" t="s">
+      <c r="H96" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="H96" s="9" t="s">
+      <c r="I96" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="I96" s="9" t="s">
+      <c r="J96" s="9" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" s="7" t="s">
         <v>323</v>
       </c>
@@ -5291,23 +5426,24 @@
       <c r="D97" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E97" s="7" t="s">
+      <c r="E97" s="7"/>
+      <c r="F97" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="F97" s="7" t="s">
+      <c r="G97" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="G97" s="7" t="s">
+      <c r="H97" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="H97" s="7" t="s">
+      <c r="I97" s="7" t="s">
         <v>327</v>
       </c>
-      <c r="I97" s="7" t="s">
+      <c r="J97" s="7" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" s="7" t="s">
         <v>381</v>
       </c>
@@ -5320,21 +5456,22 @@
       <c r="D98" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E98" s="17" t="s">
+      <c r="E98" s="7"/>
+      <c r="F98" s="17" t="s">
         <v>384</v>
       </c>
-      <c r="F98" s="7" t="s">
+      <c r="G98" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G98" s="7"/>
-      <c r="H98" s="7" t="s">
+      <c r="H98" s="7"/>
+      <c r="I98" s="7" t="s">
         <v>385</v>
       </c>
-      <c r="I98" s="7" t="s">
+      <c r="J98" s="7" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" s="9" t="s">
         <v>194</v>
       </c>
@@ -5345,42 +5482,43 @@
       <c r="D99" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="E99" s="9" t="s">
+      <c r="E99" s="9"/>
+      <c r="F99" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="F99" s="9" t="s">
+      <c r="G99" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G99" s="9" t="s">
+      <c r="H99" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="H99" s="9" t="s">
+      <c r="I99" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="I99" s="14" t="s">
+      <c r="J99" s="14" t="s">
         <v>199</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H11" r:id="rId1" display="mailto:audrey.begin-poissant@umontreal.ca" xr:uid="{708FEBAC-F938-40E8-8D55-B34C4326210F}"/>
-    <hyperlink ref="I32" r:id="rId2" xr:uid="{574D93C5-0522-4DEE-A777-CB1BD468A7B3}"/>
-    <hyperlink ref="H25" r:id="rId3" display="mailto:delphine.cado@umontreal.ca" xr:uid="{0E0BF38D-BCA7-4652-84E3-BBE8A015792A}"/>
-    <hyperlink ref="I25" r:id="rId4" xr:uid="{27792995-CED1-460A-9DC6-1C7D908E58F9}"/>
-    <hyperlink ref="I99" r:id="rId5" xr:uid="{FA15E077-C7FD-42E7-A5F3-AC50929F77F4}"/>
-    <hyperlink ref="I31" r:id="rId6" xr:uid="{2D74694A-18E3-4092-AA2F-BC65E158D410}"/>
-    <hyperlink ref="H15" r:id="rId7" display="mailto:hugo.bernier@umontreal.ca" xr:uid="{3F591457-DA50-462E-B1CA-F2F56ED9E3DD}"/>
-    <hyperlink ref="I15" r:id="rId8" xr:uid="{11A3F440-1028-45FC-8DC2-DE60A7EA0AD9}"/>
-    <hyperlink ref="H57" r:id="rId9" display="mailto:isabelle.lagadec@bib.umontreal.ca" xr:uid="{4822C834-E5A8-42FD-9734-374BFC718C85}"/>
-    <hyperlink ref="H9" r:id="rId10" display="mailto:magalie.beaudoin@umontreal.ca" xr:uid="{2D976BF0-B68A-46E5-8412-BA8BC43FD26D}"/>
-    <hyperlink ref="I9" r:id="rId11" xr:uid="{8AB273DE-5C86-4A48-AF36-BE5967CA61FD}"/>
-    <hyperlink ref="H86" r:id="rId12" display="mailto:mathieu.pigeon@umontreal.ca" xr:uid="{F73DFC6E-4D6D-42F3-84C0-454956AEC7E8}"/>
-    <hyperlink ref="H4" r:id="rId13" display="mailto:nadege.arsa@bib.umontreal.ca" xr:uid="{408AF5A3-35ED-4BF5-92B9-1B21C0C475D9}"/>
-    <hyperlink ref="I4" r:id="rId14" xr:uid="{DD84AED2-20C7-4DA6-BFBF-EEC1E7D79E1B}"/>
-    <hyperlink ref="H16" r:id="rId15" display="mailto:simon.blais.longtin@umontreal.ca" xr:uid="{EA917AC7-9087-435B-A6E7-3AE1885514AA}"/>
-    <hyperlink ref="I16" r:id="rId16" xr:uid="{CDCAA32A-F6EB-49BF-B7CF-1AA918DBB62B}"/>
-    <hyperlink ref="H68" r:id="rId17" xr:uid="{8ABC26E9-CF81-491C-8A28-B209E6620D2A}"/>
-    <hyperlink ref="I26" r:id="rId18" xr:uid="{28692D92-728B-4DFE-B003-A38AA753D55A}"/>
+    <hyperlink ref="I11" r:id="rId1" display="mailto:audrey.begin-poissant@umontreal.ca" xr:uid="{708FEBAC-F938-40E8-8D55-B34C4326210F}"/>
+    <hyperlink ref="J32" r:id="rId2" xr:uid="{574D93C5-0522-4DEE-A777-CB1BD468A7B3}"/>
+    <hyperlink ref="I25" r:id="rId3" display="mailto:delphine.cado@umontreal.ca" xr:uid="{0E0BF38D-BCA7-4652-84E3-BBE8A015792A}"/>
+    <hyperlink ref="J25" r:id="rId4" xr:uid="{27792995-CED1-460A-9DC6-1C7D908E58F9}"/>
+    <hyperlink ref="J99" r:id="rId5" xr:uid="{FA15E077-C7FD-42E7-A5F3-AC50929F77F4}"/>
+    <hyperlink ref="J31" r:id="rId6" xr:uid="{2D74694A-18E3-4092-AA2F-BC65E158D410}"/>
+    <hyperlink ref="I15" r:id="rId7" display="mailto:hugo.bernier@umontreal.ca" xr:uid="{3F591457-DA50-462E-B1CA-F2F56ED9E3DD}"/>
+    <hyperlink ref="J15" r:id="rId8" xr:uid="{11A3F440-1028-45FC-8DC2-DE60A7EA0AD9}"/>
+    <hyperlink ref="I57" r:id="rId9" display="mailto:isabelle.lagadec@bib.umontreal.ca" xr:uid="{4822C834-E5A8-42FD-9734-374BFC718C85}"/>
+    <hyperlink ref="I9" r:id="rId10" display="mailto:magalie.beaudoin@umontreal.ca" xr:uid="{2D976BF0-B68A-46E5-8412-BA8BC43FD26D}"/>
+    <hyperlink ref="J9" r:id="rId11" xr:uid="{8AB273DE-5C86-4A48-AF36-BE5967CA61FD}"/>
+    <hyperlink ref="I86" r:id="rId12" display="mailto:mathieu.pigeon@umontreal.ca" xr:uid="{F73DFC6E-4D6D-42F3-84C0-454956AEC7E8}"/>
+    <hyperlink ref="I4" r:id="rId13" display="mailto:nadege.arsa@bib.umontreal.ca" xr:uid="{408AF5A3-35ED-4BF5-92B9-1B21C0C475D9}"/>
+    <hyperlink ref="J4" r:id="rId14" xr:uid="{DD84AED2-20C7-4DA6-BFBF-EEC1E7D79E1B}"/>
+    <hyperlink ref="I16" r:id="rId15" display="mailto:simon.blais.longtin@umontreal.ca" xr:uid="{EA917AC7-9087-435B-A6E7-3AE1885514AA}"/>
+    <hyperlink ref="J16" r:id="rId16" xr:uid="{CDCAA32A-F6EB-49BF-B7CF-1AA918DBB62B}"/>
+    <hyperlink ref="I68" r:id="rId17" xr:uid="{8ABC26E9-CF81-491C-8A28-B209E6620D2A}"/>
+    <hyperlink ref="J26" r:id="rId18" xr:uid="{28692D92-728B-4DFE-B003-A38AA753D55A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>
@@ -5391,6 +5529,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f6670ae2-8190-4e72-909e-d717fe03ced5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="00db0817-461a-4a69-8eb5-8daf0756d296" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007812637FDE95774892D21861907C1625" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="9e26b686a71b543072340cfd27a56c29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f6670ae2-8190-4e72-909e-d717fe03ced5" xmlns:ns3="00db0817-461a-4a69-8eb5-8daf0756d296" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8d151e41c23af60827e9e8828a6e0ebd" ns2:_="" ns3:_="">
     <xsd:import namespace="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
@@ -5625,27 +5783,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="00db0817-461a-4a69-8eb5-8daf0756d296"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f6670ae2-8190-4e72-909e-d717fe03ced5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="00db0817-461a-4a69-8eb5-8daf0756d296" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{141ACCEB-C60B-4854-82C0-9885432D8ACB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5662,29 +5825,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="00db0817-461a-4a69-8eb5-8daf0756d296"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Correction du "i" majuscule
</commit_message>
<xml_diff>
--- a/content/personnel/liste-personnel.xlsx
+++ b/content/personnel/liste-personnel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p1212882\siteWeb\coquille-web\content\personnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C7D500-A826-4E1D-A374-68A30F7BEF9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AED33B-D304-4FE4-B029-DAEEC9F81C9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2624,8 +2624,8 @@
   <dimension ref="A1:J99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3347,7 +3347,7 @@
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7" t="s">
@@ -5529,6 +5529,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="f6670ae2-8190-4e72-909e-d717fe03ced5">
@@ -5537,15 +5546,6 @@
     <TaxCatchAll xmlns="00db0817-461a-4a69-8eb5-8daf0756d296" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5784,6 +5784,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -5796,14 +5804,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="00db0817-461a-4a69-8eb5-8daf0756d296"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Ajout du contenu pour le champ direction
</commit_message>
<xml_diff>
--- a/content/personnel/liste-personnel.xlsx
+++ b/content/personnel/liste-personnel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p1212882\siteWeb\coquille-web\content\personnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AED33B-D304-4FE4-B029-DAEEC9F81C9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9123F568-E584-49DB-86A0-1FB97E1B09A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="663">
   <si>
     <t>Borsi</t>
   </si>
@@ -2014,9 +2014,6 @@
   </si>
   <si>
     <t>direction</t>
-  </si>
-  <si>
-    <t>test direction</t>
   </si>
 </sst>
 </file>
@@ -2191,7 +2188,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2220,6 +2217,7 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -2273,8 +2271,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A0AF7E1-A614-44BF-8C48-5C26377DC552}" name="Tableau1" displayName="Tableau1" ref="A1:J99" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:J99" xr:uid="{4F6A1D8F-9220-4675-A202-2173F3493722}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A0AF7E1-A614-44BF-8C48-5C26377DC552}" name="Tableau1" displayName="Tableau1" ref="A1:J1048576" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:J1048576" xr:uid="{4F6A1D8F-9220-4675-A202-2173F3493722}">
     <filterColumn colId="6">
       <filters>
         <filter val="Direction de la recherche et des initiatives numériques"/>
@@ -2624,8 +2622,8 @@
   <dimension ref="A1:J99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2637,7 +2635,7 @@
     <col min="7" max="7" width="116.85546875" customWidth="1"/>
     <col min="8" max="8" width="44.28515625" customWidth="1"/>
     <col min="9" max="9" width="36.42578125" customWidth="1"/>
-    <col min="10" max="10" width="75.85546875" customWidth="1"/>
+    <col min="10" max="10" width="75.85546875" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2805,8 +2803,8 @@
       <c r="D6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>663</v>
+      <c r="E6" s="8" t="s">
+        <v>650</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>74</v>
@@ -2894,7 +2892,9 @@
       <c r="D9" s="7" t="s">
         <v>343</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="13" t="s">
+        <v>307</v>
+      </c>
       <c r="F9" s="17"/>
       <c r="G9" s="7" t="s">
         <v>307</v>
@@ -2922,7 +2922,9 @@
       <c r="D10" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="E10" s="9"/>
+      <c r="E10" s="12" t="s">
+        <v>403</v>
+      </c>
       <c r="F10" s="12" t="s">
         <v>403</v>
       </c>
@@ -2980,7 +2982,9 @@
       <c r="D12" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="E12" s="9"/>
+      <c r="E12" s="17" t="s">
+        <v>60</v>
+      </c>
       <c r="F12" s="9" t="s">
         <v>128</v>
       </c>
@@ -3175,7 +3179,9 @@
       <c r="D19" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="7"/>
+      <c r="E19" s="8" t="s">
+        <v>624</v>
+      </c>
       <c r="F19" s="8" t="s">
         <v>624</v>
       </c>
@@ -3263,7 +3269,9 @@
       <c r="D22" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="E22" s="9"/>
+      <c r="E22" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="F22" s="9" t="s">
         <v>54</v>
       </c>
@@ -3321,7 +3329,9 @@
       <c r="D24" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="E24" s="9"/>
+      <c r="E24" s="13" t="s">
+        <v>307</v>
+      </c>
       <c r="F24" s="13" t="s">
         <v>307</v>
       </c>
@@ -3555,7 +3565,9 @@
       <c r="D32" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="E32" s="7"/>
+      <c r="E32" s="8" t="s">
+        <v>624</v>
+      </c>
       <c r="F32" s="7"/>
       <c r="G32" s="7" t="s">
         <v>45</v>
@@ -3673,7 +3685,9 @@
       <c r="D36" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="E36" s="9"/>
+      <c r="E36" s="13" t="s">
+        <v>273</v>
+      </c>
       <c r="F36" s="13" t="s">
         <v>273</v>
       </c>
@@ -3761,7 +3775,9 @@
       <c r="D39" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="E39" s="7"/>
+      <c r="E39" s="7" t="s">
+        <v>110</v>
+      </c>
       <c r="F39" s="7"/>
       <c r="G39" s="7" t="s">
         <v>110</v>
@@ -3819,7 +3835,9 @@
       <c r="D41" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="E41" s="9"/>
+      <c r="E41" s="8" t="s">
+        <v>624</v>
+      </c>
       <c r="F41" s="9" t="s">
         <v>460</v>
       </c>
@@ -3849,7 +3867,9 @@
       <c r="D42" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E42" s="9"/>
+      <c r="E42" s="9" t="s">
+        <v>403</v>
+      </c>
       <c r="F42" s="9" t="s">
         <v>74</v>
       </c>
@@ -3989,7 +4009,9 @@
       <c r="D47" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E47" s="7"/>
+      <c r="E47" s="8" t="s">
+        <v>624</v>
+      </c>
       <c r="F47" s="7"/>
       <c r="G47" s="7" t="s">
         <v>4</v>
@@ -4017,7 +4039,9 @@
       <c r="D48" s="7" t="s">
         <v>535</v>
       </c>
-      <c r="E48" s="7"/>
+      <c r="E48" s="7" t="s">
+        <v>110</v>
+      </c>
       <c r="F48" s="7" t="s">
         <v>110</v>
       </c>
@@ -4218,7 +4242,9 @@
       <c r="D55" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E55" s="7"/>
+      <c r="E55" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="F55" s="8" t="s">
         <v>81</v>
       </c>
@@ -4336,7 +4362,9 @@
       <c r="D59" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="E59" s="7"/>
+      <c r="E59" s="8" t="s">
+        <v>624</v>
+      </c>
       <c r="F59" s="7" t="s">
         <v>74</v>
       </c>
@@ -4366,7 +4394,9 @@
       <c r="D60" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E60" s="9"/>
+      <c r="E60" s="9" t="s">
+        <v>403</v>
+      </c>
       <c r="F60" s="9" t="s">
         <v>633</v>
       </c>
@@ -4426,7 +4456,9 @@
       <c r="D62" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="E62" s="9"/>
+      <c r="E62" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="F62" s="9" t="s">
         <v>253</v>
       </c>
@@ -4456,7 +4488,9 @@
       <c r="D63" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="E63" s="7"/>
+      <c r="E63" s="8" t="s">
+        <v>624</v>
+      </c>
       <c r="F63" s="8" t="s">
         <v>370</v>
       </c>
@@ -4486,7 +4520,9 @@
       <c r="D64" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="E64" s="9"/>
+      <c r="E64" s="17" t="s">
+        <v>60</v>
+      </c>
       <c r="F64" s="9" t="s">
         <v>427</v>
       </c>
@@ -4516,7 +4552,9 @@
       <c r="D65" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="E65" s="7"/>
+      <c r="E65" s="9" t="s">
+        <v>403</v>
+      </c>
       <c r="F65" s="7" t="s">
         <v>151</v>
       </c>
@@ -4544,7 +4582,9 @@
       <c r="D66" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E66" s="11"/>
+      <c r="E66" s="8" t="s">
+        <v>650</v>
+      </c>
       <c r="F66" s="12" t="s">
         <v>370</v>
       </c>
@@ -4682,7 +4722,9 @@
       <c r="D71" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E71" s="7"/>
+      <c r="E71" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="F71" s="7" t="s">
         <v>245</v>
       </c>
@@ -4832,7 +4874,9 @@
       <c r="D76" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="E76" s="16"/>
+      <c r="E76" s="8" t="s">
+        <v>650</v>
+      </c>
       <c r="F76" s="8" t="s">
         <v>650</v>
       </c>
@@ -4860,7 +4904,9 @@
       <c r="D77" s="9" t="s">
         <v>349</v>
       </c>
-      <c r="E77" s="9"/>
+      <c r="E77" s="13" t="s">
+        <v>307</v>
+      </c>
       <c r="F77" s="9" t="s">
         <v>350</v>
       </c>
@@ -4916,7 +4962,9 @@
       <c r="D79" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E79" s="9"/>
+      <c r="E79" s="9" t="s">
+        <v>403</v>
+      </c>
       <c r="F79" s="11" t="s">
         <v>629</v>
       </c>
@@ -5228,7 +5276,9 @@
       <c r="D90" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E90" s="7"/>
+      <c r="E90" s="17" t="s">
+        <v>60</v>
+      </c>
       <c r="F90" s="17" t="s">
         <v>60</v>
       </c>
@@ -5312,7 +5362,9 @@
       <c r="D93" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="E93" s="11"/>
+      <c r="E93" s="8" t="s">
+        <v>650</v>
+      </c>
       <c r="F93" s="11"/>
       <c r="G93" s="11" t="s">
         <v>653</v>
@@ -5338,7 +5390,9 @@
       <c r="D94" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E94" s="7"/>
+      <c r="E94" s="17" t="s">
+        <v>60</v>
+      </c>
       <c r="F94" s="7" t="s">
         <v>420</v>
       </c>
@@ -5368,7 +5422,9 @@
       <c r="D95" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="E95" s="16"/>
+      <c r="E95" s="8" t="s">
+        <v>650</v>
+      </c>
       <c r="F95" s="16" t="s">
         <v>460</v>
       </c>
@@ -5529,26 +5585,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f6670ae2-8190-4e72-909e-d717fe03ced5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="00db0817-461a-4a69-8eb5-8daf0756d296" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007812637FDE95774892D21861907C1625" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="9e26b686a71b543072340cfd27a56c29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f6670ae2-8190-4e72-909e-d717fe03ced5" xmlns:ns3="00db0817-461a-4a69-8eb5-8daf0756d296" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8d151e41c23af60827e9e8828a6e0ebd" ns2:_="" ns3:_="">
     <xsd:import namespace="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
@@ -5783,10 +5819,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f6670ae2-8190-4e72-909e-d717fe03ced5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="00db0817-461a-4a69-8eb5-8daf0756d296" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{141ACCEB-C60B-4854-82C0-9885432D8ACB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
+    <ds:schemaRef ds:uri="00db0817-461a-4a69-8eb5-8daf0756d296"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5809,20 +5876,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{141ACCEB-C60B-4854-82C0-9885432D8ACB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
-    <ds:schemaRef ds:uri="00db0817-461a-4a69-8eb5-8daf0756d296"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Corrections sur le contenu de la liste de personnel
</commit_message>
<xml_diff>
--- a/content/personnel/liste-personnel.xlsx
+++ b/content/personnel/liste-personnel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p1212882\siteWeb\coquille-web\content\personnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F84E239-F94F-4F13-933D-69311AADEBED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B899ED13-06F4-4CBC-8C61-9D716B204CA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="670">
   <si>
     <t>Borsi</t>
   </si>
@@ -2014,13 +2014,34 @@
   </si>
   <si>
     <t>direction</t>
+  </si>
+  <si>
+    <t>Direction des bibliothèques sociétés et création;</t>
+  </si>
+  <si>
+    <t>Direction de la Bibliothèque des  lettres et sciences humaines et  Livres rares et collections spéciales</t>
+  </si>
+  <si>
+    <t>Direction des bibliothèques des sciences de la santé et des bibliothèques scientifiques</t>
+  </si>
+  <si>
+    <t>Direction des bibliothèques des  sciences de la santé et des  bibliothèques scientifiques</t>
+  </si>
+  <si>
+    <t>Direction de la Bibliothèque des lettres et sciences humaines et Livres rares et collections spéciales</t>
+  </si>
+  <si>
+    <t>Direction des bibliothèques Sociétés et création</t>
+  </si>
+  <si>
+    <t>Direction de la recherche et des initiatives numériques;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2106,6 +2127,11 @@
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2188,7 +2214,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2218,6 +2244,10 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -2619,11 +2649,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J99"/>
+  <dimension ref="A1:J126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E95" sqref="E95"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2803,8 +2833,8 @@
       <c r="D6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>650</v>
+      <c r="E6" s="7" t="s">
+        <v>663</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>74</v>
@@ -2892,7 +2922,7 @@
       <c r="D9" s="7" t="s">
         <v>343</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="7" t="s">
         <v>307</v>
       </c>
       <c r="F9" s="17"/>
@@ -2922,8 +2952,8 @@
       <c r="D10" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>403</v>
+      <c r="E10" t="s">
+        <v>664</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>403</v>
@@ -2952,7 +2982,9 @@
       <c r="D11" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>81</v>
+      </c>
       <c r="F11" s="9" t="s">
         <v>80</v>
       </c>
@@ -2982,7 +3014,7 @@
       <c r="D12" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="9" t="s">
         <v>60</v>
       </c>
       <c r="F12" s="9" t="s">
@@ -3068,7 +3100,9 @@
       <c r="D15" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="F15" s="7" t="s">
         <v>284</v>
       </c>
@@ -3096,7 +3130,6 @@
       <c r="D16" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="7"/>
       <c r="F16" s="17" t="s">
         <v>512</v>
       </c>
@@ -3124,6 +3157,9 @@
       <c r="D17" t="s">
         <v>11</v>
       </c>
+      <c r="E17" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="F17" s="3" t="s">
         <v>563</v>
       </c>
@@ -3151,7 +3187,6 @@
       <c r="D18" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11" t="s">
         <v>307</v>
@@ -3179,8 +3214,8 @@
       <c r="D19" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>624</v>
+      <c r="E19" s="11" t="s">
+        <v>307</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>624</v>
@@ -3211,7 +3246,9 @@
       <c r="D20" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="9"/>
+      <c r="E20" s="25" t="s">
+        <v>665</v>
+      </c>
       <c r="F20" s="13" t="s">
         <v>211</v>
       </c>
@@ -3241,7 +3278,7 @@
       <c r="D21" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="7"/>
+      <c r="E21" s="9"/>
       <c r="F21" s="7" t="s">
         <v>498</v>
       </c>
@@ -3269,9 +3306,7 @@
       <c r="D22" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>81</v>
-      </c>
+      <c r="E22" s="7"/>
       <c r="F22" s="9" t="s">
         <v>54</v>
       </c>
@@ -3299,7 +3334,9 @@
       <c r="D23" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="9"/>
+      <c r="E23" s="9" t="s">
+        <v>81</v>
+      </c>
       <c r="F23" s="9" t="s">
         <v>277</v>
       </c>
@@ -3329,9 +3366,7 @@
       <c r="D24" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="E24" s="13" t="s">
-        <v>307</v>
-      </c>
+      <c r="E24" s="9"/>
       <c r="F24" s="13" t="s">
         <v>307</v>
       </c>
@@ -3359,7 +3394,9 @@
       <c r="D25" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E25" s="7"/>
+      <c r="E25" s="9" t="s">
+        <v>307</v>
+      </c>
       <c r="F25" s="7" t="s">
         <v>165</v>
       </c>
@@ -3389,7 +3426,6 @@
       <c r="D26" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="E26" s="7"/>
       <c r="F26" s="7" t="s">
         <v>657</v>
       </c>
@@ -3445,7 +3481,7 @@
       <c r="D28" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="9"/>
+      <c r="E28" s="7"/>
       <c r="F28" s="13" t="s">
         <v>505</v>
       </c>
@@ -3475,7 +3511,9 @@
       <c r="D29" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="E29" s="7"/>
+      <c r="E29" s="9" t="s">
+        <v>81</v>
+      </c>
       <c r="F29" s="7" t="s">
         <v>204</v>
       </c>
@@ -3505,7 +3543,6 @@
       <c r="D30" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E30" s="7"/>
       <c r="F30" s="17" t="s">
         <v>447</v>
       </c>
@@ -3535,7 +3572,6 @@
       <c r="D31" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="E31" s="9"/>
       <c r="F31" s="13" t="s">
         <v>238</v>
       </c>
@@ -3565,8 +3601,8 @@
       <c r="D32" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="E32" s="9" t="s">
-        <v>624</v>
+      <c r="E32" s="17" t="s">
+        <v>307</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="7" t="s">
@@ -3625,7 +3661,9 @@
       <c r="D34" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="7"/>
+      <c r="E34" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="F34" s="7" t="s">
         <v>630</v>
       </c>
@@ -3685,9 +3723,7 @@
       <c r="D36" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="E36" s="13" t="s">
-        <v>273</v>
-      </c>
+      <c r="E36" s="9"/>
       <c r="F36" s="13" t="s">
         <v>273</v>
       </c>
@@ -3717,7 +3753,9 @@
       <c r="D37" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="9"/>
+      <c r="E37" t="s">
+        <v>666</v>
+      </c>
       <c r="F37" s="9" t="s">
         <v>625</v>
       </c>
@@ -3775,9 +3813,7 @@
       <c r="D39" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>110</v>
-      </c>
+      <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="7" t="s">
         <v>110</v>
@@ -3836,7 +3872,7 @@
         <v>252</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>624</v>
+        <v>273</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>460</v>
@@ -3867,9 +3903,7 @@
       <c r="D42" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E42" s="9" t="s">
-        <v>403</v>
-      </c>
+      <c r="E42" s="9"/>
       <c r="F42" s="9" t="s">
         <v>74</v>
       </c>
@@ -3927,7 +3961,7 @@
       <c r="D44" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E44" s="9"/>
+      <c r="E44" s="7"/>
       <c r="F44" s="13" t="s">
         <v>637</v>
       </c>
@@ -3955,7 +3989,6 @@
       <c r="D45" s="7" t="s">
         <v>641</v>
       </c>
-      <c r="E45" s="7"/>
       <c r="F45" s="17" t="s">
         <v>642</v>
       </c>
@@ -3981,7 +4014,7 @@
       <c r="D46" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E46" s="9"/>
+      <c r="E46" s="7"/>
       <c r="F46" s="9" t="s">
         <v>143</v>
       </c>
@@ -4009,9 +4042,6 @@
       <c r="D47" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E47" s="9" t="s">
-        <v>624</v>
-      </c>
       <c r="F47" s="7"/>
       <c r="G47" s="7" t="s">
         <v>4</v>
@@ -4040,7 +4070,7 @@
         <v>535</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>110</v>
+        <v>665</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>110</v>
@@ -4058,7 +4088,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" ht="45">
       <c r="A49" s="9" t="s">
         <v>387</v>
       </c>
@@ -4071,7 +4101,9 @@
       <c r="D49" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="E49" s="9"/>
+      <c r="E49" s="26" t="s">
+        <v>667</v>
+      </c>
       <c r="F49" s="13" t="s">
         <v>390</v>
       </c>
@@ -4099,7 +4131,7 @@
       <c r="D50" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E50" s="7"/>
+      <c r="E50" s="9"/>
       <c r="F50" s="7" t="s">
         <v>636</v>
       </c>
@@ -4127,7 +4159,7 @@
       <c r="D51" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E51" s="7"/>
+      <c r="E51" s="9"/>
       <c r="F51" s="7" t="s">
         <v>613</v>
       </c>
@@ -4153,7 +4185,9 @@
       <c r="D52" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="7"/>
+      <c r="E52" s="7" t="s">
+        <v>273</v>
+      </c>
       <c r="F52" s="7" t="s">
         <v>44</v>
       </c>
@@ -4213,6 +4247,9 @@
       <c r="D54" t="s">
         <v>11</v>
       </c>
+      <c r="E54" s="7" t="s">
+        <v>110</v>
+      </c>
       <c r="F54" s="3" t="s">
         <v>570</v>
       </c>
@@ -4242,8 +4279,8 @@
       <c r="D55" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E55" s="9" t="s">
-        <v>81</v>
+      <c r="E55" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="F55" s="8" t="s">
         <v>81</v>
@@ -4274,7 +4311,7 @@
       <c r="D56" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E56" s="7"/>
+      <c r="E56" s="9"/>
       <c r="F56" s="7" t="s">
         <v>29</v>
       </c>
@@ -4302,7 +4339,7 @@
       <c r="D57" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E57" s="9"/>
+      <c r="E57" s="7"/>
       <c r="F57" s="9" t="s">
         <v>626</v>
       </c>
@@ -4332,7 +4369,7 @@
       <c r="D58" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E58" s="9"/>
+      <c r="E58" s="7"/>
       <c r="F58" s="9" t="s">
         <v>54</v>
       </c>
@@ -4362,8 +4399,8 @@
       <c r="D59" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="E59" s="9" t="s">
-        <v>624</v>
+      <c r="E59" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>74</v>
@@ -4394,9 +4431,7 @@
       <c r="D60" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E60" s="9" t="s">
-        <v>403</v>
-      </c>
+      <c r="E60" s="7"/>
       <c r="F60" s="9" t="s">
         <v>633</v>
       </c>
@@ -4456,9 +4491,7 @@
       <c r="D62" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="E62" s="9" t="s">
-        <v>81</v>
-      </c>
+      <c r="E62"/>
       <c r="F62" s="9" t="s">
         <v>253</v>
       </c>
@@ -4488,8 +4521,8 @@
       <c r="D63" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="E63" s="9" t="s">
-        <v>624</v>
+      <c r="E63" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="F63" s="8" t="s">
         <v>370</v>
@@ -4520,9 +4553,7 @@
       <c r="D64" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="E64" s="9" t="s">
-        <v>60</v>
-      </c>
+      <c r="E64" s="7"/>
       <c r="F64" s="9" t="s">
         <v>427</v>
       </c>
@@ -4552,9 +4583,6 @@
       <c r="D65" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="E65" s="9" t="s">
-        <v>403</v>
-      </c>
       <c r="F65" s="7" t="s">
         <v>151</v>
       </c>
@@ -4582,9 +4610,7 @@
       <c r="D66" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E66" s="9" t="s">
-        <v>650</v>
-      </c>
+      <c r="E66" s="9"/>
       <c r="F66" s="12" t="s">
         <v>370</v>
       </c>
@@ -4612,7 +4638,6 @@
       <c r="D67" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E67" s="7"/>
       <c r="F67" s="7"/>
       <c r="G67" s="7" t="s">
         <v>60</v>
@@ -4636,7 +4661,7 @@
       <c r="D68" s="7" t="s">
         <v>648</v>
       </c>
-      <c r="E68" s="7"/>
+      <c r="E68" s="9"/>
       <c r="F68" s="17"/>
       <c r="G68" s="7" t="s">
         <v>273</v>
@@ -4662,7 +4687,9 @@
       <c r="D69" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E69" s="7"/>
+      <c r="E69" s="7" t="s">
+        <v>665</v>
+      </c>
       <c r="F69" s="7" t="s">
         <v>484</v>
       </c>
@@ -4679,7 +4706,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" ht="45">
       <c r="A70" s="7" t="s">
         <v>432</v>
       </c>
@@ -4692,7 +4719,9 @@
       <c r="D70" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E70" s="7"/>
+      <c r="E70" s="26" t="s">
+        <v>667</v>
+      </c>
       <c r="F70" s="7" t="s">
         <v>260</v>
       </c>
@@ -4722,9 +4751,7 @@
       <c r="D71" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E71" s="9" t="s">
-        <v>81</v>
-      </c>
+      <c r="E71"/>
       <c r="F71" s="7" t="s">
         <v>245</v>
       </c>
@@ -4754,7 +4781,7 @@
       <c r="D72" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E72" s="7"/>
+      <c r="E72" s="9"/>
       <c r="F72" s="7" t="s">
         <v>135</v>
       </c>
@@ -4784,7 +4811,7 @@
       <c r="D73" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E73" s="7"/>
+      <c r="E73" s="9"/>
       <c r="F73" s="16" t="s">
         <v>260</v>
       </c>
@@ -4814,7 +4841,9 @@
       <c r="D74" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E74" s="9"/>
+      <c r="E74" s="9" t="s">
+        <v>81</v>
+      </c>
       <c r="F74" s="9" t="s">
         <v>332</v>
       </c>
@@ -4844,7 +4873,9 @@
       <c r="D75" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E75" s="9"/>
+      <c r="E75" s="7" t="s">
+        <v>665</v>
+      </c>
       <c r="F75" s="13" t="s">
         <v>66</v>
       </c>
@@ -4875,7 +4906,7 @@
         <v>231</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>650</v>
+        <v>60</v>
       </c>
       <c r="F76" s="8" t="s">
         <v>650</v>
@@ -4893,7 +4924,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" ht="45">
       <c r="A77" s="9" t="s">
         <v>347</v>
       </c>
@@ -4904,8 +4935,8 @@
       <c r="D77" s="9" t="s">
         <v>349</v>
       </c>
-      <c r="E77" s="13" t="s">
-        <v>307</v>
+      <c r="E77" s="26" t="s">
+        <v>667</v>
       </c>
       <c r="F77" s="9" t="s">
         <v>350</v>
@@ -4934,7 +4965,9 @@
       <c r="D78" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E78" s="9"/>
+      <c r="E78" s="16" t="s">
+        <v>650</v>
+      </c>
       <c r="F78" s="9"/>
       <c r="G78" s="9" t="s">
         <v>224</v>
@@ -4962,8 +4995,8 @@
       <c r="D79" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E79" s="9" t="s">
-        <v>403</v>
+      <c r="E79" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="F79" s="11" t="s">
         <v>629</v>
@@ -4992,7 +5025,7 @@
       <c r="D80" s="9" t="s">
         <v>645</v>
       </c>
-      <c r="E80" s="9"/>
+      <c r="E80" s="7"/>
       <c r="F80" s="13"/>
       <c r="G80" s="9" t="s">
         <v>273</v>
@@ -5016,6 +5049,7 @@
       <c r="D81" t="s">
         <v>195</v>
       </c>
+      <c r="E81" s="7"/>
       <c r="F81" s="3" t="s">
         <v>595</v>
       </c>
@@ -5042,7 +5076,9 @@
       <c r="D82" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E82" s="7"/>
+      <c r="E82" s="7" t="s">
+        <v>273</v>
+      </c>
       <c r="F82" s="17" t="s">
         <v>218</v>
       </c>
@@ -5102,7 +5138,7 @@
       <c r="D84" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E84" s="9"/>
+      <c r="E84" s="7"/>
       <c r="F84" s="9" t="s">
         <v>158</v>
       </c>
@@ -5132,7 +5168,9 @@
       <c r="D85" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E85" s="7"/>
+      <c r="E85" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="F85" s="7" t="s">
         <v>498</v>
       </c>
@@ -5190,7 +5228,7 @@
       <c r="D87" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E87" s="9"/>
+      <c r="E87" s="7"/>
       <c r="F87" s="13" t="s">
         <v>377</v>
       </c>
@@ -5220,6 +5258,7 @@
       <c r="D88" t="s">
         <v>11</v>
       </c>
+      <c r="E88" s="7"/>
       <c r="F88" s="3" t="s">
         <v>583</v>
       </c>
@@ -5247,6 +5286,7 @@
       <c r="D89" t="s">
         <v>17</v>
       </c>
+      <c r="E89" s="9"/>
       <c r="F89" t="s">
         <v>18</v>
       </c>
@@ -5276,9 +5316,7 @@
       <c r="D90" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E90" s="17" t="s">
-        <v>60</v>
-      </c>
+      <c r="E90" s="9"/>
       <c r="F90" s="17" t="s">
         <v>60</v>
       </c>
@@ -5306,7 +5344,7 @@
       <c r="D91" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E91" s="7"/>
+      <c r="E91" s="9"/>
       <c r="F91" s="17" t="s">
         <v>121</v>
       </c>
@@ -5334,7 +5372,9 @@
       <c r="D92" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="E92" s="11"/>
+      <c r="E92" s="16" t="s">
+        <v>650</v>
+      </c>
       <c r="F92" s="11" t="s">
         <v>607</v>
       </c>
@@ -5362,9 +5402,7 @@
       <c r="D93" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="E93" s="9" t="s">
-        <v>650</v>
-      </c>
+      <c r="E93" s="9"/>
       <c r="F93" s="11"/>
       <c r="G93" s="11" t="s">
         <v>653</v>
@@ -5391,7 +5429,7 @@
         <v>127</v>
       </c>
       <c r="E94" s="9" t="s">
-        <v>60</v>
+        <v>224</v>
       </c>
       <c r="F94" s="7" t="s">
         <v>420</v>
@@ -5409,7 +5447,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" ht="45">
       <c r="A95" s="16" t="s">
         <v>457</v>
       </c>
@@ -5422,8 +5460,8 @@
       <c r="D95" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="E95" s="9" t="s">
-        <v>650</v>
+      <c r="E95" s="26" t="s">
+        <v>667</v>
       </c>
       <c r="F95" s="16" t="s">
         <v>460</v>
@@ -5454,7 +5492,9 @@
       <c r="D96" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E96" s="9"/>
+      <c r="E96" s="9" t="s">
+        <v>273</v>
+      </c>
       <c r="F96" s="9" t="s">
         <v>211</v>
       </c>
@@ -5482,7 +5522,9 @@
       <c r="D97" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E97" s="7"/>
+      <c r="E97" t="s">
+        <v>60</v>
+      </c>
       <c r="F97" s="7" t="s">
         <v>325</v>
       </c>
@@ -5512,7 +5554,9 @@
       <c r="D98" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E98" s="7"/>
+      <c r="E98" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="F98" s="17" t="s">
         <v>384</v>
       </c>
@@ -5538,7 +5582,7 @@
       <c r="D99" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="E99" s="9"/>
+      <c r="E99" s="7"/>
       <c r="F99" s="9" t="s">
         <v>196</v>
       </c>
@@ -5553,6 +5597,91 @@
       </c>
       <c r="J99" s="14" t="s">
         <v>199</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="E100" s="9"/>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="E101" s="7"/>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="E102" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="E103" s="9"/>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="E104" s="9"/>
+    </row>
+    <row r="108" spans="1:10">
+      <c r="E108" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="E109" s="7"/>
+    </row>
+    <row r="110" spans="1:10">
+      <c r="E110" s="7"/>
+    </row>
+    <row r="111" spans="1:10">
+      <c r="E111" s="11"/>
+    </row>
+    <row r="112" spans="1:10">
+      <c r="E112" s="11" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="113" spans="5:5">
+      <c r="E113" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="114" spans="5:5">
+      <c r="E114" s="7"/>
+    </row>
+    <row r="115" spans="5:5">
+      <c r="E115" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="116" spans="5:5">
+      <c r="E116" s="9"/>
+    </row>
+    <row r="117" spans="5:5">
+      <c r="E117" s="9"/>
+    </row>
+    <row r="118" spans="5:5">
+      <c r="E118" s="7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="119" spans="5:5">
+      <c r="E119" s="7"/>
+    </row>
+    <row r="121" spans="5:5">
+      <c r="E121" s="7"/>
+    </row>
+    <row r="122" spans="5:5">
+      <c r="E122" s="7"/>
+    </row>
+    <row r="123" spans="5:5">
+      <c r="E123" s="7"/>
+    </row>
+    <row r="124" spans="5:5">
+      <c r="E124" s="7" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="125" spans="5:5">
+      <c r="E125" s="7"/>
+    </row>
+    <row r="126" spans="5:5">
+      <c r="E126" s="9" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -5585,26 +5714,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f6670ae2-8190-4e72-909e-d717fe03ced5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="00db0817-461a-4a69-8eb5-8daf0756d296" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007812637FDE95774892D21861907C1625" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="9e26b686a71b543072340cfd27a56c29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f6670ae2-8190-4e72-909e-d717fe03ced5" xmlns:ns3="00db0817-461a-4a69-8eb5-8daf0756d296" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8d151e41c23af60827e9e8828a6e0ebd" ns2:_="" ns3:_="">
     <xsd:import namespace="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
@@ -5839,10 +5948,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f6670ae2-8190-4e72-909e-d717fe03ced5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="00db0817-461a-4a69-8eb5-8daf0756d296" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{141ACCEB-C60B-4854-82C0-9885432D8ACB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
+    <ds:schemaRef ds:uri="00db0817-461a-4a69-8eb5-8daf0756d296"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5865,20 +6005,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{141ACCEB-C60B-4854-82C0-9885432D8ACB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
-    <ds:schemaRef ds:uri="00db0817-461a-4a69-8eb5-8daf0756d296"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix(repertoire-personnel): Ajout de la Bibliothèque de musique pour Chantal Taillon
</commit_message>
<xml_diff>
--- a/content/personnel/liste-personnel.xlsx
+++ b/content/personnel/liste-personnel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p1212882\siteWeb\coquille-web\content\personnel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projets\coquille-web\content\personnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B899ED13-06F4-4CBC-8C61-9D716B204CA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135BA10B-B6C7-42DB-81FE-229D808B86E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11300" tabRatio="184" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="669">
   <si>
     <t>Borsi</t>
   </si>
@@ -1984,9 +1984,6 @@
   </si>
   <si>
     <t>Direction des bibliothèques sociétés et création; Bibliothèque d'aménagement; Bibliothèque de droit; Bibliothèque Thérèse-Gouin-Décarie; Bibliothèque du Campus de Laval;Bibliothèque de musique</t>
-  </si>
-  <si>
-    <t>Direction des bibliothèques sociétés et création; Bibliothèque d'aménagement; Bibliothèque de droit; Bibliothèque Thérèse-Gouin-Décarie; Bibliothèque du Campus de Laval</t>
   </si>
   <si>
     <t>Direction des bibliothèques sociétés et création; Bibliothèque d'aménagement; Bibliothèque de droit; Bibliothèque Thérèse-Gouin-Décarie; Bibliothèque du Campus de Laval; Bibliothèque de musique</t>
@@ -2651,21 +2648,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="3" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" customWidth="1"/>
+    <col min="2" max="3" width="18.81640625" customWidth="1"/>
     <col min="4" max="5" width="45" customWidth="1"/>
-    <col min="6" max="6" width="79.42578125" customWidth="1"/>
-    <col min="7" max="7" width="116.85546875" customWidth="1"/>
-    <col min="8" max="8" width="44.28515625" customWidth="1"/>
-    <col min="9" max="9" width="36.42578125" customWidth="1"/>
-    <col min="10" max="10" width="75.85546875" style="24" customWidth="1"/>
+    <col min="6" max="6" width="79.453125" customWidth="1"/>
+    <col min="7" max="7" width="116.81640625" customWidth="1"/>
+    <col min="8" max="8" width="44.26953125" customWidth="1"/>
+    <col min="9" max="9" width="36.453125" customWidth="1"/>
+    <col min="10" max="10" width="75.81640625" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2682,7 +2679,7 @@
         <v>618</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>617</v>
@@ -2834,13 +2831,13 @@
         <v>22</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>74</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>75</v>
@@ -2870,7 +2867,7 @@
         <v>631</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>441</v>
@@ -2953,7 +2950,7 @@
         <v>402</v>
       </c>
       <c r="E10" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>403</v>
@@ -3247,7 +3244,7 @@
         <v>53</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>211</v>
@@ -3415,29 +3412,29 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="7" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>164</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>81</v>
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="15" t="s">
+        <v>657</v>
+      </c>
+      <c r="J26" s="15" t="s">
         <v>658</v>
-      </c>
-      <c r="J26" s="15" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -3754,7 +3751,7 @@
         <v>11</v>
       </c>
       <c r="E37" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>625</v>
@@ -4070,7 +4067,7 @@
         <v>535</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>110</v>
@@ -4088,7 +4085,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="45">
+    <row r="49" spans="1:10" ht="29">
       <c r="A49" s="9" t="s">
         <v>387</v>
       </c>
@@ -4102,7 +4099,7 @@
         <v>195</v>
       </c>
       <c r="E49" s="26" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F49" s="13" t="s">
         <v>390</v>
@@ -4688,7 +4685,7 @@
         <v>11</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>484</v>
@@ -4706,7 +4703,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="45">
+    <row r="70" spans="1:10" ht="29">
       <c r="A70" s="7" t="s">
         <v>432</v>
       </c>
@@ -4720,7 +4717,7 @@
         <v>11</v>
       </c>
       <c r="E70" s="26" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F70" s="7" t="s">
         <v>260</v>
@@ -4874,7 +4871,7 @@
         <v>11</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F75" s="13" t="s">
         <v>66</v>
@@ -4912,7 +4909,7 @@
         <v>650</v>
       </c>
       <c r="G76" s="16" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="H76" s="16" t="s">
         <v>232</v>
@@ -4924,7 +4921,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="45">
+    <row r="77" spans="1:10" ht="29">
       <c r="A77" s="9" t="s">
         <v>347</v>
       </c>
@@ -4936,7 +4933,7 @@
         <v>349</v>
       </c>
       <c r="E77" s="26" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F77" s="9" t="s">
         <v>350</v>
@@ -5447,7 +5444,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="45">
+    <row r="95" spans="1:10" ht="29">
       <c r="A95" s="16" t="s">
         <v>457</v>
       </c>
@@ -5461,7 +5458,7 @@
         <v>362</v>
       </c>
       <c r="E95" s="26" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F95" s="16" t="s">
         <v>460</v>
@@ -5645,7 +5642,7 @@
     </row>
     <row r="115" spans="5:5">
       <c r="E115" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="116" spans="5:5">
@@ -5673,7 +5670,7 @@
     </row>
     <row r="124" spans="5:5">
       <c r="E124" s="7" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="125" spans="5:5">
@@ -5714,6 +5711,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f6670ae2-8190-4e72-909e-d717fe03ced5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="00db0817-461a-4a69-8eb5-8daf0756d296" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007812637FDE95774892D21861907C1625" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="9e26b686a71b543072340cfd27a56c29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f6670ae2-8190-4e72-909e-d717fe03ced5" xmlns:ns3="00db0817-461a-4a69-8eb5-8daf0756d296" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8d151e41c23af60827e9e8828a6e0ebd" ns2:_="" ns3:_="">
     <xsd:import namespace="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
@@ -5948,41 +5965,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f6670ae2-8190-4e72-909e-d717fe03ced5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="00db0817-461a-4a69-8eb5-8daf0756d296" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{141ACCEB-C60B-4854-82C0-9885432D8ACB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
-    <ds:schemaRef ds:uri="00db0817-461a-4a69-8eb5-8daf0756d296"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6005,9 +5991,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{141ACCEB-C60B-4854-82C0-9885432D8ACB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f6670ae2-8190-4e72-909e-d717fe03ced5"/>
+    <ds:schemaRef ds:uri="00db0817-461a-4a69-8eb5-8daf0756d296"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Mise à jour du fichier du répertoire
</commit_message>
<xml_diff>
--- a/content/personnel/liste-personnel.xlsx
+++ b/content/personnel/liste-personnel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p1212882\siteWeb\coquille-web\content\personnel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udemontreal-my.sharepoint.com/personal/mathieu_nicolas_tardif_umontreal_ca/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0359BA1A-3C3B-4D85-93D1-23695A5AB4E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{A26446F4-863B-4A00-AE77-7AFA78F7D4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11515A0B-4F6F-4D62-A083-765C240211A5}"/>
   <bookViews>
-    <workbookView xWindow="58980" yWindow="-3495" windowWidth="25455" windowHeight="28020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60555" yWindow="-2670" windowWidth="30915" windowHeight="28020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="776">
   <si>
     <t>nom</t>
   </si>
@@ -2374,12 +2385,15 @@
   <si>
     <t>marie-helene-vezina.jpg</t>
   </si>
+  <si>
+    <t>mathieu-tardif.jpg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2573,9 +2587,6 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2598,6 +2609,9 @@
           <bgColor rgb="FFB8CCE4"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -2668,29 +2682,29 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A0AF7E1-A614-44BF-8C48-5C26377DC552}" name="Tableau1" displayName="Tableau1" ref="A1:J126" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:J126" xr:uid="{4A0AF7E1-A614-44BF-8C48-5C26377DC552}"/>
-  <sortState ref="A2:J126">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J126">
     <sortCondition ref="A1:A126"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{4B04E1AF-0079-4AD2-81CA-E8A433733E21}" name="nom"/>
     <tableColumn id="2" xr3:uid="{1806D27F-AC1F-4E36-9BA8-C129073C454B}" name="prenom"/>
-    <tableColumn id="10" xr3:uid="{E3A23A48-0B2E-4806-A0DF-3FD140C193D8}" name="photo" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{E3A23A48-0B2E-4806-A0DF-3FD140C193D8}" name="photo" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{0FE88E88-BACD-4136-9DE5-D5CF43012561}" name="fonction"/>
-    <tableColumn id="9" xr3:uid="{5D8C8F40-AC09-4A58-AADB-E868267363E8}" name="direction" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{5D8C8F40-AC09-4A58-AADB-E868267363E8}" name="direction" dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{EAABD870-1607-4CF3-AAF5-8E02FDD82AD3}" name="disciplines"/>
     <tableColumn id="4" xr3:uid="{05DDFE09-1E34-4D35-BAB3-F489E7BA0330}" name="bibliotheque"/>
     <tableColumn id="5" xr3:uid="{46B2E408-5C8E-434E-9C2D-03D2C880B796}" name="telephone"/>
     <tableColumn id="6" xr3:uid="{1B50FE7B-209E-45E2-97D9-6B4E8A4571F7}" name="courriel"/>
-    <tableColumn id="7" xr3:uid="{8D15EE71-3F80-4AD2-9232-FBA3E46614DC}" name="teams" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{8D15EE71-3F80-4AD2-9232-FBA3E46614DC}" name="teams" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2728,9 +2742,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2763,26 +2777,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2815,26 +2812,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3011,11 +2991,11 @@
   <dimension ref="A1:J126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="3" width="13" customWidth="1"/>
@@ -3027,7 +3007,7 @@
     <col min="9" max="9" width="78.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3059,7 +3039,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
@@ -3089,7 +3069,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
@@ -3119,7 +3099,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
@@ -3149,7 +3129,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>31</v>
       </c>
@@ -3179,7 +3159,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>37</v>
       </c>
@@ -3211,7 +3191,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>44</v>
       </c>
@@ -3241,7 +3221,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -3270,7 +3250,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>58</v>
       </c>
@@ -3297,7 +3277,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>65</v>
       </c>
@@ -3326,7 +3306,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>71</v>
       </c>
@@ -3353,7 +3333,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>78</v>
       </c>
@@ -3382,7 +3362,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>86</v>
       </c>
@@ -3412,7 +3392,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>93</v>
       </c>
@@ -3436,7 +3416,7 @@
       </c>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>98</v>
       </c>
@@ -3464,7 +3444,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>98</v>
       </c>
@@ -3488,7 +3468,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>108</v>
       </c>
@@ -3518,7 +3498,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>114</v>
       </c>
@@ -3547,7 +3527,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>120</v>
       </c>
@@ -3572,7 +3552,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>126</v>
       </c>
@@ -3601,7 +3581,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>133</v>
       </c>
@@ -3631,7 +3611,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>140</v>
       </c>
@@ -3661,7 +3641,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>146</v>
       </c>
@@ -3688,7 +3668,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>153</v>
       </c>
@@ -3716,7 +3696,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>160</v>
       </c>
@@ -3743,7 +3723,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>165</v>
       </c>
@@ -3766,7 +3746,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>170</v>
       </c>
@@ -3794,7 +3774,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>177</v>
       </c>
@@ -3822,7 +3802,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>184</v>
       </c>
@@ -3852,7 +3832,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>189</v>
       </c>
@@ -3866,7 +3846,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>191</v>
       </c>
@@ -3889,7 +3869,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>197</v>
       </c>
@@ -3908,7 +3888,7 @@
       <c r="I32" s="14"/>
       <c r="J32" s="21"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>200</v>
       </c>
@@ -3938,7 +3918,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>206</v>
       </c>
@@ -3967,7 +3947,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>214</v>
       </c>
@@ -3997,7 +3977,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>220</v>
       </c>
@@ -4027,7 +4007,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>226</v>
       </c>
@@ -4059,7 +4039,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>233</v>
       </c>
@@ -4089,7 +4069,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>239</v>
       </c>
@@ -4119,7 +4099,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>245</v>
       </c>
@@ -4149,7 +4129,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>251</v>
       </c>
@@ -4176,7 +4156,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>258</v>
       </c>
@@ -4206,7 +4186,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>264</v>
       </c>
@@ -4236,7 +4216,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>270</v>
       </c>
@@ -4262,7 +4242,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>276</v>
       </c>
@@ -4285,7 +4265,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>281</v>
       </c>
@@ -4315,7 +4295,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>287</v>
       </c>
@@ -4339,7 +4319,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>292</v>
       </c>
@@ -4371,7 +4351,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="30">
+    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>297</v>
       </c>
@@ -4403,7 +4383,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>302</v>
       </c>
@@ -4431,7 +4411,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>309</v>
       </c>
@@ -4461,7 +4441,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>315</v>
       </c>
@@ -4485,7 +4465,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>320</v>
       </c>
@@ -4515,7 +4495,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>326</v>
       </c>
@@ -4542,7 +4522,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>326</v>
       </c>
@@ -4567,7 +4547,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>334</v>
       </c>
@@ -4597,7 +4577,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>340</v>
       </c>
@@ -4625,7 +4605,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>346</v>
       </c>
@@ -4653,7 +4633,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>352</v>
       </c>
@@ -4679,7 +4659,7 @@
       <c r="I59" s="6"/>
       <c r="J59" s="6"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>356</v>
       </c>
@@ -4709,7 +4689,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>361</v>
       </c>
@@ -4739,7 +4719,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>367</v>
       </c>
@@ -4768,7 +4748,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="63" spans="1:10" s="4" customFormat="1">
+    <row r="63" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>373</v>
       </c>
@@ -4795,7 +4775,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>378</v>
       </c>
@@ -4825,7 +4805,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="5" customFormat="1">
+    <row r="65" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>384</v>
       </c>
@@ -4851,7 +4831,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>389</v>
       </c>
@@ -4879,7 +4859,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>392</v>
       </c>
@@ -4902,7 +4882,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>396</v>
       </c>
@@ -4932,7 +4912,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>402</v>
       </c>
@@ -4964,7 +4944,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="30">
+    <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
         <v>407</v>
       </c>
@@ -4996,7 +4976,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>411</v>
       </c>
@@ -5020,7 +5000,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>416</v>
       </c>
@@ -5050,7 +5030,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>422</v>
       </c>
@@ -5075,7 +5055,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="74" spans="1:10" s="4" customFormat="1">
+    <row r="74" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
         <v>427</v>
       </c>
@@ -5104,7 +5084,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="75" spans="1:10" s="4" customFormat="1">
+    <row r="75" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>433</v>
       </c>
@@ -5136,7 +5116,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
         <v>439</v>
       </c>
@@ -5165,7 +5145,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="30">
+    <row r="77" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>445</v>
       </c>
@@ -5195,7 +5175,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="78" spans="1:10" s="4" customFormat="1">
+    <row r="78" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
         <v>451</v>
       </c>
@@ -5225,7 +5205,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>451</v>
       </c>
@@ -5248,7 +5228,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>459</v>
       </c>
@@ -5272,7 +5252,7 @@
       </c>
       <c r="J80" s="6"/>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>464</v>
       </c>
@@ -5296,7 +5276,7 @@
       </c>
       <c r="J81" s="6"/>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>469</v>
       </c>
@@ -5321,7 +5301,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>475</v>
       </c>
@@ -5351,7 +5331,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>480</v>
       </c>
@@ -5381,7 +5361,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>486</v>
       </c>
@@ -5410,7 +5390,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>492</v>
       </c>
@@ -5434,7 +5414,7 @@
       </c>
       <c r="J86" s="6"/>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>496</v>
       </c>
@@ -5464,7 +5444,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="15" t="s">
         <v>502</v>
       </c>
@@ -5494,7 +5474,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
         <v>507</v>
       </c>
@@ -5524,7 +5504,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
         <v>512</v>
       </c>
@@ -5554,7 +5534,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>518</v>
       </c>
@@ -5579,7 +5559,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="15" t="s">
         <v>523</v>
       </c>
@@ -5609,7 +5589,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
         <v>529</v>
       </c>
@@ -5637,7 +5617,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
         <v>536</v>
       </c>
@@ -5662,7 +5642,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="95" spans="1:10" s="4" customFormat="1" ht="30">
+    <row r="95" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
         <v>542</v>
       </c>
@@ -5694,7 +5674,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="96" spans="1:10" s="4" customFormat="1">
+    <row r="96" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
         <v>547</v>
       </c>
@@ -5718,7 +5698,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>552</v>
       </c>
@@ -5747,7 +5727,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
         <v>557</v>
       </c>
@@ -5779,7 +5759,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
         <v>563</v>
       </c>
@@ -5809,7 +5789,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
         <v>563</v>
       </c>
@@ -5839,7 +5819,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
         <v>574</v>
       </c>
@@ -5869,7 +5849,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="102" spans="1:10" s="5" customFormat="1">
+    <row r="102" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>578</v>
       </c>
@@ -5896,7 +5876,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="103" spans="1:10" s="5" customFormat="1">
+    <row r="103" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
         <v>582</v>
       </c>
@@ -5926,7 +5906,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
         <v>588</v>
       </c>
@@ -5950,7 +5930,7 @@
       </c>
       <c r="J104" s="10"/>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>592</v>
       </c>
@@ -5973,7 +5953,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>597</v>
       </c>
@@ -5996,7 +5976,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>602</v>
       </c>
@@ -6025,7 +6005,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
         <v>607</v>
       </c>
@@ -6052,7 +6032,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
         <v>610</v>
       </c>
@@ -6078,7 +6058,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>615</v>
       </c>
@@ -6091,7 +6071,7 @@
       <c r="E110" s="6"/>
       <c r="F110" s="6"/>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="10" t="s">
         <v>617</v>
       </c>
@@ -6121,7 +6101,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="10" t="s">
         <v>623</v>
       </c>
@@ -6147,14 +6127,16 @@
         <v>626</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
         <v>627</v>
       </c>
       <c r="B113" s="6" t="s">
         <v>628</v>
       </c>
-      <c r="C113" s="6"/>
+      <c r="C113" s="6" t="s">
+        <v>775</v>
+      </c>
       <c r="D113" s="6" t="s">
         <v>80</v>
       </c>
@@ -6174,7 +6156,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
         <v>633</v>
       </c>
@@ -6196,7 +6178,7 @@
       </c>
       <c r="J114" s="6"/>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="15" t="s">
         <v>636</v>
       </c>
@@ -6228,7 +6210,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="8" t="s">
         <v>642</v>
       </c>
@@ -6258,7 +6240,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="8" t="s">
         <v>646</v>
       </c>
@@ -6282,7 +6264,7 @@
       </c>
       <c r="J117" s="8"/>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
         <v>650</v>
       </c>
@@ -6307,7 +6289,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
         <v>655</v>
       </c>
@@ -6331,7 +6313,7 @@
       </c>
       <c r="J119" s="6"/>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>655</v>
       </c>
@@ -6357,7 +6339,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
         <v>663</v>
       </c>
@@ -6381,7 +6363,7 @@
       </c>
       <c r="J121" s="6"/>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
         <v>667</v>
       </c>
@@ -6407,7 +6389,7 @@
       </c>
       <c r="J122" s="6"/>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
         <v>672</v>
       </c>
@@ -6431,7 +6413,7 @@
       </c>
       <c r="J123" s="6"/>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
         <v>676</v>
       </c>
@@ -6461,7 +6443,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
         <v>681</v>
       </c>
@@ -6485,7 +6467,7 @@
       </c>
       <c r="J125" s="6"/>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="8" t="s">
         <v>684</v>
       </c>
@@ -6592,26 +6574,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9cb1c2f4-2737-4134-a1af-8acbe3d02830" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CC83367596A4B94585FCDD3502D89912" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="2a2c8be576c5813ed00651336e7e5f0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1" xmlns:ns3="9cb1c2f4-2737-4134-a1af-8acbe3d02830" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="38bcc58a1a25ff2f1b87145c26d2c7e5" ns2:_="" ns3:_="">
     <xsd:import namespace="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1"/>
@@ -6806,10 +6768,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9cb1c2f4-2737-4134-a1af-8acbe3d02830" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDAA9BFF-4339-414A-A7F4-1C453516523F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1"/>
+    <ds:schemaRef ds:uri="9cb1c2f4-2737-4134-a1af-8acbe3d02830"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6834,20 +6827,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDAA9BFF-4339-414A-A7F4-1C453516523F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1"/>
-    <ds:schemaRef ds:uri="9cb1c2f4-2737-4134-a1af-8acbe3d02830"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(repertoire-personnel): Autres changements divers.
</commit_message>
<xml_diff>
--- a/content/personnel/liste-personnel.xlsx
+++ b/content/personnel/liste-personnel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projets\coquille-web\content\personnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF41C5F-3313-49C2-B961-0E2E1FAEC7CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6B3619-0308-4B60-9139-73463DE9FDD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29580" yWindow="-7050" windowWidth="50280" windowHeight="23450" tabRatio="149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="790">
   <si>
     <t>nom</t>
   </si>
@@ -1883,9 +1883,6 @@
     <t>Julie</t>
   </si>
   <si>
-    <t>julie-ouelette.jpg</t>
-  </si>
-  <si>
     <t>Circulation, gestion des collections et des espaces;Prêt entre bibliothèques</t>
   </si>
   <si>
@@ -2415,6 +2412,12 @@
   </si>
   <si>
     <t>alex-sandrine-lavallee-masse.jpg</t>
+  </si>
+  <si>
+    <t>josee-vachon.jpg</t>
+  </si>
+  <si>
+    <t>julie-ouellette.jpg</t>
   </si>
 </sst>
 </file>
@@ -2724,7 +2727,7 @@
   <autoFilter ref="A1:J128" xr:uid="{4A0AF7E1-A614-44BF-8C48-5C26377DC552}">
     <filterColumn colId="0">
       <filters>
-        <filter val="Lavallée-Masse"/>
+        <filter val="Ouellette"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3072,7 +3075,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
+      <selection pane="bottomLeft" activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -3939,7 +3942,7 @@
         <v>56</v>
       </c>
       <c r="G31" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="H31" s="8" t="s">
         <v>219</v>
@@ -4109,7 +4112,7 @@
         <v>259</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="H37" s="6" t="s">
         <v>260</v>
@@ -4259,7 +4262,7 @@
         <v>296</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="H42" s="8" t="s">
         <v>297</v>
@@ -4335,7 +4338,7 @@
         <v>315</v>
       </c>
       <c r="C45" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D45" t="s">
         <v>110</v>
@@ -4450,7 +4453,7 @@
         <v>333</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>148</v>
@@ -4743,7 +4746,7 @@
         <v>396</v>
       </c>
       <c r="H59" s="10" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="I59" s="16" t="s">
         <v>397</v>
@@ -4972,7 +4975,7 @@
         <v>443</v>
       </c>
       <c r="I67" s="12" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="J67" s="17" t="s">
         <v>398</v>
@@ -5044,7 +5047,7 @@
         <v>457</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>148</v>
@@ -5073,7 +5076,7 @@
         <v>373</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>46</v>
@@ -5097,7 +5100,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" hidden="1">
       <c r="A72" t="s">
         <v>467</v>
       </c>
@@ -5105,7 +5108,7 @@
         <v>468</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="D72" t="s">
         <v>110</v>
@@ -5227,7 +5230,7 @@
         <v>493</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="H76" s="6" t="s">
         <v>494</v>
@@ -5337,10 +5340,10 @@
         <v>47</v>
       </c>
       <c r="F80" t="s">
+        <v>778</v>
+      </c>
+      <c r="G80" s="10" t="s">
         <v>779</v>
-      </c>
-      <c r="G80" s="10" t="s">
-        <v>780</v>
       </c>
       <c r="H80" s="10" t="s">
         <v>512</v>
@@ -5769,7 +5772,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="96" spans="1:10" s="4" customFormat="1" hidden="1">
+    <row r="96" spans="1:10" s="4" customFormat="1">
       <c r="A96" s="8" t="s">
         <v>609</v>
       </c>
@@ -5777,7 +5780,7 @@
         <v>610</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>611</v>
+        <v>789</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>46</v>
@@ -5786,56 +5789,56 @@
         <v>340</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="G96" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H96" s="8" t="s">
+        <v>612</v>
+      </c>
+      <c r="I96" s="8" t="s">
         <v>613</v>
       </c>
-      <c r="I96" s="8" t="s">
+      <c r="J96" s="17" t="s">
         <v>614</v>
-      </c>
-      <c r="J96" s="17" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="97" spans="1:10" s="4" customFormat="1" hidden="1">
       <c r="A97" s="8" t="s">
+        <v>615</v>
+      </c>
+      <c r="B97" s="8" t="s">
         <v>616</v>
-      </c>
-      <c r="B97" s="8" t="s">
-        <v>617</v>
       </c>
       <c r="C97" s="8"/>
       <c r="D97" s="8" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E97" s="6"/>
       <c r="F97" s="28" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G97" s="8" t="s">
         <v>288</v>
       </c>
       <c r="H97" s="8"/>
       <c r="I97" s="17" t="s">
+        <v>619</v>
+      </c>
+      <c r="J97" s="18" t="s">
         <v>620</v>
-      </c>
-      <c r="J97" s="18" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="98" spans="1:10" hidden="1">
       <c r="A98" t="s">
+        <v>621</v>
+      </c>
+      <c r="B98" t="s">
         <v>622</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" s="25" t="s">
         <v>623</v>
-      </c>
-      <c r="C98" s="25" t="s">
-        <v>624</v>
       </c>
       <c r="D98" t="s">
         <v>30</v>
@@ -5844,27 +5847,27 @@
         <v>96</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G98" t="s">
         <v>117</v>
       </c>
       <c r="I98" t="s">
+        <v>625</v>
+      </c>
+      <c r="J98" t="s">
         <v>626</v>
-      </c>
-      <c r="J98" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="99" spans="1:10" hidden="1">
       <c r="A99" s="6" t="s">
+        <v>627</v>
+      </c>
+      <c r="B99" s="6" t="s">
         <v>628</v>
       </c>
-      <c r="B99" s="6" t="s">
+      <c r="C99" s="6" t="s">
         <v>629</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>630</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>127</v>
@@ -5873,90 +5876,90 @@
         <v>96</v>
       </c>
       <c r="F99" s="15" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G99" t="s">
         <v>117</v>
       </c>
       <c r="H99" s="14" t="s">
+        <v>631</v>
+      </c>
+      <c r="I99" s="14" t="s">
         <v>632</v>
       </c>
-      <c r="I99" s="14" t="s">
+      <c r="J99" s="14" t="s">
         <v>633</v>
-      </c>
-      <c r="J99" s="14" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="100" spans="1:10" hidden="1">
       <c r="A100" s="6" t="s">
+        <v>634</v>
+      </c>
+      <c r="B100" s="6" t="s">
         <v>635</v>
       </c>
-      <c r="B100" s="6" t="s">
+      <c r="C100" s="6" t="s">
         <v>636</v>
-      </c>
-      <c r="C100" s="6" t="s">
-        <v>637</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E100" s="6"/>
       <c r="F100" s="6" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G100" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H100" s="14" t="s">
+        <v>638</v>
+      </c>
+      <c r="I100" s="14" t="s">
         <v>639</v>
       </c>
-      <c r="I100" s="14" t="s">
+      <c r="J100" s="14" t="s">
         <v>640</v>
-      </c>
-      <c r="J100" s="14" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="101" spans="1:10" hidden="1">
       <c r="A101" s="8" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B101" s="8" t="s">
+        <v>641</v>
+      </c>
+      <c r="C101" s="8" t="s">
         <v>642</v>
-      </c>
-      <c r="C101" s="8" t="s">
-        <v>643</v>
       </c>
       <c r="D101" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E101" s="8"/>
       <c r="F101" s="8" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="G101" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H101" s="10" t="s">
+        <v>644</v>
+      </c>
+      <c r="I101" s="10" t="s">
         <v>645</v>
       </c>
-      <c r="I101" s="10" t="s">
+      <c r="J101" s="10" t="s">
         <v>646</v>
-      </c>
-      <c r="J101" s="10" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="102" spans="1:10" hidden="1">
       <c r="A102" s="6" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B102" s="6" t="s">
         <v>373</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>13</v>
@@ -5969,24 +5972,24 @@
         <v>111</v>
       </c>
       <c r="H102" s="14" t="s">
+        <v>649</v>
+      </c>
+      <c r="I102" s="14" t="s">
         <v>650</v>
       </c>
-      <c r="I102" s="14" t="s">
+      <c r="J102" s="14" t="s">
         <v>651</v>
-      </c>
-      <c r="J102" s="14" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="103" spans="1:10" s="5" customFormat="1" hidden="1">
       <c r="A103" s="6" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B103" s="6" t="s">
         <v>586</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>30</v>
@@ -5995,52 +5998,52 @@
         <v>96</v>
       </c>
       <c r="F103" s="15" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="H103" s="14"/>
       <c r="I103" s="13" t="s">
+        <v>655</v>
+      </c>
+      <c r="J103" s="14" t="s">
         <v>656</v>
-      </c>
-      <c r="J103" s="14" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="104" spans="1:10" s="5" customFormat="1" hidden="1">
       <c r="A104" s="8" t="s">
+        <v>657</v>
+      </c>
+      <c r="B104" s="8" t="s">
         <v>658</v>
       </c>
-      <c r="B104" s="8" t="s">
+      <c r="C104" s="8" t="s">
         <v>659</v>
-      </c>
-      <c r="C104" s="8" t="s">
-        <v>660</v>
       </c>
       <c r="D104" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E104" s="8"/>
       <c r="F104" s="11" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="G104" s="8" t="s">
         <v>396</v>
       </c>
       <c r="H104" s="10" t="s">
+        <v>661</v>
+      </c>
+      <c r="I104" s="10" t="s">
         <v>662</v>
       </c>
-      <c r="I104" s="10" t="s">
+      <c r="J104" s="10" t="s">
         <v>663</v>
-      </c>
-      <c r="J104" s="10" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="105" spans="1:10" hidden="1">
       <c r="A105" s="8" t="s">
+        <v>664</v>
+      </c>
+      <c r="B105" s="8" t="s">
         <v>665</v>
-      </c>
-      <c r="B105" s="8" t="s">
-        <v>666</v>
       </c>
       <c r="C105" s="6"/>
       <c r="D105" s="8" t="s">
@@ -6052,42 +6055,42 @@
         <v>23</v>
       </c>
       <c r="H105" s="10" t="s">
+        <v>666</v>
+      </c>
+      <c r="I105" s="17" t="s">
         <v>667</v>
-      </c>
-      <c r="I105" s="17" t="s">
-        <v>668</v>
       </c>
       <c r="J105" s="10"/>
     </row>
     <row r="106" spans="1:10" hidden="1">
       <c r="A106" t="s">
+        <v>668</v>
+      </c>
+      <c r="B106" t="s">
         <v>669</v>
-      </c>
-      <c r="B106" t="s">
-        <v>670</v>
       </c>
       <c r="D106" t="s">
         <v>520</v>
       </c>
       <c r="G106" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="H106" s="8" t="s">
+        <v>670</v>
+      </c>
+      <c r="I106" s="18" t="s">
         <v>671</v>
       </c>
-      <c r="I106" s="18" t="s">
+      <c r="J106" s="17" t="s">
         <v>672</v>
-      </c>
-      <c r="J106" s="17" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="107" spans="1:10" hidden="1">
       <c r="A107" t="s">
+        <v>673</v>
+      </c>
+      <c r="B107" t="s">
         <v>674</v>
-      </c>
-      <c r="B107" t="s">
-        <v>675</v>
       </c>
       <c r="D107" t="s">
         <v>110</v>
@@ -6096,53 +6099,53 @@
         <v>32</v>
       </c>
       <c r="H107" t="s">
+        <v>675</v>
+      </c>
+      <c r="I107" s="18" t="s">
         <v>676</v>
       </c>
-      <c r="I107" s="18" t="s">
+      <c r="J107" s="19" t="s">
         <v>677</v>
-      </c>
-      <c r="J107" s="19" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="108" spans="1:10" hidden="1">
       <c r="A108" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B108" t="s">
         <v>62</v>
       </c>
       <c r="C108" s="25" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D108" t="s">
         <v>13</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="G108" t="s">
         <v>32</v>
       </c>
       <c r="H108" s="4" t="s">
+        <v>681</v>
+      </c>
+      <c r="I108" s="4" t="s">
         <v>682</v>
       </c>
-      <c r="I108" s="4" t="s">
+      <c r="J108" s="4" t="s">
         <v>683</v>
-      </c>
-      <c r="J108" s="4" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="109" spans="1:10" hidden="1">
       <c r="A109" s="6" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B109" s="6" t="s">
         <v>528</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>147</v>
@@ -6155,18 +6158,18 @@
         <v>141</v>
       </c>
       <c r="I109" s="14" t="s">
+        <v>686</v>
+      </c>
+      <c r="J109" s="14" t="s">
         <v>687</v>
-      </c>
-      <c r="J109" s="14" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="110" spans="1:10" hidden="1">
       <c r="A110" s="6" t="s">
+        <v>688</v>
+      </c>
+      <c r="B110" s="6" t="s">
         <v>689</v>
-      </c>
-      <c r="B110" s="6" t="s">
-        <v>690</v>
       </c>
       <c r="C110" s="6"/>
       <c r="D110" s="6" t="s">
@@ -6174,25 +6177,25 @@
       </c>
       <c r="E110" s="6"/>
       <c r="F110" s="15" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="G110" s="6" t="s">
         <v>197</v>
       </c>
       <c r="H110" s="14"/>
       <c r="I110" s="14" t="s">
+        <v>691</v>
+      </c>
+      <c r="J110" s="14" t="s">
         <v>692</v>
-      </c>
-      <c r="J110" s="14" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="111" spans="1:10" hidden="1">
       <c r="A111" t="s">
+        <v>693</v>
+      </c>
+      <c r="B111" t="s">
         <v>694</v>
-      </c>
-      <c r="B111" t="s">
-        <v>695</v>
       </c>
       <c r="C111" s="33"/>
       <c r="D111" s="6" t="s">
@@ -6203,37 +6206,37 @@
     </row>
     <row r="112" spans="1:10" hidden="1">
       <c r="A112" s="10" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B112" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C112" s="30" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D112" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E112" s="10"/>
       <c r="F112" s="10" t="s">
+        <v>697</v>
+      </c>
+      <c r="G112" s="10" t="s">
         <v>698</v>
       </c>
-      <c r="G112" s="10" t="s">
+      <c r="H112" s="10" t="s">
         <v>699</v>
       </c>
-      <c r="H112" s="10" t="s">
+      <c r="I112" s="10" t="s">
         <v>700</v>
       </c>
-      <c r="I112" s="10" t="s">
+      <c r="J112" s="10" t="s">
         <v>701</v>
-      </c>
-      <c r="J112" s="10" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="113" spans="1:10" hidden="1">
       <c r="A113" s="10" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B113" s="10" t="s">
         <v>308</v>
@@ -6248,24 +6251,24 @@
       <c r="F113" s="10"/>
       <c r="G113" s="10"/>
       <c r="H113" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="I113" s="10" t="s">
         <v>704</v>
       </c>
-      <c r="I113" s="10" t="s">
+      <c r="J113" s="10" t="s">
         <v>705</v>
-      </c>
-      <c r="J113" s="10" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="114" spans="1:10" hidden="1">
       <c r="A114" s="6" t="s">
+        <v>706</v>
+      </c>
+      <c r="B114" s="6" t="s">
         <v>707</v>
       </c>
-      <c r="B114" s="6" t="s">
+      <c r="C114" s="6" t="s">
         <v>708</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>709</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>95</v>
@@ -6277,21 +6280,21 @@
         <v>402</v>
       </c>
       <c r="H114" s="6" t="s">
+        <v>709</v>
+      </c>
+      <c r="I114" s="6" t="s">
         <v>710</v>
       </c>
-      <c r="I114" s="6" t="s">
+      <c r="J114" s="6" t="s">
         <v>711</v>
-      </c>
-      <c r="J114" s="6" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="115" spans="1:10" hidden="1">
       <c r="A115" s="6" t="s">
+        <v>712</v>
+      </c>
+      <c r="B115" s="6" t="s">
         <v>713</v>
-      </c>
-      <c r="B115" s="6" t="s">
-        <v>714</v>
       </c>
       <c r="C115" s="6"/>
       <c r="D115" s="6" t="s">
@@ -6304,51 +6307,51 @@
       </c>
       <c r="H115" s="6"/>
       <c r="I115" s="16" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="J115" s="6"/>
     </row>
     <row r="116" spans="1:10" hidden="1">
       <c r="A116" s="14" t="s">
+        <v>715</v>
+      </c>
+      <c r="B116" s="14" t="s">
         <v>716</v>
       </c>
-      <c r="B116" s="14" t="s">
+      <c r="C116" s="26" t="s">
         <v>717</v>
-      </c>
-      <c r="C116" s="26" t="s">
-        <v>718</v>
       </c>
       <c r="D116" s="14" t="s">
         <v>346</v>
       </c>
       <c r="E116" t="s">
+        <v>718</v>
+      </c>
+      <c r="F116" s="14" t="s">
         <v>719</v>
-      </c>
-      <c r="F116" s="14" t="s">
-        <v>720</v>
       </c>
       <c r="G116" s="14" t="s">
         <v>49</v>
       </c>
       <c r="H116" s="14" t="s">
+        <v>720</v>
+      </c>
+      <c r="I116" s="14" t="s">
         <v>721</v>
       </c>
-      <c r="I116" s="14" t="s">
+      <c r="J116" s="14" t="s">
         <v>722</v>
-      </c>
-      <c r="J116" s="14" t="s">
-        <v>723</v>
       </c>
     </row>
     <row r="117" spans="1:10" hidden="1">
       <c r="A117" s="8" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B117" s="8" t="s">
         <v>586</v>
       </c>
       <c r="C117" s="27" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D117" s="8" t="s">
         <v>30</v>
@@ -6361,21 +6364,21 @@
         <v>157</v>
       </c>
       <c r="H117" s="8" t="s">
+        <v>725</v>
+      </c>
+      <c r="I117" s="8" t="s">
         <v>726</v>
       </c>
-      <c r="I117" s="8" t="s">
+      <c r="J117" s="8" t="s">
         <v>727</v>
-      </c>
-      <c r="J117" s="8" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="118" spans="1:10" hidden="1">
       <c r="A118" s="8" t="s">
+        <v>728</v>
+      </c>
+      <c r="B118" s="8" t="s">
         <v>729</v>
-      </c>
-      <c r="B118" s="8" t="s">
-        <v>730</v>
       </c>
       <c r="C118" s="8"/>
       <c r="D118" s="8" t="s">
@@ -6387,19 +6390,19 @@
         <v>544</v>
       </c>
       <c r="H118" t="s">
+        <v>730</v>
+      </c>
+      <c r="I118" s="17" t="s">
         <v>731</v>
-      </c>
-      <c r="I118" s="17" t="s">
-        <v>732</v>
       </c>
       <c r="J118" s="8"/>
     </row>
     <row r="119" spans="1:10" hidden="1">
       <c r="A119" s="6" t="s">
+        <v>732</v>
+      </c>
+      <c r="B119" s="6" t="s">
         <v>733</v>
-      </c>
-      <c r="B119" s="6" t="s">
-        <v>734</v>
       </c>
       <c r="C119" s="6"/>
       <c r="D119" s="6" t="s">
@@ -6407,27 +6410,27 @@
       </c>
       <c r="E119" s="6"/>
       <c r="F119" s="15" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="G119" s="6" t="s">
         <v>288</v>
       </c>
       <c r="H119" s="6" t="s">
+        <v>735</v>
+      </c>
+      <c r="I119" s="6" t="s">
         <v>736</v>
       </c>
-      <c r="I119" s="6" t="s">
+      <c r="J119" s="6" t="s">
         <v>737</v>
-      </c>
-      <c r="J119" s="6" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="120" spans="1:10" hidden="1">
       <c r="A120" s="6" t="s">
+        <v>738</v>
+      </c>
+      <c r="B120" s="6" t="s">
         <v>739</v>
-      </c>
-      <c r="B120" s="6" t="s">
-        <v>740</v>
       </c>
       <c r="C120" s="6"/>
       <c r="D120" s="6" t="s">
@@ -6442,70 +6445,70 @@
         <v>526</v>
       </c>
       <c r="I120" s="16" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="J120" s="6"/>
     </row>
     <row r="121" spans="1:10" hidden="1">
       <c r="A121" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B121" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D121" t="s">
         <v>56</v>
       </c>
       <c r="F121" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="G121" t="s">
         <v>368</v>
       </c>
       <c r="H121" s="8" t="s">
+        <v>743</v>
+      </c>
+      <c r="I121" s="18" t="s">
         <v>744</v>
       </c>
-      <c r="I121" s="18" t="s">
+      <c r="J121" s="17" t="s">
         <v>745</v>
-      </c>
-      <c r="J121" s="17" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="122" spans="1:10" hidden="1">
       <c r="A122" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B122" t="s">
         <v>610</v>
       </c>
       <c r="C122" s="6"/>
       <c r="D122" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E122" s="6" t="s">
         <v>47</v>
       </c>
       <c r="F122" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="G122" t="s">
         <v>49</v>
       </c>
       <c r="H122" t="s">
+        <v>783</v>
+      </c>
+      <c r="I122" s="32" t="s">
         <v>784</v>
-      </c>
-      <c r="I122" s="32" t="s">
-        <v>785</v>
       </c>
       <c r="J122" s="31"/>
     </row>
     <row r="123" spans="1:10" hidden="1">
       <c r="A123" s="6" t="s">
+        <v>746</v>
+      </c>
+      <c r="B123" s="6" t="s">
         <v>747</v>
-      </c>
-      <c r="B123" s="6" t="s">
-        <v>748</v>
       </c>
       <c r="C123" s="6"/>
       <c r="D123" s="6" t="s">
@@ -6517,45 +6520,47 @@
         <v>65</v>
       </c>
       <c r="H123" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="I123" s="16" t="s">
         <v>749</v>
-      </c>
-      <c r="I123" s="16" t="s">
-        <v>750</v>
       </c>
       <c r="J123" s="6"/>
     </row>
     <row r="124" spans="1:10" hidden="1">
       <c r="A124" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="B124" s="6" t="s">
         <v>751</v>
       </c>
-      <c r="B124" s="6" t="s">
-        <v>752</v>
-      </c>
-      <c r="C124" s="29"/>
+      <c r="C124" s="29" t="s">
+        <v>788</v>
+      </c>
       <c r="D124" s="6" t="s">
         <v>110</v>
       </c>
       <c r="E124" s="6"/>
       <c r="F124" s="6" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="G124" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H124" s="6" t="s">
+        <v>753</v>
+      </c>
+      <c r="I124" s="16" t="s">
         <v>754</v>
-      </c>
-      <c r="I124" s="16" t="s">
-        <v>755</v>
       </c>
       <c r="J124" s="6"/>
     </row>
     <row r="125" spans="1:10" hidden="1">
       <c r="A125" s="6" t="s">
+        <v>755</v>
+      </c>
+      <c r="B125" s="6" t="s">
         <v>756</v>
-      </c>
-      <c r="B125" s="6" t="s">
-        <v>757</v>
       </c>
       <c r="C125" s="26"/>
       <c r="D125" s="6" t="s">
@@ -6567,49 +6572,49 @@
         <v>65</v>
       </c>
       <c r="H125" s="6" t="s">
+        <v>757</v>
+      </c>
+      <c r="I125" s="16" t="s">
         <v>758</v>
-      </c>
-      <c r="I125" s="16" t="s">
-        <v>759</v>
       </c>
       <c r="J125" s="6"/>
     </row>
     <row r="126" spans="1:10" hidden="1">
       <c r="A126" s="6" t="s">
+        <v>759</v>
+      </c>
+      <c r="B126" s="6" t="s">
         <v>760</v>
       </c>
-      <c r="B126" s="6" t="s">
+      <c r="C126" s="29" t="s">
         <v>761</v>
-      </c>
-      <c r="C126" s="29" t="s">
-        <v>762</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E126" s="6" t="s">
+        <v>762</v>
+      </c>
+      <c r="F126" s="15" t="s">
         <v>763</v>
-      </c>
-      <c r="F126" s="15" t="s">
-        <v>764</v>
       </c>
       <c r="G126" t="s">
         <v>117</v>
       </c>
       <c r="H126" s="6"/>
       <c r="I126" s="6" t="s">
+        <v>764</v>
+      </c>
+      <c r="J126" s="6" t="s">
         <v>765</v>
-      </c>
-      <c r="J126" s="6" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="127" spans="1:10" hidden="1">
       <c r="A127" s="6" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="C127" s="6"/>
       <c r="D127" s="6" t="s">
@@ -6621,16 +6626,16 @@
         <v>111</v>
       </c>
       <c r="H127" s="6" t="s">
+        <v>767</v>
+      </c>
+      <c r="I127" s="16" t="s">
         <v>768</v>
-      </c>
-      <c r="I127" s="16" t="s">
-        <v>769</v>
       </c>
       <c r="J127" s="6"/>
     </row>
     <row r="128" spans="1:10" hidden="1">
       <c r="A128" s="8" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B128" s="8" t="s">
         <v>278</v>
@@ -6643,7 +6648,7 @@
         <v>87</v>
       </c>
       <c r="F128" s="8" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="G128" t="s">
         <v>551</v>
@@ -6652,10 +6657,10 @@
         <v>575</v>
       </c>
       <c r="I128" s="8" t="s">
+        <v>771</v>
+      </c>
+      <c r="J128" s="12" t="s">
         <v>772</v>
-      </c>
-      <c r="J128" s="12" t="s">
-        <v>773</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(repertoire-personnel): Ajustement des fiches d'Amélie Élizabeth Lévesque et Julie Trépanier
</commit_message>
<xml_diff>
--- a/content/personnel/liste-personnel.xlsx
+++ b/content/personnel/liste-personnel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projets\coquille-web\content\personnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6B3619-0308-4B60-9139-73463DE9FDD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E75754B-D3ED-405B-A03B-F22A4737E566}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29580" yWindow="-7050" windowWidth="50280" windowHeight="23450" tabRatio="149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2387,15 +2387,9 @@
     <t>Référence et offre pédagogique de première ligne - Bibliothèque de droit, Bibliothèque de musique</t>
   </si>
   <si>
-    <t>Bibliothèque d'aménagement;Bibliothèque Thérèse-Gouin-Décarie;Bibliothèque du Campus de Laval</t>
-  </si>
-  <si>
     <t>Trépanier</t>
   </si>
   <si>
-    <t>Cherre de service</t>
-  </si>
-  <si>
     <t>Référence et offre pédagogique de première ligne - Bibliothèques d'aménagement, Thérèse-Gouin-Décarie et Campus de l'UdeM à Laval</t>
   </si>
   <si>
@@ -2418,6 +2412,12 @@
   </si>
   <si>
     <t>julie-ouellette.jpg</t>
+  </si>
+  <si>
+    <t>Bibliothèque d'aménagement;;Bibliothèque Thérèse-Gouin-Décarie;Bibliothèque du Campus de Laval</t>
+  </si>
+  <si>
+    <t>Bibliothèque de droit;Bibliothèque de musique</t>
   </si>
 </sst>
 </file>
@@ -2727,12 +2727,12 @@
   <autoFilter ref="A1:J128" xr:uid="{4A0AF7E1-A614-44BF-8C48-5C26377DC552}">
     <filterColumn colId="0">
       <filters>
-        <filter val="Ouellette"/>
+        <filter val="Lévesque"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState ref="A2:J128">
-    <sortCondition ref="A1:A128"/>
+  <sortState ref="A122:J122">
+    <sortCondition descending="1" ref="A1:A128"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{4B04E1AF-0079-4AD2-81CA-E8A433733E21}" name="nom"/>
@@ -3073,9 +3073,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C129" sqref="C129"/>
+      <selection pane="bottomLeft" activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -4338,7 +4338,7 @@
         <v>315</v>
       </c>
       <c r="C45" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="D45" t="s">
         <v>110</v>
@@ -5076,7 +5076,7 @@
         <v>373</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>46</v>
@@ -5108,7 +5108,7 @@
         <v>468</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="D72" t="s">
         <v>110</v>
@@ -5301,7 +5301,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="79" spans="1:10" s="4" customFormat="1" hidden="1">
+    <row r="79" spans="1:10" s="4" customFormat="1">
       <c r="A79" s="6" t="s">
         <v>510</v>
       </c>
@@ -5325,7 +5325,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="80" spans="1:10" hidden="1">
+    <row r="80" spans="1:10">
       <c r="A80" s="10" t="s">
         <v>510</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>778</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>779</v>
+        <v>789</v>
       </c>
       <c r="H80" s="10" t="s">
         <v>512</v>
@@ -5772,7 +5772,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="96" spans="1:10" s="4" customFormat="1">
+    <row r="96" spans="1:10" s="4" customFormat="1" hidden="1">
       <c r="A96" s="8" t="s">
         <v>609</v>
       </c>
@@ -5780,7 +5780,7 @@
         <v>610</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>46</v>
@@ -6477,29 +6477,29 @@
     </row>
     <row r="122" spans="1:10" hidden="1">
       <c r="A122" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B122" t="s">
         <v>610</v>
       </c>
       <c r="C122" s="6"/>
       <c r="D122" t="s">
-        <v>781</v>
+        <v>170</v>
       </c>
       <c r="E122" s="6" t="s">
         <v>47</v>
       </c>
       <c r="F122" t="s">
+        <v>780</v>
+      </c>
+      <c r="G122" t="s">
+        <v>788</v>
+      </c>
+      <c r="H122" t="s">
+        <v>781</v>
+      </c>
+      <c r="I122" s="32" t="s">
         <v>782</v>
-      </c>
-      <c r="G122" t="s">
-        <v>49</v>
-      </c>
-      <c r="H122" t="s">
-        <v>783</v>
-      </c>
-      <c r="I122" s="32" t="s">
-        <v>784</v>
       </c>
       <c r="J122" s="31"/>
     </row>
@@ -6535,7 +6535,7 @@
         <v>751</v>
       </c>
       <c r="C124" s="29" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>110</v>
@@ -6741,12 +6741,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9cb1c2f4-2737-4134-a1af-8acbe3d02830" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6945,20 +6947,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9cb1c2f4-2737-4134-a1af-8acbe3d02830" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9cb1c2f4-2737-4134-a1af-8acbe3d02830"/>
+    <ds:schemaRef ds:uri="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6983,18 +6992,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9cb1c2f4-2737-4134-a1af-8acbe3d02830"/>
-    <ds:schemaRef ds:uri="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "feat(repertoire-personnel): Ajustement des fiches d'Amélie Élizabeth Lévesque et Julie Trépanier"
This reverts commit 328d311742392d67f4da1b72b7db3f6ceadc5c63.
</commit_message>
<xml_diff>
--- a/content/personnel/liste-personnel.xlsx
+++ b/content/personnel/liste-personnel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projets\coquille-web\content\personnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E75754B-D3ED-405B-A03B-F22A4737E566}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6B3619-0308-4B60-9139-73463DE9FDD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29580" yWindow="-7050" windowWidth="50280" windowHeight="23450" tabRatio="149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2387,9 +2387,15 @@
     <t>Référence et offre pédagogique de première ligne - Bibliothèque de droit, Bibliothèque de musique</t>
   </si>
   <si>
+    <t>Bibliothèque d'aménagement;Bibliothèque Thérèse-Gouin-Décarie;Bibliothèque du Campus de Laval</t>
+  </si>
+  <si>
     <t>Trépanier</t>
   </si>
   <si>
+    <t>Cherre de service</t>
+  </si>
+  <si>
     <t>Référence et offre pédagogique de première ligne - Bibliothèques d'aménagement, Thérèse-Gouin-Décarie et Campus de l'UdeM à Laval</t>
   </si>
   <si>
@@ -2412,12 +2418,6 @@
   </si>
   <si>
     <t>julie-ouellette.jpg</t>
-  </si>
-  <si>
-    <t>Bibliothèque d'aménagement;;Bibliothèque Thérèse-Gouin-Décarie;Bibliothèque du Campus de Laval</t>
-  </si>
-  <si>
-    <t>Bibliothèque de droit;Bibliothèque de musique</t>
   </si>
 </sst>
 </file>
@@ -2727,12 +2727,12 @@
   <autoFilter ref="A1:J128" xr:uid="{4A0AF7E1-A614-44BF-8C48-5C26377DC552}">
     <filterColumn colId="0">
       <filters>
-        <filter val="Lévesque"/>
+        <filter val="Ouellette"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState ref="A122:J122">
-    <sortCondition descending="1" ref="A1:A128"/>
+  <sortState ref="A2:J128">
+    <sortCondition ref="A1:A128"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{4B04E1AF-0079-4AD2-81CA-E8A433733E21}" name="nom"/>
@@ -3073,9 +3073,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F80" sqref="F80"/>
+      <selection pane="bottomLeft" activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -4338,7 +4338,7 @@
         <v>315</v>
       </c>
       <c r="C45" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D45" t="s">
         <v>110</v>
@@ -5076,7 +5076,7 @@
         <v>373</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>46</v>
@@ -5108,7 +5108,7 @@
         <v>468</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="D72" t="s">
         <v>110</v>
@@ -5301,7 +5301,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="79" spans="1:10" s="4" customFormat="1">
+    <row r="79" spans="1:10" s="4" customFormat="1" hidden="1">
       <c r="A79" s="6" t="s">
         <v>510</v>
       </c>
@@ -5325,7 +5325,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" hidden="1">
       <c r="A80" s="10" t="s">
         <v>510</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>778</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>789</v>
+        <v>779</v>
       </c>
       <c r="H80" s="10" t="s">
         <v>512</v>
@@ -5772,7 +5772,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="96" spans="1:10" s="4" customFormat="1" hidden="1">
+    <row r="96" spans="1:10" s="4" customFormat="1">
       <c r="A96" s="8" t="s">
         <v>609</v>
       </c>
@@ -5780,7 +5780,7 @@
         <v>610</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>46</v>
@@ -6477,29 +6477,29 @@
     </row>
     <row r="122" spans="1:10" hidden="1">
       <c r="A122" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="B122" t="s">
         <v>610</v>
       </c>
       <c r="C122" s="6"/>
       <c r="D122" t="s">
-        <v>170</v>
+        <v>781</v>
       </c>
       <c r="E122" s="6" t="s">
         <v>47</v>
       </c>
       <c r="F122" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="G122" t="s">
-        <v>788</v>
+        <v>49</v>
       </c>
       <c r="H122" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="I122" s="32" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="J122" s="31"/>
     </row>
@@ -6535,7 +6535,7 @@
         <v>751</v>
       </c>
       <c r="C124" s="29" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>110</v>
@@ -6741,14 +6741,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9cb1c2f4-2737-4134-a1af-8acbe3d02830" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6947,27 +6945,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9cb1c2f4-2737-4134-a1af-8acbe3d02830" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9cb1c2f4-2737-4134-a1af-8acbe3d02830"/>
-    <ds:schemaRef ds:uri="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6992,9 +6983,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9cb1c2f4-2737-4134-a1af-8acbe3d02830"/>
+    <ds:schemaRef ds:uri="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(repertoire-personnel): Ajout du Centre de conservation Lionel-Groulx à Myriam Boyer
</commit_message>
<xml_diff>
--- a/content/personnel/liste-personnel.xlsx
+++ b/content/personnel/liste-personnel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projets\coquille-web\content\personnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F452EBF-040B-4B50-AF75-CD68D00A2892}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9357DE76-E356-409F-8638-34C040D2ADEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1890" yWindow="3180" windowWidth="33570" windowHeight="23450" tabRatio="149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -538,9 +538,6 @@
   </si>
   <si>
     <t>Cheffe de service</t>
-  </si>
-  <si>
-    <t>Gestion des collections et numérisation</t>
   </si>
   <si>
     <t>514 343-6111, poste 13788</t>
@@ -2415,6 +2412,9 @@
   </si>
   <si>
     <t>Bibliothèque de droit;Bibliothèque de musique</t>
+  </si>
+  <si>
+    <t>Gestion des collections et numérisation;Centre de conservation Lionel-Groulx</t>
   </si>
 </sst>
 </file>
@@ -3061,8 +3061,8 @@
   <dimension ref="A1:J128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E122" sqref="E122"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -3366,10 +3366,10 @@
         <v>81</v>
       </c>
       <c r="F10" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>82</v>
@@ -3731,24 +3731,24 @@
         <v>87</v>
       </c>
       <c r="G23" s="8" t="s">
+        <v>788</v>
+      </c>
+      <c r="H23" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="H23" s="8" t="s">
+      <c r="I23" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="J23" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>176</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8" t="s">
@@ -3756,30 +3756,30 @@
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="H24" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="H24" s="8" t="s">
+      <c r="I24" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="J24" s="8" t="s">
         <v>180</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="C25" s="8" t="s">
         <v>183</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>184</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>80</v>
@@ -3789,21 +3789,21 @@
       </c>
       <c r="F25" s="11"/>
       <c r="H25" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="I25" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="J25" s="8" t="s">
         <v>186</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
+        <v>187</v>
+      </c>
+      <c r="B26" t="s">
         <v>188</v>
-      </c>
-      <c r="B26" t="s">
-        <v>189</v>
       </c>
       <c r="D26" t="s">
         <v>110</v>
@@ -3812,49 +3812,49 @@
         <v>32</v>
       </c>
       <c r="H26" t="s">
+        <v>189</v>
+      </c>
+      <c r="I26" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="I26" s="18" t="s">
+      <c r="J26" s="18" t="s">
         <v>191</v>
-      </c>
-      <c r="J26" s="18" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>194</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="H27" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="I27" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="I27" s="13" t="s">
+      <c r="J27" s="13" t="s">
         <v>199</v>
-      </c>
-      <c r="J27" s="13" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>201</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>202</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6" t="s">
@@ -3862,57 +3862,57 @@
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="H28" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="I28" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="I28" s="6" t="s">
+      <c r="J28" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="C29" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>210</v>
-      </c>
       <c r="D29" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F29" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="G29" t="s">
         <v>211</v>
-      </c>
-      <c r="G29" t="s">
-        <v>212</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="J29" s="13" t="s">
         <v>213</v>
-      </c>
-      <c r="J29" s="13" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
+        <v>214</v>
+      </c>
+      <c r="B30" t="s">
         <v>215</v>
-      </c>
-      <c r="B30" t="s">
-        <v>216</v>
       </c>
       <c r="D30" t="s">
         <v>30</v>
@@ -3926,37 +3926,37 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
+        <v>216</v>
+      </c>
+      <c r="B31" t="s">
         <v>217</v>
-      </c>
-      <c r="B31" t="s">
-        <v>218</v>
       </c>
       <c r="D31" t="s">
         <v>56</v>
       </c>
       <c r="G31" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="H31" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="I31" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="I31" s="18" t="s">
+      <c r="J31" s="17" t="s">
         <v>220</v>
-      </c>
-      <c r="J31" s="17" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>223</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E32" s="15" t="s">
         <v>72</v>
@@ -3968,370 +3968,370 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="C33" s="8" t="s">
         <v>226</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>227</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="H33" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="G33" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="H33" s="8" t="s">
+      <c r="I33" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="J33" s="8" t="s">
         <v>230</v>
-      </c>
-      <c r="J33" s="8" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="C34" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="D34" s="6" t="s">
         <v>234</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>235</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>96</v>
       </c>
       <c r="F34" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H34" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="I34" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="I34" s="6" t="s">
+      <c r="J34" s="6" t="s">
         <v>238</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>241</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>242</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H35" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="I35" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="I35" s="6" t="s">
+      <c r="J35" s="6" t="s">
         <v>245</v>
-      </c>
-      <c r="J35" s="6" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="C36" s="8" t="s">
         <v>248</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>249</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>30</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H36" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="I36" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="I36" s="8" t="s">
+      <c r="J36" s="12" t="s">
         <v>252</v>
-      </c>
-      <c r="J36" s="12" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="C37" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="D37" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="E37" t="s">
         <v>257</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>258</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" s="8" t="s">
+        <v>772</v>
+      </c>
+      <c r="H37" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="G37" s="8" t="s">
-        <v>773</v>
-      </c>
-      <c r="H37" s="6" t="s">
+      <c r="I37" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="I37" s="6" t="s">
+      <c r="J37" s="13" t="s">
         <v>261</v>
-      </c>
-      <c r="J37" s="13" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="C38" s="8" t="s">
         <v>264</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>265</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="H38" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="G38" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="H38" s="8" t="s">
+      <c r="I38" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="I38" s="8" t="s">
+      <c r="J38" s="8" t="s">
         <v>268</v>
-      </c>
-      <c r="J38" s="8" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="C39" s="6" t="s">
         <v>271</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>272</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E39" s="6"/>
       <c r="F39" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>65</v>
       </c>
       <c r="H39" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="I39" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="I39" s="6" t="s">
+      <c r="J39" s="6" t="s">
         <v>275</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>278</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>279</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H40" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="I40" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="I40" s="6" t="s">
+      <c r="J40" s="6" t="s">
         <v>282</v>
-      </c>
-      <c r="J40" s="6" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="B41" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="C41" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="D41" s="8" t="s">
         <v>286</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>287</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="28" t="s">
+        <v>288</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="H41" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="G41" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="H41" s="8" t="s">
+      <c r="I41" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="I41" s="8" t="s">
+      <c r="J41" s="8" t="s">
         <v>291</v>
-      </c>
-      <c r="J41" s="8" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="C42" s="8" t="s">
         <v>294</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>295</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>774</v>
+      </c>
+      <c r="H42" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="G42" s="8" t="s">
-        <v>775</v>
-      </c>
-      <c r="H42" s="8" t="s">
+      <c r="I42" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="I42" s="8" t="s">
+      <c r="J42" s="8" t="s">
         <v>298</v>
-      </c>
-      <c r="J42" s="8" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="C43" s="8" t="s">
         <v>301</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>302</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G43" s="8" t="s">
         <v>65</v>
       </c>
       <c r="H43" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="I43" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="I43" s="8" t="s">
+      <c r="J43" s="8" t="s">
         <v>305</v>
-      </c>
-      <c r="J43" s="8" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>307</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>308</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="H44" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="H44" s="6" t="s">
+      <c r="I44" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="I44" s="6" t="s">
+      <c r="J44" s="6" t="s">
         <v>312</v>
-      </c>
-      <c r="J44" s="6" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
+        <v>313</v>
+      </c>
+      <c r="B45" t="s">
         <v>314</v>
       </c>
-      <c r="B45" t="s">
-        <v>315</v>
-      </c>
       <c r="C45" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D45" t="s">
         <v>110</v>
@@ -4340,51 +4340,51 @@
         <v>32</v>
       </c>
       <c r="H45" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="I45" s="18" t="s">
         <v>316</v>
       </c>
-      <c r="I45" s="18" t="s">
+      <c r="J45" s="18" t="s">
         <v>317</v>
-      </c>
-      <c r="J45" s="18" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="C46" s="6" t="s">
         <v>320</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>321</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E46" s="6"/>
       <c r="F46" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>65</v>
       </c>
       <c r="H46" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="I46" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="I46" s="6" t="s">
+      <c r="J46" s="6" t="s">
         <v>324</v>
-      </c>
-      <c r="J46" s="6" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
+        <v>325</v>
+      </c>
+      <c r="B47" t="s">
         <v>326</v>
-      </c>
-      <c r="B47" t="s">
-        <v>327</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" t="s">
@@ -4394,24 +4394,24 @@
         <v>32</v>
       </c>
       <c r="H47" t="s">
+        <v>327</v>
+      </c>
+      <c r="I47" s="18" t="s">
         <v>328</v>
       </c>
-      <c r="I47" s="18" t="s">
+      <c r="J47" s="18" t="s">
         <v>329</v>
-      </c>
-      <c r="J47" s="18" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="C48" s="6" t="s">
         <v>332</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>333</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>170</v>
@@ -4426,60 +4426,60 @@
         <v>149</v>
       </c>
       <c r="H48" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="I48" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="I48" s="8" t="s">
+      <c r="J48" s="8" t="s">
         <v>335</v>
-      </c>
-      <c r="J48" s="8" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="C49" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="C49" s="6" t="s">
-        <v>333</v>
-      </c>
       <c r="D49" s="8" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>148</v>
       </c>
       <c r="F49" s="8"/>
       <c r="G49" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H49" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="I49" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="I49" s="8" t="s">
+      <c r="J49" s="8" t="s">
         <v>335</v>
-      </c>
-      <c r="J49" s="8" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>337</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="C50" s="8" t="s">
         <v>338</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>339</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>46</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>48</v>
@@ -4488,21 +4488,21 @@
         <v>32</v>
       </c>
       <c r="H50" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="I50" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="I50" s="8" t="s">
+      <c r="J50" s="8" t="s">
         <v>342</v>
-      </c>
-      <c r="J50" s="8" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>344</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>345</v>
       </c>
       <c r="C51" s="8"/>
       <c r="D51" s="8" t="s">
@@ -4510,113 +4510,113 @@
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="G51" s="8" t="s">
         <v>346</v>
       </c>
-      <c r="G51" s="8" t="s">
+      <c r="H51" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="H51" s="8" t="s">
+      <c r="I51" s="8" t="s">
         <v>348</v>
       </c>
-      <c r="I51" s="8" t="s">
+      <c r="J51" s="8" t="s">
         <v>349</v>
-      </c>
-      <c r="J51" s="8" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="B52" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="C52" s="8" t="s">
         <v>352</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>353</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E52" s="8"/>
       <c r="F52" s="11" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G52" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H52" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="I52" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="I52" s="8" t="s">
+      <c r="J52" s="8" t="s">
         <v>356</v>
-      </c>
-      <c r="J52" s="8" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>358</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>359</v>
       </c>
       <c r="C53" s="6"/>
       <c r="D53" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E53" s="6"/>
       <c r="F53" s="15" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H53" s="6"/>
       <c r="I53" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="J53" s="18" t="s">
         <v>362</v>
-      </c>
-      <c r="J53" s="18" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="B54" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="C54" s="8" t="s">
         <v>365</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>366</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E54" s="8"/>
       <c r="F54" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="G54" s="8" t="s">
         <v>367</v>
       </c>
-      <c r="G54" s="8" t="s">
+      <c r="H54" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="H54" s="8" t="s">
+      <c r="I54" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="I54" s="8" t="s">
+      <c r="J54" s="8" t="s">
         <v>370</v>
-      </c>
-      <c r="J54" s="8" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55" s="6" t="s">
@@ -4630,48 +4630,48 @@
         <v>150</v>
       </c>
       <c r="I55" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="J55" s="6" t="s">
         <v>379</v>
-      </c>
-      <c r="J55" s="6" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="C56" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="D56" s="6" t="s">
         <v>374</v>
       </c>
-      <c r="D56" s="6" t="s">
-        <v>375</v>
-      </c>
       <c r="E56" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F56" s="6"/>
       <c r="H56" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I56" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="J56" s="16" t="s">
         <v>376</v>
-      </c>
-      <c r="J56" s="16" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="C57" s="8" t="s">
         <v>382</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>383</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>30</v>
@@ -4680,24 +4680,24 @@
         <v>96</v>
       </c>
       <c r="F57" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="H57" s="8" t="s">
         <v>384</v>
       </c>
-      <c r="H57" s="8" t="s">
+      <c r="I57" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="I57" s="8" t="s">
+      <c r="J57" s="8" t="s">
         <v>386</v>
-      </c>
-      <c r="J57" s="8" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>388</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>389</v>
       </c>
       <c r="C58" s="6"/>
       <c r="D58" s="6" t="s">
@@ -4705,27 +4705,27 @@
       </c>
       <c r="E58" s="6"/>
       <c r="F58" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G58" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H58" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="I58" s="6" t="s">
         <v>391</v>
       </c>
-      <c r="I58" s="6" t="s">
+      <c r="J58" s="16" t="s">
         <v>392</v>
-      </c>
-      <c r="J58" s="16" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C59" s="6"/>
       <c r="D59" s="6" t="s">
@@ -4733,27 +4733,27 @@
       </c>
       <c r="E59" s="6"/>
       <c r="F59" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="G59" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="G59" s="6" t="s">
+      <c r="H59" s="10" t="s">
+        <v>658</v>
+      </c>
+      <c r="I59" s="16" t="s">
         <v>396</v>
       </c>
-      <c r="H59" s="10" t="s">
-        <v>659</v>
-      </c>
-      <c r="I59" s="16" t="s">
+      <c r="J59" s="22" t="s">
         <v>397</v>
-      </c>
-      <c r="J59" s="22" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>399</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>400</v>
       </c>
       <c r="C60" s="6"/>
       <c r="D60" s="6" t="s">
@@ -4763,115 +4763,115 @@
         <v>96</v>
       </c>
       <c r="F60" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="G60" s="6" t="s">
         <v>401</v>
       </c>
-      <c r="G60" s="6" t="s">
+      <c r="H60" s="6" t="s">
         <v>402</v>
-      </c>
-      <c r="H60" s="6" t="s">
-        <v>403</v>
       </c>
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C61" s="6" t="s">
         <v>404</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>405</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E61" s="6"/>
       <c r="F61" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="H61" s="6" t="s">
         <v>406</v>
       </c>
-      <c r="G61" s="6" t="s">
-        <v>368</v>
-      </c>
-      <c r="H61" s="6" t="s">
+      <c r="I61" s="6" t="s">
         <v>407</v>
       </c>
-      <c r="I61" s="6" t="s">
+      <c r="J61" s="6" t="s">
         <v>408</v>
-      </c>
-      <c r="J61" s="6" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="B62" s="8" t="s">
         <v>410</v>
       </c>
-      <c r="B62" s="8" t="s">
+      <c r="C62" s="8" t="s">
         <v>411</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>412</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>30</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G62" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H62" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="I62" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="I62" s="8" t="s">
+      <c r="J62" s="8" t="s">
         <v>415</v>
-      </c>
-      <c r="J62" s="8" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" t="s">
+        <v>416</v>
+      </c>
+      <c r="B63" t="s">
         <v>417</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" s="25" t="s">
         <v>418</v>
-      </c>
-      <c r="C63" s="25" t="s">
-        <v>419</v>
       </c>
       <c r="D63" t="s">
         <v>13</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G63" t="s">
         <v>15</v>
       </c>
       <c r="H63" t="s">
+        <v>420</v>
+      </c>
+      <c r="I63" t="s">
         <v>421</v>
       </c>
-      <c r="I63" t="s">
+      <c r="J63" t="s">
         <v>422</v>
-      </c>
-      <c r="J63" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="64" spans="1:10" s="4" customFormat="1">
       <c r="A64" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="B64" s="6" t="s">
         <v>424</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="C64" s="6" t="s">
         <v>425</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>426</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>147</v>
@@ -4881,51 +4881,51 @@
       </c>
       <c r="F64" s="7"/>
       <c r="H64" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="I64" s="6" t="s">
         <v>427</v>
       </c>
-      <c r="I64" s="6" t="s">
+      <c r="J64" s="6" t="s">
         <v>428</v>
-      </c>
-      <c r="J64" s="6" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="B65" s="6" t="s">
         <v>430</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="C65" s="6" t="s">
         <v>431</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>432</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E65" s="6"/>
       <c r="F65" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G65" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H65" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="I65" s="6" t="s">
         <v>434</v>
       </c>
-      <c r="I65" s="6" t="s">
+      <c r="J65" s="6" t="s">
         <v>435</v>
-      </c>
-      <c r="J65" s="6" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="66" spans="1:10" s="5" customFormat="1">
       <c r="A66" t="s">
+        <v>436</v>
+      </c>
+      <c r="B66" t="s">
         <v>437</v>
-      </c>
-      <c r="B66" t="s">
-        <v>438</v>
       </c>
       <c r="C66"/>
       <c r="D66" t="s">
@@ -4934,24 +4934,24 @@
       <c r="E66"/>
       <c r="F66"/>
       <c r="G66" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H66" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="I66" s="18" t="s">
         <v>439</v>
       </c>
-      <c r="I66" s="18" t="s">
+      <c r="J66" s="17" t="s">
         <v>440</v>
-      </c>
-      <c r="J66" s="17" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="8" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="8" t="s">
@@ -4959,24 +4959,24 @@
       </c>
       <c r="E67" s="8"/>
       <c r="F67" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="G67" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="G67" s="8" t="s">
-        <v>396</v>
-      </c>
       <c r="H67" s="8" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I67" s="12" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="J67" s="17" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B68" t="s">
         <v>120</v>
@@ -4988,24 +4988,24 @@
         <v>32</v>
       </c>
       <c r="H68" s="21" t="s">
+        <v>444</v>
+      </c>
+      <c r="I68" s="18" t="s">
         <v>445</v>
       </c>
-      <c r="I68" s="18" t="s">
+      <c r="J68" s="18" t="s">
         <v>446</v>
-      </c>
-      <c r="J68" s="18" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="B69" s="8" t="s">
         <v>448</v>
       </c>
-      <c r="B69" s="8" t="s">
+      <c r="C69" s="8" t="s">
         <v>449</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>450</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>127</v>
@@ -5014,33 +5014,33 @@
         <v>87</v>
       </c>
       <c r="F69" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="G69" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="H69" s="8" t="s">
         <v>451</v>
       </c>
-      <c r="G69" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="H69" s="8" t="s">
+      <c r="I69" s="8" t="s">
         <v>452</v>
       </c>
-      <c r="I69" s="8" t="s">
+      <c r="J69" s="8" t="s">
         <v>453</v>
-      </c>
-      <c r="J69" s="8" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="B70" s="6" t="s">
         <v>455</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="C70" s="6" t="s">
         <v>456</v>
       </c>
-      <c r="C70" s="6" t="s">
-        <v>457</v>
-      </c>
       <c r="D70" s="6" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>148</v>
@@ -5052,56 +5052,56 @@
         <v>149</v>
       </c>
       <c r="H70" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="I70" s="6" t="s">
         <v>458</v>
       </c>
-      <c r="I70" s="6" t="s">
+      <c r="J70" s="6" t="s">
         <v>459</v>
-      </c>
-      <c r="J70" s="6" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="8" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>46</v>
       </c>
       <c r="E71" s="23" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G71" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H71" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="I71" s="8" t="s">
         <v>463</v>
       </c>
-      <c r="I71" s="8" t="s">
+      <c r="J71" s="17" t="s">
         <v>464</v>
-      </c>
-      <c r="J71" s="17" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
+        <v>465</v>
+      </c>
+      <c r="B72" t="s">
         <v>466</v>
       </c>
-      <c r="B72" t="s">
-        <v>467</v>
-      </c>
       <c r="C72" s="6" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D72" t="s">
         <v>110</v>
@@ -5110,51 +5110,51 @@
         <v>32</v>
       </c>
       <c r="H72" s="21" t="s">
+        <v>467</v>
+      </c>
+      <c r="I72" s="18" t="s">
         <v>468</v>
       </c>
-      <c r="I72" s="18" t="s">
+      <c r="J72" s="18" t="s">
         <v>469</v>
-      </c>
-      <c r="J72" s="18" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="B73" s="8" t="s">
         <v>471</v>
       </c>
-      <c r="B73" s="8" t="s">
+      <c r="C73" s="6" t="s">
         <v>472</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>473</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E73" s="8"/>
       <c r="F73" s="8" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G73" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H73" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="I73" s="8" t="s">
         <v>475</v>
       </c>
-      <c r="I73" s="8" t="s">
+      <c r="J73" s="8" t="s">
         <v>476</v>
-      </c>
-      <c r="J73" s="8" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74" t="s">
+        <v>477</v>
+      </c>
+      <c r="B74" t="s">
         <v>478</v>
-      </c>
-      <c r="B74" t="s">
-        <v>479</v>
       </c>
       <c r="C74" s="6"/>
       <c r="D74" s="8" t="s">
@@ -5162,27 +5162,27 @@
       </c>
       <c r="E74" s="8"/>
       <c r="F74" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G74" s="8" t="s">
         <v>87</v>
       </c>
       <c r="H74" t="s">
+        <v>480</v>
+      </c>
+      <c r="I74" s="18" t="s">
         <v>481</v>
-      </c>
-      <c r="I74" s="18" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="75" spans="1:10" s="4" customFormat="1">
       <c r="A75" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="B75" s="8" t="s">
         <v>483</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="C75" s="6" t="s">
         <v>484</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>485</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>170</v>
@@ -5191,27 +5191,27 @@
         <v>87</v>
       </c>
       <c r="G75" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H75" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="I75" s="8" t="s">
         <v>486</v>
       </c>
-      <c r="I75" s="8" t="s">
+      <c r="J75" s="8" t="s">
         <v>487</v>
-      </c>
-      <c r="J75" s="8" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="76" spans="1:10" s="4" customFormat="1">
       <c r="A76" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="B76" s="6" t="s">
         <v>489</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="C76" s="6" t="s">
         <v>490</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>491</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>170</v>
@@ -5220,30 +5220,30 @@
         <v>148</v>
       </c>
       <c r="F76" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="G76" s="8" t="s">
+        <v>772</v>
+      </c>
+      <c r="H76" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="G76" s="8" t="s">
-        <v>773</v>
-      </c>
-      <c r="H76" s="6" t="s">
+      <c r="I76" s="6" t="s">
         <v>493</v>
       </c>
-      <c r="I76" s="6" t="s">
+      <c r="J76" s="6" t="s">
         <v>494</v>
-      </c>
-      <c r="J76" s="6" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="B77" s="8" t="s">
         <v>496</v>
       </c>
-      <c r="B77" s="8" t="s">
+      <c r="C77" s="6" t="s">
         <v>497</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>498</v>
       </c>
       <c r="D77" s="8" t="s">
         <v>170</v>
@@ -5255,51 +5255,51 @@
         <v>117</v>
       </c>
       <c r="H77" s="8" t="s">
+        <v>498</v>
+      </c>
+      <c r="I77" s="8" t="s">
         <v>499</v>
       </c>
-      <c r="I77" s="8" t="s">
+      <c r="J77" s="8" t="s">
         <v>500</v>
-      </c>
-      <c r="J77" s="8" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="B78" s="6" t="s">
         <v>502</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="C78" s="6" t="s">
         <v>503</v>
       </c>
-      <c r="C78" s="6" t="s">
-        <v>504</v>
-      </c>
       <c r="D78" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E78" s="23" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F78" s="6"/>
       <c r="G78" s="6" t="s">
         <v>157</v>
       </c>
       <c r="H78" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="I78" s="6" t="s">
         <v>505</v>
       </c>
-      <c r="I78" s="6" t="s">
+      <c r="J78" s="6" t="s">
         <v>506</v>
-      </c>
-      <c r="J78" s="6" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="79" spans="1:10" s="4" customFormat="1">
       <c r="A79" s="6" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C79" s="6"/>
       <c r="D79" s="6" t="s">
@@ -5312,18 +5312,18 @@
       <c r="G79"/>
       <c r="H79" s="6"/>
       <c r="I79" s="6" t="s">
+        <v>513</v>
+      </c>
+      <c r="J79" s="6" t="s">
         <v>514</v>
-      </c>
-      <c r="J79" s="6" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="10" t="s">
+        <v>507</v>
+      </c>
+      <c r="B80" s="10" t="s">
         <v>508</v>
-      </c>
-      <c r="B80" s="10" t="s">
-        <v>509</v>
       </c>
       <c r="C80" s="10"/>
       <c r="D80" s="10" t="s">
@@ -5333,31 +5333,31 @@
         <v>47</v>
       </c>
       <c r="F80" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="H80" s="10" t="s">
+        <v>509</v>
+      </c>
+      <c r="I80" s="10" t="s">
         <v>510</v>
       </c>
-      <c r="I80" s="10" t="s">
+      <c r="J80" s="10" t="s">
         <v>511</v>
-      </c>
-      <c r="J80" s="10" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="B81" s="6" t="s">
         <v>516</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>517</v>
       </c>
       <c r="C81" s="6"/>
       <c r="D81" s="6" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E81" s="6"/>
       <c r="F81" s="6"/>
@@ -5365,134 +5365,134 @@
         <v>65</v>
       </c>
       <c r="H81" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="I81" s="16" t="s">
         <v>519</v>
-      </c>
-      <c r="I81" s="16" t="s">
-        <v>520</v>
       </c>
       <c r="J81" s="6"/>
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="6" t="s">
+        <v>520</v>
+      </c>
+      <c r="B82" s="6" t="s">
         <v>521</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>522</v>
       </c>
       <c r="C82" s="6"/>
       <c r="D82" s="6" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E82" s="6"/>
       <c r="F82" s="6"/>
       <c r="G82" s="6" t="s">
+        <v>522</v>
+      </c>
+      <c r="H82" s="6" t="s">
         <v>523</v>
       </c>
-      <c r="H82" s="6" t="s">
+      <c r="I82" s="16" t="s">
         <v>524</v>
-      </c>
-      <c r="I82" s="16" t="s">
-        <v>525</v>
       </c>
       <c r="J82" s="6"/>
     </row>
     <row r="83" spans="1:10">
       <c r="A83" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="B83" s="6" t="s">
         <v>526</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>527</v>
       </c>
       <c r="C83" s="6"/>
       <c r="D83" s="6" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E83" s="6"/>
       <c r="F83" s="28" t="s">
+        <v>528</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H83" s="14" t="s">
         <v>529</v>
       </c>
-      <c r="G83" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="H83" s="14" t="s">
+      <c r="I83" s="16" t="s">
         <v>530</v>
       </c>
-      <c r="I83" s="16" t="s">
+      <c r="J83" s="16" t="s">
         <v>531</v>
-      </c>
-      <c r="J83" s="16" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="84" spans="1:10">
       <c r="A84" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="B84" s="6" t="s">
         <v>533</v>
       </c>
-      <c r="B84" s="6" t="s">
+      <c r="C84" s="6" t="s">
         <v>534</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>535</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E84" s="6"/>
       <c r="F84" s="6" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G84" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H84" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="I84" s="6" t="s">
         <v>537</v>
       </c>
-      <c r="I84" s="6" t="s">
-        <v>538</v>
-      </c>
       <c r="J84" s="6" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="6" t="s">
+        <v>538</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="C85" s="6" t="s">
         <v>539</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>438</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>540</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E85" s="6"/>
       <c r="F85" s="6" t="s">
+        <v>540</v>
+      </c>
+      <c r="G85" s="6" t="s">
         <v>541</v>
       </c>
-      <c r="G85" s="6" t="s">
+      <c r="H85" s="6" t="s">
         <v>542</v>
       </c>
-      <c r="H85" s="6" t="s">
+      <c r="I85" s="6" t="s">
         <v>543</v>
       </c>
-      <c r="I85" s="6" t="s">
+      <c r="J85" s="6" t="s">
         <v>544</v>
-      </c>
-      <c r="J85" s="6" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="B86" s="6" t="s">
         <v>546</v>
       </c>
-      <c r="B86" s="6" t="s">
+      <c r="C86" s="6" t="s">
         <v>547</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>548</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>46</v>
@@ -5501,28 +5501,28 @@
         <v>87</v>
       </c>
       <c r="G86" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="H86" s="6" t="s">
         <v>549</v>
       </c>
-      <c r="H86" s="6" t="s">
+      <c r="I86" s="6" t="s">
         <v>550</v>
       </c>
-      <c r="I86" s="6" t="s">
+      <c r="J86" s="6" t="s">
         <v>551</v>
-      </c>
-      <c r="J86" s="6" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="6" t="s">
+        <v>552</v>
+      </c>
+      <c r="B87" s="6" t="s">
         <v>553</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>554</v>
       </c>
       <c r="C87" s="6"/>
       <c r="D87" s="6" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E87" s="6"/>
       <c r="F87" s="6"/>
@@ -5530,82 +5530,82 @@
         <v>111</v>
       </c>
       <c r="H87" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="I87" s="16" t="s">
         <v>555</v>
-      </c>
-      <c r="I87" s="16" t="s">
-        <v>556</v>
       </c>
       <c r="J87" s="6"/>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="B88" s="6" t="s">
         <v>557</v>
       </c>
-      <c r="B88" s="6" t="s">
+      <c r="C88" s="6" t="s">
         <v>558</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>559</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E88" s="6"/>
       <c r="F88" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="G88" s="6" t="s">
+        <v>522</v>
+      </c>
+      <c r="H88" s="6" t="s">
         <v>560</v>
       </c>
-      <c r="G88" s="6" t="s">
-        <v>523</v>
-      </c>
-      <c r="H88" s="6" t="s">
+      <c r="I88" s="6" t="s">
         <v>561</v>
       </c>
-      <c r="I88" s="6" t="s">
+      <c r="J88" s="6" t="s">
         <v>562</v>
-      </c>
-      <c r="J88" s="6" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="89" spans="1:10">
       <c r="A89" s="14" t="s">
+        <v>563</v>
+      </c>
+      <c r="B89" s="14" t="s">
         <v>564</v>
       </c>
-      <c r="B89" s="14" t="s">
+      <c r="C89" s="6" t="s">
         <v>565</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>566</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E89" s="6"/>
       <c r="F89" s="14" t="s">
+        <v>540</v>
+      </c>
+      <c r="G89" s="14" t="s">
         <v>541</v>
       </c>
-      <c r="G89" s="14" t="s">
-        <v>542</v>
-      </c>
       <c r="H89" s="14" t="s">
+        <v>566</v>
+      </c>
+      <c r="I89" s="14" t="s">
         <v>567</v>
       </c>
-      <c r="I89" s="14" t="s">
+      <c r="J89" s="14" t="s">
         <v>568</v>
-      </c>
-      <c r="J89" s="14" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="90" spans="1:10">
       <c r="A90" s="8" t="s">
+        <v>569</v>
+      </c>
+      <c r="B90" s="8" t="s">
         <v>570</v>
       </c>
-      <c r="B90" s="8" t="s">
+      <c r="C90" s="6" t="s">
         <v>571</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>572</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>127</v>
@@ -5618,51 +5618,51 @@
         <v>87</v>
       </c>
       <c r="H90" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="I90" s="8" t="s">
         <v>573</v>
       </c>
-      <c r="I90" s="8" t="s">
+      <c r="J90" s="8" t="s">
         <v>574</v>
-      </c>
-      <c r="J90" s="8" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91" s="8" t="s">
+        <v>575</v>
+      </c>
+      <c r="B91" s="8" t="s">
         <v>576</v>
       </c>
-      <c r="B91" s="8" t="s">
+      <c r="C91" s="6" t="s">
         <v>577</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>578</v>
       </c>
       <c r="D91" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E91" s="8"/>
       <c r="F91" s="11" t="s">
+        <v>578</v>
+      </c>
+      <c r="G91" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="H91" s="8" t="s">
         <v>579</v>
       </c>
-      <c r="G91" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="H91" s="8" t="s">
+      <c r="I91" s="8" t="s">
         <v>580</v>
       </c>
-      <c r="I91" s="8" t="s">
+      <c r="J91" s="8" t="s">
         <v>581</v>
-      </c>
-      <c r="J91" s="8" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="92" spans="1:10">
       <c r="A92" t="s">
+        <v>582</v>
+      </c>
+      <c r="B92" t="s">
         <v>583</v>
-      </c>
-      <c r="B92" t="s">
-        <v>584</v>
       </c>
       <c r="C92" s="6"/>
       <c r="D92" s="8" t="s">
@@ -5670,168 +5670,168 @@
       </c>
       <c r="E92" s="8"/>
       <c r="F92" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G92" s="8" t="s">
         <v>87</v>
       </c>
       <c r="H92" t="s">
+        <v>585</v>
+      </c>
+      <c r="I92" s="18" t="s">
         <v>586</v>
-      </c>
-      <c r="I92" s="18" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="14" t="s">
+        <v>587</v>
+      </c>
+      <c r="B93" s="14" t="s">
         <v>588</v>
       </c>
-      <c r="B93" s="14" t="s">
+      <c r="C93" s="14" t="s">
         <v>589</v>
       </c>
-      <c r="C93" s="14" t="s">
-        <v>590</v>
-      </c>
       <c r="D93" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E93" s="14" t="s">
         <v>47</v>
       </c>
       <c r="F93" s="7"/>
       <c r="G93" s="14" t="s">
+        <v>590</v>
+      </c>
+      <c r="H93" s="14" t="s">
         <v>591</v>
       </c>
-      <c r="H93" s="14" t="s">
+      <c r="I93" s="14" t="s">
         <v>592</v>
       </c>
-      <c r="I93" s="14" t="s">
+      <c r="J93" s="14" t="s">
         <v>593</v>
-      </c>
-      <c r="J93" s="14" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="94" spans="1:10">
       <c r="A94" s="8" t="s">
+        <v>594</v>
+      </c>
+      <c r="B94" s="8" t="s">
         <v>595</v>
-      </c>
-      <c r="B94" s="8" t="s">
-        <v>596</v>
       </c>
       <c r="C94" s="8"/>
       <c r="D94" s="8" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E94" s="8"/>
       <c r="F94" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G94" s="8" t="s">
         <v>72</v>
       </c>
       <c r="H94" s="8" t="s">
+        <v>598</v>
+      </c>
+      <c r="I94" s="8" t="s">
         <v>599</v>
       </c>
-      <c r="I94" s="8" t="s">
+      <c r="J94" s="8" t="s">
         <v>600</v>
-      </c>
-      <c r="J94" s="8" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="8" t="s">
+        <v>601</v>
+      </c>
+      <c r="B95" s="8" t="s">
         <v>602</v>
-      </c>
-      <c r="B95" s="8" t="s">
-        <v>603</v>
       </c>
       <c r="C95" s="8"/>
       <c r="D95" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F95" s="8"/>
       <c r="H95" s="8" t="s">
+        <v>603</v>
+      </c>
+      <c r="I95" s="8" t="s">
         <v>604</v>
       </c>
-      <c r="I95" s="8" t="s">
+      <c r="J95" s="8" t="s">
         <v>605</v>
-      </c>
-      <c r="J95" s="8" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="96" spans="1:10" s="4" customFormat="1">
       <c r="A96" s="8" t="s">
+        <v>606</v>
+      </c>
+      <c r="B96" s="8" t="s">
         <v>607</v>
       </c>
-      <c r="B96" s="8" t="s">
-        <v>608</v>
-      </c>
       <c r="C96" s="8" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>46</v>
       </c>
       <c r="E96" s="23" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="G96" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H96" s="8" t="s">
+        <v>609</v>
+      </c>
+      <c r="I96" s="8" t="s">
         <v>610</v>
       </c>
-      <c r="I96" s="8" t="s">
+      <c r="J96" s="17" t="s">
         <v>611</v>
-      </c>
-      <c r="J96" s="17" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="97" spans="1:10" s="4" customFormat="1">
       <c r="A97" s="8" t="s">
+        <v>612</v>
+      </c>
+      <c r="B97" s="8" t="s">
         <v>613</v>
-      </c>
-      <c r="B97" s="8" t="s">
-        <v>614</v>
       </c>
       <c r="C97" s="8"/>
       <c r="D97" s="8" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E97" s="6"/>
       <c r="F97" s="28" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H97" s="8"/>
       <c r="I97" s="17" t="s">
+        <v>616</v>
+      </c>
+      <c r="J97" s="18" t="s">
         <v>617</v>
-      </c>
-      <c r="J97" s="18" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" t="s">
+        <v>618</v>
+      </c>
+      <c r="B98" t="s">
         <v>619</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" s="25" t="s">
         <v>620</v>
-      </c>
-      <c r="C98" s="25" t="s">
-        <v>621</v>
       </c>
       <c r="D98" t="s">
         <v>30</v>
@@ -5840,27 +5840,27 @@
         <v>96</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="G98" t="s">
         <v>117</v>
       </c>
       <c r="I98" t="s">
+        <v>622</v>
+      </c>
+      <c r="J98" t="s">
         <v>623</v>
-      </c>
-      <c r="J98" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="99" spans="1:10">
       <c r="A99" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="B99" s="6" t="s">
         <v>625</v>
       </c>
-      <c r="B99" s="6" t="s">
+      <c r="C99" s="6" t="s">
         <v>626</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>627</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>127</v>
@@ -5869,90 +5869,90 @@
         <v>96</v>
       </c>
       <c r="F99" s="15" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G99" t="s">
         <v>117</v>
       </c>
       <c r="H99" s="14" t="s">
+        <v>628</v>
+      </c>
+      <c r="I99" s="14" t="s">
         <v>629</v>
       </c>
-      <c r="I99" s="14" t="s">
+      <c r="J99" s="14" t="s">
         <v>630</v>
-      </c>
-      <c r="J99" s="14" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" s="6" t="s">
+        <v>631</v>
+      </c>
+      <c r="B100" s="6" t="s">
         <v>632</v>
       </c>
-      <c r="B100" s="6" t="s">
+      <c r="C100" s="6" t="s">
         <v>633</v>
-      </c>
-      <c r="C100" s="6" t="s">
-        <v>634</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E100" s="6"/>
       <c r="F100" s="6" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G100" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H100" s="14" t="s">
+        <v>635</v>
+      </c>
+      <c r="I100" s="14" t="s">
         <v>636</v>
       </c>
-      <c r="I100" s="14" t="s">
+      <c r="J100" s="14" t="s">
         <v>637</v>
-      </c>
-      <c r="J100" s="14" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="101" spans="1:10">
       <c r="A101" s="8" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B101" s="8" t="s">
+        <v>638</v>
+      </c>
+      <c r="C101" s="8" t="s">
         <v>639</v>
-      </c>
-      <c r="C101" s="8" t="s">
-        <v>640</v>
       </c>
       <c r="D101" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E101" s="8"/>
       <c r="F101" s="8" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="G101" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H101" s="10" t="s">
+        <v>641</v>
+      </c>
+      <c r="I101" s="10" t="s">
         <v>642</v>
       </c>
-      <c r="I101" s="10" t="s">
+      <c r="J101" s="10" t="s">
         <v>643</v>
-      </c>
-      <c r="J101" s="10" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="102" spans="1:10">
       <c r="A102" s="6" t="s">
+        <v>644</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="C102" s="6" t="s">
         <v>645</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>373</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>646</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>13</v>
@@ -5965,24 +5965,24 @@
         <v>111</v>
       </c>
       <c r="H102" s="14" t="s">
+        <v>646</v>
+      </c>
+      <c r="I102" s="14" t="s">
         <v>647</v>
       </c>
-      <c r="I102" s="14" t="s">
+      <c r="J102" s="14" t="s">
         <v>648</v>
-      </c>
-      <c r="J102" s="14" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="103" spans="1:10" s="5" customFormat="1">
       <c r="A103" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>583</v>
+      </c>
+      <c r="C103" s="6" t="s">
         <v>650</v>
-      </c>
-      <c r="B103" s="6" t="s">
-        <v>584</v>
-      </c>
-      <c r="C103" s="6" t="s">
-        <v>651</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>30</v>
@@ -5991,52 +5991,52 @@
         <v>96</v>
       </c>
       <c r="F103" s="15" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="H103" s="14"/>
       <c r="I103" s="13" t="s">
+        <v>652</v>
+      </c>
+      <c r="J103" s="14" t="s">
         <v>653</v>
-      </c>
-      <c r="J103" s="14" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="104" spans="1:10" s="5" customFormat="1">
       <c r="A104" s="8" t="s">
+        <v>654</v>
+      </c>
+      <c r="B104" s="8" t="s">
         <v>655</v>
       </c>
-      <c r="B104" s="8" t="s">
+      <c r="C104" s="8" t="s">
         <v>656</v>
-      </c>
-      <c r="C104" s="8" t="s">
-        <v>657</v>
       </c>
       <c r="D104" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E104" s="8"/>
       <c r="F104" s="11" t="s">
+        <v>657</v>
+      </c>
+      <c r="G104" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="H104" s="10" t="s">
         <v>658</v>
       </c>
-      <c r="G104" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="H104" s="10" t="s">
+      <c r="I104" s="10" t="s">
         <v>659</v>
       </c>
-      <c r="I104" s="10" t="s">
+      <c r="J104" s="10" t="s">
         <v>660</v>
-      </c>
-      <c r="J104" s="10" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="105" spans="1:10">
       <c r="A105" s="8" t="s">
+        <v>661</v>
+      </c>
+      <c r="B105" s="8" t="s">
         <v>662</v>
-      </c>
-      <c r="B105" s="8" t="s">
-        <v>663</v>
       </c>
       <c r="C105" s="6"/>
       <c r="D105" s="8" t="s">
@@ -6048,42 +6048,42 @@
         <v>23</v>
       </c>
       <c r="H105" s="10" t="s">
+        <v>663</v>
+      </c>
+      <c r="I105" s="17" t="s">
         <v>664</v>
-      </c>
-      <c r="I105" s="17" t="s">
-        <v>665</v>
       </c>
       <c r="J105" s="10"/>
     </row>
     <row r="106" spans="1:10">
       <c r="A106" t="s">
+        <v>665</v>
+      </c>
+      <c r="B106" t="s">
         <v>666</v>
       </c>
-      <c r="B106" t="s">
+      <c r="D106" t="s">
+        <v>517</v>
+      </c>
+      <c r="G106" t="s">
+        <v>774</v>
+      </c>
+      <c r="H106" s="8" t="s">
         <v>667</v>
       </c>
-      <c r="D106" t="s">
-        <v>518</v>
-      </c>
-      <c r="G106" t="s">
-        <v>775</v>
-      </c>
-      <c r="H106" s="8" t="s">
+      <c r="I106" s="18" t="s">
         <v>668</v>
       </c>
-      <c r="I106" s="18" t="s">
+      <c r="J106" s="17" t="s">
         <v>669</v>
-      </c>
-      <c r="J106" s="17" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="107" spans="1:10">
       <c r="A107" t="s">
+        <v>670</v>
+      </c>
+      <c r="B107" t="s">
         <v>671</v>
-      </c>
-      <c r="B107" t="s">
-        <v>672</v>
       </c>
       <c r="D107" t="s">
         <v>110</v>
@@ -6092,53 +6092,53 @@
         <v>32</v>
       </c>
       <c r="H107" t="s">
+        <v>672</v>
+      </c>
+      <c r="I107" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="I107" s="18" t="s">
+      <c r="J107" s="19" t="s">
         <v>674</v>
-      </c>
-      <c r="J107" s="19" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="108" spans="1:10">
       <c r="A108" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B108" t="s">
         <v>62</v>
       </c>
       <c r="C108" s="25" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="D108" t="s">
         <v>13</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="G108" t="s">
         <v>32</v>
       </c>
       <c r="H108" s="4" t="s">
+        <v>678</v>
+      </c>
+      <c r="I108" s="4" t="s">
         <v>679</v>
       </c>
-      <c r="I108" s="4" t="s">
+      <c r="J108" s="4" t="s">
         <v>680</v>
-      </c>
-      <c r="J108" s="4" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="109" spans="1:10">
       <c r="A109" s="6" t="s">
+        <v>681</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="C109" s="6" t="s">
         <v>682</v>
-      </c>
-      <c r="B109" s="6" t="s">
-        <v>526</v>
-      </c>
-      <c r="C109" s="6" t="s">
-        <v>683</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>147</v>
@@ -6151,18 +6151,18 @@
         <v>141</v>
       </c>
       <c r="I109" s="14" t="s">
+        <v>683</v>
+      </c>
+      <c r="J109" s="14" t="s">
         <v>684</v>
-      </c>
-      <c r="J109" s="14" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="110" spans="1:10">
       <c r="A110" s="6" t="s">
+        <v>685</v>
+      </c>
+      <c r="B110" s="6" t="s">
         <v>686</v>
-      </c>
-      <c r="B110" s="6" t="s">
-        <v>687</v>
       </c>
       <c r="C110" s="6"/>
       <c r="D110" s="6" t="s">
@@ -6170,28 +6170,28 @@
       </c>
       <c r="E110" s="6"/>
       <c r="F110" s="15" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H110" s="14"/>
       <c r="I110" s="14" t="s">
+        <v>688</v>
+      </c>
+      <c r="J110" s="14" t="s">
         <v>689</v>
-      </c>
-      <c r="J110" s="14" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="111" spans="1:10">
       <c r="A111" t="s">
+        <v>690</v>
+      </c>
+      <c r="B111" t="s">
         <v>691</v>
       </c>
-      <c r="B111" t="s">
-        <v>692</v>
-      </c>
       <c r="D111" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E111" s="6"/>
       <c r="F111" s="6"/>
@@ -6201,40 +6201,40 @@
     </row>
     <row r="112" spans="1:10">
       <c r="A112" s="10" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B112" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D112" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E112" s="10"/>
       <c r="F112" s="10" t="s">
+        <v>694</v>
+      </c>
+      <c r="G112" s="10" t="s">
         <v>695</v>
       </c>
-      <c r="G112" s="10" t="s">
+      <c r="H112" s="10" t="s">
         <v>696</v>
       </c>
-      <c r="H112" s="10" t="s">
+      <c r="I112" s="10" t="s">
         <v>697</v>
       </c>
-      <c r="I112" s="10" t="s">
+      <c r="J112" s="10" t="s">
         <v>698</v>
-      </c>
-      <c r="J112" s="10" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="113" spans="1:10">
       <c r="A113" s="10" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B113" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C113" s="10"/>
       <c r="D113" s="10" t="s">
@@ -6246,24 +6246,24 @@
       <c r="F113" s="10"/>
       <c r="G113" s="10"/>
       <c r="H113" s="10" t="s">
+        <v>700</v>
+      </c>
+      <c r="I113" s="10" t="s">
         <v>701</v>
       </c>
-      <c r="I113" s="10" t="s">
+      <c r="J113" s="10" t="s">
         <v>702</v>
-      </c>
-      <c r="J113" s="10" t="s">
-        <v>703</v>
       </c>
     </row>
     <row r="114" spans="1:10">
       <c r="A114" s="6" t="s">
+        <v>703</v>
+      </c>
+      <c r="B114" s="6" t="s">
         <v>704</v>
       </c>
-      <c r="B114" s="6" t="s">
+      <c r="C114" s="6" t="s">
         <v>705</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>706</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>95</v>
@@ -6272,24 +6272,24 @@
         <v>96</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H114" s="6" t="s">
+        <v>706</v>
+      </c>
+      <c r="I114" s="6" t="s">
         <v>707</v>
       </c>
-      <c r="I114" s="6" t="s">
+      <c r="J114" s="6" t="s">
         <v>708</v>
-      </c>
-      <c r="J114" s="6" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="115" spans="1:10">
       <c r="A115" s="6" t="s">
+        <v>709</v>
+      </c>
+      <c r="B115" s="6" t="s">
         <v>710</v>
-      </c>
-      <c r="B115" s="6" t="s">
-        <v>711</v>
       </c>
       <c r="C115" s="6"/>
       <c r="D115" s="6" t="s">
@@ -6298,55 +6298,55 @@
       <c r="E115" s="6"/>
       <c r="F115" s="6"/>
       <c r="G115" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="H115" s="6"/>
       <c r="I115" s="16" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="J115" s="6"/>
     </row>
     <row r="116" spans="1:10">
       <c r="A116" s="14" t="s">
+        <v>712</v>
+      </c>
+      <c r="B116" s="14" t="s">
         <v>713</v>
       </c>
-      <c r="B116" s="14" t="s">
+      <c r="C116" s="26" t="s">
         <v>714</v>
       </c>
-      <c r="C116" s="26" t="s">
+      <c r="D116" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="E116" t="s">
         <v>715</v>
       </c>
-      <c r="D116" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="E116" t="s">
+      <c r="F116" s="14" t="s">
         <v>716</v>
-      </c>
-      <c r="F116" s="14" t="s">
-        <v>717</v>
       </c>
       <c r="G116" s="14" t="s">
         <v>49</v>
       </c>
       <c r="H116" s="14" t="s">
+        <v>717</v>
+      </c>
+      <c r="I116" s="14" t="s">
         <v>718</v>
       </c>
-      <c r="I116" s="14" t="s">
+      <c r="J116" s="14" t="s">
         <v>719</v>
-      </c>
-      <c r="J116" s="14" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="117" spans="1:10">
       <c r="A117" s="8" t="s">
+        <v>720</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>583</v>
+      </c>
+      <c r="C117" s="27" t="s">
         <v>721</v>
-      </c>
-      <c r="B117" s="8" t="s">
-        <v>584</v>
-      </c>
-      <c r="C117" s="27" t="s">
-        <v>722</v>
       </c>
       <c r="D117" s="8" t="s">
         <v>30</v>
@@ -6359,21 +6359,21 @@
         <v>157</v>
       </c>
       <c r="H117" s="8" t="s">
+        <v>722</v>
+      </c>
+      <c r="I117" s="8" t="s">
         <v>723</v>
       </c>
-      <c r="I117" s="8" t="s">
+      <c r="J117" s="8" t="s">
         <v>724</v>
-      </c>
-      <c r="J117" s="8" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="118" spans="1:10">
       <c r="A118" s="8" t="s">
+        <v>725</v>
+      </c>
+      <c r="B118" s="8" t="s">
         <v>726</v>
-      </c>
-      <c r="B118" s="8" t="s">
-        <v>727</v>
       </c>
       <c r="C118" s="8"/>
       <c r="D118" s="8" t="s">
@@ -6382,22 +6382,22 @@
       <c r="E118" s="8"/>
       <c r="F118" s="8"/>
       <c r="G118" s="8" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="H118" t="s">
+        <v>727</v>
+      </c>
+      <c r="I118" s="17" t="s">
         <v>728</v>
-      </c>
-      <c r="I118" s="17" t="s">
-        <v>729</v>
       </c>
       <c r="J118" s="8"/>
     </row>
     <row r="119" spans="1:10">
       <c r="A119" s="6" t="s">
+        <v>729</v>
+      </c>
+      <c r="B119" s="6" t="s">
         <v>730</v>
-      </c>
-      <c r="B119" s="6" t="s">
-        <v>731</v>
       </c>
       <c r="C119" s="6"/>
       <c r="D119" s="6" t="s">
@@ -6405,77 +6405,77 @@
       </c>
       <c r="E119" s="6"/>
       <c r="F119" s="15" t="s">
+        <v>731</v>
+      </c>
+      <c r="G119" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H119" s="6" t="s">
         <v>732</v>
       </c>
-      <c r="G119" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="H119" s="6" t="s">
+      <c r="I119" s="6" t="s">
         <v>733</v>
       </c>
-      <c r="I119" s="6" t="s">
+      <c r="J119" s="6" t="s">
         <v>734</v>
-      </c>
-      <c r="J119" s="6" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="120" spans="1:10">
       <c r="A120" s="6" t="s">
+        <v>735</v>
+      </c>
+      <c r="B120" s="6" t="s">
         <v>736</v>
-      </c>
-      <c r="B120" s="6" t="s">
-        <v>737</v>
       </c>
       <c r="C120" s="6"/>
       <c r="D120" s="6" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E120" s="6"/>
       <c r="F120" s="6"/>
       <c r="G120" s="6" t="s">
+        <v>522</v>
+      </c>
+      <c r="H120" s="8" t="s">
         <v>523</v>
       </c>
-      <c r="H120" s="8" t="s">
-        <v>524</v>
-      </c>
       <c r="I120" s="16" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="J120" s="6"/>
     </row>
     <row r="121" spans="1:10">
       <c r="A121" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B121" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D121" t="s">
         <v>56</v>
       </c>
       <c r="F121" t="s">
+        <v>739</v>
+      </c>
+      <c r="G121" t="s">
+        <v>367</v>
+      </c>
+      <c r="H121" s="8" t="s">
         <v>740</v>
       </c>
-      <c r="G121" t="s">
-        <v>368</v>
-      </c>
-      <c r="H121" s="8" t="s">
+      <c r="I121" s="18" t="s">
         <v>741</v>
       </c>
-      <c r="I121" s="18" t="s">
+      <c r="J121" s="17" t="s">
         <v>742</v>
-      </c>
-      <c r="J121" s="17" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="122" spans="1:10">
       <c r="A122" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B122" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C122" s="6"/>
       <c r="D122" t="s">
@@ -6485,24 +6485,24 @@
         <v>47</v>
       </c>
       <c r="F122" t="s">
+        <v>778</v>
+      </c>
+      <c r="G122" t="s">
+        <v>776</v>
+      </c>
+      <c r="H122" t="s">
         <v>779</v>
       </c>
-      <c r="G122" t="s">
-        <v>777</v>
-      </c>
-      <c r="H122" t="s">
+      <c r="I122" s="29" t="s">
         <v>780</v>
-      </c>
-      <c r="I122" s="29" t="s">
-        <v>781</v>
       </c>
     </row>
     <row r="123" spans="1:10">
       <c r="A123" s="6" t="s">
+        <v>743</v>
+      </c>
+      <c r="B123" s="6" t="s">
         <v>744</v>
-      </c>
-      <c r="B123" s="6" t="s">
-        <v>745</v>
       </c>
       <c r="C123" s="6"/>
       <c r="D123" s="6" t="s">
@@ -6514,51 +6514,51 @@
         <v>65</v>
       </c>
       <c r="H123" s="6" t="s">
+        <v>745</v>
+      </c>
+      <c r="I123" s="16" t="s">
         <v>746</v>
-      </c>
-      <c r="I123" s="16" t="s">
-        <v>747</v>
       </c>
       <c r="J123" s="6"/>
     </row>
     <row r="124" spans="1:10">
       <c r="A124" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="B124" s="6" t="s">
         <v>748</v>
       </c>
-      <c r="B124" s="6" t="s">
-        <v>749</v>
-      </c>
       <c r="C124" s="6" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>110</v>
       </c>
       <c r="E124" s="6"/>
       <c r="F124" s="6" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="G124" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H124" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="I124" s="16" t="s">
         <v>751</v>
-      </c>
-      <c r="I124" s="16" t="s">
-        <v>752</v>
       </c>
       <c r="J124" s="6"/>
     </row>
     <row r="125" spans="1:10">
       <c r="A125" s="6" t="s">
+        <v>752</v>
+      </c>
+      <c r="B125" s="6" t="s">
         <v>753</v>
-      </c>
-      <c r="B125" s="6" t="s">
-        <v>754</v>
       </c>
       <c r="C125" s="26"/>
       <c r="D125" s="6" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E125" s="6"/>
       <c r="F125" s="6"/>
@@ -6566,49 +6566,49 @@
         <v>65</v>
       </c>
       <c r="H125" s="6" t="s">
+        <v>754</v>
+      </c>
+      <c r="I125" s="16" t="s">
         <v>755</v>
-      </c>
-      <c r="I125" s="16" t="s">
-        <v>756</v>
       </c>
       <c r="J125" s="6"/>
     </row>
     <row r="126" spans="1:10">
       <c r="A126" s="6" t="s">
+        <v>756</v>
+      </c>
+      <c r="B126" s="6" t="s">
         <v>757</v>
       </c>
-      <c r="B126" s="6" t="s">
+      <c r="C126" s="6" t="s">
         <v>758</v>
-      </c>
-      <c r="C126" s="6" t="s">
-        <v>759</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E126" s="6" t="s">
+        <v>759</v>
+      </c>
+      <c r="F126" s="15" t="s">
         <v>760</v>
-      </c>
-      <c r="F126" s="15" t="s">
-        <v>761</v>
       </c>
       <c r="G126" t="s">
         <v>117</v>
       </c>
       <c r="H126" s="6"/>
       <c r="I126" s="6" t="s">
+        <v>761</v>
+      </c>
+      <c r="J126" s="6" t="s">
         <v>762</v>
-      </c>
-      <c r="J126" s="6" t="s">
-        <v>763</v>
       </c>
     </row>
     <row r="127" spans="1:10">
       <c r="A127" s="6" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C127" s="6"/>
       <c r="D127" s="6" t="s">
@@ -6620,19 +6620,19 @@
         <v>111</v>
       </c>
       <c r="H127" s="6" t="s">
+        <v>764</v>
+      </c>
+      <c r="I127" s="16" t="s">
         <v>765</v>
-      </c>
-      <c r="I127" s="16" t="s">
-        <v>766</v>
       </c>
       <c r="J127" s="6"/>
     </row>
     <row r="128" spans="1:10">
       <c r="A128" s="8" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C128" s="8"/>
       <c r="D128" s="8" t="s">
@@ -6642,19 +6642,19 @@
         <v>87</v>
       </c>
       <c r="F128" s="8" t="s">
+        <v>767</v>
+      </c>
+      <c r="G128" t="s">
+        <v>548</v>
+      </c>
+      <c r="H128" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="I128" s="8" t="s">
         <v>768</v>
       </c>
-      <c r="G128" t="s">
-        <v>549</v>
-      </c>
-      <c r="H128" s="8" t="s">
-        <v>573</v>
-      </c>
-      <c r="I128" s="8" t="s">
+      <c r="J128" s="12" t="s">
         <v>769</v>
-      </c>
-      <c r="J128" s="12" t="s">
-        <v>770</v>
       </c>
     </row>
   </sheetData>
@@ -6735,14 +6735,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9cb1c2f4-2737-4134-a1af-8acbe3d02830" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6941,27 +6939,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9cb1c2f4-2737-4134-a1af-8acbe3d02830" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9cb1c2f4-2737-4134-a1af-8acbe3d02830"/>
-    <ds:schemaRef ds:uri="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6986,9 +6977,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9cb1c2f4-2737-4134-a1af-8acbe3d02830"/>
+    <ds:schemaRef ds:uri="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(repertoire-personnel): Changements au répertoire du personnel
</commit_message>
<xml_diff>
--- a/content/personnel/liste-personnel.xlsx
+++ b/content/personnel/liste-personnel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projets\coquille-web\content\personnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9357DE76-E356-409F-8638-34C040D2ADEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86E65F6-050C-4067-852B-F5A4626C1260}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1890" yWindow="3180" windowWidth="33570" windowHeight="23450" tabRatio="149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -556,9 +556,6 @@
   </si>
   <si>
     <t>Accueil et prêt</t>
-  </si>
-  <si>
-    <t>Centre de conservation Lionel-Groulx</t>
   </si>
   <si>
     <t>514 343-6111, poste 42680</t>
@@ -2414,7 +2411,10 @@
     <t>Bibliothèque de droit;Bibliothèque de musique</t>
   </si>
   <si>
-    <t>Gestion des collections et numérisation;Centre de conservation Lionel-Groulx</t>
+    <t>Centre de conservation Lionel-Groulx;Centre de conservation Marcel-Laurin</t>
+  </si>
+  <si>
+    <t>Gestion des collections et numérisation;Centre de conservation Lionel-Groulx;Centre de conservation Marcel-Laurin</t>
   </si>
 </sst>
 </file>
@@ -2717,7 +2717,15 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A0AF7E1-A614-44BF-8C48-5C26377DC552}" name="Tableau1" displayName="Tableau1" ref="A1:J128" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:J128" xr:uid="{4A0AF7E1-A614-44BF-8C48-5C26377DC552}"/>
+  <autoFilter ref="A1:J128" xr:uid="{4A0AF7E1-A614-44BF-8C48-5C26377DC552}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Boyer"/>
+        <filter val="Brazeau"/>
+        <filter val="Lalonde"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:J128">
     <sortCondition ref="A1:A128"/>
   </sortState>
@@ -3060,9 +3068,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomLeft" activeCell="G133" sqref="G133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -3111,7 +3119,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" hidden="1">
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
@@ -3141,7 +3149,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" hidden="1">
       <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
@@ -3171,7 +3179,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" hidden="1">
       <c r="A4" s="6" t="s">
         <v>27</v>
       </c>
@@ -3201,7 +3209,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" hidden="1">
       <c r="A5" s="8" t="s">
         <v>36</v>
       </c>
@@ -3231,7 +3239,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" hidden="1">
       <c r="A6" s="6" t="s">
         <v>43</v>
       </c>
@@ -3263,7 +3271,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" hidden="1">
       <c r="A7" s="8" t="s">
         <v>53</v>
       </c>
@@ -3293,7 +3301,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" hidden="1">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -3322,7 +3330,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" hidden="1">
       <c r="A9" s="6" t="s">
         <v>69</v>
       </c>
@@ -3349,7 +3357,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" hidden="1">
       <c r="A10" s="8" t="s">
         <v>77</v>
       </c>
@@ -3366,10 +3374,10 @@
         <v>81</v>
       </c>
       <c r="F10" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>82</v>
@@ -3381,7 +3389,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" hidden="1">
       <c r="A11" s="8" t="s">
         <v>85</v>
       </c>
@@ -3408,7 +3416,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" hidden="1">
       <c r="A12" s="8" t="s">
         <v>92</v>
       </c>
@@ -3437,7 +3445,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" hidden="1">
       <c r="A13" s="8" t="s">
         <v>101</v>
       </c>
@@ -3467,7 +3475,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" hidden="1">
       <c r="A14" s="8" t="s">
         <v>108</v>
       </c>
@@ -3491,7 +3499,7 @@
       </c>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" hidden="1">
       <c r="A15" s="6" t="s">
         <v>114</v>
       </c>
@@ -3519,7 +3527,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" hidden="1">
       <c r="A16" t="s">
         <v>114</v>
       </c>
@@ -3543,7 +3551,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" hidden="1">
       <c r="A17" s="6" t="s">
         <v>124</v>
       </c>
@@ -3573,7 +3581,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" hidden="1">
       <c r="A18" t="s">
         <v>131</v>
       </c>
@@ -3602,7 +3610,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" hidden="1">
       <c r="A19" s="10" t="s">
         <v>138</v>
       </c>
@@ -3627,7 +3635,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" hidden="1">
       <c r="A20" s="6" t="s">
         <v>144</v>
       </c>
@@ -3656,7 +3664,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" hidden="1">
       <c r="A21" s="8" t="s">
         <v>153</v>
       </c>
@@ -3686,7 +3694,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" hidden="1">
       <c r="A22" s="6" t="s">
         <v>161</v>
       </c>
@@ -3759,27 +3767,27 @@
         <v>176</v>
       </c>
       <c r="G24" s="8" t="s">
+        <v>787</v>
+      </c>
+      <c r="H24" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="H24" s="8" t="s">
+      <c r="I24" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="J24" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="J24" s="8" t="s">
+    </row>
+    <row r="25" spans="1:10" hidden="1">
+      <c r="A25" s="8" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="8" t="s">
+      <c r="B25" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="C25" s="8" t="s">
         <v>182</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>183</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>80</v>
@@ -3789,21 +3797,21 @@
       </c>
       <c r="F25" s="11"/>
       <c r="H25" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="I25" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="J25" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="J25" s="8" t="s">
+    </row>
+    <row r="26" spans="1:10" hidden="1">
+      <c r="A26" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
         <v>187</v>
-      </c>
-      <c r="B26" t="s">
-        <v>188</v>
       </c>
       <c r="D26" t="s">
         <v>110</v>
@@ -3812,49 +3820,49 @@
         <v>32</v>
       </c>
       <c r="H26" t="s">
+        <v>188</v>
+      </c>
+      <c r="I26" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="I26" s="18" t="s">
+      <c r="J26" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="J26" s="18" t="s">
+    </row>
+    <row r="27" spans="1:10" hidden="1">
+      <c r="A27" s="6" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="6" t="s">
+      <c r="B27" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>193</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="H27" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="I27" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="I27" s="13" t="s">
+      <c r="J27" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="J27" s="13" t="s">
+    </row>
+    <row r="28" spans="1:10" hidden="1">
+      <c r="A28" s="6" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="6" t="s">
+      <c r="B28" s="6" t="s">
         <v>200</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>201</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6" t="s">
@@ -3862,57 +3870,57 @@
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="H28" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="I28" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="I28" s="6" t="s">
+      <c r="J28" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="J28" s="6" t="s">
+    </row>
+    <row r="29" spans="1:10" hidden="1">
+      <c r="A29" s="6" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="6" t="s">
+      <c r="B29" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="C29" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="D29" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F29" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="G29" t="s">
         <v>210</v>
-      </c>
-      <c r="G29" t="s">
-        <v>211</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="J29" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="J29" s="13" t="s">
+    </row>
+    <row r="30" spans="1:10" hidden="1">
+      <c r="A30" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
         <v>214</v>
-      </c>
-      <c r="B30" t="s">
-        <v>215</v>
       </c>
       <c r="D30" t="s">
         <v>30</v>
@@ -3924,39 +3932,39 @@
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" hidden="1">
       <c r="A31" t="s">
+        <v>215</v>
+      </c>
+      <c r="B31" t="s">
         <v>216</v>
-      </c>
-      <c r="B31" t="s">
-        <v>217</v>
       </c>
       <c r="D31" t="s">
         <v>56</v>
       </c>
       <c r="G31" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H31" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="I31" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="I31" s="18" t="s">
+      <c r="J31" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="J31" s="17" t="s">
+    </row>
+    <row r="32" spans="1:10" hidden="1">
+      <c r="A32" s="6" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="6" t="s">
+      <c r="B32" s="6" t="s">
         <v>221</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>222</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E32" s="15" t="s">
         <v>72</v>
@@ -3966,372 +3974,372 @@
       <c r="I32" s="13"/>
       <c r="J32" s="20"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" hidden="1">
       <c r="A33" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="C33" s="8" t="s">
         <v>225</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>226</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="H33" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="G33" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="H33" s="8" t="s">
+      <c r="I33" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="J33" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="J33" s="8" t="s">
+    </row>
+    <row r="34" spans="1:10" hidden="1">
+      <c r="A34" s="6" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="6" t="s">
+      <c r="B34" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="C34" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="D34" s="6" t="s">
         <v>233</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>234</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>96</v>
       </c>
       <c r="F34" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="H34" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="I34" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="I34" s="6" t="s">
+      <c r="J34" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="J34" s="6" t="s">
+    </row>
+    <row r="35" spans="1:10" hidden="1">
+      <c r="A35" s="6" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="6" t="s">
+      <c r="B35" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>240</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>241</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H35" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="I35" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="I35" s="6" t="s">
+      <c r="J35" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="J35" s="6" t="s">
+    </row>
+    <row r="36" spans="1:10" hidden="1">
+      <c r="A36" s="8" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="8" t="s">
+      <c r="B36" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="C36" s="8" t="s">
         <v>247</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>248</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>30</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H36" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="I36" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="I36" s="8" t="s">
+      <c r="J36" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="J36" s="12" t="s">
+    </row>
+    <row r="37" spans="1:10" hidden="1">
+      <c r="A37" s="6" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="6" t="s">
+      <c r="B37" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="C37" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="D37" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="E37" t="s">
         <v>256</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>257</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" s="8" t="s">
+        <v>771</v>
+      </c>
+      <c r="H37" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="G37" s="8" t="s">
-        <v>772</v>
-      </c>
-      <c r="H37" s="6" t="s">
+      <c r="I37" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="I37" s="6" t="s">
+      <c r="J37" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="J37" s="13" t="s">
+    </row>
+    <row r="38" spans="1:10" hidden="1">
+      <c r="A38" s="8" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="8" t="s">
+      <c r="B38" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="C38" s="8" t="s">
         <v>263</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>264</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="H38" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="G38" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="H38" s="8" t="s">
+      <c r="I38" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="I38" s="8" t="s">
+      <c r="J38" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="J38" s="8" t="s">
+    </row>
+    <row r="39" spans="1:10" hidden="1">
+      <c r="A39" s="6" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="6" t="s">
+      <c r="B39" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="C39" s="6" t="s">
         <v>270</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>271</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E39" s="6"/>
       <c r="F39" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>65</v>
       </c>
       <c r="H39" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="I39" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="I39" s="6" t="s">
+      <c r="J39" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="J39" s="6" t="s">
+    </row>
+    <row r="40" spans="1:10" hidden="1">
+      <c r="A40" s="6" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="6" t="s">
+      <c r="B40" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>277</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>278</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H40" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="I40" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="I40" s="6" t="s">
+      <c r="J40" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="J40" s="6" t="s">
+    </row>
+    <row r="41" spans="1:10" hidden="1">
+      <c r="A41" s="8" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="8" t="s">
+      <c r="B41" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="C41" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="D41" s="8" t="s">
         <v>285</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>286</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="H41" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="G41" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="H41" s="8" t="s">
+      <c r="I41" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="I41" s="8" t="s">
+      <c r="J41" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="J41" s="8" t="s">
+    </row>
+    <row r="42" spans="1:10" hidden="1">
+      <c r="A42" s="8" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="8" t="s">
+      <c r="B42" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="C42" s="8" t="s">
         <v>293</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>294</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>773</v>
+      </c>
+      <c r="H42" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="G42" s="8" t="s">
-        <v>774</v>
-      </c>
-      <c r="H42" s="8" t="s">
+      <c r="I42" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="I42" s="8" t="s">
+      <c r="J42" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="J42" s="8" t="s">
+    </row>
+    <row r="43" spans="1:10" hidden="1">
+      <c r="A43" s="8" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="8" t="s">
+      <c r="B43" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="C43" s="8" t="s">
         <v>300</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>301</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G43" s="8" t="s">
         <v>65</v>
       </c>
       <c r="H43" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="I43" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="I43" s="8" t="s">
+      <c r="J43" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="J43" s="8" t="s">
+    </row>
+    <row r="44" spans="1:10" hidden="1">
+      <c r="A44" s="6" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="6" t="s">
+      <c r="B44" s="6" t="s">
         <v>306</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>307</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="H44" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="H44" s="6" t="s">
+      <c r="I44" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="I44" s="6" t="s">
+      <c r="J44" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="J44" s="6" t="s">
+    </row>
+    <row r="45" spans="1:10" hidden="1">
+      <c r="A45" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="A45" t="s">
+      <c r="B45" t="s">
         <v>313</v>
       </c>
-      <c r="B45" t="s">
-        <v>314</v>
-      </c>
       <c r="C45" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D45" t="s">
         <v>110</v>
@@ -4340,51 +4348,51 @@
         <v>32</v>
       </c>
       <c r="H45" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="I45" s="18" t="s">
         <v>315</v>
       </c>
-      <c r="I45" s="18" t="s">
+      <c r="J45" s="18" t="s">
         <v>316</v>
       </c>
-      <c r="J45" s="18" t="s">
+    </row>
+    <row r="46" spans="1:10" hidden="1">
+      <c r="A46" s="6" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="6" t="s">
+      <c r="B46" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="C46" s="6" t="s">
         <v>319</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>320</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E46" s="6"/>
       <c r="F46" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>65</v>
       </c>
       <c r="H46" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="I46" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="I46" s="6" t="s">
+      <c r="J46" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="J46" s="6" t="s">
+    </row>
+    <row r="47" spans="1:10" hidden="1">
+      <c r="A47" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="A47" t="s">
+      <c r="B47" t="s">
         <v>325</v>
-      </c>
-      <c r="B47" t="s">
-        <v>326</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" t="s">
@@ -4394,24 +4402,24 @@
         <v>32</v>
       </c>
       <c r="H47" t="s">
+        <v>326</v>
+      </c>
+      <c r="I47" s="18" t="s">
         <v>327</v>
       </c>
-      <c r="I47" s="18" t="s">
+      <c r="J47" s="18" t="s">
         <v>328</v>
       </c>
-      <c r="J47" s="18" t="s">
+    </row>
+    <row r="48" spans="1:10" hidden="1">
+      <c r="A48" s="8" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="8" t="s">
+      <c r="B48" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="C48" s="6" t="s">
         <v>331</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>332</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>170</v>
@@ -4426,60 +4434,60 @@
         <v>149</v>
       </c>
       <c r="H48" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="I48" s="8" t="s">
         <v>333</v>
       </c>
-      <c r="I48" s="8" t="s">
+      <c r="J48" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="J48" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
+    </row>
+    <row r="49" spans="1:10" hidden="1">
       <c r="A49" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="C49" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="C49" s="6" t="s">
-        <v>332</v>
-      </c>
       <c r="D49" s="8" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>148</v>
       </c>
       <c r="F49" s="8"/>
       <c r="G49" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H49" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="I49" s="8" t="s">
         <v>333</v>
       </c>
-      <c r="I49" s="8" t="s">
+      <c r="J49" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="J49" s="8" t="s">
+    </row>
+    <row r="50" spans="1:10" hidden="1">
+      <c r="A50" s="8" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="50" spans="1:10">
-      <c r="A50" s="8" t="s">
+      <c r="B50" s="8" t="s">
         <v>336</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="C50" s="8" t="s">
         <v>337</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>338</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>46</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>48</v>
@@ -4488,21 +4496,21 @@
         <v>32</v>
       </c>
       <c r="H50" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="I50" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="I50" s="8" t="s">
+      <c r="J50" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="J50" s="8" t="s">
+    </row>
+    <row r="51" spans="1:10" hidden="1">
+      <c r="A51" s="8" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="51" spans="1:10">
-      <c r="A51" s="8" t="s">
+      <c r="B51" s="8" t="s">
         <v>343</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>344</v>
       </c>
       <c r="C51" s="8"/>
       <c r="D51" s="8" t="s">
@@ -4510,113 +4518,113 @@
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="G51" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="G51" s="8" t="s">
+      <c r="H51" s="8" t="s">
         <v>346</v>
       </c>
-      <c r="H51" s="8" t="s">
+      <c r="I51" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="I51" s="8" t="s">
+      <c r="J51" s="8" t="s">
         <v>348</v>
       </c>
-      <c r="J51" s="8" t="s">
+    </row>
+    <row r="52" spans="1:10" hidden="1">
+      <c r="A52" s="8" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="52" spans="1:10">
-      <c r="A52" s="8" t="s">
+      <c r="B52" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="C52" s="8" t="s">
         <v>351</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>352</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E52" s="8"/>
       <c r="F52" s="11" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G52" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H52" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="I52" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="I52" s="8" t="s">
+      <c r="J52" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="J52" s="8" t="s">
+    </row>
+    <row r="53" spans="1:10" hidden="1">
+      <c r="A53" s="6" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="53" spans="1:10">
-      <c r="A53" s="6" t="s">
+      <c r="B53" s="6" t="s">
         <v>357</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>358</v>
       </c>
       <c r="C53" s="6"/>
       <c r="D53" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E53" s="6"/>
       <c r="F53" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H53" s="6"/>
       <c r="I53" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="J53" s="18" t="s">
         <v>361</v>
       </c>
-      <c r="J53" s="18" t="s">
+    </row>
+    <row r="54" spans="1:10" hidden="1">
+      <c r="A54" s="8" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="54" spans="1:10">
-      <c r="A54" s="8" t="s">
+      <c r="B54" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="C54" s="8" t="s">
         <v>364</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>365</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E54" s="8"/>
       <c r="F54" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="G54" s="8" t="s">
         <v>366</v>
       </c>
-      <c r="G54" s="8" t="s">
+      <c r="H54" s="8" t="s">
         <v>367</v>
       </c>
-      <c r="H54" s="8" t="s">
+      <c r="I54" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="I54" s="8" t="s">
+      <c r="J54" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="J54" s="8" t="s">
+    </row>
+    <row r="55" spans="1:10" hidden="1">
+      <c r="A55" s="6" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="55" spans="1:10">
-      <c r="A55" s="6" t="s">
-        <v>371</v>
-      </c>
       <c r="B55" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55" s="6" t="s">
@@ -4630,48 +4638,48 @@
         <v>150</v>
       </c>
       <c r="I55" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="J55" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="J55" s="6" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
+    </row>
+    <row r="56" spans="1:10" hidden="1">
       <c r="A56" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="C56" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="D56" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="D56" s="6" t="s">
-        <v>374</v>
-      </c>
       <c r="E56" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F56" s="6"/>
       <c r="H56" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I56" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="J56" s="16" t="s">
         <v>375</v>
       </c>
-      <c r="J56" s="16" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
+    </row>
+    <row r="57" spans="1:10" hidden="1">
       <c r="A57" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="C57" s="8" t="s">
         <v>381</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>382</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>30</v>
@@ -4680,24 +4688,24 @@
         <v>96</v>
       </c>
       <c r="F57" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="H57" s="8" t="s">
         <v>383</v>
       </c>
-      <c r="H57" s="8" t="s">
+      <c r="I57" s="8" t="s">
         <v>384</v>
       </c>
-      <c r="I57" s="8" t="s">
+      <c r="J57" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="J57" s="8" t="s">
+    </row>
+    <row r="58" spans="1:10" hidden="1">
+      <c r="A58" s="6" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="58" spans="1:10">
-      <c r="A58" s="6" t="s">
+      <c r="B58" s="6" t="s">
         <v>387</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>388</v>
       </c>
       <c r="C58" s="6"/>
       <c r="D58" s="6" t="s">
@@ -4705,27 +4713,27 @@
       </c>
       <c r="E58" s="6"/>
       <c r="F58" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G58" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H58" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="I58" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="I58" s="6" t="s">
+      <c r="J58" s="16" t="s">
         <v>391</v>
       </c>
-      <c r="J58" s="16" t="s">
+    </row>
+    <row r="59" spans="1:10" hidden="1">
+      <c r="A59" s="6" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="59" spans="1:10">
-      <c r="A59" s="6" t="s">
-        <v>393</v>
-      </c>
       <c r="B59" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C59" s="6"/>
       <c r="D59" s="6" t="s">
@@ -4733,27 +4741,27 @@
       </c>
       <c r="E59" s="6"/>
       <c r="F59" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="G59" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="G59" s="6" t="s">
+      <c r="H59" s="10" t="s">
+        <v>657</v>
+      </c>
+      <c r="I59" s="16" t="s">
         <v>395</v>
       </c>
-      <c r="H59" s="10" t="s">
-        <v>658</v>
-      </c>
-      <c r="I59" s="16" t="s">
+      <c r="J59" s="22" t="s">
         <v>396</v>
       </c>
-      <c r="J59" s="22" t="s">
+    </row>
+    <row r="60" spans="1:10" hidden="1">
+      <c r="A60" s="6" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="60" spans="1:10">
-      <c r="A60" s="6" t="s">
+      <c r="B60" s="6" t="s">
         <v>398</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>399</v>
       </c>
       <c r="C60" s="6"/>
       <c r="D60" s="6" t="s">
@@ -4763,115 +4771,115 @@
         <v>96</v>
       </c>
       <c r="F60" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="G60" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="G60" s="6" t="s">
+      <c r="H60" s="6" t="s">
         <v>401</v>
-      </c>
-      <c r="H60" s="6" t="s">
-        <v>402</v>
       </c>
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" hidden="1">
       <c r="A61" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="C61" s="6" t="s">
         <v>403</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>404</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E61" s="6"/>
       <c r="F61" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="H61" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="G61" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="H61" s="6" t="s">
+      <c r="I61" s="6" t="s">
         <v>406</v>
       </c>
-      <c r="I61" s="6" t="s">
+      <c r="J61" s="6" t="s">
         <v>407</v>
       </c>
-      <c r="J61" s="6" t="s">
+    </row>
+    <row r="62" spans="1:10" hidden="1">
+      <c r="A62" s="8" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="62" spans="1:10">
-      <c r="A62" s="8" t="s">
+      <c r="B62" s="8" t="s">
         <v>409</v>
       </c>
-      <c r="B62" s="8" t="s">
+      <c r="C62" s="8" t="s">
         <v>410</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>411</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>30</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G62" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H62" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="I62" s="8" t="s">
         <v>413</v>
       </c>
-      <c r="I62" s="8" t="s">
+      <c r="J62" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="J62" s="8" t="s">
+    </row>
+    <row r="63" spans="1:10" hidden="1">
+      <c r="A63" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="63" spans="1:10">
-      <c r="A63" t="s">
+      <c r="B63" t="s">
         <v>416</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" s="25" t="s">
         <v>417</v>
-      </c>
-      <c r="C63" s="25" t="s">
-        <v>418</v>
       </c>
       <c r="D63" t="s">
         <v>13</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G63" t="s">
         <v>15</v>
       </c>
       <c r="H63" t="s">
+        <v>419</v>
+      </c>
+      <c r="I63" t="s">
         <v>420</v>
       </c>
-      <c r="I63" t="s">
+      <c r="J63" t="s">
         <v>421</v>
       </c>
-      <c r="J63" t="s">
+    </row>
+    <row r="64" spans="1:10" s="4" customFormat="1" hidden="1">
+      <c r="A64" s="6" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" s="4" customFormat="1">
-      <c r="A64" s="6" t="s">
+      <c r="B64" s="6" t="s">
         <v>423</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="C64" s="6" t="s">
         <v>424</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>425</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>147</v>
@@ -4881,51 +4889,51 @@
       </c>
       <c r="F64" s="7"/>
       <c r="H64" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="I64" s="6" t="s">
         <v>426</v>
       </c>
-      <c r="I64" s="6" t="s">
+      <c r="J64" s="6" t="s">
         <v>427</v>
       </c>
-      <c r="J64" s="6" t="s">
+    </row>
+    <row r="65" spans="1:10" hidden="1">
+      <c r="A65" s="6" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="65" spans="1:10">
-      <c r="A65" s="6" t="s">
+      <c r="B65" s="6" t="s">
         <v>429</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="C65" s="6" t="s">
         <v>430</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>431</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E65" s="6"/>
       <c r="F65" s="6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G65" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H65" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="I65" s="6" t="s">
         <v>433</v>
       </c>
-      <c r="I65" s="6" t="s">
+      <c r="J65" s="6" t="s">
         <v>434</v>
       </c>
-      <c r="J65" s="6" t="s">
+    </row>
+    <row r="66" spans="1:10" s="5" customFormat="1" hidden="1">
+      <c r="A66" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" s="5" customFormat="1">
-      <c r="A66" t="s">
+      <c r="B66" t="s">
         <v>436</v>
-      </c>
-      <c r="B66" t="s">
-        <v>437</v>
       </c>
       <c r="C66"/>
       <c r="D66" t="s">
@@ -4934,24 +4942,24 @@
       <c r="E66"/>
       <c r="F66"/>
       <c r="G66" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H66" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="I66" s="18" t="s">
         <v>438</v>
       </c>
-      <c r="I66" s="18" t="s">
+      <c r="J66" s="17" t="s">
         <v>439</v>
       </c>
-      <c r="J66" s="17" t="s">
+    </row>
+    <row r="67" spans="1:10" hidden="1">
+      <c r="A67" s="8" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="67" spans="1:10">
-      <c r="A67" s="8" t="s">
-        <v>441</v>
-      </c>
       <c r="B67" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="8" t="s">
@@ -4959,24 +4967,24 @@
       </c>
       <c r="E67" s="8"/>
       <c r="F67" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="G67" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="G67" s="8" t="s">
-        <v>395</v>
-      </c>
       <c r="H67" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="I67" s="12" t="s">
+        <v>769</v>
+      </c>
+      <c r="J67" s="17" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" hidden="1">
+      <c r="A68" t="s">
         <v>442</v>
-      </c>
-      <c r="I67" s="12" t="s">
-        <v>770</v>
-      </c>
-      <c r="J67" s="17" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10">
-      <c r="A68" t="s">
-        <v>443</v>
       </c>
       <c r="B68" t="s">
         <v>120</v>
@@ -4988,24 +4996,24 @@
         <v>32</v>
       </c>
       <c r="H68" s="21" t="s">
+        <v>443</v>
+      </c>
+      <c r="I68" s="18" t="s">
         <v>444</v>
       </c>
-      <c r="I68" s="18" t="s">
+      <c r="J68" s="18" t="s">
         <v>445</v>
-      </c>
-      <c r="J68" s="18" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="8" t="s">
+        <v>446</v>
+      </c>
+      <c r="B69" s="8" t="s">
         <v>447</v>
       </c>
-      <c r="B69" s="8" t="s">
+      <c r="C69" s="8" t="s">
         <v>448</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>449</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>127</v>
@@ -5014,33 +5022,33 @@
         <v>87</v>
       </c>
       <c r="F69" s="8" t="s">
+        <v>449</v>
+      </c>
+      <c r="G69" s="8" t="s">
+        <v>787</v>
+      </c>
+      <c r="H69" s="8" t="s">
         <v>450</v>
       </c>
-      <c r="G69" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="H69" s="8" t="s">
+      <c r="I69" s="8" t="s">
         <v>451</v>
       </c>
-      <c r="I69" s="8" t="s">
+      <c r="J69" s="8" t="s">
         <v>452</v>
       </c>
-      <c r="J69" s="8" t="s">
+    </row>
+    <row r="70" spans="1:10" hidden="1">
+      <c r="A70" s="6" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="70" spans="1:10">
-      <c r="A70" s="6" t="s">
+      <c r="B70" s="6" t="s">
         <v>454</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="C70" s="6" t="s">
         <v>455</v>
       </c>
-      <c r="C70" s="6" t="s">
-        <v>456</v>
-      </c>
       <c r="D70" s="6" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>148</v>
@@ -5052,56 +5060,56 @@
         <v>149</v>
       </c>
       <c r="H70" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="I70" s="6" t="s">
         <v>457</v>
       </c>
-      <c r="I70" s="6" t="s">
+      <c r="J70" s="6" t="s">
         <v>458</v>
       </c>
-      <c r="J70" s="6" t="s">
+    </row>
+    <row r="71" spans="1:10" hidden="1">
+      <c r="A71" s="8" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="71" spans="1:10">
-      <c r="A71" s="8" t="s">
-        <v>460</v>
-      </c>
       <c r="B71" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>46</v>
       </c>
       <c r="E71" s="23" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G71" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H71" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="I71" s="8" t="s">
         <v>462</v>
       </c>
-      <c r="I71" s="8" t="s">
+      <c r="J71" s="17" t="s">
         <v>463</v>
       </c>
-      <c r="J71" s="17" t="s">
+    </row>
+    <row r="72" spans="1:10" hidden="1">
+      <c r="A72" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="72" spans="1:10">
-      <c r="A72" t="s">
+      <c r="B72" t="s">
         <v>465</v>
       </c>
-      <c r="B72" t="s">
-        <v>466</v>
-      </c>
       <c r="C72" s="6" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D72" t="s">
         <v>110</v>
@@ -5110,51 +5118,51 @@
         <v>32</v>
       </c>
       <c r="H72" s="21" t="s">
+        <v>466</v>
+      </c>
+      <c r="I72" s="18" t="s">
         <v>467</v>
       </c>
-      <c r="I72" s="18" t="s">
+      <c r="J72" s="18" t="s">
         <v>468</v>
       </c>
-      <c r="J72" s="18" t="s">
+    </row>
+    <row r="73" spans="1:10" hidden="1">
+      <c r="A73" s="8" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="73" spans="1:10">
-      <c r="A73" s="8" t="s">
+      <c r="B73" s="8" t="s">
         <v>470</v>
       </c>
-      <c r="B73" s="8" t="s">
+      <c r="C73" s="6" t="s">
         <v>471</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>472</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E73" s="8"/>
       <c r="F73" s="8" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G73" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H73" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="I73" s="8" t="s">
         <v>474</v>
       </c>
-      <c r="I73" s="8" t="s">
+      <c r="J73" s="8" t="s">
         <v>475</v>
       </c>
-      <c r="J73" s="8" t="s">
+    </row>
+    <row r="74" spans="1:10" hidden="1">
+      <c r="A74" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="74" spans="1:10">
-      <c r="A74" t="s">
+      <c r="B74" t="s">
         <v>477</v>
-      </c>
-      <c r="B74" t="s">
-        <v>478</v>
       </c>
       <c r="C74" s="6"/>
       <c r="D74" s="8" t="s">
@@ -5162,27 +5170,27 @@
       </c>
       <c r="E74" s="8"/>
       <c r="F74" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G74" s="8" t="s">
         <v>87</v>
       </c>
       <c r="H74" t="s">
+        <v>479</v>
+      </c>
+      <c r="I74" s="18" t="s">
         <v>480</v>
       </c>
-      <c r="I74" s="18" t="s">
+    </row>
+    <row r="75" spans="1:10" s="4" customFormat="1" hidden="1">
+      <c r="A75" s="8" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" s="4" customFormat="1">
-      <c r="A75" s="8" t="s">
+      <c r="B75" s="8" t="s">
         <v>482</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="C75" s="6" t="s">
         <v>483</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>484</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>170</v>
@@ -5191,27 +5199,27 @@
         <v>87</v>
       </c>
       <c r="G75" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H75" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="I75" s="8" t="s">
         <v>485</v>
       </c>
-      <c r="I75" s="8" t="s">
+      <c r="J75" s="8" t="s">
         <v>486</v>
       </c>
-      <c r="J75" s="8" t="s">
+    </row>
+    <row r="76" spans="1:10" s="4" customFormat="1" hidden="1">
+      <c r="A76" s="6" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" s="4" customFormat="1">
-      <c r="A76" s="6" t="s">
+      <c r="B76" s="6" t="s">
         <v>488</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="C76" s="6" t="s">
         <v>489</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>490</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>170</v>
@@ -5220,30 +5228,30 @@
         <v>148</v>
       </c>
       <c r="F76" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="G76" s="8" t="s">
+        <v>771</v>
+      </c>
+      <c r="H76" s="6" t="s">
         <v>491</v>
       </c>
-      <c r="G76" s="8" t="s">
-        <v>772</v>
-      </c>
-      <c r="H76" s="6" t="s">
+      <c r="I76" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="I76" s="6" t="s">
+      <c r="J76" s="6" t="s">
         <v>493</v>
       </c>
-      <c r="J76" s="6" t="s">
+    </row>
+    <row r="77" spans="1:10" hidden="1">
+      <c r="A77" s="8" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="77" spans="1:10">
-      <c r="A77" s="8" t="s">
+      <c r="B77" s="8" t="s">
         <v>495</v>
       </c>
-      <c r="B77" s="8" t="s">
+      <c r="C77" s="6" t="s">
         <v>496</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>497</v>
       </c>
       <c r="D77" s="8" t="s">
         <v>170</v>
@@ -5255,51 +5263,51 @@
         <v>117</v>
       </c>
       <c r="H77" s="8" t="s">
+        <v>497</v>
+      </c>
+      <c r="I77" s="8" t="s">
         <v>498</v>
       </c>
-      <c r="I77" s="8" t="s">
+      <c r="J77" s="8" t="s">
         <v>499</v>
       </c>
-      <c r="J77" s="8" t="s">
+    </row>
+    <row r="78" spans="1:10" hidden="1">
+      <c r="A78" s="6" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="78" spans="1:10">
-      <c r="A78" s="6" t="s">
+      <c r="B78" s="6" t="s">
         <v>501</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="C78" s="6" t="s">
         <v>502</v>
       </c>
-      <c r="C78" s="6" t="s">
-        <v>503</v>
-      </c>
       <c r="D78" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E78" s="23" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F78" s="6"/>
       <c r="G78" s="6" t="s">
         <v>157</v>
       </c>
       <c r="H78" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="I78" s="6" t="s">
         <v>504</v>
       </c>
-      <c r="I78" s="6" t="s">
+      <c r="J78" s="6" t="s">
         <v>505</v>
       </c>
-      <c r="J78" s="6" t="s">
+    </row>
+    <row r="79" spans="1:10" s="4" customFormat="1" hidden="1">
+      <c r="A79" s="6" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" s="4" customFormat="1">
-      <c r="A79" s="6" t="s">
-        <v>507</v>
-      </c>
       <c r="B79" s="6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C79" s="6"/>
       <c r="D79" s="6" t="s">
@@ -5312,18 +5320,18 @@
       <c r="G79"/>
       <c r="H79" s="6"/>
       <c r="I79" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="J79" s="6" t="s">
         <v>513</v>
       </c>
-      <c r="J79" s="6" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10">
+    </row>
+    <row r="80" spans="1:10" hidden="1">
       <c r="A80" s="10" t="s">
+        <v>506</v>
+      </c>
+      <c r="B80" s="10" t="s">
         <v>507</v>
-      </c>
-      <c r="B80" s="10" t="s">
-        <v>508</v>
       </c>
       <c r="C80" s="10"/>
       <c r="D80" s="10" t="s">
@@ -5333,31 +5341,31 @@
         <v>47</v>
       </c>
       <c r="F80" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="H80" s="10" t="s">
+        <v>508</v>
+      </c>
+      <c r="I80" s="10" t="s">
         <v>509</v>
       </c>
-      <c r="I80" s="10" t="s">
+      <c r="J80" s="10" t="s">
         <v>510</v>
       </c>
-      <c r="J80" s="10" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10">
+    </row>
+    <row r="81" spans="1:10" hidden="1">
       <c r="A81" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="B81" s="6" t="s">
         <v>515</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>516</v>
       </c>
       <c r="C81" s="6"/>
       <c r="D81" s="6" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E81" s="6"/>
       <c r="F81" s="6"/>
@@ -5365,134 +5373,134 @@
         <v>65</v>
       </c>
       <c r="H81" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="I81" s="16" t="s">
         <v>518</v>
       </c>
-      <c r="I81" s="16" t="s">
+      <c r="J81" s="6"/>
+    </row>
+    <row r="82" spans="1:10" hidden="1">
+      <c r="A82" s="6" t="s">
         <v>519</v>
       </c>
-      <c r="J81" s="6"/>
-    </row>
-    <row r="82" spans="1:10">
-      <c r="A82" s="6" t="s">
+      <c r="B82" s="6" t="s">
         <v>520</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>521</v>
       </c>
       <c r="C82" s="6"/>
       <c r="D82" s="6" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E82" s="6"/>
       <c r="F82" s="6"/>
       <c r="G82" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="H82" s="6" t="s">
         <v>522</v>
       </c>
-      <c r="H82" s="6" t="s">
+      <c r="I82" s="16" t="s">
         <v>523</v>
       </c>
-      <c r="I82" s="16" t="s">
+      <c r="J82" s="6"/>
+    </row>
+    <row r="83" spans="1:10" hidden="1">
+      <c r="A83" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="J82" s="6"/>
-    </row>
-    <row r="83" spans="1:10">
-      <c r="A83" s="6" t="s">
+      <c r="B83" s="6" t="s">
         <v>525</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>526</v>
       </c>
       <c r="C83" s="6"/>
       <c r="D83" s="6" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E83" s="6"/>
       <c r="F83" s="28" t="s">
+        <v>527</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="H83" s="14" t="s">
         <v>528</v>
       </c>
-      <c r="G83" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="H83" s="14" t="s">
+      <c r="I83" s="16" t="s">
         <v>529</v>
       </c>
-      <c r="I83" s="16" t="s">
+      <c r="J83" s="16" t="s">
         <v>530</v>
       </c>
-      <c r="J83" s="16" t="s">
+    </row>
+    <row r="84" spans="1:10" hidden="1">
+      <c r="A84" s="6" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="84" spans="1:10">
-      <c r="A84" s="6" t="s">
+      <c r="B84" s="6" t="s">
         <v>532</v>
       </c>
-      <c r="B84" s="6" t="s">
+      <c r="C84" s="6" t="s">
         <v>533</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>534</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E84" s="6"/>
       <c r="F84" s="6" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G84" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H84" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="I84" s="6" t="s">
         <v>536</v>
       </c>
-      <c r="I84" s="6" t="s">
+      <c r="J84" s="6" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" hidden="1">
+      <c r="A85" s="6" t="s">
         <v>537</v>
       </c>
-      <c r="J84" s="6" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10">
-      <c r="A85" s="6" t="s">
+      <c r="B85" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="C85" s="6" t="s">
         <v>538</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>437</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>539</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E85" s="6"/>
       <c r="F85" s="6" t="s">
+        <v>539</v>
+      </c>
+      <c r="G85" s="6" t="s">
         <v>540</v>
       </c>
-      <c r="G85" s="6" t="s">
+      <c r="H85" s="6" t="s">
         <v>541</v>
       </c>
-      <c r="H85" s="6" t="s">
+      <c r="I85" s="6" t="s">
         <v>542</v>
       </c>
-      <c r="I85" s="6" t="s">
+      <c r="J85" s="6" t="s">
         <v>543</v>
       </c>
-      <c r="J85" s="6" t="s">
+    </row>
+    <row r="86" spans="1:10" hidden="1">
+      <c r="A86" s="6" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="86" spans="1:10">
-      <c r="A86" s="6" t="s">
+      <c r="B86" s="6" t="s">
         <v>545</v>
       </c>
-      <c r="B86" s="6" t="s">
+      <c r="C86" s="6" t="s">
         <v>546</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>547</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>46</v>
@@ -5501,28 +5509,28 @@
         <v>87</v>
       </c>
       <c r="G86" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="H86" s="6" t="s">
         <v>548</v>
       </c>
-      <c r="H86" s="6" t="s">
+      <c r="I86" s="6" t="s">
         <v>549</v>
       </c>
-      <c r="I86" s="6" t="s">
+      <c r="J86" s="6" t="s">
         <v>550</v>
       </c>
-      <c r="J86" s="6" t="s">
+    </row>
+    <row r="87" spans="1:10" hidden="1">
+      <c r="A87" s="6" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="87" spans="1:10">
-      <c r="A87" s="6" t="s">
+      <c r="B87" s="6" t="s">
         <v>552</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>553</v>
       </c>
       <c r="C87" s="6"/>
       <c r="D87" s="6" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E87" s="6"/>
       <c r="F87" s="6"/>
@@ -5530,82 +5538,82 @@
         <v>111</v>
       </c>
       <c r="H87" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="I87" s="16" t="s">
         <v>554</v>
       </c>
-      <c r="I87" s="16" t="s">
+      <c r="J87" s="6"/>
+    </row>
+    <row r="88" spans="1:10" hidden="1">
+      <c r="A88" s="6" t="s">
         <v>555</v>
       </c>
-      <c r="J87" s="6"/>
-    </row>
-    <row r="88" spans="1:10">
-      <c r="A88" s="6" t="s">
+      <c r="B88" s="6" t="s">
         <v>556</v>
       </c>
-      <c r="B88" s="6" t="s">
+      <c r="C88" s="6" t="s">
         <v>557</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>558</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E88" s="6"/>
       <c r="F88" s="6" t="s">
+        <v>558</v>
+      </c>
+      <c r="G88" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="H88" s="6" t="s">
         <v>559</v>
       </c>
-      <c r="G88" s="6" t="s">
-        <v>522</v>
-      </c>
-      <c r="H88" s="6" t="s">
+      <c r="I88" s="6" t="s">
         <v>560</v>
       </c>
-      <c r="I88" s="6" t="s">
+      <c r="J88" s="6" t="s">
         <v>561</v>
       </c>
-      <c r="J88" s="6" t="s">
+    </row>
+    <row r="89" spans="1:10" hidden="1">
+      <c r="A89" s="14" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="89" spans="1:10">
-      <c r="A89" s="14" t="s">
+      <c r="B89" s="14" t="s">
         <v>563</v>
       </c>
-      <c r="B89" s="14" t="s">
+      <c r="C89" s="6" t="s">
         <v>564</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>565</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E89" s="6"/>
       <c r="F89" s="14" t="s">
+        <v>539</v>
+      </c>
+      <c r="G89" s="14" t="s">
         <v>540</v>
       </c>
-      <c r="G89" s="14" t="s">
-        <v>541</v>
-      </c>
       <c r="H89" s="14" t="s">
+        <v>565</v>
+      </c>
+      <c r="I89" s="14" t="s">
         <v>566</v>
       </c>
-      <c r="I89" s="14" t="s">
+      <c r="J89" s="14" t="s">
         <v>567</v>
       </c>
-      <c r="J89" s="14" t="s">
+    </row>
+    <row r="90" spans="1:10" hidden="1">
+      <c r="A90" s="8" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="90" spans="1:10">
-      <c r="A90" s="8" t="s">
+      <c r="B90" s="8" t="s">
         <v>569</v>
       </c>
-      <c r="B90" s="8" t="s">
+      <c r="C90" s="6" t="s">
         <v>570</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>571</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>127</v>
@@ -5618,51 +5626,51 @@
         <v>87</v>
       </c>
       <c r="H90" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="I90" s="8" t="s">
         <v>572</v>
       </c>
-      <c r="I90" s="8" t="s">
+      <c r="J90" s="8" t="s">
         <v>573</v>
       </c>
-      <c r="J90" s="8" t="s">
+    </row>
+    <row r="91" spans="1:10" hidden="1">
+      <c r="A91" s="8" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="91" spans="1:10">
-      <c r="A91" s="8" t="s">
+      <c r="B91" s="8" t="s">
         <v>575</v>
       </c>
-      <c r="B91" s="8" t="s">
+      <c r="C91" s="6" t="s">
         <v>576</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>577</v>
       </c>
       <c r="D91" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E91" s="8"/>
       <c r="F91" s="11" t="s">
+        <v>577</v>
+      </c>
+      <c r="G91" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="H91" s="8" t="s">
         <v>578</v>
       </c>
-      <c r="G91" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="H91" s="8" t="s">
+      <c r="I91" s="8" t="s">
         <v>579</v>
       </c>
-      <c r="I91" s="8" t="s">
+      <c r="J91" s="8" t="s">
         <v>580</v>
       </c>
-      <c r="J91" s="8" t="s">
+    </row>
+    <row r="92" spans="1:10" hidden="1">
+      <c r="A92" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="92" spans="1:10">
-      <c r="A92" t="s">
+      <c r="B92" t="s">
         <v>582</v>
-      </c>
-      <c r="B92" t="s">
-        <v>583</v>
       </c>
       <c r="C92" s="6"/>
       <c r="D92" s="8" t="s">
@@ -5670,168 +5678,168 @@
       </c>
       <c r="E92" s="8"/>
       <c r="F92" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G92" s="8" t="s">
         <v>87</v>
       </c>
       <c r="H92" t="s">
+        <v>584</v>
+      </c>
+      <c r="I92" s="18" t="s">
         <v>585</v>
       </c>
-      <c r="I92" s="18" t="s">
+    </row>
+    <row r="93" spans="1:10" hidden="1">
+      <c r="A93" s="14" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="93" spans="1:10">
-      <c r="A93" s="14" t="s">
+      <c r="B93" s="14" t="s">
         <v>587</v>
       </c>
-      <c r="B93" s="14" t="s">
+      <c r="C93" s="14" t="s">
         <v>588</v>
       </c>
-      <c r="C93" s="14" t="s">
-        <v>589</v>
-      </c>
       <c r="D93" s="14" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E93" s="14" t="s">
         <v>47</v>
       </c>
       <c r="F93" s="7"/>
       <c r="G93" s="14" t="s">
+        <v>589</v>
+      </c>
+      <c r="H93" s="14" t="s">
         <v>590</v>
       </c>
-      <c r="H93" s="14" t="s">
+      <c r="I93" s="14" t="s">
         <v>591</v>
       </c>
-      <c r="I93" s="14" t="s">
+      <c r="J93" s="14" t="s">
         <v>592</v>
       </c>
-      <c r="J93" s="14" t="s">
+    </row>
+    <row r="94" spans="1:10" hidden="1">
+      <c r="A94" s="8" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="94" spans="1:10">
-      <c r="A94" s="8" t="s">
+      <c r="B94" s="8" t="s">
         <v>594</v>
-      </c>
-      <c r="B94" s="8" t="s">
-        <v>595</v>
       </c>
       <c r="C94" s="8"/>
       <c r="D94" s="8" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E94" s="8"/>
       <c r="F94" s="8" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G94" s="8" t="s">
         <v>72</v>
       </c>
       <c r="H94" s="8" t="s">
+        <v>597</v>
+      </c>
+      <c r="I94" s="8" t="s">
         <v>598</v>
       </c>
-      <c r="I94" s="8" t="s">
+      <c r="J94" s="8" t="s">
         <v>599</v>
       </c>
-      <c r="J94" s="8" t="s">
+    </row>
+    <row r="95" spans="1:10" hidden="1">
+      <c r="A95" s="8" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="95" spans="1:10">
-      <c r="A95" s="8" t="s">
+      <c r="B95" s="8" t="s">
         <v>601</v>
-      </c>
-      <c r="B95" s="8" t="s">
-        <v>602</v>
       </c>
       <c r="C95" s="8"/>
       <c r="D95" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F95" s="8"/>
       <c r="H95" s="8" t="s">
+        <v>602</v>
+      </c>
+      <c r="I95" s="8" t="s">
         <v>603</v>
       </c>
-      <c r="I95" s="8" t="s">
+      <c r="J95" s="8" t="s">
         <v>604</v>
       </c>
-      <c r="J95" s="8" t="s">
+    </row>
+    <row r="96" spans="1:10" s="4" customFormat="1" hidden="1">
+      <c r="A96" s="8" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" s="4" customFormat="1">
-      <c r="A96" s="8" t="s">
+      <c r="B96" s="8" t="s">
         <v>606</v>
       </c>
-      <c r="B96" s="8" t="s">
-        <v>607</v>
-      </c>
       <c r="C96" s="8" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>46</v>
       </c>
       <c r="E96" s="23" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G96" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H96" s="8" t="s">
+        <v>608</v>
+      </c>
+      <c r="I96" s="8" t="s">
         <v>609</v>
       </c>
-      <c r="I96" s="8" t="s">
+      <c r="J96" s="17" t="s">
         <v>610</v>
       </c>
-      <c r="J96" s="17" t="s">
+    </row>
+    <row r="97" spans="1:10" s="4" customFormat="1" hidden="1">
+      <c r="A97" s="8" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" s="4" customFormat="1">
-      <c r="A97" s="8" t="s">
+      <c r="B97" s="8" t="s">
         <v>612</v>
-      </c>
-      <c r="B97" s="8" t="s">
-        <v>613</v>
       </c>
       <c r="C97" s="8"/>
       <c r="D97" s="8" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E97" s="6"/>
       <c r="F97" s="28" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H97" s="8"/>
       <c r="I97" s="17" t="s">
+        <v>615</v>
+      </c>
+      <c r="J97" s="18" t="s">
         <v>616</v>
       </c>
-      <c r="J97" s="18" t="s">
+    </row>
+    <row r="98" spans="1:10" hidden="1">
+      <c r="A98" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="98" spans="1:10">
-      <c r="A98" t="s">
+      <c r="B98" t="s">
         <v>618</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" s="25" t="s">
         <v>619</v>
-      </c>
-      <c r="C98" s="25" t="s">
-        <v>620</v>
       </c>
       <c r="D98" t="s">
         <v>30</v>
@@ -5840,27 +5848,27 @@
         <v>96</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G98" t="s">
         <v>117</v>
       </c>
       <c r="I98" t="s">
+        <v>621</v>
+      </c>
+      <c r="J98" t="s">
         <v>622</v>
       </c>
-      <c r="J98" t="s">
+    </row>
+    <row r="99" spans="1:10" hidden="1">
+      <c r="A99" s="6" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="99" spans="1:10">
-      <c r="A99" s="6" t="s">
+      <c r="B99" s="6" t="s">
         <v>624</v>
       </c>
-      <c r="B99" s="6" t="s">
+      <c r="C99" s="6" t="s">
         <v>625</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>626</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>127</v>
@@ -5869,90 +5877,90 @@
         <v>96</v>
       </c>
       <c r="F99" s="15" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G99" t="s">
         <v>117</v>
       </c>
       <c r="H99" s="14" t="s">
+        <v>627</v>
+      </c>
+      <c r="I99" s="14" t="s">
         <v>628</v>
       </c>
-      <c r="I99" s="14" t="s">
+      <c r="J99" s="14" t="s">
         <v>629</v>
       </c>
-      <c r="J99" s="14" t="s">
+    </row>
+    <row r="100" spans="1:10" hidden="1">
+      <c r="A100" s="6" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="100" spans="1:10">
-      <c r="A100" s="6" t="s">
+      <c r="B100" s="6" t="s">
         <v>631</v>
       </c>
-      <c r="B100" s="6" t="s">
+      <c r="C100" s="6" t="s">
         <v>632</v>
-      </c>
-      <c r="C100" s="6" t="s">
-        <v>633</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E100" s="6"/>
       <c r="F100" s="6" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G100" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H100" s="14" t="s">
+        <v>634</v>
+      </c>
+      <c r="I100" s="14" t="s">
         <v>635</v>
       </c>
-      <c r="I100" s="14" t="s">
+      <c r="J100" s="14" t="s">
         <v>636</v>
       </c>
-      <c r="J100" s="14" t="s">
+    </row>
+    <row r="101" spans="1:10" hidden="1">
+      <c r="A101" s="8" t="s">
+        <v>630</v>
+      </c>
+      <c r="B101" s="8" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="101" spans="1:10">
-      <c r="A101" s="8" t="s">
-        <v>631</v>
-      </c>
-      <c r="B101" s="8" t="s">
+      <c r="C101" s="8" t="s">
         <v>638</v>
-      </c>
-      <c r="C101" s="8" t="s">
-        <v>639</v>
       </c>
       <c r="D101" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E101" s="8"/>
       <c r="F101" s="8" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="G101" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H101" s="10" t="s">
+        <v>640</v>
+      </c>
+      <c r="I101" s="10" t="s">
         <v>641</v>
       </c>
-      <c r="I101" s="10" t="s">
+      <c r="J101" s="10" t="s">
         <v>642</v>
       </c>
-      <c r="J101" s="10" t="s">
+    </row>
+    <row r="102" spans="1:10" hidden="1">
+      <c r="A102" s="6" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="102" spans="1:10">
-      <c r="A102" s="6" t="s">
+      <c r="B102" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="C102" s="6" t="s">
         <v>644</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>372</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>645</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>13</v>
@@ -5965,24 +5973,24 @@
         <v>111</v>
       </c>
       <c r="H102" s="14" t="s">
+        <v>645</v>
+      </c>
+      <c r="I102" s="14" t="s">
         <v>646</v>
       </c>
-      <c r="I102" s="14" t="s">
+      <c r="J102" s="14" t="s">
         <v>647</v>
       </c>
-      <c r="J102" s="14" t="s">
+    </row>
+    <row r="103" spans="1:10" s="5" customFormat="1" hidden="1">
+      <c r="A103" s="6" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" s="5" customFormat="1">
-      <c r="A103" s="6" t="s">
+      <c r="B103" s="6" t="s">
+        <v>582</v>
+      </c>
+      <c r="C103" s="6" t="s">
         <v>649</v>
-      </c>
-      <c r="B103" s="6" t="s">
-        <v>583</v>
-      </c>
-      <c r="C103" s="6" t="s">
-        <v>650</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>30</v>
@@ -5991,52 +5999,52 @@
         <v>96</v>
       </c>
       <c r="F103" s="15" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="H103" s="14"/>
       <c r="I103" s="13" t="s">
+        <v>651</v>
+      </c>
+      <c r="J103" s="14" t="s">
         <v>652</v>
       </c>
-      <c r="J103" s="14" t="s">
+    </row>
+    <row r="104" spans="1:10" s="5" customFormat="1" hidden="1">
+      <c r="A104" s="8" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" s="5" customFormat="1">
-      <c r="A104" s="8" t="s">
+      <c r="B104" s="8" t="s">
         <v>654</v>
       </c>
-      <c r="B104" s="8" t="s">
+      <c r="C104" s="8" t="s">
         <v>655</v>
-      </c>
-      <c r="C104" s="8" t="s">
-        <v>656</v>
       </c>
       <c r="D104" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E104" s="8"/>
       <c r="F104" s="11" t="s">
+        <v>656</v>
+      </c>
+      <c r="G104" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="H104" s="10" t="s">
         <v>657</v>
       </c>
-      <c r="G104" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="H104" s="10" t="s">
+      <c r="I104" s="10" t="s">
         <v>658</v>
       </c>
-      <c r="I104" s="10" t="s">
+      <c r="J104" s="10" t="s">
         <v>659</v>
       </c>
-      <c r="J104" s="10" t="s">
+    </row>
+    <row r="105" spans="1:10" hidden="1">
+      <c r="A105" s="8" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="105" spans="1:10">
-      <c r="A105" s="8" t="s">
+      <c r="B105" s="8" t="s">
         <v>661</v>
-      </c>
-      <c r="B105" s="8" t="s">
-        <v>662</v>
       </c>
       <c r="C105" s="6"/>
       <c r="D105" s="8" t="s">
@@ -6048,42 +6056,42 @@
         <v>23</v>
       </c>
       <c r="H105" s="10" t="s">
+        <v>662</v>
+      </c>
+      <c r="I105" s="17" t="s">
         <v>663</v>
       </c>
-      <c r="I105" s="17" t="s">
+      <c r="J105" s="10"/>
+    </row>
+    <row r="106" spans="1:10" hidden="1">
+      <c r="A106" t="s">
         <v>664</v>
       </c>
-      <c r="J105" s="10"/>
-    </row>
-    <row r="106" spans="1:10">
-      <c r="A106" t="s">
+      <c r="B106" t="s">
         <v>665</v>
       </c>
-      <c r="B106" t="s">
+      <c r="D106" t="s">
+        <v>516</v>
+      </c>
+      <c r="G106" t="s">
+        <v>773</v>
+      </c>
+      <c r="H106" s="8" t="s">
         <v>666</v>
       </c>
-      <c r="D106" t="s">
-        <v>517</v>
-      </c>
-      <c r="G106" t="s">
-        <v>774</v>
-      </c>
-      <c r="H106" s="8" t="s">
+      <c r="I106" s="18" t="s">
         <v>667</v>
       </c>
-      <c r="I106" s="18" t="s">
+      <c r="J106" s="17" t="s">
         <v>668</v>
       </c>
-      <c r="J106" s="17" t="s">
+    </row>
+    <row r="107" spans="1:10" hidden="1">
+      <c r="A107" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="107" spans="1:10">
-      <c r="A107" t="s">
+      <c r="B107" t="s">
         <v>670</v>
-      </c>
-      <c r="B107" t="s">
-        <v>671</v>
       </c>
       <c r="D107" t="s">
         <v>110</v>
@@ -6092,53 +6100,53 @@
         <v>32</v>
       </c>
       <c r="H107" t="s">
+        <v>671</v>
+      </c>
+      <c r="I107" s="18" t="s">
         <v>672</v>
       </c>
-      <c r="I107" s="18" t="s">
+      <c r="J107" s="19" t="s">
         <v>673</v>
       </c>
-      <c r="J107" s="19" t="s">
+    </row>
+    <row r="108" spans="1:10" hidden="1">
+      <c r="A108" t="s">
         <v>674</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10">
-      <c r="A108" t="s">
-        <v>675</v>
       </c>
       <c r="B108" t="s">
         <v>62</v>
       </c>
       <c r="C108" s="25" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D108" t="s">
         <v>13</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="G108" t="s">
         <v>32</v>
       </c>
       <c r="H108" s="4" t="s">
+        <v>677</v>
+      </c>
+      <c r="I108" s="4" t="s">
         <v>678</v>
       </c>
-      <c r="I108" s="4" t="s">
+      <c r="J108" s="4" t="s">
         <v>679</v>
       </c>
-      <c r="J108" s="4" t="s">
+    </row>
+    <row r="109" spans="1:10" hidden="1">
+      <c r="A109" s="6" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="109" spans="1:10">
-      <c r="A109" s="6" t="s">
+      <c r="B109" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="C109" s="6" t="s">
         <v>681</v>
-      </c>
-      <c r="B109" s="6" t="s">
-        <v>525</v>
-      </c>
-      <c r="C109" s="6" t="s">
-        <v>682</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>147</v>
@@ -6151,18 +6159,18 @@
         <v>141</v>
       </c>
       <c r="I109" s="14" t="s">
+        <v>682</v>
+      </c>
+      <c r="J109" s="14" t="s">
         <v>683</v>
       </c>
-      <c r="J109" s="14" t="s">
+    </row>
+    <row r="110" spans="1:10" hidden="1">
+      <c r="A110" s="6" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="110" spans="1:10">
-      <c r="A110" s="6" t="s">
+      <c r="B110" s="6" t="s">
         <v>685</v>
-      </c>
-      <c r="B110" s="6" t="s">
-        <v>686</v>
       </c>
       <c r="C110" s="6"/>
       <c r="D110" s="6" t="s">
@@ -6170,28 +6178,28 @@
       </c>
       <c r="E110" s="6"/>
       <c r="F110" s="15" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H110" s="14"/>
       <c r="I110" s="14" t="s">
+        <v>687</v>
+      </c>
+      <c r="J110" s="14" t="s">
         <v>688</v>
       </c>
-      <c r="J110" s="14" t="s">
+    </row>
+    <row r="111" spans="1:10" hidden="1">
+      <c r="A111" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="111" spans="1:10">
-      <c r="A111" t="s">
+      <c r="B111" t="s">
         <v>690</v>
       </c>
-      <c r="B111" t="s">
-        <v>691</v>
-      </c>
       <c r="D111" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E111" s="6"/>
       <c r="F111" s="6"/>
@@ -6199,42 +6207,42 @@
         <v>32</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" hidden="1">
       <c r="A112" s="10" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B112" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D112" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E112" s="10"/>
       <c r="F112" s="10" t="s">
+        <v>693</v>
+      </c>
+      <c r="G112" s="10" t="s">
         <v>694</v>
       </c>
-      <c r="G112" s="10" t="s">
+      <c r="H112" s="10" t="s">
         <v>695</v>
       </c>
-      <c r="H112" s="10" t="s">
+      <c r="I112" s="10" t="s">
         <v>696</v>
       </c>
-      <c r="I112" s="10" t="s">
+      <c r="J112" s="10" t="s">
         <v>697</v>
       </c>
-      <c r="J112" s="10" t="s">
+    </row>
+    <row r="113" spans="1:10" hidden="1">
+      <c r="A113" s="10" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="113" spans="1:10">
-      <c r="A113" s="10" t="s">
-        <v>699</v>
-      </c>
       <c r="B113" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C113" s="10"/>
       <c r="D113" s="10" t="s">
@@ -6246,24 +6254,24 @@
       <c r="F113" s="10"/>
       <c r="G113" s="10"/>
       <c r="H113" s="10" t="s">
+        <v>699</v>
+      </c>
+      <c r="I113" s="10" t="s">
         <v>700</v>
       </c>
-      <c r="I113" s="10" t="s">
+      <c r="J113" s="10" t="s">
         <v>701</v>
       </c>
-      <c r="J113" s="10" t="s">
+    </row>
+    <row r="114" spans="1:10" hidden="1">
+      <c r="A114" s="6" t="s">
         <v>702</v>
       </c>
-    </row>
-    <row r="114" spans="1:10">
-      <c r="A114" s="6" t="s">
+      <c r="B114" s="6" t="s">
         <v>703</v>
       </c>
-      <c r="B114" s="6" t="s">
+      <c r="C114" s="6" t="s">
         <v>704</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>705</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>95</v>
@@ -6272,24 +6280,24 @@
         <v>96</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H114" s="6" t="s">
+        <v>705</v>
+      </c>
+      <c r="I114" s="6" t="s">
         <v>706</v>
       </c>
-      <c r="I114" s="6" t="s">
+      <c r="J114" s="6" t="s">
         <v>707</v>
       </c>
-      <c r="J114" s="6" t="s">
+    </row>
+    <row r="115" spans="1:10" hidden="1">
+      <c r="A115" s="6" t="s">
         <v>708</v>
       </c>
-    </row>
-    <row r="115" spans="1:10">
-      <c r="A115" s="6" t="s">
+      <c r="B115" s="6" t="s">
         <v>709</v>
-      </c>
-      <c r="B115" s="6" t="s">
-        <v>710</v>
       </c>
       <c r="C115" s="6"/>
       <c r="D115" s="6" t="s">
@@ -6298,55 +6306,55 @@
       <c r="E115" s="6"/>
       <c r="F115" s="6"/>
       <c r="G115" s="6" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H115" s="6"/>
       <c r="I115" s="16" t="s">
+        <v>710</v>
+      </c>
+      <c r="J115" s="6"/>
+    </row>
+    <row r="116" spans="1:10" hidden="1">
+      <c r="A116" s="14" t="s">
         <v>711</v>
       </c>
-      <c r="J115" s="6"/>
-    </row>
-    <row r="116" spans="1:10">
-      <c r="A116" s="14" t="s">
+      <c r="B116" s="14" t="s">
         <v>712</v>
       </c>
-      <c r="B116" s="14" t="s">
+      <c r="C116" s="26" t="s">
         <v>713</v>
       </c>
-      <c r="C116" s="26" t="s">
+      <c r="D116" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="E116" t="s">
         <v>714</v>
       </c>
-      <c r="D116" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="E116" t="s">
+      <c r="F116" s="14" t="s">
         <v>715</v>
-      </c>
-      <c r="F116" s="14" t="s">
-        <v>716</v>
       </c>
       <c r="G116" s="14" t="s">
         <v>49</v>
       </c>
       <c r="H116" s="14" t="s">
+        <v>716</v>
+      </c>
+      <c r="I116" s="14" t="s">
         <v>717</v>
       </c>
-      <c r="I116" s="14" t="s">
+      <c r="J116" s="14" t="s">
         <v>718</v>
       </c>
-      <c r="J116" s="14" t="s">
+    </row>
+    <row r="117" spans="1:10" hidden="1">
+      <c r="A117" s="8" t="s">
         <v>719</v>
       </c>
-    </row>
-    <row r="117" spans="1:10">
-      <c r="A117" s="8" t="s">
+      <c r="B117" s="8" t="s">
+        <v>582</v>
+      </c>
+      <c r="C117" s="27" t="s">
         <v>720</v>
-      </c>
-      <c r="B117" s="8" t="s">
-        <v>583</v>
-      </c>
-      <c r="C117" s="27" t="s">
-        <v>721</v>
       </c>
       <c r="D117" s="8" t="s">
         <v>30</v>
@@ -6359,21 +6367,21 @@
         <v>157</v>
       </c>
       <c r="H117" s="8" t="s">
+        <v>721</v>
+      </c>
+      <c r="I117" s="8" t="s">
         <v>722</v>
       </c>
-      <c r="I117" s="8" t="s">
+      <c r="J117" s="8" t="s">
         <v>723</v>
       </c>
-      <c r="J117" s="8" t="s">
+    </row>
+    <row r="118" spans="1:10" hidden="1">
+      <c r="A118" s="8" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="118" spans="1:10">
-      <c r="A118" s="8" t="s">
+      <c r="B118" s="8" t="s">
         <v>725</v>
-      </c>
-      <c r="B118" s="8" t="s">
-        <v>726</v>
       </c>
       <c r="C118" s="8"/>
       <c r="D118" s="8" t="s">
@@ -6382,22 +6390,22 @@
       <c r="E118" s="8"/>
       <c r="F118" s="8"/>
       <c r="G118" s="8" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H118" t="s">
+        <v>726</v>
+      </c>
+      <c r="I118" s="17" t="s">
         <v>727</v>
       </c>
-      <c r="I118" s="17" t="s">
+      <c r="J118" s="8"/>
+    </row>
+    <row r="119" spans="1:10" hidden="1">
+      <c r="A119" s="6" t="s">
         <v>728</v>
       </c>
-      <c r="J118" s="8"/>
-    </row>
-    <row r="119" spans="1:10">
-      <c r="A119" s="6" t="s">
+      <c r="B119" s="6" t="s">
         <v>729</v>
-      </c>
-      <c r="B119" s="6" t="s">
-        <v>730</v>
       </c>
       <c r="C119" s="6"/>
       <c r="D119" s="6" t="s">
@@ -6405,77 +6413,77 @@
       </c>
       <c r="E119" s="6"/>
       <c r="F119" s="15" t="s">
+        <v>730</v>
+      </c>
+      <c r="G119" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="H119" s="6" t="s">
         <v>731</v>
       </c>
-      <c r="G119" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="H119" s="6" t="s">
+      <c r="I119" s="6" t="s">
         <v>732</v>
       </c>
-      <c r="I119" s="6" t="s">
+      <c r="J119" s="6" t="s">
         <v>733</v>
       </c>
-      <c r="J119" s="6" t="s">
+    </row>
+    <row r="120" spans="1:10" hidden="1">
+      <c r="A120" s="6" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="120" spans="1:10">
-      <c r="A120" s="6" t="s">
+      <c r="B120" s="6" t="s">
         <v>735</v>
-      </c>
-      <c r="B120" s="6" t="s">
-        <v>736</v>
       </c>
       <c r="C120" s="6"/>
       <c r="D120" s="6" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E120" s="6"/>
       <c r="F120" s="6"/>
       <c r="G120" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="H120" s="8" t="s">
         <v>522</v>
       </c>
-      <c r="H120" s="8" t="s">
-        <v>523</v>
-      </c>
       <c r="I120" s="16" t="s">
+        <v>736</v>
+      </c>
+      <c r="J120" s="6"/>
+    </row>
+    <row r="121" spans="1:10" hidden="1">
+      <c r="A121" t="s">
+        <v>734</v>
+      </c>
+      <c r="B121" t="s">
         <v>737</v>
-      </c>
-      <c r="J120" s="6"/>
-    </row>
-    <row r="121" spans="1:10">
-      <c r="A121" t="s">
-        <v>735</v>
-      </c>
-      <c r="B121" t="s">
-        <v>738</v>
       </c>
       <c r="D121" t="s">
         <v>56</v>
       </c>
       <c r="F121" t="s">
+        <v>738</v>
+      </c>
+      <c r="G121" t="s">
+        <v>366</v>
+      </c>
+      <c r="H121" s="8" t="s">
         <v>739</v>
       </c>
-      <c r="G121" t="s">
-        <v>367</v>
-      </c>
-      <c r="H121" s="8" t="s">
+      <c r="I121" s="18" t="s">
         <v>740</v>
       </c>
-      <c r="I121" s="18" t="s">
+      <c r="J121" s="17" t="s">
         <v>741</v>
       </c>
-      <c r="J121" s="17" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10">
+    </row>
+    <row r="122" spans="1:10" hidden="1">
       <c r="A122" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B122" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C122" s="6"/>
       <c r="D122" t="s">
@@ -6485,24 +6493,24 @@
         <v>47</v>
       </c>
       <c r="F122" t="s">
+        <v>777</v>
+      </c>
+      <c r="G122" t="s">
+        <v>775</v>
+      </c>
+      <c r="H122" t="s">
         <v>778</v>
       </c>
-      <c r="G122" t="s">
-        <v>776</v>
-      </c>
-      <c r="H122" t="s">
+      <c r="I122" s="29" t="s">
         <v>779</v>
       </c>
-      <c r="I122" s="29" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10">
+    </row>
+    <row r="123" spans="1:10" hidden="1">
       <c r="A123" s="6" t="s">
+        <v>742</v>
+      </c>
+      <c r="B123" s="6" t="s">
         <v>743</v>
-      </c>
-      <c r="B123" s="6" t="s">
-        <v>744</v>
       </c>
       <c r="C123" s="6"/>
       <c r="D123" s="6" t="s">
@@ -6514,51 +6522,51 @@
         <v>65</v>
       </c>
       <c r="H123" s="6" t="s">
+        <v>744</v>
+      </c>
+      <c r="I123" s="16" t="s">
         <v>745</v>
       </c>
-      <c r="I123" s="16" t="s">
+      <c r="J123" s="6"/>
+    </row>
+    <row r="124" spans="1:10" hidden="1">
+      <c r="A124" s="6" t="s">
         <v>746</v>
       </c>
-      <c r="J123" s="6"/>
-    </row>
-    <row r="124" spans="1:10">
-      <c r="A124" s="6" t="s">
+      <c r="B124" s="6" t="s">
         <v>747</v>
       </c>
-      <c r="B124" s="6" t="s">
-        <v>748</v>
-      </c>
       <c r="C124" s="6" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>110</v>
       </c>
       <c r="E124" s="6"/>
       <c r="F124" s="6" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G124" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H124" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="I124" s="16" t="s">
         <v>750</v>
       </c>
-      <c r="I124" s="16" t="s">
+      <c r="J124" s="6"/>
+    </row>
+    <row r="125" spans="1:10" hidden="1">
+      <c r="A125" s="6" t="s">
         <v>751</v>
       </c>
-      <c r="J124" s="6"/>
-    </row>
-    <row r="125" spans="1:10">
-      <c r="A125" s="6" t="s">
+      <c r="B125" s="6" t="s">
         <v>752</v>
-      </c>
-      <c r="B125" s="6" t="s">
-        <v>753</v>
       </c>
       <c r="C125" s="26"/>
       <c r="D125" s="6" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E125" s="6"/>
       <c r="F125" s="6"/>
@@ -6566,49 +6574,49 @@
         <v>65</v>
       </c>
       <c r="H125" s="6" t="s">
+        <v>753</v>
+      </c>
+      <c r="I125" s="16" t="s">
         <v>754</v>
       </c>
-      <c r="I125" s="16" t="s">
+      <c r="J125" s="6"/>
+    </row>
+    <row r="126" spans="1:10" hidden="1">
+      <c r="A126" s="6" t="s">
         <v>755</v>
       </c>
-      <c r="J125" s="6"/>
-    </row>
-    <row r="126" spans="1:10">
-      <c r="A126" s="6" t="s">
+      <c r="B126" s="6" t="s">
         <v>756</v>
       </c>
-      <c r="B126" s="6" t="s">
+      <c r="C126" s="6" t="s">
         <v>757</v>
-      </c>
-      <c r="C126" s="6" t="s">
-        <v>758</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E126" s="6" t="s">
+        <v>758</v>
+      </c>
+      <c r="F126" s="15" t="s">
         <v>759</v>
-      </c>
-      <c r="F126" s="15" t="s">
-        <v>760</v>
       </c>
       <c r="G126" t="s">
         <v>117</v>
       </c>
       <c r="H126" s="6"/>
       <c r="I126" s="6" t="s">
+        <v>760</v>
+      </c>
+      <c r="J126" s="6" t="s">
         <v>761</v>
       </c>
-      <c r="J126" s="6" t="s">
+    </row>
+    <row r="127" spans="1:10" hidden="1">
+      <c r="A127" s="6" t="s">
         <v>762</v>
       </c>
-    </row>
-    <row r="127" spans="1:10">
-      <c r="A127" s="6" t="s">
-        <v>763</v>
-      </c>
       <c r="B127" s="6" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C127" s="6"/>
       <c r="D127" s="6" t="s">
@@ -6620,19 +6628,19 @@
         <v>111</v>
       </c>
       <c r="H127" s="6" t="s">
+        <v>763</v>
+      </c>
+      <c r="I127" s="16" t="s">
         <v>764</v>
       </c>
-      <c r="I127" s="16" t="s">
+      <c r="J127" s="6"/>
+    </row>
+    <row r="128" spans="1:10" hidden="1">
+      <c r="A128" s="8" t="s">
         <v>765</v>
       </c>
-      <c r="J127" s="6"/>
-    </row>
-    <row r="128" spans="1:10">
-      <c r="A128" s="8" t="s">
-        <v>766</v>
-      </c>
       <c r="B128" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C128" s="8"/>
       <c r="D128" s="8" t="s">
@@ -6642,19 +6650,19 @@
         <v>87</v>
       </c>
       <c r="F128" s="8" t="s">
+        <v>766</v>
+      </c>
+      <c r="G128" t="s">
+        <v>547</v>
+      </c>
+      <c r="H128" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="I128" s="8" t="s">
         <v>767</v>
       </c>
-      <c r="G128" t="s">
-        <v>548</v>
-      </c>
-      <c r="H128" s="8" t="s">
-        <v>572</v>
-      </c>
-      <c r="I128" s="8" t="s">
+      <c r="J128" s="12" t="s">
         <v>768</v>
-      </c>
-      <c r="J128" s="12" t="s">
-        <v>769</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(repertoire-personnel): Correction de plusieurs déclinaisons différentes de "Bibliothèque du campus de l'UdeM à Laval"
</commit_message>
<xml_diff>
--- a/content/personnel/liste-personnel.xlsx
+++ b/content/personnel/liste-personnel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projets\coquille-web\content\personnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45787D0-19AA-4168-B764-43E1BABE0292}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC761E77-A8EF-4D15-88D9-E59C4ABBB4BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1890" yWindow="3180" windowWidth="33570" windowHeight="23450" tabRatio="149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="793">
   <si>
     <t>nom</t>
   </si>
@@ -169,9 +169,6 @@
   </si>
   <si>
     <t>Soutien à la recherche et à l’enseignement</t>
-  </si>
-  <si>
-    <t>Bibliothèque d'aménagement;Bibliothèque de droit;Bibliothèque Thérèse-Gouin-Décarie;Bibliothèque du Campus de Laval;Bibliothèque de musique</t>
   </si>
   <si>
     <t>514 343-6111, poste 1707</t>
@@ -1814,9 +1811,6 @@
     <t>France-nadeau.jpg</t>
   </si>
   <si>
-    <t>Bibliothèque d'aménagement; Bibliothèque de droit; Bibliothèque Thérèse-Gouin-Décarie; Bibliothèque du Campus de Laval; Bibliothèque de musique</t>
-  </si>
-  <si>
     <t>514 343-6111, poste 3256</t>
   </si>
   <si>
@@ -2372,9 +2366,6 @@
     <t>Référence et offre pédagogique de première ligne - Bibliothèque de droit, Bibliothèque de musique</t>
   </si>
   <si>
-    <t>Bibliothèque d'aménagement;Bibliothèque Thérèse-Gouin-Décarie;Bibliothèque du Campus de Laval</t>
-  </si>
-  <si>
     <t>Trépanier</t>
   </si>
   <si>
@@ -2426,10 +2417,16 @@
     <t>eve.baribeau.marchand@umontreal.ca</t>
   </si>
   <si>
-    <t>Bibliothèque du campus de l’UdeM à Laval</t>
-  </si>
-  <si>
     <t>Référence et offre pédagogique de première ligne, psychoéducation, psychologie, sciences de l'éducation, sciences infirmières, travail social – premier cycle</t>
+  </si>
+  <si>
+    <t>Bibliothèque d'aménagement;Bibliothèque de droit;Bibliothèque Thérèse-Gouin-Décarie;Bibliothèque du campus de l'UdeM à Laval;Bibliothèque de musique</t>
+  </si>
+  <si>
+    <t>Bibliothèque d'aménagement; Bibliothèque de droit; Bibliothèque Thérèse-Gouin-Décarie; Bibliothèque du campus de l'UdeM à Laval; Bibliothèque de musique</t>
+  </si>
+  <si>
+    <t>Bibliothèque d'aménagement;Bibliothèque Thérèse-Gouin-Décarie;Bibliothèque du campus de l'UdeM à Laval</t>
   </si>
 </sst>
 </file>
@@ -3077,9 +3074,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G123" sqref="G123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -3175,10 +3172,10 @@
         <v>46</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>792</v>
+        <v>22</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>23</v>
@@ -3270,743 +3267,743 @@
         <v>47</v>
       </c>
       <c r="G6" s="6" t="s">
+        <v>790</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="J6" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>55</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>22</v>
       </c>
       <c r="H7" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="J7" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="B8" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="G8" t="s">
         <v>15</v>
       </c>
       <c r="H8" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="I8" s="28" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="J8" s="29"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
         <v>60</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="24" t="s">
         <v>61</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>62</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" t="s">
         <v>63</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="I9" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="J9" t="s">
         <v>66</v>
-      </c>
-      <c r="J9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="G10" t="s">
         <v>71</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="I10" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="J10" s="13" t="s">
         <v>74</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="E11" t="s">
         <v>79</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
+        <v>690</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>781</v>
+      </c>
+      <c r="H11" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F11" t="s">
-        <v>692</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>784</v>
-      </c>
-      <c r="H11" s="10" t="s">
+      <c r="I11" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="J11" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="F12" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="H12" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="I12" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="J12" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="C13" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="E13" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="H13" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="I13" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="J13" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="C14" s="8" t="s">
         <v>101</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>102</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H14" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="I14" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="I14" s="10" t="s">
+      <c r="J14" s="8" t="s">
         <v>105</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>108</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="I15" s="17" t="s">
         <v>111</v>
-      </c>
-      <c r="I15" s="17" t="s">
-        <v>112</v>
       </c>
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>113</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>114</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F16" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G16" t="s">
         <v>115</v>
-      </c>
-      <c r="G16" t="s">
-        <v>116</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="J16" s="13" t="s">
         <v>117</v>
-      </c>
-      <c r="J16" s="13" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G17" t="s">
         <v>31</v>
       </c>
       <c r="H17" t="s">
+        <v>119</v>
+      </c>
+      <c r="I17" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="I17" s="18" t="s">
+      <c r="J17" s="18" t="s">
         <v>121</v>
-      </c>
-      <c r="J17" s="18" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E18" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>127</v>
-      </c>
       <c r="G18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="J18" s="13" t="s">
         <v>128</v>
-      </c>
-      <c r="J18" s="13" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" t="s">
         <v>130</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" s="24" t="s">
         <v>131</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>132</v>
       </c>
       <c r="D19" t="s">
         <v>13</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G19" t="s">
         <v>15</v>
       </c>
       <c r="H19" t="s">
+        <v>133</v>
+      </c>
+      <c r="I19" t="s">
         <v>134</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>135</v>
-      </c>
-      <c r="J19" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>137</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>138</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F20" s="10"/>
       <c r="H20" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="I20" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="J20" s="10" t="s">
         <v>141</v>
-      </c>
-      <c r="J20" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="E21" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="G21" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="H21" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="I21" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="J21" s="6" t="s">
         <v>150</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="C22" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>154</v>
-      </c>
       <c r="D22" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="G22" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="H22" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="I22" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="J22" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="C23" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>162</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H23" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="G23" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H23" s="6" t="s">
+      <c r="I23" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="J23" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="J23" s="9" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>167</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>168</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>784</v>
+      </c>
+      <c r="H24" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="E24" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>787</v>
-      </c>
-      <c r="H24" s="8" t="s">
+      <c r="I24" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="J24" s="8" t="s">
         <v>171</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>174</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>783</v>
+      </c>
+      <c r="H25" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="G25" s="8" t="s">
-        <v>786</v>
-      </c>
-      <c r="H25" s="8" t="s">
+      <c r="I25" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="J25" s="8" t="s">
         <v>177</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="C26" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="D26" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F26" s="11"/>
       <c r="H26" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="I26" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="I26" s="8" t="s">
+      <c r="J26" s="8" t="s">
         <v>183</v>
-      </c>
-      <c r="J26" s="8" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B27" t="s">
         <v>185</v>
       </c>
-      <c r="B27" t="s">
-        <v>186</v>
-      </c>
       <c r="D27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G27" t="s">
         <v>31</v>
       </c>
       <c r="H27" t="s">
+        <v>186</v>
+      </c>
+      <c r="I27" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="I27" s="18" t="s">
+      <c r="J27" s="18" t="s">
         <v>188</v>
-      </c>
-      <c r="J27" s="18" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>191</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="H28" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="I28" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="I28" s="13" t="s">
+      <c r="J28" s="13" t="s">
         <v>196</v>
-      </c>
-      <c r="J28" s="13" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>199</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="G29" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="H29" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="H29" s="6" t="s">
+      <c r="I29" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="I29" s="6" t="s">
+      <c r="J29" s="6" t="s">
         <v>203</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="D30" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F30" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="D30" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="F30" s="6" t="s">
+      <c r="G30" t="s">
         <v>208</v>
-      </c>
-      <c r="G30" t="s">
-        <v>209</v>
       </c>
       <c r="H30" s="6"/>
       <c r="I30" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="J30" s="13" t="s">
         <v>210</v>
-      </c>
-      <c r="J30" s="13" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
+        <v>211</v>
+      </c>
+      <c r="B31" t="s">
         <v>212</v>
-      </c>
-      <c r="B31" t="s">
-        <v>213</v>
       </c>
       <c r="D31" t="s">
         <v>29</v>
       </c>
       <c r="F31" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="G31" t="s">
         <v>155</v>
-      </c>
-      <c r="G31" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
+        <v>213</v>
+      </c>
+      <c r="B32" t="s">
         <v>214</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" t="s">
+        <v>54</v>
+      </c>
+      <c r="G32" t="s">
+        <v>770</v>
+      </c>
+      <c r="H32" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D32" t="s">
-        <v>55</v>
-      </c>
-      <c r="G32" t="s">
-        <v>772</v>
-      </c>
-      <c r="H32" s="8" t="s">
+      <c r="I32" s="18" t="s">
         <v>216</v>
       </c>
-      <c r="I32" s="18" t="s">
+      <c r="J32" s="17" t="s">
         <v>217</v>
-      </c>
-      <c r="J32" s="17" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>219</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>220</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="14"/>
@@ -4015,518 +4012,518 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="C34" s="8" t="s">
         <v>223</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>224</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="H34" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="G34" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="H34" s="8" t="s">
+      <c r="I34" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="I34" s="8" t="s">
+      <c r="J34" s="8" t="s">
         <v>227</v>
-      </c>
-      <c r="J34" s="8" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="D35" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="E35" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F35" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F35" s="6" t="s">
+      <c r="H35" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="H35" s="6" t="s">
+      <c r="I35" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="I35" s="6" t="s">
+      <c r="J35" s="6" t="s">
         <v>235</v>
-      </c>
-      <c r="J35" s="6" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>238</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>239</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H36" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="I36" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="I36" s="6" t="s">
+      <c r="J36" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="J36" s="6" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="C37" s="8" t="s">
         <v>245</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>246</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E37" s="8"/>
       <c r="F37" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>31</v>
       </c>
       <c r="H37" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="I37" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="I37" s="8" t="s">
+      <c r="J37" s="12" t="s">
         <v>249</v>
-      </c>
-      <c r="J37" s="12" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="C38" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="D38" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="E38" t="s">
         <v>254</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>255</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" s="8" t="s">
+        <v>768</v>
+      </c>
+      <c r="H38" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="G38" s="8" t="s">
-        <v>770</v>
-      </c>
-      <c r="H38" s="6" t="s">
+      <c r="I38" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="I38" s="6" t="s">
+      <c r="J38" s="13" t="s">
         <v>258</v>
-      </c>
-      <c r="J38" s="13" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="B39" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="C39" s="8" t="s">
         <v>261</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>262</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="H39" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="G39" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="H39" s="8" t="s">
+      <c r="I39" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="I39" s="8" t="s">
+      <c r="J39" s="8" t="s">
         <v>265</v>
-      </c>
-      <c r="J39" s="8" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>268</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>269</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H40" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="G40" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H40" s="6" t="s">
+      <c r="I40" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="I40" s="6" t="s">
+      <c r="J40" s="6" t="s">
         <v>272</v>
-      </c>
-      <c r="J40" s="6" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="C41" s="6" t="s">
         <v>275</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>276</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>31</v>
       </c>
       <c r="H41" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I41" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="I41" s="6" t="s">
+      <c r="J41" s="6" t="s">
         <v>279</v>
-      </c>
-      <c r="J41" s="6" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="C42" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="D42" s="8" t="s">
         <v>283</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>284</v>
       </c>
       <c r="E42" s="6"/>
       <c r="F42" s="27" t="s">
+        <v>285</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="H42" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="G42" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="H42" s="8" t="s">
+      <c r="I42" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="I42" s="8" t="s">
+      <c r="J42" s="8" t="s">
         <v>288</v>
-      </c>
-      <c r="J42" s="8" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="C43" s="8" t="s">
         <v>291</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>292</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>770</v>
+      </c>
+      <c r="H43" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="G43" s="8" t="s">
-        <v>772</v>
-      </c>
-      <c r="H43" s="8" t="s">
+      <c r="I43" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="I43" s="8" t="s">
+      <c r="J43" s="8" t="s">
         <v>295</v>
-      </c>
-      <c r="J43" s="8" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="C44" s="8" t="s">
         <v>298</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>299</v>
       </c>
       <c r="D44" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E44" s="8"/>
       <c r="F44" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H44" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="G44" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H44" s="8" t="s">
+      <c r="I44" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="I44" s="8" t="s">
+      <c r="J44" s="8" t="s">
         <v>302</v>
-      </c>
-      <c r="J44" s="8" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>304</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>305</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="H45" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="H45" s="6" t="s">
+      <c r="I45" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="I45" s="6" t="s">
+      <c r="J45" s="6" t="s">
         <v>309</v>
-      </c>
-      <c r="J45" s="6" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
+        <v>310</v>
+      </c>
+      <c r="B46" t="s">
         <v>311</v>
       </c>
-      <c r="B46" t="s">
-        <v>312</v>
-      </c>
       <c r="C46" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="D46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G46" t="s">
         <v>31</v>
       </c>
       <c r="H46" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="I46" s="18" t="s">
         <v>313</v>
       </c>
-      <c r="I46" s="18" t="s">
+      <c r="J46" s="18" t="s">
         <v>314</v>
-      </c>
-      <c r="J46" s="18" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="C47" s="6" t="s">
         <v>317</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>318</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E47" s="6"/>
       <c r="F47" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H47" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="G47" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H47" s="6" t="s">
+      <c r="I47" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="I47" s="6" t="s">
+      <c r="J47" s="6" t="s">
         <v>321</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
+        <v>322</v>
+      </c>
+      <c r="B48" t="s">
         <v>323</v>
-      </c>
-      <c r="B48" t="s">
-        <v>324</v>
       </c>
       <c r="C48" s="6"/>
       <c r="D48" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G48" t="s">
         <v>31</v>
       </c>
       <c r="H48" t="s">
+        <v>324</v>
+      </c>
+      <c r="I48" s="18" t="s">
         <v>325</v>
       </c>
-      <c r="I48" s="18" t="s">
+      <c r="J48" s="18" t="s">
         <v>326</v>
-      </c>
-      <c r="J48" s="18" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>328</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="C49" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="C49" s="6" t="s">
-        <v>330</v>
-      </c>
       <c r="D49" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H49" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="I49" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="I49" s="8" t="s">
+      <c r="J49" s="8" t="s">
         <v>332</v>
-      </c>
-      <c r="J49" s="8" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>328</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="C50" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="C50" s="6" t="s">
-        <v>330</v>
-      </c>
       <c r="D50" s="8" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F50" s="8"/>
       <c r="G50" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H50" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="I50" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="I50" s="8" t="s">
+      <c r="J50" s="8" t="s">
         <v>332</v>
-      </c>
-      <c r="J50" s="8" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="C51" s="8" t="s">
         <v>335</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>336</v>
       </c>
       <c r="D51" s="8" t="s">
         <v>45</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>47</v>
@@ -4535,216 +4532,216 @@
         <v>31</v>
       </c>
       <c r="H51" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="I51" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="I51" s="8" t="s">
+      <c r="J51" s="8" t="s">
         <v>339</v>
-      </c>
-      <c r="J51" s="8" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="B52" s="8" t="s">
         <v>341</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>342</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E52" s="8"/>
       <c r="F52" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="G52" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="G52" s="8" t="s">
+      <c r="H52" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="H52" s="8" t="s">
+      <c r="I52" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="I52" s="8" t="s">
+      <c r="J52" s="8" t="s">
         <v>346</v>
-      </c>
-      <c r="J52" s="8" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="B53" s="8" t="s">
         <v>348</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="C53" s="8" t="s">
         <v>349</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>350</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E53" s="8"/>
       <c r="F53" s="11" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G53" s="8" t="s">
         <v>31</v>
       </c>
       <c r="H53" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="I53" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="I53" s="8" t="s">
+      <c r="J53" s="8" t="s">
         <v>353</v>
-      </c>
-      <c r="J53" s="8" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>355</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>356</v>
       </c>
       <c r="C54" s="6"/>
       <c r="D54" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E54" s="6"/>
       <c r="F54" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H54" s="6"/>
       <c r="I54" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="J54" s="18" t="s">
         <v>359</v>
-      </c>
-      <c r="J54" s="18" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="B55" s="8" t="s">
         <v>361</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="C55" s="8" t="s">
         <v>362</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>363</v>
       </c>
       <c r="D55" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E55" s="8"/>
       <c r="F55" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="G55" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="G55" s="8" t="s">
+      <c r="H55" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="H55" s="8" t="s">
+      <c r="I55" s="8" t="s">
         <v>366</v>
       </c>
-      <c r="I55" s="8" t="s">
+      <c r="J55" s="8" t="s">
         <v>367</v>
-      </c>
-      <c r="J55" s="8" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C56" s="6"/>
       <c r="D56" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F56" s="6"/>
       <c r="H56" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I56" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="J56" s="6" t="s">
         <v>376</v>
-      </c>
-      <c r="J56" s="6" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="C57" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="D57" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="D57" s="6" t="s">
-        <v>372</v>
-      </c>
       <c r="E57" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F57" s="6"/>
       <c r="H57" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I57" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="J57" s="16" t="s">
         <v>373</v>
-      </c>
-      <c r="J57" s="16" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B58" s="8" t="s">
         <v>378</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="C58" s="8" t="s">
         <v>379</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>380</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F58" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="H58" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="H58" s="8" t="s">
+      <c r="I58" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="I58" s="8" t="s">
+      <c r="J58" s="8" t="s">
         <v>383</v>
-      </c>
-      <c r="J58" s="8" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>385</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>386</v>
       </c>
       <c r="C59" s="6"/>
       <c r="D59" s="6" t="s">
@@ -4752,455 +4749,455 @@
       </c>
       <c r="E59" s="6"/>
       <c r="F59" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G59" s="6" t="s">
         <v>31</v>
       </c>
       <c r="H59" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="I59" s="6" t="s">
         <v>388</v>
       </c>
-      <c r="I59" s="6" t="s">
+      <c r="J59" s="16" t="s">
         <v>389</v>
-      </c>
-      <c r="J59" s="16" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C60" s="6"/>
       <c r="D60" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E60" s="6"/>
       <c r="F60" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="G60" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="G60" s="6" t="s">
+      <c r="H60" s="10" t="s">
+        <v>654</v>
+      </c>
+      <c r="I60" s="16" t="s">
         <v>393</v>
       </c>
-      <c r="H60" s="10" t="s">
-        <v>656</v>
-      </c>
-      <c r="I60" s="16" t="s">
+      <c r="J60" s="22" t="s">
         <v>394</v>
-      </c>
-      <c r="J60" s="22" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>396</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>397</v>
       </c>
       <c r="C61" s="6"/>
       <c r="D61" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F61" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="G61" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="G61" s="6" t="s">
+      <c r="H61" s="6" t="s">
         <v>399</v>
-      </c>
-      <c r="H61" s="6" t="s">
-        <v>400</v>
       </c>
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="C62" s="6" t="s">
         <v>401</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>402</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E62" s="6"/>
       <c r="F62" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="H62" s="6" t="s">
         <v>403</v>
       </c>
-      <c r="G62" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="H62" s="6" t="s">
+      <c r="I62" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="I62" s="6" t="s">
+      <c r="J62" s="6" t="s">
         <v>405</v>
-      </c>
-      <c r="J62" s="6" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="B63" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="B63" s="8" t="s">
+      <c r="C63" s="8" t="s">
         <v>408</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>409</v>
       </c>
       <c r="D63" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E63" s="8"/>
       <c r="F63" s="8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G63" s="8" t="s">
         <v>31</v>
       </c>
       <c r="H63" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="I63" s="8" t="s">
         <v>411</v>
       </c>
-      <c r="I63" s="8" t="s">
+      <c r="J63" s="8" t="s">
         <v>412</v>
-      </c>
-      <c r="J63" s="8" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="64" spans="1:10" s="4" customFormat="1">
       <c r="A64" t="s">
+        <v>413</v>
+      </c>
+      <c r="B64" t="s">
         <v>414</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" s="25" t="s">
         <v>415</v>
-      </c>
-      <c r="C64" s="25" t="s">
-        <v>416</v>
       </c>
       <c r="D64" t="s">
         <v>13</v>
       </c>
       <c r="E64"/>
       <c r="F64" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G64" t="s">
         <v>15</v>
       </c>
       <c r="H64" t="s">
+        <v>417</v>
+      </c>
+      <c r="I64" t="s">
         <v>418</v>
       </c>
-      <c r="I64" t="s">
+      <c r="J64" t="s">
         <v>419</v>
-      </c>
-      <c r="J64" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="B65" s="6" t="s">
         <v>421</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="C65" s="6" t="s">
         <v>422</v>
       </c>
-      <c r="C65" s="6" t="s">
-        <v>423</v>
-      </c>
       <c r="D65" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F65" s="7"/>
       <c r="G65" s="4"/>
       <c r="H65" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="I65" s="6" t="s">
         <v>424</v>
       </c>
-      <c r="I65" s="6" t="s">
+      <c r="J65" s="6" t="s">
         <v>425</v>
-      </c>
-      <c r="J65" s="6" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="66" spans="1:10" s="5" customFormat="1">
       <c r="A66" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>427</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="C66" s="6" t="s">
         <v>428</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>429</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E66" s="6"/>
       <c r="F66" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G66" s="6" t="s">
         <v>31</v>
       </c>
       <c r="H66" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="I66" s="6" t="s">
         <v>431</v>
       </c>
-      <c r="I66" s="6" t="s">
+      <c r="J66" s="6" t="s">
         <v>432</v>
-      </c>
-      <c r="J66" s="6" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" t="s">
+        <v>433</v>
+      </c>
+      <c r="B67" t="s">
         <v>434</v>
       </c>
-      <c r="B67" t="s">
+      <c r="D67" t="s">
+        <v>54</v>
+      </c>
+      <c r="G67" t="s">
+        <v>364</v>
+      </c>
+      <c r="H67" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="D67" t="s">
-        <v>55</v>
-      </c>
-      <c r="G67" t="s">
-        <v>365</v>
-      </c>
-      <c r="H67" s="8" t="s">
+      <c r="I67" s="18" t="s">
         <v>436</v>
       </c>
-      <c r="I67" s="18" t="s">
+      <c r="J67" s="17" t="s">
         <v>437</v>
-      </c>
-      <c r="J67" s="17" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="8" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C68" s="8"/>
       <c r="D68" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E68" s="8"/>
       <c r="F68" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="G68" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="G68" s="8" t="s">
-        <v>393</v>
-      </c>
       <c r="H68" s="8" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="I68" s="12" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="J68" s="17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B69" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D69" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G69" t="s">
         <v>31</v>
       </c>
       <c r="H69" s="21" t="s">
+        <v>441</v>
+      </c>
+      <c r="I69" s="18" t="s">
         <v>442</v>
       </c>
-      <c r="I69" s="18" t="s">
+      <c r="J69" s="18" t="s">
         <v>443</v>
-      </c>
-      <c r="J69" s="18" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="B70" s="8" t="s">
         <v>445</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="C70" s="8" t="s">
         <v>446</v>
       </c>
-      <c r="C70" s="8" t="s">
+      <c r="D70" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E70" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F70" s="8" t="s">
         <v>447</v>
       </c>
-      <c r="D70" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="E70" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="F70" s="8" t="s">
+      <c r="G70" s="8" t="s">
+        <v>783</v>
+      </c>
+      <c r="H70" s="8" t="s">
         <v>448</v>
       </c>
-      <c r="G70" s="8" t="s">
-        <v>786</v>
-      </c>
-      <c r="H70" s="8" t="s">
+      <c r="I70" s="8" t="s">
         <v>449</v>
       </c>
-      <c r="I70" s="8" t="s">
+      <c r="J70" s="8" t="s">
         <v>450</v>
-      </c>
-      <c r="J70" s="8" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="B71" s="6" t="s">
         <v>452</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="C71" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="C71" s="6" t="s">
-        <v>454</v>
-      </c>
       <c r="D71" s="6" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>47</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H71" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="I71" s="6" t="s">
         <v>455</v>
       </c>
-      <c r="I71" s="6" t="s">
+      <c r="J71" s="6" t="s">
         <v>456</v>
-      </c>
-      <c r="J71" s="6" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" s="8" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="D72" s="8" t="s">
         <v>45</v>
       </c>
       <c r="E72" s="23" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G72" s="8" t="s">
         <v>31</v>
       </c>
       <c r="H72" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="I72" s="8" t="s">
         <v>460</v>
       </c>
-      <c r="I72" s="8" t="s">
+      <c r="J72" s="17" t="s">
         <v>461</v>
-      </c>
-      <c r="J72" s="17" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73" t="s">
+        <v>462</v>
+      </c>
+      <c r="B73" t="s">
         <v>463</v>
       </c>
-      <c r="B73" t="s">
-        <v>464</v>
-      </c>
       <c r="C73" s="6" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="D73" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G73" t="s">
         <v>31</v>
       </c>
       <c r="H73" s="21" t="s">
+        <v>464</v>
+      </c>
+      <c r="I73" s="18" t="s">
         <v>465</v>
       </c>
-      <c r="I73" s="18" t="s">
+      <c r="J73" s="18" t="s">
         <v>466</v>
-      </c>
-      <c r="J73" s="18" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="B74" s="8" t="s">
         <v>468</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="C74" s="6" t="s">
         <v>469</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>470</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E74" s="8"/>
       <c r="F74" s="8" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G74" s="8" t="s">
         <v>31</v>
       </c>
       <c r="H74" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="I74" s="8" t="s">
         <v>472</v>
       </c>
-      <c r="I74" s="8" t="s">
+      <c r="J74" s="8" t="s">
         <v>473</v>
-      </c>
-      <c r="J74" s="8" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="75" spans="1:10" s="4" customFormat="1">
       <c r="A75" t="s">
+        <v>474</v>
+      </c>
+      <c r="B75" t="s">
         <v>475</v>
-      </c>
-      <c r="B75" t="s">
-        <v>476</v>
       </c>
       <c r="C75" s="6"/>
       <c r="D75" s="8" t="s">
@@ -5208,168 +5205,168 @@
       </c>
       <c r="E75" s="8"/>
       <c r="F75" t="s">
+        <v>476</v>
+      </c>
+      <c r="G75" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H75" t="s">
         <v>477</v>
       </c>
-      <c r="G75" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="H75" t="s">
+      <c r="I75" s="18" t="s">
         <v>478</v>
-      </c>
-      <c r="I75" s="18" t="s">
-        <v>479</v>
       </c>
       <c r="J75"/>
     </row>
     <row r="76" spans="1:10" s="4" customFormat="1">
       <c r="A76" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="B76" s="8" t="s">
         <v>480</v>
       </c>
-      <c r="B76" s="8" t="s">
+      <c r="C76" s="6" t="s">
         <v>481</v>
       </c>
-      <c r="C76" s="6" t="s">
+      <c r="D76" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="E76" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G76" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H76" s="8" t="s">
         <v>482</v>
       </c>
-      <c r="D76" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E76" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G76" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="H76" s="8" t="s">
+      <c r="I76" s="8" t="s">
         <v>483</v>
       </c>
-      <c r="I76" s="8" t="s">
+      <c r="J76" s="8" t="s">
         <v>484</v>
-      </c>
-      <c r="J76" s="8" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="B77" s="6" t="s">
         <v>486</v>
       </c>
-      <c r="B77" s="6" t="s">
+      <c r="C77" s="6" t="s">
         <v>487</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="D77" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="F77" s="7" t="s">
         <v>488</v>
       </c>
-      <c r="D77" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="F77" s="7" t="s">
+      <c r="G77" s="8" t="s">
+        <v>768</v>
+      </c>
+      <c r="H77" s="6" t="s">
         <v>489</v>
       </c>
-      <c r="G77" s="8" t="s">
-        <v>770</v>
-      </c>
-      <c r="H77" s="6" t="s">
+      <c r="I77" s="6" t="s">
         <v>490</v>
       </c>
-      <c r="I77" s="6" t="s">
+      <c r="J77" s="6" t="s">
         <v>491</v>
-      </c>
-      <c r="J77" s="6" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="8" t="s">
+        <v>492</v>
+      </c>
+      <c r="B78" s="8" t="s">
         <v>493</v>
       </c>
-      <c r="B78" s="8" t="s">
+      <c r="C78" s="6" t="s">
         <v>494</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="D78" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="E78" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G78" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="H78" s="8" t="s">
         <v>495</v>
       </c>
-      <c r="D78" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E78" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="G78" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="H78" s="8" t="s">
+      <c r="I78" s="8" t="s">
         <v>496</v>
       </c>
-      <c r="I78" s="8" t="s">
+      <c r="J78" s="8" t="s">
         <v>497</v>
-      </c>
-      <c r="J78" s="8" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="79" spans="1:10" s="4" customFormat="1">
       <c r="A79" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="B79" s="6" t="s">
         <v>499</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="C79" s="6" t="s">
         <v>500</v>
       </c>
-      <c r="C79" s="6" t="s">
-        <v>501</v>
-      </c>
       <c r="D79" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E79" s="23" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F79" s="6"/>
       <c r="G79" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H79" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="I79" s="6" t="s">
         <v>502</v>
       </c>
-      <c r="I79" s="6" t="s">
+      <c r="J79" s="6" t="s">
         <v>503</v>
-      </c>
-      <c r="J79" s="6" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="6" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C80" s="6"/>
       <c r="D80" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F80" s="6"/>
       <c r="H80" s="6"/>
       <c r="I80" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="J80" s="6" t="s">
         <v>511</v>
-      </c>
-      <c r="J80" s="6" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="10" t="s">
+        <v>504</v>
+      </c>
+      <c r="B81" s="10" t="s">
         <v>505</v>
-      </c>
-      <c r="B81" s="10" t="s">
-        <v>506</v>
       </c>
       <c r="C81" s="10"/>
       <c r="D81" s="10" t="s">
@@ -5379,336 +5376,336 @@
         <v>46</v>
       </c>
       <c r="F81" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="G81" s="10" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="H81" s="10" t="s">
+        <v>506</v>
+      </c>
+      <c r="I81" s="10" t="s">
         <v>507</v>
       </c>
-      <c r="I81" s="10" t="s">
+      <c r="J81" s="10" t="s">
         <v>508</v>
-      </c>
-      <c r="J81" s="10" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="B82" s="6" t="s">
         <v>513</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>514</v>
       </c>
       <c r="C82" s="6"/>
       <c r="D82" s="6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E82" s="6"/>
       <c r="F82" s="6"/>
       <c r="G82" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H82" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="I82" s="16" t="s">
         <v>516</v>
-      </c>
-      <c r="I82" s="16" t="s">
-        <v>517</v>
       </c>
       <c r="J82" s="6"/>
     </row>
     <row r="83" spans="1:10">
       <c r="A83" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="B83" s="6" t="s">
         <v>518</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>519</v>
       </c>
       <c r="C83" s="6"/>
       <c r="D83" s="6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E83" s="6"/>
       <c r="F83" s="6"/>
       <c r="G83" s="6" t="s">
+        <v>519</v>
+      </c>
+      <c r="H83" s="6" t="s">
         <v>520</v>
       </c>
-      <c r="H83" s="6" t="s">
+      <c r="I83" s="16" t="s">
         <v>521</v>
-      </c>
-      <c r="I83" s="16" t="s">
-        <v>522</v>
       </c>
       <c r="J83" s="6"/>
     </row>
     <row r="84" spans="1:10">
       <c r="A84" s="6" t="s">
+        <v>522</v>
+      </c>
+      <c r="B84" s="6" t="s">
         <v>523</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>524</v>
       </c>
       <c r="C84" s="6"/>
       <c r="D84" s="6" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E84" s="6"/>
       <c r="F84" s="27" t="s">
+        <v>525</v>
+      </c>
+      <c r="G84" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="H84" s="14" t="s">
         <v>526</v>
       </c>
-      <c r="G84" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="H84" s="14" t="s">
+      <c r="I84" s="16" t="s">
         <v>527</v>
       </c>
-      <c r="I84" s="16" t="s">
+      <c r="J84" s="16" t="s">
         <v>528</v>
-      </c>
-      <c r="J84" s="16" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="6" t="s">
+        <v>529</v>
+      </c>
+      <c r="B85" s="6" t="s">
         <v>530</v>
       </c>
-      <c r="B85" s="6" t="s">
+      <c r="C85" s="6" t="s">
         <v>531</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>532</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E85" s="6"/>
       <c r="F85" s="6" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G85" s="6" t="s">
         <v>31</v>
       </c>
       <c r="H85" s="6" t="s">
+        <v>533</v>
+      </c>
+      <c r="I85" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="I85" s="6" t="s">
-        <v>535</v>
-      </c>
       <c r="J85" s="6" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="C86" s="6" t="s">
         <v>536</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>435</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>537</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E86" s="6"/>
       <c r="F86" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="G86" s="6" t="s">
         <v>538</v>
       </c>
-      <c r="G86" s="6" t="s">
+      <c r="H86" s="6" t="s">
         <v>539</v>
       </c>
-      <c r="H86" s="6" t="s">
+      <c r="I86" s="6" t="s">
         <v>540</v>
       </c>
-      <c r="I86" s="6" t="s">
+      <c r="J86" s="6" t="s">
         <v>541</v>
-      </c>
-      <c r="J86" s="6" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="B87" s="6" t="s">
         <v>543</v>
       </c>
-      <c r="B87" s="6" t="s">
+      <c r="C87" s="6" t="s">
         <v>544</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>545</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>45</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G87" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="H87" s="6" t="s">
         <v>546</v>
       </c>
-      <c r="H87" s="6" t="s">
+      <c r="I87" s="6" t="s">
         <v>547</v>
       </c>
-      <c r="I87" s="6" t="s">
+      <c r="J87" s="6" t="s">
         <v>548</v>
-      </c>
-      <c r="J87" s="6" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="B88" s="6" t="s">
         <v>550</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>551</v>
       </c>
       <c r="C88" s="6"/>
       <c r="D88" s="6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E88" s="6"/>
       <c r="F88" s="6"/>
       <c r="G88" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H88" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="I88" s="16" t="s">
         <v>552</v>
-      </c>
-      <c r="I88" s="16" t="s">
-        <v>553</v>
       </c>
       <c r="J88" s="6"/>
     </row>
     <row r="89" spans="1:10">
       <c r="A89" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="B89" s="6" t="s">
         <v>554</v>
       </c>
-      <c r="B89" s="6" t="s">
+      <c r="C89" s="6" t="s">
         <v>555</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>556</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E89" s="6"/>
       <c r="F89" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="G89" s="6" t="s">
+        <v>519</v>
+      </c>
+      <c r="H89" s="6" t="s">
         <v>557</v>
       </c>
-      <c r="G89" s="6" t="s">
-        <v>520</v>
-      </c>
-      <c r="H89" s="6" t="s">
+      <c r="I89" s="6" t="s">
         <v>558</v>
       </c>
-      <c r="I89" s="6" t="s">
+      <c r="J89" s="6" t="s">
         <v>559</v>
-      </c>
-      <c r="J89" s="6" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="90" spans="1:10">
       <c r="A90" s="14" t="s">
+        <v>560</v>
+      </c>
+      <c r="B90" s="14" t="s">
         <v>561</v>
       </c>
-      <c r="B90" s="14" t="s">
+      <c r="C90" s="6" t="s">
         <v>562</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>563</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E90" s="6"/>
       <c r="F90" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="G90" s="14" t="s">
         <v>538</v>
       </c>
-      <c r="G90" s="14" t="s">
-        <v>539</v>
-      </c>
       <c r="H90" s="14" t="s">
+        <v>563</v>
+      </c>
+      <c r="I90" s="14" t="s">
         <v>564</v>
       </c>
-      <c r="I90" s="14" t="s">
+      <c r="J90" s="14" t="s">
         <v>565</v>
-      </c>
-      <c r="J90" s="14" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91" s="8" t="s">
+        <v>566</v>
+      </c>
+      <c r="B91" s="8" t="s">
         <v>567</v>
       </c>
-      <c r="B91" s="8" t="s">
+      <c r="C91" s="6" t="s">
         <v>568</v>
       </c>
-      <c r="C91" s="6" t="s">
-        <v>569</v>
-      </c>
       <c r="D91" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E91" s="8"/>
       <c r="F91" s="8" t="s">
         <v>30</v>
       </c>
       <c r="G91" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H91" s="8" t="s">
+        <v>569</v>
+      </c>
+      <c r="I91" s="8" t="s">
         <v>570</v>
       </c>
-      <c r="I91" s="8" t="s">
+      <c r="J91" s="8" t="s">
         <v>571</v>
-      </c>
-      <c r="J91" s="8" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="92" spans="1:10">
       <c r="A92" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="B92" s="8" t="s">
         <v>573</v>
       </c>
-      <c r="B92" s="8" t="s">
+      <c r="C92" s="6" t="s">
         <v>574</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>575</v>
       </c>
       <c r="D92" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E92" s="8"/>
       <c r="F92" s="11" t="s">
+        <v>575</v>
+      </c>
+      <c r="G92" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="H92" s="8" t="s">
         <v>576</v>
       </c>
-      <c r="G92" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="H92" s="8" t="s">
+      <c r="I92" s="8" t="s">
         <v>577</v>
       </c>
-      <c r="I92" s="8" t="s">
+      <c r="J92" s="8" t="s">
         <v>578</v>
-      </c>
-      <c r="J92" s="8" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" t="s">
+        <v>579</v>
+      </c>
+      <c r="B93" t="s">
         <v>580</v>
-      </c>
-      <c r="B93" t="s">
-        <v>581</v>
       </c>
       <c r="C93" s="6"/>
       <c r="D93" s="8" t="s">
@@ -5716,378 +5713,378 @@
       </c>
       <c r="E93" s="8"/>
       <c r="F93" t="s">
+        <v>581</v>
+      </c>
+      <c r="G93" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H93" t="s">
         <v>582</v>
       </c>
-      <c r="G93" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="H93" t="s">
+      <c r="I93" s="18" t="s">
         <v>583</v>
-      </c>
-      <c r="I93" s="18" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="94" spans="1:10">
       <c r="A94" s="14" t="s">
+        <v>584</v>
+      </c>
+      <c r="B94" s="14" t="s">
         <v>585</v>
       </c>
-      <c r="B94" s="14" t="s">
+      <c r="C94" s="14" t="s">
         <v>586</v>
       </c>
-      <c r="C94" s="14" t="s">
-        <v>587</v>
-      </c>
       <c r="D94" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E94" s="14" t="s">
         <v>46</v>
       </c>
       <c r="F94" s="7"/>
       <c r="G94" s="14" t="s">
+        <v>791</v>
+      </c>
+      <c r="H94" s="14" t="s">
+        <v>587</v>
+      </c>
+      <c r="I94" s="14" t="s">
         <v>588</v>
       </c>
-      <c r="H94" s="14" t="s">
+      <c r="J94" s="14" t="s">
         <v>589</v>
-      </c>
-      <c r="I94" s="14" t="s">
-        <v>590</v>
-      </c>
-      <c r="J94" s="14" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="8" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="C95" s="8"/>
       <c r="D95" s="8" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E95" s="8"/>
       <c r="F95" s="8" t="s">
+        <v>593</v>
+      </c>
+      <c r="G95" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H95" s="8" t="s">
+        <v>594</v>
+      </c>
+      <c r="I95" s="8" t="s">
         <v>595</v>
       </c>
-      <c r="G95" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="H95" s="8" t="s">
+      <c r="J95" s="8" t="s">
         <v>596</v>
-      </c>
-      <c r="I95" s="8" t="s">
-        <v>597</v>
-      </c>
-      <c r="J95" s="8" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="96" spans="1:10" s="4" customFormat="1">
       <c r="A96" s="8" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C96" s="8"/>
       <c r="D96" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F96" s="8"/>
       <c r="G96"/>
       <c r="H96" s="8" t="s">
+        <v>599</v>
+      </c>
+      <c r="I96" s="8" t="s">
+        <v>600</v>
+      </c>
+      <c r="J96" s="8" t="s">
         <v>601</v>
-      </c>
-      <c r="I96" s="8" t="s">
-        <v>602</v>
-      </c>
-      <c r="J96" s="8" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="97" spans="1:10" s="4" customFormat="1">
       <c r="A97" s="8" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>45</v>
       </c>
       <c r="E97" s="23" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="G97" s="8" t="s">
         <v>31</v>
       </c>
       <c r="H97" s="8" t="s">
+        <v>605</v>
+      </c>
+      <c r="I97" s="8" t="s">
+        <v>606</v>
+      </c>
+      <c r="J97" s="17" t="s">
         <v>607</v>
-      </c>
-      <c r="I97" s="8" t="s">
-        <v>608</v>
-      </c>
-      <c r="J97" s="17" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" s="8" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="C98" s="8"/>
       <c r="D98" s="8" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="E98" s="6"/>
       <c r="F98" s="27" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="G98" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H98" s="8"/>
       <c r="I98" s="17" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="J98" s="18" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="99" spans="1:10">
       <c r="A99" t="s">
+        <v>614</v>
+      </c>
+      <c r="B99" t="s">
+        <v>615</v>
+      </c>
+      <c r="C99" s="25" t="s">
         <v>616</v>
-      </c>
-      <c r="B99" t="s">
-        <v>617</v>
-      </c>
-      <c r="C99" s="25" t="s">
-        <v>618</v>
       </c>
       <c r="D99" t="s">
         <v>29</v>
       </c>
       <c r="E99" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F99" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="G99" t="s">
+        <v>115</v>
+      </c>
+      <c r="I99" t="s">
+        <v>618</v>
+      </c>
+      <c r="J99" t="s">
         <v>619</v>
-      </c>
-      <c r="G99" t="s">
-        <v>116</v>
-      </c>
-      <c r="I99" t="s">
-        <v>620</v>
-      </c>
-      <c r="J99" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>621</v>
+      </c>
+      <c r="C100" s="6" t="s">
         <v>622</v>
       </c>
-      <c r="B100" s="6" t="s">
+      <c r="D100" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E100" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F100" s="15" t="s">
         <v>623</v>
       </c>
-      <c r="C100" s="6" t="s">
+      <c r="G100" t="s">
+        <v>115</v>
+      </c>
+      <c r="H100" s="14" t="s">
         <v>624</v>
       </c>
-      <c r="D100" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="E100" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F100" s="15" t="s">
+      <c r="I100" s="14" t="s">
         <v>625</v>
       </c>
-      <c r="G100" t="s">
-        <v>116</v>
-      </c>
-      <c r="H100" s="14" t="s">
+      <c r="J100" s="14" t="s">
         <v>626</v>
-      </c>
-      <c r="I100" s="14" t="s">
-        <v>627</v>
-      </c>
-      <c r="J100" s="14" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="101" spans="1:10">
       <c r="A101" s="6" t="s">
+        <v>627</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="C101" s="6" t="s">
         <v>629</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>630</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>631</v>
       </c>
       <c r="D101" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E101" s="6"/>
       <c r="F101" s="6" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="G101" s="6" t="s">
         <v>31</v>
       </c>
       <c r="H101" s="14" t="s">
+        <v>631</v>
+      </c>
+      <c r="I101" s="14" t="s">
+        <v>632</v>
+      </c>
+      <c r="J101" s="14" t="s">
         <v>633</v>
-      </c>
-      <c r="I101" s="14" t="s">
-        <v>634</v>
-      </c>
-      <c r="J101" s="14" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="102" spans="1:10">
       <c r="A102" s="8" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D102" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E102" s="8"/>
       <c r="F102" s="8" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="G102" s="8" t="s">
         <v>31</v>
       </c>
       <c r="H102" s="10" t="s">
+        <v>637</v>
+      </c>
+      <c r="I102" s="10" t="s">
+        <v>638</v>
+      </c>
+      <c r="J102" s="10" t="s">
         <v>639</v>
-      </c>
-      <c r="I102" s="10" t="s">
-        <v>640</v>
-      </c>
-      <c r="J102" s="10" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="103" spans="1:10" s="5" customFormat="1">
       <c r="A103" s="6" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E103" s="6"/>
       <c r="F103" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H103" s="14" t="s">
+        <v>642</v>
+      </c>
+      <c r="I103" s="14" t="s">
+        <v>643</v>
+      </c>
+      <c r="J103" s="14" t="s">
         <v>644</v>
-      </c>
-      <c r="I103" s="14" t="s">
-        <v>645</v>
-      </c>
-      <c r="J103" s="14" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="104" spans="1:10" s="5" customFormat="1">
       <c r="A104" s="6" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F104" s="15" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="H104" s="14"/>
       <c r="I104" s="13" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="J104" s="14" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="105" spans="1:10">
       <c r="A105" s="8" t="s">
+        <v>650</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>651</v>
+      </c>
+      <c r="C105" s="8" t="s">
         <v>652</v>
-      </c>
-      <c r="B105" s="8" t="s">
-        <v>653</v>
-      </c>
-      <c r="C105" s="8" t="s">
-        <v>654</v>
       </c>
       <c r="D105" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E105" s="8"/>
       <c r="F105" s="11" t="s">
+        <v>653</v>
+      </c>
+      <c r="G105" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="H105" s="10" t="s">
+        <v>654</v>
+      </c>
+      <c r="I105" s="10" t="s">
         <v>655</v>
       </c>
-      <c r="G105" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="H105" s="10" t="s">
+      <c r="J105" s="10" t="s">
         <v>656</v>
-      </c>
-      <c r="I105" s="10" t="s">
-        <v>657</v>
-      </c>
-      <c r="J105" s="10" t="s">
-        <v>658</v>
       </c>
     </row>
     <row r="106" spans="1:10">
       <c r="A106" s="8" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C106" s="6"/>
       <c r="D106" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E106" s="8"/>
       <c r="F106" s="11"/>
@@ -6095,121 +6092,121 @@
         <v>22</v>
       </c>
       <c r="H106" s="10" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="I106" s="17" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="J106" s="10"/>
     </row>
     <row r="107" spans="1:10">
       <c r="A107" t="s">
+        <v>661</v>
+      </c>
+      <c r="B107" t="s">
+        <v>662</v>
+      </c>
+      <c r="D107" t="s">
+        <v>514</v>
+      </c>
+      <c r="G107" t="s">
+        <v>770</v>
+      </c>
+      <c r="H107" s="8" t="s">
         <v>663</v>
       </c>
-      <c r="B107" t="s">
+      <c r="I107" s="18" t="s">
         <v>664</v>
       </c>
-      <c r="D107" t="s">
-        <v>515</v>
-      </c>
-      <c r="G107" t="s">
-        <v>772</v>
-      </c>
-      <c r="H107" s="8" t="s">
+      <c r="J107" s="17" t="s">
         <v>665</v>
-      </c>
-      <c r="I107" s="18" t="s">
-        <v>666</v>
-      </c>
-      <c r="J107" s="17" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="108" spans="1:10">
       <c r="A108" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B108" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="D108" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G108" t="s">
         <v>31</v>
       </c>
       <c r="H108" t="s">
+        <v>668</v>
+      </c>
+      <c r="I108" s="18" t="s">
+        <v>669</v>
+      </c>
+      <c r="J108" s="19" t="s">
         <v>670</v>
-      </c>
-      <c r="I108" s="18" t="s">
-        <v>671</v>
-      </c>
-      <c r="J108" s="19" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="109" spans="1:10">
       <c r="A109" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B109" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C109" s="25" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="D109" t="s">
         <v>13</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="G109" t="s">
         <v>31</v>
       </c>
       <c r="H109" s="4" t="s">
+        <v>674</v>
+      </c>
+      <c r="I109" s="4" t="s">
+        <v>675</v>
+      </c>
+      <c r="J109" s="4" t="s">
         <v>676</v>
-      </c>
-      <c r="I109" s="4" t="s">
-        <v>677</v>
-      </c>
-      <c r="J109" s="4" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="110" spans="1:10">
       <c r="A110" s="6" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F110" s="15"/>
       <c r="H110" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I110" s="14" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="J110" s="14" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="111" spans="1:10">
       <c r="A111" s="6" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C111" s="6"/>
       <c r="D111" s="6" t="s">
@@ -6217,28 +6214,28 @@
       </c>
       <c r="E111" s="6"/>
       <c r="F111" s="15" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H111" s="14"/>
       <c r="I111" s="14" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="J111" s="14" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="112" spans="1:10">
       <c r="A112" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B112" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E112" s="6"/>
       <c r="F112" s="6"/>
@@ -6248,44 +6245,44 @@
     </row>
     <row r="113" spans="1:10">
       <c r="A113" s="10" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B113" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="D113" s="10" t="s">
         <v>29</v>
       </c>
       <c r="E113" s="10"/>
       <c r="F113" s="10" t="s">
+        <v>690</v>
+      </c>
+      <c r="G113" s="10" t="s">
+        <v>691</v>
+      </c>
+      <c r="H113" s="10" t="s">
         <v>692</v>
       </c>
-      <c r="G113" s="10" t="s">
+      <c r="I113" s="10" t="s">
         <v>693</v>
       </c>
-      <c r="H113" s="10" t="s">
+      <c r="J113" s="10" t="s">
         <v>694</v>
-      </c>
-      <c r="I113" s="10" t="s">
-        <v>695</v>
-      </c>
-      <c r="J113" s="10" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="114" spans="1:10">
       <c r="A114" s="10" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="B114" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C114" s="10"/>
       <c r="D114" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E114" s="10" t="s">
         <v>46</v>
@@ -6293,415 +6290,415 @@
       <c r="F114" s="10"/>
       <c r="G114" s="10"/>
       <c r="H114" s="10" t="s">
+        <v>696</v>
+      </c>
+      <c r="I114" s="10" t="s">
+        <v>697</v>
+      </c>
+      <c r="J114" s="10" t="s">
         <v>698</v>
-      </c>
-      <c r="I114" s="10" t="s">
-        <v>699</v>
-      </c>
-      <c r="J114" s="10" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="115" spans="1:10">
       <c r="A115" s="6" t="s">
+        <v>699</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>700</v>
+      </c>
+      <c r="C115" s="6" t="s">
         <v>701</v>
       </c>
-      <c r="B115" s="6" t="s">
+      <c r="D115" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E115" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G115" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="H115" s="6" t="s">
         <v>702</v>
       </c>
-      <c r="C115" s="6" t="s">
+      <c r="I115" s="6" t="s">
         <v>703</v>
       </c>
-      <c r="D115" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E115" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="G115" s="6" t="s">
-        <v>399</v>
-      </c>
-      <c r="H115" s="6" t="s">
+      <c r="J115" s="6" t="s">
         <v>704</v>
-      </c>
-      <c r="I115" s="6" t="s">
-        <v>705</v>
-      </c>
-      <c r="J115" s="6" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="116" spans="1:10">
       <c r="A116" s="6" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="C116" s="26"/>
       <c r="D116" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E116" s="6"/>
       <c r="F116" s="6"/>
       <c r="G116" s="6" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H116" s="6"/>
       <c r="I116" s="16" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="J116" s="6"/>
     </row>
     <row r="117" spans="1:10">
       <c r="A117" s="14" t="s">
+        <v>708</v>
+      </c>
+      <c r="B117" s="14" t="s">
+        <v>709</v>
+      </c>
+      <c r="C117" s="26" t="s">
         <v>710</v>
       </c>
-      <c r="B117" s="14" t="s">
+      <c r="D117" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="E117" t="s">
         <v>711</v>
       </c>
-      <c r="C117" s="26" t="s">
+      <c r="F117" s="14" t="s">
         <v>712</v>
       </c>
-      <c r="D117" s="14" t="s">
-        <v>343</v>
-      </c>
-      <c r="E117" t="s">
+      <c r="G117" s="14" t="s">
+        <v>790</v>
+      </c>
+      <c r="H117" s="14" t="s">
         <v>713</v>
       </c>
-      <c r="F117" s="14" t="s">
+      <c r="I117" s="14" t="s">
         <v>714</v>
       </c>
-      <c r="G117" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="H117" s="14" t="s">
+      <c r="J117" s="14" t="s">
         <v>715</v>
-      </c>
-      <c r="I117" s="14" t="s">
-        <v>716</v>
-      </c>
-      <c r="J117" s="14" t="s">
-        <v>717</v>
       </c>
     </row>
     <row r="118" spans="1:10">
       <c r="A118" s="8" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C118" s="31" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="D118" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E118" s="8"/>
       <c r="F118" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="G118" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="G118" s="8" t="s">
-        <v>156</v>
-      </c>
       <c r="H118" s="8" t="s">
+        <v>718</v>
+      </c>
+      <c r="I118" s="8" t="s">
+        <v>719</v>
+      </c>
+      <c r="J118" s="8" t="s">
         <v>720</v>
-      </c>
-      <c r="I118" s="8" t="s">
-        <v>721</v>
-      </c>
-      <c r="J118" s="8" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="119" spans="1:10">
       <c r="A119" s="8" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="C119" s="8"/>
       <c r="D119" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E119" s="8"/>
       <c r="F119" s="8"/>
       <c r="G119" s="8" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H119" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="I119" s="17" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="J119" s="8"/>
     </row>
     <row r="120" spans="1:10">
       <c r="A120" s="6" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="C120" s="6"/>
       <c r="D120" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E120" s="6"/>
       <c r="F120" s="15" t="s">
+        <v>727</v>
+      </c>
+      <c r="G120" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="H120" s="6" t="s">
+        <v>728</v>
+      </c>
+      <c r="I120" s="6" t="s">
         <v>729</v>
       </c>
-      <c r="G120" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="H120" s="6" t="s">
+      <c r="J120" s="6" t="s">
         <v>730</v>
-      </c>
-      <c r="I120" s="6" t="s">
-        <v>731</v>
-      </c>
-      <c r="J120" s="6" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="121" spans="1:10">
       <c r="A121" s="6" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="C121" s="6"/>
       <c r="D121" s="6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E121" s="6"/>
       <c r="F121" s="6"/>
       <c r="G121" s="6" t="s">
+        <v>519</v>
+      </c>
+      <c r="H121" s="8" t="s">
         <v>520</v>
       </c>
-      <c r="H121" s="8" t="s">
-        <v>521</v>
-      </c>
       <c r="I121" s="16" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="J121" s="6"/>
     </row>
     <row r="122" spans="1:10">
       <c r="A122" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B122" t="s">
+        <v>734</v>
+      </c>
+      <c r="D122" t="s">
+        <v>54</v>
+      </c>
+      <c r="F122" t="s">
+        <v>735</v>
+      </c>
+      <c r="G122" t="s">
+        <v>364</v>
+      </c>
+      <c r="H122" s="8" t="s">
         <v>736</v>
       </c>
-      <c r="D122" t="s">
-        <v>55</v>
-      </c>
-      <c r="F122" t="s">
+      <c r="I122" s="18" t="s">
         <v>737</v>
       </c>
-      <c r="G122" t="s">
-        <v>365</v>
-      </c>
-      <c r="H122" s="8" t="s">
+      <c r="J122" s="17" t="s">
         <v>738</v>
-      </c>
-      <c r="I122" s="18" t="s">
-        <v>739</v>
-      </c>
-      <c r="J122" s="17" t="s">
-        <v>740</v>
       </c>
     </row>
     <row r="123" spans="1:10">
       <c r="A123" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="B123" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C123" s="6"/>
       <c r="D123" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E123" s="6" t="s">
         <v>46</v>
       </c>
       <c r="F123" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="G123" t="s">
+        <v>792</v>
+      </c>
+      <c r="H123" t="s">
         <v>774</v>
       </c>
-      <c r="H123" t="s">
-        <v>777</v>
-      </c>
       <c r="I123" s="28" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
     </row>
     <row r="124" spans="1:10">
       <c r="A124" s="6" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C124" s="6"/>
       <c r="D124" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E124" s="6"/>
       <c r="F124" s="6"/>
       <c r="G124" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H124" s="6" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="I124" s="16" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="J124" s="6"/>
     </row>
     <row r="125" spans="1:10">
       <c r="A125" s="6" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="C125" s="26" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E125" s="6"/>
       <c r="F125" s="6" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="G125" s="6" t="s">
         <v>31</v>
       </c>
       <c r="H125" s="6" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="I125" s="16" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="J125" s="6"/>
     </row>
     <row r="126" spans="1:10">
       <c r="A126" s="6" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C126" s="30"/>
       <c r="D126" s="6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E126" s="6"/>
       <c r="F126" s="6"/>
       <c r="G126" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H126" s="6" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="I126" s="16" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="J126" s="6"/>
     </row>
     <row r="127" spans="1:10">
       <c r="A127" s="6" t="s">
+        <v>752</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>753</v>
+      </c>
+      <c r="C127" s="6" t="s">
         <v>754</v>
-      </c>
-      <c r="B127" s="6" t="s">
-        <v>755</v>
-      </c>
-      <c r="C127" s="6" t="s">
-        <v>756</v>
       </c>
       <c r="D127" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E127" s="6" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F127" s="15" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="G127" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H127" s="6"/>
       <c r="I127" s="6" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="J127" s="6" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="128" spans="1:10">
       <c r="A128" s="6" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="C128" s="6"/>
       <c r="D128" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E128" s="6"/>
       <c r="F128" s="15"/>
       <c r="G128" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H128" s="6" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="I128" s="16" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="J128" s="6"/>
     </row>
     <row r="129" spans="1:10">
       <c r="A129" s="8" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C129" s="8"/>
       <c r="D129" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E129" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F129" s="8" t="s">
+        <v>763</v>
+      </c>
+      <c r="G129" t="s">
+        <v>545</v>
+      </c>
+      <c r="H129" s="8" t="s">
+        <v>569</v>
+      </c>
+      <c r="I129" s="8" t="s">
+        <v>764</v>
+      </c>
+      <c r="J129" s="12" t="s">
         <v>765</v>
-      </c>
-      <c r="G129" t="s">
-        <v>546</v>
-      </c>
-      <c r="H129" s="8" t="s">
-        <v>570</v>
-      </c>
-      <c r="I129" s="8" t="s">
-        <v>766</v>
-      </c>
-      <c r="J129" s="12" t="s">
-        <v>767</v>
       </c>
     </row>
   </sheetData>
@@ -6783,12 +6780,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9cb1c2f4-2737-4134-a1af-8acbe3d02830" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6987,20 +6986,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9cb1c2f4-2737-4134-a1af-8acbe3d02830" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9cb1c2f4-2737-4134-a1af-8acbe3d02830"/>
+    <ds:schemaRef ds:uri="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7025,18 +7031,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9cb1c2f4-2737-4134-a1af-8acbe3d02830"/>
-    <ds:schemaRef ds:uri="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(repertoire-personnel): Ajout d'une photo
</commit_message>
<xml_diff>
--- a/content/personnel/liste-personnel.xlsx
+++ b/content/personnel/liste-personnel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projets\coquille-web\content\personnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC761E77-A8EF-4D15-88D9-E59C4ABBB4BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2736C18B-B9FB-4A04-A403-B01EDB133122}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="3180" windowWidth="33570" windowHeight="23450" tabRatio="149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1890" yWindow="3180" windowWidth="33570" windowHeight="23445" tabRatio="149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="795">
   <si>
     <t>nom</t>
   </si>
@@ -2427,6 +2427,12 @@
   </si>
   <si>
     <t>Bibliothèque d'aménagement;Bibliothèque Thérèse-Gouin-Décarie;Bibliothèque du campus de l'UdeM à Laval</t>
+  </si>
+  <si>
+    <t>Gestion des collections et numérisation</t>
+  </si>
+  <si>
+    <t>myriam-boyer</t>
   </si>
 </sst>
 </file>
@@ -3074,23 +3080,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G123" sqref="G123"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D134" sqref="D134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.453125" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="38.453125" customWidth="1"/>
-    <col min="4" max="4" width="28.1796875" customWidth="1"/>
-    <col min="5" max="5" width="83.453125" customWidth="1"/>
-    <col min="6" max="6" width="75.54296875" customWidth="1"/>
-    <col min="7" max="7" width="128.7265625" customWidth="1"/>
-    <col min="8" max="8" width="31.7265625" customWidth="1"/>
-    <col min="9" max="9" width="78.7265625" customWidth="1"/>
-    <col min="10" max="10" width="20.81640625" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="6" max="6" width="75.5703125" customWidth="1"/>
+    <col min="7" max="7" width="128.7109375" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" customWidth="1"/>
+    <col min="9" max="9" width="78.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3767,12 +3773,17 @@
       <c r="B24" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="C24" s="8"/>
+      <c r="C24" s="8" t="s">
+        <v>794</v>
+      </c>
       <c r="D24" s="8" t="s">
         <v>168</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>85</v>
+      </c>
+      <c r="F24" t="s">
+        <v>793</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>784</v>
@@ -4509,7 +4520,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" ht="30">
       <c r="A51" s="8" t="s">
         <v>333</v>
       </c>
@@ -5104,7 +5115,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" ht="30">
       <c r="A72" s="8" t="s">
         <v>457</v>
       </c>
@@ -5308,7 +5319,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="79" spans="1:10" s="4" customFormat="1">
+    <row r="79" spans="1:10" s="4" customFormat="1" ht="30">
       <c r="A79" s="6" t="s">
         <v>498</v>
       </c>
@@ -5809,7 +5820,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="97" spans="1:10" s="4" customFormat="1">
+    <row r="97" spans="1:10" s="4" customFormat="1" ht="30">
       <c r="A97" s="8" t="s">
         <v>602</v>
       </c>
@@ -6780,14 +6791,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9cb1c2f4-2737-4134-a1af-8acbe3d02830" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6986,27 +6995,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9cb1c2f4-2737-4134-a1af-8acbe3d02830" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9cb1c2f4-2737-4134-a1af-8acbe3d02830"/>
-    <ds:schemaRef ds:uri="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7031,9 +7033,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9cb1c2f4-2737-4134-a1af-8acbe3d02830"/>
+    <ds:schemaRef ds:uri="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(repertoire-personnel): Ajout d'une vingtaine de photos pour du personnel déjà dans le répertoire.
</commit_message>
<xml_diff>
--- a/content/personnel/liste-personnel.xlsx
+++ b/content/personnel/liste-personnel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udemontreal-my.sharepoint.com/personal/mathieu_nicolas_tardif_umontreal_ca/Documents/Bureau/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projets\coquille-web\content\personnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72C6E749-598E-4F18-AEA8-9B5B0A33115B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5DA5A0-0C4D-4454-9349-D442C5A6701D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4635" yWindow="4635" windowWidth="43200" windowHeight="23445" tabRatio="149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4640" yWindow="4640" windowWidth="43200" windowHeight="23450" tabRatio="149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="813">
   <si>
     <t>nom</t>
   </si>
@@ -1808,9 +1808,6 @@
     <t>France</t>
   </si>
   <si>
-    <t>France-nadeau.jpg</t>
-  </si>
-  <si>
     <t>514 343-6111, poste 3256</t>
   </si>
   <si>
@@ -2436,13 +2433,67 @@
   </si>
   <si>
     <t>caroline-patenaude.jpg</t>
+  </si>
+  <si>
+    <t>ann-mary-sotomayor.jpg</t>
+  </si>
+  <si>
+    <t>audrey-begin-poisson.jpg</t>
+  </si>
+  <si>
+    <t>benoit-mayrand.jpg</t>
+  </si>
+  <si>
+    <t>mathieu-murray-samuel.jpg</t>
+  </si>
+  <si>
+    <t>juliette-tirard-collet.jpg</t>
+  </si>
+  <si>
+    <t>chloe-sinotte.jpg</t>
+  </si>
+  <si>
+    <t>frederic-tremblay.jpg</t>
+  </si>
+  <si>
+    <t>delphine-cado.jpg</t>
+  </si>
+  <si>
+    <t>eve-baribeau-marchand.jpg</t>
+  </si>
+  <si>
+    <t>fanny-c-brochu.jpg</t>
+  </si>
+  <si>
+    <t>siv-kham-chao.jpg</t>
+  </si>
+  <si>
+    <t>france-nadeau.jpg</t>
+  </si>
+  <si>
+    <t>guylaine-brazeau.jpg</t>
+  </si>
+  <si>
+    <t>isabelle-giguere.jpg</t>
+  </si>
+  <si>
+    <t>karine-theriault-dube.jpg</t>
+  </si>
+  <si>
+    <t>marie-france-bernier.jpg</t>
+  </si>
+  <si>
+    <t>noemie-charest-bourbon.jpg</t>
+  </si>
+  <si>
+    <t>yan-vallee.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2738,7 +2789,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A0AF7E1-A614-44BF-8C48-5C26377DC552}" name="Tableau1" displayName="Tableau1" ref="A1:J129" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:J129" xr:uid="{4A0AF7E1-A614-44BF-8C48-5C26377DC552}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J129">
+  <sortState ref="A2:J129">
     <sortCondition ref="A1:A129"/>
   </sortState>
   <tableColumns count="10">
@@ -2758,9 +2809,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2798,9 +2849,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2833,9 +2884,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2868,9 +2936,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3047,25 +3132,25 @@
   <dimension ref="A1:J129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D97" sqref="D97"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1"/>
-    <col min="5" max="5" width="83.42578125" customWidth="1"/>
-    <col min="6" max="6" width="75.5703125" customWidth="1"/>
-    <col min="7" max="7" width="128.7109375" customWidth="1"/>
-    <col min="8" max="8" width="31.7109375" customWidth="1"/>
-    <col min="9" max="9" width="78.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="38.453125" customWidth="1"/>
+    <col min="4" max="4" width="28.1796875" customWidth="1"/>
+    <col min="5" max="5" width="83.453125" customWidth="1"/>
+    <col min="6" max="6" width="75.54296875" customWidth="1"/>
+    <col min="7" max="7" width="128.7265625" customWidth="1"/>
+    <col min="8" max="8" width="31.7265625" customWidth="1"/>
+    <col min="9" max="9" width="78.7265625" customWidth="1"/>
+    <col min="10" max="10" width="20.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3097,7 +3182,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
@@ -3127,7 +3212,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
@@ -3144,7 +3229,7 @@
         <v>46</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>22</v>
@@ -3159,7 +3244,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="6" t="s">
         <v>26</v>
       </c>
@@ -3189,7 +3274,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="8" t="s">
         <v>35</v>
       </c>
@@ -3219,7 +3304,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="6" t="s">
         <v>42</v>
       </c>
@@ -3239,7 +3324,7 @@
         <v>47</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>48</v>
@@ -3251,7 +3336,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="8" t="s">
         <v>51</v>
       </c>
@@ -3281,14 +3366,16 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B8" t="s">
-        <v>621</v>
-      </c>
-      <c r="C8" s="6"/>
+        <v>620</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>803</v>
+      </c>
       <c r="D8" t="s">
         <v>108</v>
       </c>
@@ -3296,19 +3383,19 @@
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="G8" t="s">
         <v>15</v>
       </c>
       <c r="H8" t="s">
+        <v>785</v>
+      </c>
+      <c r="I8" s="28" t="s">
         <v>786</v>
       </c>
-      <c r="I8" s="28" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -3337,7 +3424,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="6" t="s">
         <v>67</v>
       </c>
@@ -3364,7 +3451,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="8" t="s">
         <v>75</v>
       </c>
@@ -3381,10 +3468,10 @@
         <v>79</v>
       </c>
       <c r="F11" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>80</v>
@@ -3396,14 +3483,16 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="8" t="s">
         <v>83</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>796</v>
+      </c>
       <c r="D12" s="8" t="s">
         <v>84</v>
       </c>
@@ -3423,7 +3512,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="8" t="s">
         <v>90</v>
       </c>
@@ -3452,7 +3541,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="8" t="s">
         <v>99</v>
       </c>
@@ -3482,7 +3571,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="8" t="s">
         <v>106</v>
       </c>
@@ -3506,7 +3595,7 @@
       </c>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="6" t="s">
         <v>112</v>
       </c>
@@ -3534,14 +3623,16 @@
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>112</v>
       </c>
       <c r="B17" t="s">
         <v>118</v>
       </c>
-      <c r="C17" s="6"/>
+      <c r="C17" s="6" t="s">
+        <v>810</v>
+      </c>
       <c r="D17" t="s">
         <v>108</v>
       </c>
@@ -3558,7 +3649,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="6" t="s">
         <v>122</v>
       </c>
@@ -3588,7 +3679,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>129</v>
       </c>
@@ -3617,7 +3708,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="10" t="s">
         <v>136</v>
       </c>
@@ -3642,7 +3733,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="6" t="s">
         <v>142</v>
       </c>
@@ -3671,7 +3762,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="8" t="s">
         <v>151</v>
       </c>
@@ -3701,7 +3792,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="6" t="s">
         <v>159</v>
       </c>
@@ -3731,7 +3822,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="8" t="s">
         <v>166</v>
       </c>
@@ -3739,7 +3830,7 @@
         <v>167</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>168</v>
@@ -3748,10 +3839,10 @@
         <v>85</v>
       </c>
       <c r="F24" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>169</v>
@@ -3763,14 +3854,16 @@
         <v>171</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="8" t="s">
         <v>172</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="C25" s="8"/>
+      <c r="C25" s="8" t="s">
+        <v>807</v>
+      </c>
       <c r="D25" s="8" t="s">
         <v>54</v>
       </c>
@@ -3779,7 +3872,7 @@
         <v>174</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>175</v>
@@ -3791,7 +3884,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="8" t="s">
         <v>178</v>
       </c>
@@ -3818,13 +3911,16 @@
         <v>183</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>184</v>
       </c>
       <c r="B27" t="s">
         <v>185</v>
       </c>
+      <c r="C27" t="s">
+        <v>804</v>
+      </c>
       <c r="D27" t="s">
         <v>108</v>
       </c>
@@ -3841,14 +3937,16 @@
         <v>188</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="6" t="s">
         <v>189</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="C28" s="6"/>
+      <c r="C28" s="6" t="s">
+        <v>802</v>
+      </c>
       <c r="D28" s="6" t="s">
         <v>191</v>
       </c>
@@ -3869,14 +3967,16 @@
         <v>196</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="6" t="s">
         <v>197</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="C29" s="6"/>
+      <c r="C29" s="6" t="s">
+        <v>805</v>
+      </c>
       <c r="D29" s="6" t="s">
         <v>54</v>
       </c>
@@ -3897,7 +3997,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="6" t="s">
         <v>204</v>
       </c>
@@ -3927,13 +4027,16 @@
         <v>210</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>211</v>
       </c>
       <c r="B31" t="s">
         <v>212</v>
       </c>
+      <c r="C31" t="s">
+        <v>811</v>
+      </c>
       <c r="D31" t="s">
         <v>29</v>
       </c>
@@ -3944,7 +4047,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>213</v>
       </c>
@@ -3955,7 +4058,7 @@
         <v>54</v>
       </c>
       <c r="G32" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="H32" s="8" t="s">
         <v>215</v>
@@ -3967,7 +4070,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="6" t="s">
         <v>218</v>
       </c>
@@ -3986,7 +4089,7 @@
       <c r="I33" s="13"/>
       <c r="J33" s="20"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="8" t="s">
         <v>221</v>
       </c>
@@ -4016,7 +4119,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="6" t="s">
         <v>228</v>
       </c>
@@ -4045,7 +4148,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="6" t="s">
         <v>236</v>
       </c>
@@ -4075,7 +4178,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="8" t="s">
         <v>243</v>
       </c>
@@ -4105,7 +4208,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="6" t="s">
         <v>250</v>
       </c>
@@ -4125,7 +4228,7 @@
         <v>255</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>256</v>
@@ -4137,7 +4240,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="8" t="s">
         <v>259</v>
       </c>
@@ -4167,7 +4270,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="6" t="s">
         <v>266</v>
       </c>
@@ -4197,7 +4300,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="6" t="s">
         <v>273</v>
       </c>
@@ -4227,7 +4330,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="8" t="s">
         <v>280</v>
       </c>
@@ -4257,7 +4360,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="8" t="s">
         <v>289</v>
       </c>
@@ -4275,7 +4378,7 @@
         <v>292</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="H43" s="8" t="s">
         <v>293</v>
@@ -4287,7 +4390,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="8" t="s">
         <v>296</v>
       </c>
@@ -4317,7 +4420,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="6" t="s">
         <v>303</v>
       </c>
@@ -4343,7 +4446,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
         <v>310</v>
       </c>
@@ -4351,7 +4454,7 @@
         <v>311</v>
       </c>
       <c r="C46" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D46" t="s">
         <v>108</v>
@@ -4369,7 +4472,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="6" t="s">
         <v>315</v>
       </c>
@@ -4399,7 +4502,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" t="s">
         <v>322</v>
       </c>
@@ -4423,7 +4526,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="8" t="s">
         <v>327</v>
       </c>
@@ -4455,7 +4558,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="8" t="s">
         <v>327</v>
       </c>
@@ -4466,7 +4569,7 @@
         <v>329</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>146</v>
@@ -4485,7 +4588,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="8" t="s">
         <v>333</v>
       </c>
@@ -4517,7 +4620,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="8" t="s">
         <v>340</v>
       </c>
@@ -4545,7 +4648,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="8" t="s">
         <v>347</v>
       </c>
@@ -4575,7 +4678,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="6" t="s">
         <v>354</v>
       </c>
@@ -4601,7 +4704,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="8" t="s">
         <v>360</v>
       </c>
@@ -4631,7 +4734,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="6" t="s">
         <v>368</v>
       </c>
@@ -4656,7 +4759,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="6" t="s">
         <v>368</v>
       </c>
@@ -4683,7 +4786,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="8" t="s">
         <v>377</v>
       </c>
@@ -4712,7 +4815,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="6" t="s">
         <v>384</v>
       </c>
@@ -4720,7 +4823,7 @@
         <v>385</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>13</v>
@@ -4742,7 +4845,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="6" t="s">
         <v>390</v>
       </c>
@@ -4761,7 +4864,7 @@
         <v>392</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I60" s="16" t="s">
         <v>393</v>
@@ -4770,14 +4873,16 @@
         <v>394</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="6" t="s">
         <v>395</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="C61" s="6"/>
+      <c r="C61" s="6" t="s">
+        <v>808</v>
+      </c>
       <c r="D61" s="6" t="s">
         <v>29</v>
       </c>
@@ -4796,7 +4901,7 @@
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="6" t="s">
         <v>400</v>
       </c>
@@ -4826,7 +4931,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="8" t="s">
         <v>406</v>
       </c>
@@ -4856,7 +4961,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="64" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" s="4" customFormat="1">
       <c r="A64" t="s">
         <v>413</v>
       </c>
@@ -4886,7 +4991,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="6" t="s">
         <v>420</v>
       </c>
@@ -4914,7 +5019,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="66" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" s="5" customFormat="1">
       <c r="A66" s="6" t="s">
         <v>426</v>
       </c>
@@ -4944,7 +5049,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" t="s">
         <v>433</v>
       </c>
@@ -4967,7 +5072,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="8" t="s">
         <v>438</v>
       </c>
@@ -4989,13 +5094,13 @@
         <v>439</v>
       </c>
       <c r="I68" s="12" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="J68" s="17" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" t="s">
         <v>440</v>
       </c>
@@ -5018,7 +5123,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="8" t="s">
         <v>444</v>
       </c>
@@ -5038,7 +5143,7 @@
         <v>447</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="H70" s="8" t="s">
         <v>448</v>
@@ -5050,7 +5155,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="6" t="s">
         <v>451</v>
       </c>
@@ -5061,7 +5166,7 @@
         <v>453</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>146</v>
@@ -5082,7 +5187,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="8" t="s">
         <v>457</v>
       </c>
@@ -5090,7 +5195,7 @@
         <v>369</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="D72" s="8" t="s">
         <v>45</v>
@@ -5114,7 +5219,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" t="s">
         <v>462</v>
       </c>
@@ -5122,7 +5227,7 @@
         <v>463</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D73" t="s">
         <v>108</v>
@@ -5140,7 +5245,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="8" t="s">
         <v>467</v>
       </c>
@@ -5170,7 +5275,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="75" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" s="4" customFormat="1">
       <c r="A75" t="s">
         <v>474</v>
       </c>
@@ -5196,7 +5301,7 @@
       </c>
       <c r="J75"/>
     </row>
-    <row r="76" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" s="4" customFormat="1">
       <c r="A76" s="8" t="s">
         <v>479</v>
       </c>
@@ -5225,7 +5330,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="6" t="s">
         <v>485</v>
       </c>
@@ -5245,7 +5350,7 @@
         <v>488</v>
       </c>
       <c r="G77" s="8" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="H77" s="6" t="s">
         <v>489</v>
@@ -5257,7 +5362,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="8" t="s">
         <v>492</v>
       </c>
@@ -5286,7 +5391,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="79" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" s="4" customFormat="1">
       <c r="A79" s="6" t="s">
         <v>498</v>
       </c>
@@ -5316,7 +5421,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="6" t="s">
         <v>504</v>
       </c>
@@ -5339,7 +5444,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="10" t="s">
         <v>504</v>
       </c>
@@ -5354,10 +5459,10 @@
         <v>46</v>
       </c>
       <c r="F81" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="G81" s="10" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H81" s="10" t="s">
         <v>506</v>
@@ -5369,7 +5474,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="6" t="s">
         <v>512</v>
       </c>
@@ -5393,7 +5498,7 @@
       </c>
       <c r="J82" s="6"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="6" t="s">
         <v>517</v>
       </c>
@@ -5417,7 +5522,7 @@
       </c>
       <c r="J83" s="6"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="6" t="s">
         <v>522</v>
       </c>
@@ -5445,7 +5550,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="6" t="s">
         <v>529</v>
       </c>
@@ -5475,7 +5580,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="6" t="s">
         <v>535</v>
       </c>
@@ -5505,7 +5610,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="6" t="s">
         <v>542</v>
       </c>
@@ -5534,14 +5639,16 @@
         <v>548</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="6" t="s">
         <v>549</v>
       </c>
       <c r="B88" s="6" t="s">
         <v>550</v>
       </c>
-      <c r="C88" s="6"/>
+      <c r="C88" s="6" t="s">
+        <v>797</v>
+      </c>
       <c r="D88" s="6" t="s">
         <v>514</v>
       </c>
@@ -5558,7 +5665,7 @@
       </c>
       <c r="J88" s="6"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="6" t="s">
         <v>553</v>
       </c>
@@ -5588,7 +5695,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="14" t="s">
         <v>560</v>
       </c>
@@ -5618,7 +5725,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="8" t="s">
         <v>566</v>
       </c>
@@ -5648,7 +5755,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="8" t="s">
         <v>572</v>
       </c>
@@ -5678,14 +5785,16 @@
         <v>578</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" t="s">
         <v>579</v>
       </c>
       <c r="B93" t="s">
         <v>580</v>
       </c>
-      <c r="C93" s="6"/>
+      <c r="C93" s="6" t="s">
+        <v>798</v>
+      </c>
       <c r="D93" s="8" t="s">
         <v>29</v>
       </c>
@@ -5703,7 +5812,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="14" t="s">
         <v>584</v>
       </c>
@@ -5711,7 +5820,7 @@
         <v>585</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>586</v>
+        <v>806</v>
       </c>
       <c r="D94" s="14" t="s">
         <v>283</v>
@@ -5721,52 +5830,52 @@
       </c>
       <c r="F94" s="7"/>
       <c r="G94" s="14" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="H94" s="14" t="s">
+        <v>586</v>
+      </c>
+      <c r="I94" s="14" t="s">
         <v>587</v>
       </c>
-      <c r="I94" s="14" t="s">
+      <c r="J94" s="14" t="s">
         <v>588</v>
       </c>
-      <c r="J94" s="14" t="s">
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95" s="8" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="8" t="s">
+      <c r="B95" s="8" t="s">
         <v>590</v>
-      </c>
-      <c r="B95" s="8" t="s">
-        <v>591</v>
       </c>
       <c r="C95" s="8"/>
       <c r="D95" s="8" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E95" s="8"/>
       <c r="F95" s="8" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G95" s="8" t="s">
         <v>70</v>
       </c>
       <c r="H95" s="8" t="s">
+        <v>593</v>
+      </c>
+      <c r="I95" s="8" t="s">
         <v>594</v>
       </c>
-      <c r="I95" s="8" t="s">
+      <c r="J95" s="8" t="s">
         <v>595</v>
       </c>
-      <c r="J95" s="8" t="s">
+    </row>
+    <row r="96" spans="1:10" s="4" customFormat="1">
+      <c r="A96" s="8" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="8" t="s">
+      <c r="B96" s="8" t="s">
         <v>597</v>
-      </c>
-      <c r="B96" s="8" t="s">
-        <v>598</v>
       </c>
       <c r="C96" s="8"/>
       <c r="D96" s="8" t="s">
@@ -5778,24 +5887,24 @@
       <c r="F96" s="8"/>
       <c r="G96"/>
       <c r="H96" s="8" t="s">
+        <v>598</v>
+      </c>
+      <c r="I96" s="8" t="s">
         <v>599</v>
       </c>
-      <c r="I96" s="8" t="s">
+      <c r="J96" s="8" t="s">
         <v>600</v>
       </c>
-      <c r="J96" s="8" t="s">
+    </row>
+    <row r="97" spans="1:10" s="4" customFormat="1">
+      <c r="A97" s="8" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A97" s="8" t="s">
+      <c r="B97" s="8" t="s">
         <v>602</v>
       </c>
-      <c r="B97" s="8" t="s">
-        <v>603</v>
-      </c>
       <c r="C97" s="8" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>45</v>
@@ -5804,56 +5913,56 @@
         <v>336</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="G97" s="8" t="s">
         <v>31</v>
       </c>
       <c r="H97" s="8" t="s">
+        <v>604</v>
+      </c>
+      <c r="I97" s="8" t="s">
         <v>605</v>
       </c>
-      <c r="I97" s="8" t="s">
+      <c r="J97" s="17" t="s">
         <v>606</v>
       </c>
-      <c r="J97" s="17" t="s">
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98" s="8" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" s="8" t="s">
+      <c r="B98" s="8" t="s">
         <v>608</v>
-      </c>
-      <c r="B98" s="8" t="s">
-        <v>609</v>
       </c>
       <c r="C98" s="8"/>
       <c r="D98" s="8" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E98" s="6"/>
       <c r="F98" s="27" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G98" s="8" t="s">
         <v>284</v>
       </c>
       <c r="H98" s="8"/>
       <c r="I98" s="17" t="s">
+        <v>611</v>
+      </c>
+      <c r="J98" s="18" t="s">
         <v>612</v>
       </c>
-      <c r="J98" s="18" t="s">
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="B99" t="s">
         <v>614</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" s="25" t="s">
         <v>615</v>
-      </c>
-      <c r="C99" s="25" t="s">
-        <v>616</v>
       </c>
       <c r="D99" t="s">
         <v>29</v>
@@ -5862,27 +5971,27 @@
         <v>94</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="G99" t="s">
         <v>115</v>
       </c>
       <c r="I99" t="s">
+        <v>617</v>
+      </c>
+      <c r="J99" t="s">
         <v>618</v>
       </c>
-      <c r="J99" t="s">
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" s="6" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" s="6" t="s">
+      <c r="B100" s="6" t="s">
         <v>620</v>
       </c>
-      <c r="B100" s="6" t="s">
+      <c r="C100" s="6" t="s">
         <v>621</v>
-      </c>
-      <c r="C100" s="6" t="s">
-        <v>622</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>125</v>
@@ -5891,90 +6000,90 @@
         <v>94</v>
       </c>
       <c r="F100" s="15" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G100" t="s">
         <v>115</v>
       </c>
       <c r="H100" s="14" t="s">
+        <v>623</v>
+      </c>
+      <c r="I100" s="14" t="s">
         <v>624</v>
       </c>
-      <c r="I100" s="14" t="s">
+      <c r="J100" s="14" t="s">
         <v>625</v>
       </c>
-      <c r="J100" s="14" t="s">
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" s="6" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" s="6" t="s">
+      <c r="B101" s="6" t="s">
         <v>627</v>
       </c>
-      <c r="B101" s="6" t="s">
-        <v>628</v>
-      </c>
       <c r="C101" s="6" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D101" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E101" s="6"/>
       <c r="F101" s="6" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="G101" s="6" t="s">
         <v>31</v>
       </c>
       <c r="H101" s="14" t="s">
+        <v>629</v>
+      </c>
+      <c r="I101" s="14" t="s">
         <v>630</v>
       </c>
-      <c r="I101" s="14" t="s">
+      <c r="J101" s="14" t="s">
         <v>631</v>
       </c>
-      <c r="J101" s="14" t="s">
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102" s="8" t="s">
+        <v>626</v>
+      </c>
+      <c r="B102" s="8" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" s="8" t="s">
-        <v>627</v>
-      </c>
-      <c r="B102" s="8" t="s">
+      <c r="C102" s="8" t="s">
         <v>633</v>
-      </c>
-      <c r="C102" s="8" t="s">
-        <v>634</v>
       </c>
       <c r="D102" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E102" s="8"/>
       <c r="F102" s="8" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G102" s="8" t="s">
         <v>31</v>
       </c>
       <c r="H102" s="10" t="s">
+        <v>635</v>
+      </c>
+      <c r="I102" s="10" t="s">
         <v>636</v>
       </c>
-      <c r="I102" s="10" t="s">
+      <c r="J102" s="10" t="s">
         <v>637</v>
       </c>
-      <c r="J102" s="10" t="s">
+    </row>
+    <row r="103" spans="1:10" s="5" customFormat="1">
+      <c r="A103" s="6" t="s">
         <v>638</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="6" t="s">
-        <v>639</v>
       </c>
       <c r="B103" s="6" t="s">
         <v>369</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>13</v>
@@ -5987,24 +6096,24 @@
         <v>109</v>
       </c>
       <c r="H103" s="14" t="s">
+        <v>640</v>
+      </c>
+      <c r="I103" s="14" t="s">
         <v>641</v>
       </c>
-      <c r="I103" s="14" t="s">
+      <c r="J103" s="14" t="s">
         <v>642</v>
       </c>
-      <c r="J103" s="14" t="s">
+    </row>
+    <row r="104" spans="1:10" s="5" customFormat="1">
+      <c r="A104" s="6" t="s">
         <v>643</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="6" t="s">
-        <v>644</v>
       </c>
       <c r="B104" s="6" t="s">
         <v>580</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>29</v>
@@ -6013,52 +6122,52 @@
         <v>94</v>
       </c>
       <c r="F104" s="15" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="H104" s="14"/>
       <c r="I104" s="13" t="s">
+        <v>646</v>
+      </c>
+      <c r="J104" s="14" t="s">
         <v>647</v>
       </c>
-      <c r="J104" s="14" t="s">
+    </row>
+    <row r="105" spans="1:10">
+      <c r="A105" s="8" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A105" s="8" t="s">
+      <c r="B105" s="8" t="s">
         <v>649</v>
       </c>
-      <c r="B105" s="8" t="s">
+      <c r="C105" s="8" t="s">
         <v>650</v>
-      </c>
-      <c r="C105" s="8" t="s">
-        <v>651</v>
       </c>
       <c r="D105" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E105" s="8"/>
       <c r="F105" s="11" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G105" s="8" t="s">
         <v>392</v>
       </c>
       <c r="H105" s="10" t="s">
+        <v>652</v>
+      </c>
+      <c r="I105" s="10" t="s">
         <v>653</v>
       </c>
-      <c r="I105" s="10" t="s">
+      <c r="J105" s="10" t="s">
         <v>654</v>
       </c>
-      <c r="J105" s="10" t="s">
+    </row>
+    <row r="106" spans="1:10">
+      <c r="A106" s="8" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="8" t="s">
+      <c r="B106" s="8" t="s">
         <v>656</v>
-      </c>
-      <c r="B106" s="8" t="s">
-        <v>657</v>
       </c>
       <c r="C106" s="6"/>
       <c r="D106" s="8" t="s">
@@ -6070,42 +6179,42 @@
         <v>22</v>
       </c>
       <c r="H106" s="10" t="s">
+        <v>657</v>
+      </c>
+      <c r="I106" s="17" t="s">
         <v>658</v>
       </c>
-      <c r="I106" s="17" t="s">
+      <c r="J106" s="10"/>
+    </row>
+    <row r="107" spans="1:10">
+      <c r="A107" t="s">
         <v>659</v>
       </c>
-      <c r="J106" s="10"/>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="B107" t="s">
         <v>660</v>
-      </c>
-      <c r="B107" t="s">
-        <v>661</v>
       </c>
       <c r="D107" t="s">
         <v>514</v>
       </c>
       <c r="G107" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="H107" s="8" t="s">
+        <v>661</v>
+      </c>
+      <c r="I107" s="18" t="s">
         <v>662</v>
       </c>
-      <c r="I107" s="18" t="s">
+      <c r="J107" s="17" t="s">
         <v>663</v>
       </c>
-      <c r="J107" s="17" t="s">
+    </row>
+    <row r="108" spans="1:10">
+      <c r="A108" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="B108" t="s">
         <v>665</v>
-      </c>
-      <c r="B108" t="s">
-        <v>666</v>
       </c>
       <c r="D108" t="s">
         <v>108</v>
@@ -6114,53 +6223,53 @@
         <v>31</v>
       </c>
       <c r="H108" t="s">
+        <v>666</v>
+      </c>
+      <c r="I108" s="18" t="s">
         <v>667</v>
       </c>
-      <c r="I108" s="18" t="s">
+      <c r="J108" s="19" t="s">
         <v>668</v>
       </c>
-      <c r="J108" s="19" t="s">
+    </row>
+    <row r="109" spans="1:10">
+      <c r="A109" t="s">
         <v>669</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>670</v>
       </c>
       <c r="B109" t="s">
         <v>60</v>
       </c>
       <c r="C109" s="25" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="D109" t="s">
         <v>13</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G109" t="s">
         <v>31</v>
       </c>
       <c r="H109" s="4" t="s">
+        <v>672</v>
+      </c>
+      <c r="I109" s="4" t="s">
         <v>673</v>
       </c>
-      <c r="I109" s="4" t="s">
+      <c r="J109" s="4" t="s">
         <v>674</v>
       </c>
-      <c r="J109" s="4" t="s">
+    </row>
+    <row r="110" spans="1:10">
+      <c r="A110" s="6" t="s">
         <v>675</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A110" s="6" t="s">
-        <v>676</v>
       </c>
       <c r="B110" s="6" t="s">
         <v>522</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>145</v>
@@ -6173,44 +6282,49 @@
         <v>139</v>
       </c>
       <c r="I110" s="14" t="s">
+        <v>677</v>
+      </c>
+      <c r="J110" s="14" t="s">
         <v>678</v>
       </c>
-      <c r="J110" s="14" t="s">
+    </row>
+    <row r="111" spans="1:10">
+      <c r="A111" s="6" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" s="6" t="s">
+      <c r="B111" s="6" t="s">
         <v>680</v>
       </c>
-      <c r="B111" s="6" t="s">
-        <v>681</v>
-      </c>
-      <c r="C111" s="6"/>
+      <c r="C111" s="6" t="s">
+        <v>800</v>
+      </c>
       <c r="D111" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E111" s="6"/>
       <c r="F111" s="15" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="G111" s="6" t="s">
         <v>193</v>
       </c>
       <c r="H111" s="14"/>
       <c r="I111" s="14" t="s">
+        <v>682</v>
+      </c>
+      <c r="J111" s="14" t="s">
         <v>683</v>
       </c>
-      <c r="J111" s="14" t="s">
+    </row>
+    <row r="112" spans="1:10">
+      <c r="A112" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="B112" t="s">
         <v>685</v>
       </c>
-      <c r="B112" t="s">
-        <v>686</v>
+      <c r="C112" t="s">
+        <v>795</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>305</v>
@@ -6221,39 +6335,39 @@
         <v>31</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10">
       <c r="A113" s="10" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B113" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D113" s="10" t="s">
         <v>29</v>
       </c>
       <c r="E113" s="10"/>
       <c r="F113" s="10" t="s">
+        <v>688</v>
+      </c>
+      <c r="G113" s="10" t="s">
         <v>689</v>
       </c>
-      <c r="G113" s="10" t="s">
+      <c r="H113" s="10" t="s">
         <v>690</v>
       </c>
-      <c r="H113" s="10" t="s">
+      <c r="I113" s="10" t="s">
         <v>691</v>
       </c>
-      <c r="I113" s="10" t="s">
+      <c r="J113" s="10" t="s">
         <v>692</v>
       </c>
-      <c r="J113" s="10" t="s">
+    </row>
+    <row r="114" spans="1:10">
+      <c r="A114" s="10" t="s">
         <v>693</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114" s="10" t="s">
-        <v>694</v>
       </c>
       <c r="B114" s="10" t="s">
         <v>304</v>
@@ -6268,24 +6382,24 @@
       <c r="F114" s="10"/>
       <c r="G114" s="10"/>
       <c r="H114" s="10" t="s">
+        <v>694</v>
+      </c>
+      <c r="I114" s="10" t="s">
         <v>695</v>
       </c>
-      <c r="I114" s="10" t="s">
+      <c r="J114" s="10" t="s">
         <v>696</v>
       </c>
-      <c r="J114" s="10" t="s">
+    </row>
+    <row r="115" spans="1:10">
+      <c r="A115" s="6" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" s="6" t="s">
+      <c r="B115" s="6" t="s">
         <v>698</v>
       </c>
-      <c r="B115" s="6" t="s">
+      <c r="C115" s="6" t="s">
         <v>699</v>
-      </c>
-      <c r="C115" s="6" t="s">
-        <v>700</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>93</v>
@@ -6297,23 +6411,25 @@
         <v>398</v>
       </c>
       <c r="H115" s="6" t="s">
+        <v>700</v>
+      </c>
+      <c r="I115" s="6" t="s">
         <v>701</v>
       </c>
-      <c r="I115" s="6" t="s">
+      <c r="J115" s="6" t="s">
         <v>702</v>
       </c>
-      <c r="J115" s="6" t="s">
+    </row>
+    <row r="116" spans="1:10">
+      <c r="A116" s="6" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" s="6" t="s">
+      <c r="B116" s="6" t="s">
         <v>704</v>
       </c>
-      <c r="B116" s="6" t="s">
-        <v>705</v>
-      </c>
-      <c r="C116" s="26"/>
+      <c r="C116" s="26" t="s">
+        <v>809</v>
+      </c>
       <c r="D116" s="6" t="s">
         <v>108</v>
       </c>
@@ -6324,51 +6440,51 @@
       </c>
       <c r="H116" s="6"/>
       <c r="I116" s="16" t="s">
+        <v>705</v>
+      </c>
+      <c r="J116" s="6"/>
+    </row>
+    <row r="117" spans="1:10">
+      <c r="A117" s="14" t="s">
         <v>706</v>
       </c>
-      <c r="J116" s="6"/>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A117" s="14" t="s">
+      <c r="B117" s="14" t="s">
         <v>707</v>
       </c>
-      <c r="B117" s="14" t="s">
+      <c r="C117" s="26" t="s">
         <v>708</v>
-      </c>
-      <c r="C117" s="26" t="s">
-        <v>709</v>
       </c>
       <c r="D117" s="14" t="s">
         <v>342</v>
       </c>
       <c r="E117" t="s">
+        <v>709</v>
+      </c>
+      <c r="F117" s="14" t="s">
         <v>710</v>
       </c>
-      <c r="F117" s="14" t="s">
+      <c r="G117" s="14" t="s">
+        <v>788</v>
+      </c>
+      <c r="H117" s="14" t="s">
         <v>711</v>
       </c>
-      <c r="G117" s="14" t="s">
-        <v>789</v>
-      </c>
-      <c r="H117" s="14" t="s">
+      <c r="I117" s="14" t="s">
         <v>712</v>
       </c>
-      <c r="I117" s="14" t="s">
+      <c r="J117" s="14" t="s">
         <v>713</v>
       </c>
-      <c r="J117" s="14" t="s">
+    </row>
+    <row r="118" spans="1:10">
+      <c r="A118" s="8" t="s">
         <v>714</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A118" s="8" t="s">
-        <v>715</v>
       </c>
       <c r="B118" s="8" t="s">
         <v>580</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D118" s="8" t="s">
         <v>29</v>
@@ -6381,21 +6497,21 @@
         <v>155</v>
       </c>
       <c r="H118" s="8" t="s">
+        <v>716</v>
+      </c>
+      <c r="I118" s="8" t="s">
         <v>717</v>
       </c>
-      <c r="I118" s="8" t="s">
+      <c r="J118" s="8" t="s">
         <v>718</v>
       </c>
-      <c r="J118" s="8" t="s">
+    </row>
+    <row r="119" spans="1:10">
+      <c r="A119" s="8" t="s">
         <v>719</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A119" s="8" t="s">
+      <c r="B119" s="8" t="s">
         <v>720</v>
-      </c>
-      <c r="B119" s="8" t="s">
-        <v>721</v>
       </c>
       <c r="C119" s="8"/>
       <c r="D119" s="8" t="s">
@@ -6407,49 +6523,53 @@
         <v>538</v>
       </c>
       <c r="H119" t="s">
+        <v>721</v>
+      </c>
+      <c r="I119" s="17" t="s">
         <v>722</v>
       </c>
-      <c r="I119" s="17" t="s">
+      <c r="J119" s="8"/>
+    </row>
+    <row r="120" spans="1:10">
+      <c r="A120" s="6" t="s">
         <v>723</v>
       </c>
-      <c r="J119" s="8"/>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A120" s="6" t="s">
+      <c r="B120" s="6" t="s">
         <v>724</v>
       </c>
-      <c r="B120" s="6" t="s">
-        <v>725</v>
-      </c>
-      <c r="C120" s="6"/>
+      <c r="C120" s="6" t="s">
+        <v>799</v>
+      </c>
       <c r="D120" s="6" t="s">
         <v>125</v>
       </c>
       <c r="E120" s="6"/>
       <c r="F120" s="15" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="G120" s="6" t="s">
         <v>284</v>
       </c>
       <c r="H120" s="6" t="s">
+        <v>726</v>
+      </c>
+      <c r="I120" s="6" t="s">
         <v>727</v>
       </c>
-      <c r="I120" s="6" t="s">
+      <c r="J120" s="6" t="s">
         <v>728</v>
       </c>
-      <c r="J120" s="6" t="s">
+    </row>
+    <row r="121" spans="1:10">
+      <c r="A121" s="6" t="s">
         <v>729</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A121" s="6" t="s">
+      <c r="B121" s="6" t="s">
         <v>730</v>
       </c>
-      <c r="B121" s="6" t="s">
-        <v>731</v>
-      </c>
-      <c r="C121" s="6"/>
+      <c r="C121" s="6" t="s">
+        <v>801</v>
+      </c>
       <c r="D121" s="6" t="s">
         <v>514</v>
       </c>
@@ -6462,42 +6582,42 @@
         <v>520</v>
       </c>
       <c r="I121" s="16" t="s">
+        <v>731</v>
+      </c>
+      <c r="J121" s="6"/>
+    </row>
+    <row r="122" spans="1:10">
+      <c r="A122" t="s">
+        <v>729</v>
+      </c>
+      <c r="B122" t="s">
         <v>732</v>
-      </c>
-      <c r="J121" s="6"/>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>730</v>
-      </c>
-      <c r="B122" t="s">
-        <v>733</v>
       </c>
       <c r="D122" t="s">
         <v>54</v>
       </c>
       <c r="F122" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="G122" t="s">
         <v>364</v>
       </c>
       <c r="H122" s="8" t="s">
+        <v>734</v>
+      </c>
+      <c r="I122" s="18" t="s">
         <v>735</v>
       </c>
-      <c r="I122" s="18" t="s">
+      <c r="J122" s="17" t="s">
         <v>736</v>
       </c>
-      <c r="J122" s="17" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:10">
       <c r="A123" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="B123" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C123" s="6"/>
       <c r="D123" t="s">
@@ -6507,24 +6627,24 @@
         <v>46</v>
       </c>
       <c r="F123" t="s">
+        <v>771</v>
+      </c>
+      <c r="G123" t="s">
+        <v>790</v>
+      </c>
+      <c r="H123" t="s">
         <v>772</v>
       </c>
-      <c r="G123" t="s">
-        <v>791</v>
-      </c>
-      <c r="H123" t="s">
+      <c r="I123" s="28" t="s">
         <v>773</v>
       </c>
-      <c r="I123" s="28" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:10">
       <c r="A124" s="6" t="s">
+        <v>737</v>
+      </c>
+      <c r="B124" s="6" t="s">
         <v>738</v>
-      </c>
-      <c r="B124" s="6" t="s">
-        <v>739</v>
       </c>
       <c r="C124" s="6"/>
       <c r="D124" s="6" t="s">
@@ -6536,49 +6656,51 @@
         <v>63</v>
       </c>
       <c r="H124" s="6" t="s">
+        <v>739</v>
+      </c>
+      <c r="I124" s="16" t="s">
         <v>740</v>
       </c>
-      <c r="I124" s="16" t="s">
+      <c r="J124" s="6"/>
+    </row>
+    <row r="125" spans="1:10">
+      <c r="A125" s="6" t="s">
         <v>741</v>
       </c>
-      <c r="J124" s="6"/>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A125" s="6" t="s">
+      <c r="B125" s="6" t="s">
         <v>742</v>
       </c>
-      <c r="B125" s="6" t="s">
-        <v>743</v>
-      </c>
       <c r="C125" s="26" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="D125" s="6" t="s">
         <v>108</v>
       </c>
       <c r="E125" s="6"/>
       <c r="F125" s="6" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="G125" s="6" t="s">
         <v>31</v>
       </c>
       <c r="H125" s="6" t="s">
+        <v>744</v>
+      </c>
+      <c r="I125" s="16" t="s">
         <v>745</v>
       </c>
-      <c r="I125" s="16" t="s">
+      <c r="J125" s="6"/>
+    </row>
+    <row r="126" spans="1:10">
+      <c r="A126" s="6" t="s">
         <v>746</v>
       </c>
-      <c r="J125" s="6"/>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A126" s="6" t="s">
+      <c r="B126" s="6" t="s">
         <v>747</v>
       </c>
-      <c r="B126" s="6" t="s">
-        <v>748</v>
-      </c>
-      <c r="C126" s="6"/>
+      <c r="C126" s="6" t="s">
+        <v>812</v>
+      </c>
       <c r="D126" s="6" t="s">
         <v>514</v>
       </c>
@@ -6588,49 +6710,49 @@
         <v>63</v>
       </c>
       <c r="H126" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="I126" s="16" t="s">
         <v>749</v>
       </c>
-      <c r="I126" s="16" t="s">
+      <c r="J126" s="6"/>
+    </row>
+    <row r="127" spans="1:10">
+      <c r="A127" s="6" t="s">
         <v>750</v>
       </c>
-      <c r="J126" s="6"/>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A127" s="6" t="s">
+      <c r="B127" s="6" t="s">
         <v>751</v>
       </c>
-      <c r="B127" s="6" t="s">
+      <c r="C127" s="6" t="s">
         <v>752</v>
-      </c>
-      <c r="C127" s="6" t="s">
-        <v>753</v>
       </c>
       <c r="D127" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E127" s="6" t="s">
+        <v>753</v>
+      </c>
+      <c r="F127" s="15" t="s">
         <v>754</v>
-      </c>
-      <c r="F127" s="15" t="s">
-        <v>755</v>
       </c>
       <c r="G127" t="s">
         <v>115</v>
       </c>
       <c r="H127" s="6"/>
       <c r="I127" s="6" t="s">
+        <v>755</v>
+      </c>
+      <c r="J127" s="6" t="s">
         <v>756</v>
       </c>
-      <c r="J127" s="6" t="s">
+    </row>
+    <row r="128" spans="1:10">
+      <c r="A128" s="6" t="s">
         <v>757</v>
       </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A128" s="6" t="s">
-        <v>758</v>
-      </c>
       <c r="B128" s="6" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C128" s="6"/>
       <c r="D128" s="6" t="s">
@@ -6642,16 +6764,16 @@
         <v>109</v>
       </c>
       <c r="H128" s="6" t="s">
+        <v>758</v>
+      </c>
+      <c r="I128" s="16" t="s">
         <v>759</v>
       </c>
-      <c r="I128" s="16" t="s">
+      <c r="J128" s="6"/>
+    </row>
+    <row r="129" spans="1:10">
+      <c r="A129" s="8" t="s">
         <v>760</v>
-      </c>
-      <c r="J128" s="6"/>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A129" s="8" t="s">
-        <v>761</v>
       </c>
       <c r="B129" s="8" t="s">
         <v>274</v>
@@ -6664,7 +6786,7 @@
         <v>85</v>
       </c>
       <c r="F129" s="8" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="G129" t="s">
         <v>545</v>
@@ -6673,10 +6795,10 @@
         <v>569</v>
       </c>
       <c r="I129" s="8" t="s">
+        <v>762</v>
+      </c>
+      <c r="J129" s="12" t="s">
         <v>763</v>
-      </c>
-      <c r="J129" s="12" t="s">
-        <v>764</v>
       </c>
     </row>
   </sheetData>
@@ -6758,12 +6880,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9cb1c2f4-2737-4134-a1af-8acbe3d02830" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6962,20 +7086,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9cb1c2f4-2737-4134-a1af-8acbe3d02830" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9cb1c2f4-2737-4134-a1af-8acbe3d02830"/>
+    <ds:schemaRef ds:uri="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7000,18 +7131,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBEF5B7A-066E-4CFA-AECB-2B495BA6263D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747C807-31DC-4949-A88C-18B7D05A7D8F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9cb1c2f4-2737-4134-a1af-8acbe3d02830"/>
-    <ds:schemaRef ds:uri="7c5d7804-4d0b-4e60-9ce8-4dcaa1999ed1"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>